<commit_message>
[24.06.07 17:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="943" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03F980D5-0FB0-4AAF-ADD4-7C7CC7851A22}"/>
+  <xr:revisionPtr revIDLastSave="944" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88AAC7FA-117D-4EF1-B9BD-2FBC0C49EFFC}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="885" windowWidth="26910" windowHeight="13470" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1335" yWindow="795" windowWidth="26910" windowHeight="13470" tabRatio="877" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Type de vecteurs" sheetId="37" r:id="rId16"/>
     <sheet name="Niveau de prise en charge" sheetId="31" r:id="rId17"/>
     <sheet name="Type de devenir du patient" sheetId="35" r:id="rId18"/>
-    <sheet name="Effet à obtenir" sheetId="10" r:id="rId19"/>
+    <sheet name="#Effet à obtenir" sheetId="10" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -8182,7 +8182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
   <dimension ref="A1:K220"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -8755,11 +8755,11 @@
         <v>1934</v>
       </c>
       <c r="C21" s="35" t="str">
-        <f>'Effet à obtenir'!$B$1</f>
+        <f>'#Effet à obtenir'!$B$1</f>
         <v>CISU</v>
       </c>
       <c r="D21" s="35" t="str">
-        <f>'Effet à obtenir'!$B$2</f>
+        <f>'#Effet à obtenir'!$B$2</f>
         <v>CodeEffet_a_obtenir</v>
       </c>
       <c r="E21" s="38" t="s">
@@ -15538,8 +15538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
[24.06.10 18:04] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="965" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29C78338-9B41-4E4C-8812-6A522D25CDFA}"/>
+  <xr:revisionPtr revIDLastSave="966" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C13653A-A307-46DD-BE54-30F24EB7ECC1}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="240" windowWidth="23655" windowHeight="13470" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6288,13 +6288,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -6307,6 +6300,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -6460,7 +6459,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6470,6 +6468,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -8217,7 +8216,7 @@
   <dimension ref="A1:K220"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -8289,7 +8288,7 @@
       <c r="A5" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="42" t="s">
         <v>1922</v>
       </c>
       <c r="C5" s="31" t="str">
@@ -8320,7 +8319,7 @@
       <c r="A6" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="43" t="s">
         <v>1928</v>
       </c>
       <c r="C6" s="31" t="str">
@@ -8351,7 +8350,7 @@
       <c r="A7" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="43" t="s">
         <v>1929</v>
       </c>
       <c r="C7" s="31" t="str">
@@ -8382,10 +8381,10 @@
       <c r="A8" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="43" t="s">
         <v>1954</v>
       </c>
-      <c r="C8" s="42" t="str">
+      <c r="C8" s="40" t="str">
         <f>'Motif de recours médico-secouri'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -8413,7 +8412,7 @@
       <c r="A9" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="43" t="s">
         <v>1925</v>
       </c>
       <c r="C9" s="31" t="str">
@@ -8442,7 +8441,7 @@
       <c r="A10" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="43" t="s">
         <v>1934</v>
       </c>
       <c r="C10" s="31" t="str">
@@ -8471,10 +8470,10 @@
       <c r="A11" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="43" t="s">
         <v>1930</v>
       </c>
-      <c r="C11" s="43" t="str">
+      <c r="C11" s="41" t="str">
         <f>'Nombre de patients-victimes'!$B$1</f>
         <v>CISU</v>
       </c>
@@ -8500,7 +8499,7 @@
       <c r="A12" s="31" t="s">
         <v>1924</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="43" t="s">
         <v>1931</v>
       </c>
       <c r="C12" s="31" t="str">
@@ -8531,7 +8530,7 @@
       <c r="A13" s="31" t="s">
         <v>1924</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="43" t="s">
         <v>1932</v>
       </c>
       <c r="C13" s="31" t="str">
@@ -8562,7 +8561,7 @@
       <c r="A14" s="32" t="s">
         <v>1941</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="43" t="s">
         <v>1935</v>
       </c>
       <c r="C14" s="31" t="str">
@@ -8593,7 +8592,7 @@
       <c r="A15" s="32" t="s">
         <v>1941</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="43" t="s">
         <v>1936</v>
       </c>
       <c r="C15" s="31" t="str">
@@ -8622,7 +8621,7 @@
       <c r="A16" s="31" t="s">
         <v>1942</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="43" t="s">
         <v>1937</v>
       </c>
       <c r="C16" s="31" t="str">
@@ -8653,10 +8652,10 @@
       <c r="A17" s="31" t="s">
         <v>1951</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="43" t="s">
         <v>1939</v>
       </c>
-      <c r="C17" s="41" t="str">
+      <c r="C17" s="39" t="str">
         <f>'Type de ressource'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -8686,7 +8685,7 @@
       <c r="A18" s="32" t="s">
         <v>1951</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="43" t="s">
         <v>1953</v>
       </c>
       <c r="C18" s="31" t="str">
@@ -8719,7 +8718,7 @@
       <c r="A19" s="31" t="s">
         <v>1951</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="43" t="s">
         <v>1949</v>
       </c>
       <c r="C19" s="31" t="str">
@@ -8754,7 +8753,7 @@
       <c r="A20" s="31" t="s">
         <v>1942</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="43" t="s">
         <v>1938</v>
       </c>
       <c r="C20" s="31" t="str">
@@ -8785,7 +8784,7 @@
       <c r="A21" s="32" t="s">
         <v>1952</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="43" t="s">
         <v>1933</v>
       </c>
       <c r="C21" s="31" t="str">

</xml_diff>

<commit_message>
[24.06.13 11:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="966" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C13653A-A307-46DD-BE54-30F24EB7ECC1}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="240" windowWidth="23655" windowHeight="13470" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3540" yWindow="2835" windowWidth="21600" windowHeight="11295" tabRatio="877" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -6449,12 +6449,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6469,6 +6463,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -7820,10 +7820,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
-<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
@@ -8215,7 +8211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
   <dimension ref="A1:K220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -8232,12 +8228,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="37"/>
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="20"/>
@@ -8288,7 +8284,7 @@
       <c r="A5" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>1922</v>
       </c>
       <c r="C5" s="31" t="str">
@@ -8319,7 +8315,7 @@
       <c r="A6" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="41" t="s">
         <v>1928</v>
       </c>
       <c r="C6" s="31" t="str">
@@ -8350,7 +8346,7 @@
       <c r="A7" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="41" t="s">
         <v>1929</v>
       </c>
       <c r="C7" s="31" t="str">
@@ -8381,10 +8377,10 @@
       <c r="A8" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="41" t="s">
         <v>1954</v>
       </c>
-      <c r="C8" s="40" t="str">
+      <c r="C8" s="38" t="str">
         <f>'Motif de recours médico-secouri'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -8412,7 +8408,7 @@
       <c r="A9" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="41" t="s">
         <v>1925</v>
       </c>
       <c r="C9" s="31" t="str">
@@ -8441,7 +8437,7 @@
       <c r="A10" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>1934</v>
       </c>
       <c r="C10" s="31" t="str">
@@ -8470,10 +8466,10 @@
       <c r="A11" s="31" t="s">
         <v>1921</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="41" t="s">
         <v>1930</v>
       </c>
-      <c r="C11" s="41" t="str">
+      <c r="C11" s="39" t="str">
         <f>'Nombre de patients-victimes'!$B$1</f>
         <v>CISU</v>
       </c>
@@ -8499,7 +8495,7 @@
       <c r="A12" s="31" t="s">
         <v>1924</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="41" t="s">
         <v>1931</v>
       </c>
       <c r="C12" s="31" t="str">
@@ -8530,7 +8526,7 @@
       <c r="A13" s="31" t="s">
         <v>1924</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="41" t="s">
         <v>1932</v>
       </c>
       <c r="C13" s="31" t="str">
@@ -8561,7 +8557,7 @@
       <c r="A14" s="32" t="s">
         <v>1941</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="41" t="s">
         <v>1935</v>
       </c>
       <c r="C14" s="31" t="str">
@@ -8592,7 +8588,7 @@
       <c r="A15" s="32" t="s">
         <v>1941</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="41" t="s">
         <v>1936</v>
       </c>
       <c r="C15" s="31" t="str">
@@ -8621,7 +8617,7 @@
       <c r="A16" s="31" t="s">
         <v>1942</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="41" t="s">
         <v>1937</v>
       </c>
       <c r="C16" s="31" t="str">
@@ -8652,10 +8648,10 @@
       <c r="A17" s="31" t="s">
         <v>1951</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="41" t="s">
         <v>1939</v>
       </c>
-      <c r="C17" s="39" t="str">
+      <c r="C17" s="37" t="str">
         <f>'Type de ressource'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -8685,7 +8681,7 @@
       <c r="A18" s="32" t="s">
         <v>1951</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="41" t="s">
         <v>1953</v>
       </c>
       <c r="C18" s="31" t="str">
@@ -8718,7 +8714,7 @@
       <c r="A19" s="31" t="s">
         <v>1951</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="41" t="s">
         <v>1949</v>
       </c>
       <c r="C19" s="31" t="str">
@@ -8753,7 +8749,7 @@
       <c r="A20" s="31" t="s">
         <v>1942</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="41" t="s">
         <v>1938</v>
       </c>
       <c r="C20" s="31" t="str">
@@ -8784,7 +8780,7 @@
       <c r="A21" s="32" t="s">
         <v>1952</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="41" t="s">
         <v>1933</v>
       </c>
       <c r="C21" s="31" t="str">
@@ -12167,8 +12163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEEF6AB4-B57F-443F-8D0D-BF02A9C5B3B9}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -13358,7 +13354,7 @@
       </c>
       <c r="F13" s="18"/>
     </row>
-    <row r="14" spans="1:6" s="38" customFormat="1">
+    <row r="14" spans="1:6" s="36" customFormat="1">
       <c r="A14" s="21" t="s">
         <v>1687</v>
       </c>
@@ -13369,7 +13365,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="38" customFormat="1">
+    <row r="15" spans="1:6" s="36" customFormat="1">
       <c r="A15" s="21" t="s">
         <v>1914</v>
       </c>
@@ -25455,6 +25451,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -25504,15 +25509,6 @@
     </l0a6b4600f484920bbceae0813174244>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25930,27 +25926,27 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[24.06.13 17:43] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="981" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8452B9F3-DD8D-4E72-AAAF-63A765275180}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="180" windowWidth="27585" windowHeight="13020" tabRatio="877" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1395" yWindow="345" windowWidth="24855" windowHeight="14055" tabRatio="877" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -6265,12 +6265,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6282,6 +6276,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6309,6 +6309,234 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6568,120 +6796,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -7502,120 +7616,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -7635,126 +7635,126 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="A9:F308" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A9:F188" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A9:D46" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A9:E61" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A9:E30" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{865D8B57-135B-4BFA-938D-B62BC39AC970}" name="Code"/>
     <tableColumn id="2" xr3:uid="{E07D1CE2-997E-4A59-9869-D1EFB60F0809}" name="Libellé niveau 1"/>
     <tableColumn id="5" xr3:uid="{A8693491-C517-461F-B62C-F068AE507B25}" name="Libellé niveau 2"/>
-    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A9:F30" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9B470DB1-BD5A-4D37-B9A2-613B4968664F}" name="Code"/>
-    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A9:E55" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A9:D14" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8042,12 +8042,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="20"/>
@@ -14720,7 +14720,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2"/>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>1856</v>
       </c>
       <c r="C10" s="2"/>
@@ -14729,7 +14729,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2"/>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="41" t="s">
         <v>1857</v>
       </c>
       <c r="C11" s="2"/>
@@ -14738,7 +14738,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2"/>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="41" t="s">
         <v>1858</v>
       </c>
       <c r="C12" s="2"/>
@@ -14747,7 +14747,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2"/>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="41" t="s">
         <v>1859</v>
       </c>
       <c r="C13" s="2"/>
@@ -14756,7 +14756,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2"/>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="41" t="s">
         <v>1860</v>
       </c>
       <c r="C14" s="2"/>
@@ -14765,7 +14765,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2"/>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="41" t="s">
         <v>1861</v>
       </c>
       <c r="C15" s="2"/>
@@ -14774,7 +14774,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="42" t="s">
         <v>1862</v>
       </c>
       <c r="C16" s="2"/>
@@ -14783,7 +14783,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2"/>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="41" t="s">
         <v>1863</v>
       </c>
       <c r="C17" s="2"/>
@@ -14792,7 +14792,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="41" t="s">
         <v>1864</v>
       </c>
       <c r="C18" s="2"/>
@@ -14801,7 +14801,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2"/>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="41" t="s">
         <v>1865</v>
       </c>
       <c r="C19" s="2"/>
@@ -14810,7 +14810,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2"/>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="41" t="s">
         <v>1866</v>
       </c>
       <c r="C20" s="2"/>
@@ -14819,7 +14819,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2"/>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="41" t="s">
         <v>1867</v>
       </c>
       <c r="C21" s="2"/>
@@ -14828,7 +14828,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2"/>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="41" t="s">
         <v>1868</v>
       </c>
       <c r="C22" s="2"/>
@@ -14837,7 +14837,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2"/>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="44" t="s">
         <v>1869</v>
       </c>
       <c r="C23" s="2"/>
@@ -14846,7 +14846,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2"/>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="41" t="s">
         <v>1870</v>
       </c>
       <c r="C24" s="2"/>
@@ -14855,7 +14855,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2"/>
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="44" t="s">
         <v>1871</v>
       </c>
       <c r="C25" s="2"/>
@@ -14864,7 +14864,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2"/>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="41" t="s">
         <v>1872</v>
       </c>
       <c r="C26" s="2"/>
@@ -14873,7 +14873,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2"/>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="42" t="s">
         <v>1873</v>
       </c>
       <c r="C27" s="2"/>
@@ -14882,7 +14882,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2"/>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="42" t="s">
         <v>1874</v>
       </c>
       <c r="C28" s="2"/>
@@ -14891,7 +14891,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2"/>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="42" t="s">
         <v>1875</v>
       </c>
       <c r="C29" s="2"/>
@@ -14900,7 +14900,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2"/>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="42" t="s">
         <v>1876</v>
       </c>
       <c r="C30" s="2"/>
@@ -14909,7 +14909,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2"/>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="43" t="s">
         <v>1877</v>
       </c>
       <c r="C31" s="2"/>
@@ -15101,7 +15101,7 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
@@ -23229,7 +23229,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE40BA41-A85C-4FB9-AA6F-684436E03697}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
@@ -25002,6 +25004,67 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25415,68 +25478,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25494,30 +25522,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.06.18 09:39] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="981" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8452B9F3-DD8D-4E72-AAAF-63A765275180}"/>
+  <xr:revisionPtr revIDLastSave="1019" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01280EC0-CB16-4FFA-A576-6317120C6325}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1395" yWindow="345" windowWidth="24855" windowHeight="14055" tabRatio="877" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="345" windowWidth="24975" windowHeight="13035" tabRatio="877" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -30,8 +30,10 @@
     <sheet name="Niveau de prise en charge" sheetId="31" r:id="rId15"/>
     <sheet name="Type de devenir du patient" sheetId="35" r:id="rId16"/>
     <sheet name="#Effet à obtenir" sheetId="10" r:id="rId17"/>
-    <sheet name="#Nombre de patients-victimes" sheetId="2" r:id="rId18"/>
-    <sheet name="#Informations sur le requérant" sheetId="4" r:id="rId19"/>
+    <sheet name="#Delai d'intervention demande" sheetId="40" r:id="rId18"/>
+    <sheet name="#Delai de réponse" sheetId="39" r:id="rId19"/>
+    <sheet name="#Nombre de patients-victimes" sheetId="2" r:id="rId20"/>
+    <sheet name="#Informations sur le requérant" sheetId="4" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$4:$K$20</definedName>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2412" uniqueCount="1878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="1948">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -5910,12 +5912,222 @@
   <si>
     <t>Demander l'ouverture d'accès</t>
   </si>
+  <si>
+    <t>NOMENC_EXEC_ENTITE</t>
+  </si>
+  <si>
+    <t>OK0</t>
+  </si>
+  <si>
+    <t>Immédiat</t>
+  </si>
+  <si>
+    <t>OK15M</t>
+  </si>
+  <si>
+    <t>OK30M</t>
+  </si>
+  <si>
+    <t>OK45M</t>
+  </si>
+  <si>
+    <t>OK1H</t>
+  </si>
+  <si>
+    <t>OK2H</t>
+  </si>
+  <si>
+    <t>OK4H</t>
+  </si>
+  <si>
+    <t>OK12H</t>
+  </si>
+  <si>
+    <t>OK24H</t>
+  </si>
+  <si>
+    <t>OKSP</t>
+  </si>
+  <si>
+    <t>INDISPO</t>
+  </si>
+  <si>
+    <t>Indisponible</t>
+  </si>
+  <si>
+    <t>NRPMV</t>
+  </si>
+  <si>
+    <t>Non déclenché car non joignable</t>
+  </si>
+  <si>
+    <t>REFUS</t>
+  </si>
+  <si>
+    <t>Autres refus</t>
+  </si>
+  <si>
+    <t>Accord pour une mise en œuvre immédiate en vue d'une prise en charge dès que possible</t>
+  </si>
+  <si>
+    <t>Moyen sollicité indisponible</t>
+  </si>
+  <si>
+    <t>La ressource n'a pas pu être engagé car impossibilité de la déclencher (moyens de déclenchement non joignable)</t>
+  </si>
+  <si>
+    <t>Refus d'engagement du moyen sollicité</t>
+  </si>
+  <si>
+    <t>NOMENC_EXEC_DECISION</t>
+  </si>
+  <si>
+    <t>DEL0</t>
+  </si>
+  <si>
+    <t>DEL15M</t>
+  </si>
+  <si>
+    <t>DEL30M</t>
+  </si>
+  <si>
+    <t>DEL45M</t>
+  </si>
+  <si>
+    <t>DEL1H</t>
+  </si>
+  <si>
+    <t>DEL2H</t>
+  </si>
+  <si>
+    <t>DEL4H</t>
+  </si>
+  <si>
+    <t>A réaliser dans les 4 heures</t>
+  </si>
+  <si>
+    <t>DEL12H</t>
+  </si>
+  <si>
+    <t>DEL24H</t>
+  </si>
+  <si>
+    <t>DELSP</t>
+  </si>
+  <si>
+    <t>Délai non précisé</t>
+  </si>
+  <si>
+    <t>A réaliser dans le quart d’heure</t>
+  </si>
+  <si>
+    <t>A réaliser dans la demi-heure</t>
+  </si>
+  <si>
+    <t>A réaliser dans les 45 minutes</t>
+  </si>
+  <si>
+    <t>A réaliser dans l'heure</t>
+  </si>
+  <si>
+    <t>A réaliser dans les 2 heures</t>
+  </si>
+  <si>
+    <t>A réaliser dans les 12 heures</t>
+  </si>
+  <si>
+    <t>A réaliser dans les 24 heures</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge souhaitée dans les 30 minutes</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge souhaitée dans les 45 minutes</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge souhaitée dans les 60 minutes</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge souhaitée dans les 2 heures</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge souhaitée dans les 4 heures maxi</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge souhaitée dans les 12 heures</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge souhaitée dans les 24 heures</t>
+  </si>
+  <si>
+    <t>La décision est validée sans précision du délai souhaité</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge dans les 15 minutes maximum</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge dans les 30 minutes</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge dans les 45 minutes</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge dans les 60 minutes</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge dans les 2 heures</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge dans les 4heures</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge dans les 12 heures</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge dans les 24 heures</t>
+  </si>
+  <si>
+    <t>Accord pour une prise en charge sans délai spécifié mais maximum dans 24 heures</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans le quart d’heure</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans la demi-heure</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans les 45 minutes</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans l'heure</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans les 2 heures</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans les 4 heures</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans les 12 heures</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans les 24 heures</t>
+  </si>
+  <si>
+    <t>Accepté, sera réalisé dans un délai non précisé</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge immédiate</t>
+  </si>
+  <si>
+    <t>La décision est validée pour une prise en charge souhaitée dans les 15 minutes maxi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6074,6 +6286,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -6181,7 +6421,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6283,6 +6523,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -6290,7 +6535,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="76">
     <dxf>
       <fill>
         <patternFill>
@@ -6309,6 +6554,270 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7635,126 +8144,154 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="A9:F308" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="68"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A9:D14" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="A9:F188" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A9:D46" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A9:E61" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A9:E30" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{865D8B57-135B-4BFA-938D-B62BC39AC970}" name="Code"/>
     <tableColumn id="2" xr3:uid="{E07D1CE2-997E-4A59-9869-D1EFB60F0809}" name="Libellé niveau 1"/>
     <tableColumn id="5" xr3:uid="{A8693491-C517-461F-B62C-F068AE507B25}" name="Libellé niveau 2"/>
-    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A9:F30" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9B470DB1-BD5A-4D37-B9A2-613B4968664F}" name="Code"/>
-    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A9:E55" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A9:D14" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A9:E55" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}" name="Table13611" displayName="Table13611" ref="A9:E55" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A9:E55" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{FE27AEC6-A24C-4178-99A7-1B2812152DC5}" name="Code" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{EB0C358C-6506-4607-BF79-8A517F8D75A1}" name="Libellé niveau 1" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{6068A160-E74F-4F9B-B66D-B8B2A21807F0}" name="Libellé niveau 2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{F5E953CB-171A-4B76-B54B-CA690E7F0F8D}" name="Description" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{7CB61F33-9B59-4443-8AA1-CF748FC4482A}" name="Commentaire" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14626,8 +15163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -15095,85 +15632,88 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E537A6-C63B-444A-987C-2E8C3CA81E02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1CA169-4FB0-43D8-9F60-FA4DC3576143}">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="80.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>1311</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1900</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
-        <v>45191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -15181,161 +15721,488 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>1298</v>
-      </c>
-      <c r="B10" s="24">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>1299</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
-        <v>1300</v>
-      </c>
-      <c r="B11" s="24">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
-        <v>1302</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>1303</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>1304</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
-        <v>1305</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1306</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>1307</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
-        <v>1308</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>1309</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>1310</v>
-      </c>
-      <c r="D14" s="2"/>
+    <row r="10" spans="1:5" s="36" customFormat="1">
+      <c r="A10" s="21" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="21" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="36" customFormat="1">
+      <c r="A11" s="21" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="21" t="s">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="36" customFormat="1">
+      <c r="A12" s="21" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>1914</v>
+      </c>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="21" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="36" customFormat="1">
+      <c r="A13" s="21" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>1915</v>
+      </c>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="21" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="36" customFormat="1">
+      <c r="A14" s="21" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>1916</v>
+      </c>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="21" t="s">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="36" customFormat="1">
+      <c r="A15" s="21" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>1917</v>
+      </c>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="21" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="36" customFormat="1">
+      <c r="A16" s="21" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>1908</v>
+      </c>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="21" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="36" customFormat="1">
+      <c r="A17" s="21" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="21" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="36" customFormat="1">
+      <c r="A18" s="21" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>1919</v>
+      </c>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="21" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="36" customFormat="1">
+      <c r="A19" s="21" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="21" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="47"/>
+    </row>
+    <row r="22" spans="1:5" s="50" customFormat="1">
+      <c r="A22" s="48"/>
+      <c r="B22" s="48"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="48"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0545B1B-517B-4CE5-AAD0-165B9A1E1BDF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95F9426-BF9A-4F69-8DB7-E6D9FAB47FDC}">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>1311</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" s="3" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
-        <v>45191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" s="6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="6"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -15343,95 +16210,414 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>26</v>
-      </c>
+    <row r="10" spans="1:5">
+      <c r="A10" s="21" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="21" t="s">
+        <v>1896</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="21" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="21" t="s">
+        <v>1928</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="21" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>1938</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="21" t="s">
+        <v>1929</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="21" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>1939</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="21" t="s">
+        <v>1930</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="21" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="21" t="s">
+        <v>1931</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="21" t="s">
+        <v>1885</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="21" t="s">
+        <v>1932</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="21" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>1942</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="21" t="s">
+        <v>1933</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="21" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="21" t="s">
+        <v>1934</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="21" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>1944</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="21" t="s">
+        <v>1935</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="21" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="21" t="s">
+        <v>1936</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="21" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>1891</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="21" t="s">
+        <v>1897</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="21" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>1893</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="21" t="s">
+        <v>1898</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" s="50" customFormat="1">
+      <c r="A22" s="48" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="48" t="s">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19285,6 +20471,353 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E537A6-C63B-444A-987C-2E8C3CA81E02}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B10" s="24">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B11" s="24">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0545B1B-517B-4CE5-AAD0-165B9A1E1BDF}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
@@ -23229,7 +24762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE40BA41-A85C-4FB9-AA6F-684436E03697}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -25004,67 +26537,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25478,33 +26950,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25522,4 +27029,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.06.18 15:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1019" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01280EC0-CB16-4FFA-A576-6317120C6325}"/>
+  <xr:revisionPtr revIDLastSave="1023" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6679DB7-E770-4851-A087-4846D7905FA1}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="345" windowWidth="24975" windowHeight="13035" tabRatio="877" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="345" windowWidth="24975" windowHeight="13035" tabRatio="877" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="1948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="1970">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -6121,6 +6121,72 @@
   </si>
   <si>
     <t>La décision est validée pour une prise en charge souhaitée dans les 15 minutes maxi</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>E02</t>
+  </si>
+  <si>
+    <t>E03</t>
+  </si>
+  <si>
+    <t>E04</t>
+  </si>
+  <si>
+    <t>E05</t>
+  </si>
+  <si>
+    <t>E06</t>
+  </si>
+  <si>
+    <t>E07</t>
+  </si>
+  <si>
+    <t>E08</t>
+  </si>
+  <si>
+    <t>E09</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>E15</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>E17</t>
+  </si>
+  <si>
+    <t>E18</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>E21</t>
+  </si>
+  <si>
+    <t>E22</t>
   </si>
 </sst>
 </file>
@@ -6517,17 +6583,17 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -6574,6 +6640,102 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -6838,102 +7000,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -8159,26 +8225,26 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A9:D14" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8270,28 +8336,28 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A9:E55" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}" name="Table13611" displayName="Table13611" ref="A9:E55" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}" name="Table13611" displayName="Table13611" ref="A9:E55" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A9:E55" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE27AEC6-A24C-4178-99A7-1B2812152DC5}" name="Code" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{EB0C358C-6506-4607-BF79-8A517F8D75A1}" name="Libellé niveau 1" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{6068A160-E74F-4F9B-B66D-B8B2A21807F0}" name="Libellé niveau 2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{F5E953CB-171A-4B76-B54B-CA690E7F0F8D}" name="Description" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{7CB61F33-9B59-4443-8AA1-CF748FC4482A}" name="Commentaire" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{FE27AEC6-A24C-4178-99A7-1B2812152DC5}" name="Code" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{EB0C358C-6506-4607-BF79-8A517F8D75A1}" name="Libellé niveau 1" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{6068A160-E74F-4F9B-B66D-B8B2A21807F0}" name="Libellé niveau 2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{F5E953CB-171A-4B76-B54B-CA690E7F0F8D}" name="Description" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{7CB61F33-9B59-4443-8AA1-CF748FC4482A}" name="Commentaire" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8579,12 +8645,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="20"/>
@@ -15163,8 +15229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -15256,7 +15322,9 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>1948</v>
+      </c>
       <c r="B10" s="41" t="s">
         <v>1856</v>
       </c>
@@ -15265,7 +15333,9 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>1949</v>
+      </c>
       <c r="B11" s="41" t="s">
         <v>1857</v>
       </c>
@@ -15274,7 +15344,9 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>1950</v>
+      </c>
       <c r="B12" s="41" t="s">
         <v>1858</v>
       </c>
@@ -15283,7 +15355,9 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>1951</v>
+      </c>
       <c r="B13" s="41" t="s">
         <v>1859</v>
       </c>
@@ -15292,7 +15366,9 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>1952</v>
+      </c>
       <c r="B14" s="41" t="s">
         <v>1860</v>
       </c>
@@ -15301,7 +15377,9 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>1953</v>
+      </c>
       <c r="B15" s="41" t="s">
         <v>1861</v>
       </c>
@@ -15310,7 +15388,9 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>1954</v>
+      </c>
       <c r="B16" s="42" t="s">
         <v>1862</v>
       </c>
@@ -15319,7 +15399,9 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>1955</v>
+      </c>
       <c r="B17" s="41" t="s">
         <v>1863</v>
       </c>
@@ -15328,7 +15410,9 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>1956</v>
+      </c>
       <c r="B18" s="41" t="s">
         <v>1864</v>
       </c>
@@ -15337,7 +15421,9 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>1957</v>
+      </c>
       <c r="B19" s="41" t="s">
         <v>1865</v>
       </c>
@@ -15346,7 +15432,9 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>1958</v>
+      </c>
       <c r="B20" s="41" t="s">
         <v>1866</v>
       </c>
@@ -15355,7 +15443,9 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>1959</v>
+      </c>
       <c r="B21" s="41" t="s">
         <v>1867</v>
       </c>
@@ -15364,7 +15454,9 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>1960</v>
+      </c>
       <c r="B22" s="41" t="s">
         <v>1868</v>
       </c>
@@ -15373,7 +15465,9 @@
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="2"/>
+      <c r="A23" s="2" t="s">
+        <v>1961</v>
+      </c>
       <c r="B23" s="44" t="s">
         <v>1869</v>
       </c>
@@ -15382,7 +15476,9 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>1962</v>
+      </c>
       <c r="B24" s="41" t="s">
         <v>1870</v>
       </c>
@@ -15391,7 +15487,9 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>1963</v>
+      </c>
       <c r="B25" s="44" t="s">
         <v>1871</v>
       </c>
@@ -15400,7 +15498,9 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="2"/>
+      <c r="A26" s="2" t="s">
+        <v>1964</v>
+      </c>
       <c r="B26" s="41" t="s">
         <v>1872</v>
       </c>
@@ -15409,7 +15509,9 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>1965</v>
+      </c>
       <c r="B27" s="42" t="s">
         <v>1873</v>
       </c>
@@ -15418,7 +15520,9 @@
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="2"/>
+      <c r="A28" s="2" t="s">
+        <v>1966</v>
+      </c>
       <c r="B28" s="42" t="s">
         <v>1874</v>
       </c>
@@ -15427,7 +15531,9 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>1967</v>
+      </c>
       <c r="B29" s="42" t="s">
         <v>1875</v>
       </c>
@@ -15436,7 +15542,9 @@
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="2"/>
+      <c r="A30" s="2" t="s">
+        <v>1968</v>
+      </c>
       <c r="B30" s="42" t="s">
         <v>1876</v>
       </c>
@@ -15445,7 +15553,9 @@
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>1969</v>
+      </c>
       <c r="B31" s="43" t="s">
         <v>1877</v>
       </c>
@@ -15638,7 +15748,7 @@
   </sheetPr>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -15737,8 +15847,8 @@
       <c r="B10" s="21" t="s">
         <v>1880</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
       <c r="E10" s="21" t="s">
         <v>1946</v>
       </c>
@@ -15750,8 +15860,8 @@
       <c r="B11" s="21" t="s">
         <v>1913</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
       <c r="E11" s="21" t="s">
         <v>1947</v>
       </c>
@@ -15763,8 +15873,8 @@
       <c r="B12" s="21" t="s">
         <v>1914</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="21" t="s">
         <v>1920</v>
       </c>
@@ -15776,8 +15886,8 @@
       <c r="B13" s="21" t="s">
         <v>1915</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="21" t="s">
         <v>1921</v>
       </c>
@@ -15789,8 +15899,8 @@
       <c r="B14" s="21" t="s">
         <v>1916</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="21" t="s">
         <v>1922</v>
       </c>
@@ -15802,8 +15912,8 @@
       <c r="B15" s="21" t="s">
         <v>1917</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
       <c r="E15" s="21" t="s">
         <v>1923</v>
       </c>
@@ -15815,8 +15925,8 @@
       <c r="B16" s="21" t="s">
         <v>1908</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="21" t="s">
         <v>1924</v>
       </c>
@@ -15828,8 +15938,8 @@
       <c r="B17" s="21" t="s">
         <v>1918</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
       <c r="E17" s="21" t="s">
         <v>1925</v>
       </c>
@@ -15841,8 +15951,8 @@
       <c r="B18" s="21" t="s">
         <v>1919</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="21" t="s">
         <v>1926</v>
       </c>
@@ -15854,8 +15964,8 @@
       <c r="B19" s="21" t="s">
         <v>1912</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="21" t="s">
         <v>1927</v>
       </c>
@@ -15872,14 +15982,14 @@
       <c r="B21" s="21"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="47"/>
-    </row>
-    <row r="22" spans="1:5" s="50" customFormat="1">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="48"/>
+      <c r="E21" s="45"/>
+    </row>
+    <row r="22" spans="1:5" s="48" customFormat="1">
+      <c r="A22" s="46"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="46"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2"/>
@@ -16375,16 +16485,16 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" s="50" customFormat="1">
-      <c r="A22" s="48" t="s">
+    <row r="22" spans="1:5" s="48" customFormat="1">
+      <c r="A22" s="46" t="s">
         <v>1894</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="46" t="s">
         <v>1895</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="48" t="s">
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="46" t="s">
         <v>1899</v>
       </c>
     </row>
@@ -26951,15 +27061,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -27011,6 +27112,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
   <ds:schemaRefs>
@@ -27032,27 +27142,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.06.24 09:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -26708,8 +26708,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="4317e20fb51ec4e85b8666dabb09ede3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b908cdd69cb0859c51683a5db1834d0" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -26772,12 +26772,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -26890,7 +26890,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -26909,7 +26909,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -26982,7 +26982,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -27031,8 +27031,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -27148,21 +27148,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477C49D6-F5F6-4D23-B822-AB2FD62E49A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32A1607C-5E5F-439E-B62E-A69106800C3A}"/>
 </file>
</xml_diff>

<commit_message>
[24.06.24 09:55] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1026" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E838BB7B-E5B2-4254-BDE3-E7319E109BEF}"/>
+  <xr:revisionPtr revIDLastSave="1028" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22E751DD-E313-3247-A164-FDB798066A6E}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="760" windowWidth="24980" windowHeight="13040" tabRatio="877" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15230,7 +15230,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -26647,67 +26647,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="4317e20fb51ec4e85b8666dabb09ede3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b908cdd69cb0859c51683a5db1834d0" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -27121,20 +27060,83 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32A1607C-5E5F-439E-B62E-A69106800C3A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27148,5 +27150,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32A1607C-5E5F-439E-B62E-A69106800C3A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.06.25 17:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1028" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22E751DD-E313-3247-A164-FDB798066A6E}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="760" windowWidth="24980" windowHeight="13040" tabRatio="877" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="877" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -11829,7 +11829,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E9" sqref="E9:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -15229,7 +15229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -16741,8 +16741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -25928,7 +25928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29F356B-BB22-47DE-A619-877383F0285B}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -26647,6 +26647,67 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="4317e20fb51ec4e85b8666dabb09ede3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b908cdd69cb0859c51683a5db1834d0" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -27060,68 +27121,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32A1607C-5E5F-439E-B62E-A69106800C3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27139,30 +27165,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.07.02 09:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1028" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22E751DD-E313-3247-A164-FDB798066A6E}"/>
+  <xr:revisionPtr revIDLastSave="1035" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C7BB4F8-520C-4D49-B69C-1057BCFDD770}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="877" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10050" yWindow="570" windowWidth="16500" windowHeight="13980" tabRatio="877" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2535" uniqueCount="1970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="1947">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -5853,51 +5853,15 @@
     <t>Demander un soutien médico psychologique</t>
   </si>
   <si>
-    <t>Demander une prise en charge médicale</t>
-  </si>
-  <si>
     <t>Demander une prise en charge para médicale</t>
   </si>
   <si>
     <t>Autre demande de concours au SAMU</t>
   </si>
   <si>
-    <t>Demander le transport d'une personne</t>
-  </si>
-  <si>
-    <t>Demander la recherche de personne(s) ensevelie(s)</t>
-  </si>
-  <si>
     <t>Demander de relever une personne</t>
   </si>
   <si>
-    <t>Demander d'extraire ou degager une personne</t>
-  </si>
-  <si>
-    <t>Demander un appui pour évacuation</t>
-  </si>
-  <si>
-    <t>Lutter contre l'incendie</t>
-  </si>
-  <si>
-    <t>Demander une levée de doute CO</t>
-  </si>
-  <si>
-    <t>Demander une levée de doute NRBC</t>
-  </si>
-  <si>
-    <t>Demander une levée de doute d'odeur/fumée suspecte</t>
-  </si>
-  <si>
-    <t>Demander un appui technique</t>
-  </si>
-  <si>
-    <t>Demander une prise en charge de nombreuses victimes</t>
-  </si>
-  <si>
-    <t>Autre demande de concours au SIS</t>
-  </si>
-  <si>
     <t>Demander un transfert interétablissement</t>
   </si>
   <si>
@@ -5907,9 +5871,6 @@
     <t>Demander un transport bariatrique</t>
   </si>
   <si>
-    <t>Demander l'ouverture d'accès</t>
-  </si>
-  <si>
     <t>NOMENC_EXEC_ENTITE</t>
   </si>
   <si>
@@ -6120,73 +6081,43 @@
     <t>La décision est validée pour une prise en charge souhaitée dans les 15 minutes maxi</t>
   </si>
   <si>
-    <t>E01</t>
-  </si>
-  <si>
-    <t>E02</t>
-  </si>
-  <si>
-    <t>E03</t>
-  </si>
-  <si>
-    <t>E04</t>
-  </si>
-  <si>
-    <t>E05</t>
-  </si>
-  <si>
-    <t>E06</t>
-  </si>
-  <si>
-    <t>E07</t>
-  </si>
-  <si>
-    <t>E08</t>
-  </si>
-  <si>
-    <t>E09</t>
-  </si>
-  <si>
-    <t>E10</t>
-  </si>
-  <si>
-    <t>E11</t>
-  </si>
-  <si>
-    <t>E12</t>
-  </si>
-  <si>
-    <t>E13</t>
-  </si>
-  <si>
-    <t>E14</t>
-  </si>
-  <si>
-    <t>E15</t>
-  </si>
-  <si>
-    <t>E16</t>
-  </si>
-  <si>
-    <t>E17</t>
-  </si>
-  <si>
-    <t>E18</t>
-  </si>
-  <si>
-    <t>E19</t>
-  </si>
-  <si>
-    <t>E20</t>
-  </si>
-  <si>
-    <t>E21</t>
-  </si>
-  <si>
-    <t>E22</t>
-  </si>
-  <si>
     <t>Code_Effet_a_obtenir</t>
+  </si>
+  <si>
+    <t>Demander une prise en charge de médecine d'urgence</t>
+  </si>
+  <si>
+    <t>Demander une prise en charge de médecine générale</t>
+  </si>
+  <si>
+    <t>Demander une prise en charge de nombreuses patients/victimes</t>
+  </si>
+  <si>
+    <t>SAP</t>
+  </si>
+  <si>
+    <t>REGUL</t>
+  </si>
+  <si>
+    <t>CUMP</t>
+  </si>
+  <si>
+    <t>SAMU</t>
+  </si>
+  <si>
+    <t>RELEVE</t>
+  </si>
+  <si>
+    <t>NOVI</t>
+  </si>
+  <si>
+    <t>TIH</t>
+  </si>
+  <si>
+    <t>BRANCARD</t>
+  </si>
+  <si>
+    <t>BARIA</t>
   </si>
 </sst>
 </file>
@@ -6487,7 +6418,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6594,10 +6525,25 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
@@ -8629,22 +8575,22 @@
   <dimension ref="A1:K219"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="31" style="28" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="28" customWidth="1"/>
-    <col min="4" max="4" width="37.1640625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="28" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="28" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="28" customWidth="1"/>
     <col min="7" max="11" width="9" style="28" customWidth="1"/>
-    <col min="12" max="16384" width="11.5" style="28"/>
+    <col min="12" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="50"/>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -8662,7 +8608,7 @@
       <c r="B3" s="20"/>
       <c r="C3" s="20"/>
     </row>
-    <row r="4" spans="1:11" s="30" customFormat="1">
+    <row r="4" spans="1:11" s="30" customFormat="1" ht="15">
       <c r="A4" s="29" t="s">
         <v>1850</v>
       </c>
@@ -8697,7 +8643,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8728,7 +8674,7 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8759,7 +8705,7 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8790,7 +8736,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8821,7 +8767,7 @@
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8850,7 +8796,7 @@
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8879,7 +8825,7 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" s="31" t="s">
         <v>1825</v>
       </c>
@@ -8910,7 +8856,7 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" s="31" t="s">
         <v>1825</v>
       </c>
@@ -8941,7 +8887,7 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="32" t="s">
         <v>1841</v>
       </c>
@@ -8972,7 +8918,7 @@
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="32" t="s">
         <v>1841</v>
       </c>
@@ -9001,7 +8947,7 @@
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="31" t="s">
         <v>1842</v>
       </c>
@@ -9032,7 +8978,7 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="31" t="s">
         <v>1851</v>
       </c>
@@ -9065,7 +9011,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" ht="15">
       <c r="A17" s="32" t="s">
         <v>1851</v>
       </c>
@@ -9098,7 +9044,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" s="31" t="s">
         <v>1851</v>
       </c>
@@ -9133,7 +9079,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="15">
       <c r="A19" s="31" t="s">
         <v>1842</v>
       </c>
@@ -9164,7 +9110,7 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="15">
       <c r="A20" s="32" t="s">
         <v>1852</v>
       </c>
@@ -9193,7 +9139,7 @@
       </c>
       <c r="K20" s="34"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="15">
       <c r="A21" s="32"/>
       <c r="B21" s="35"/>
       <c r="C21" s="31"/>
@@ -11832,13 +11778,13 @@
       <selection activeCell="E9" sqref="E9:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
-    <col min="6" max="6" width="61.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -11992,14 +11938,14 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12421,14 +12367,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12866,13 +12812,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13316,12 +13262,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14297,13 +14243,13 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14719,13 +14665,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15229,17 +15175,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15256,7 +15202,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1969</v>
+        <v>1934</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -15322,8 +15268,8 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>1947</v>
+      <c r="A10" s="52" t="s">
+        <v>1938</v>
       </c>
       <c r="B10" s="41" t="s">
         <v>1855</v>
@@ -15333,8 +15279,8 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
-        <v>1948</v>
+      <c r="A11" s="53" t="s">
+        <v>1939</v>
       </c>
       <c r="B11" s="41" t="s">
         <v>1856</v>
@@ -15344,8 +15290,8 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
-        <v>1949</v>
+      <c r="A12" s="54" t="s">
+        <v>1940</v>
       </c>
       <c r="B12" s="41" t="s">
         <v>1857</v>
@@ -15355,210 +15301,170 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
-        <v>1950</v>
+      <c r="A13" s="54" t="s">
+        <v>1580</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>1858</v>
+        <v>1935</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
-        <v>1951</v>
+      <c r="A14" s="54" t="s">
+        <v>1444</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>1859</v>
+        <v>1936</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>1952</v>
+      <c r="A15" s="54" t="s">
+        <v>1573</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>1860</v>
+        <v>1858</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="2" t="s">
-        <v>1953</v>
+      <c r="A16" s="54" t="s">
+        <v>1941</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>1861</v>
+        <v>1859</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="2" t="s">
-        <v>1954</v>
+      <c r="A17" s="55" t="s">
+        <v>1942</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="2" t="s">
-        <v>1955</v>
+      <c r="A18" s="56" t="s">
+        <v>1943</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>1863</v>
+        <v>1937</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
-        <v>1956</v>
+      <c r="A19" s="54" t="s">
+        <v>1944</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>1864</v>
+        <v>1861</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="2" t="s">
-        <v>1957</v>
+      <c r="A20" s="54" t="s">
+        <v>1945</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>1865</v>
+        <v>1862</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="2" t="s">
-        <v>1958</v>
+      <c r="A21" s="54" t="s">
+        <v>1946</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>1866</v>
+        <v>1863</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>1959</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>1867</v>
-      </c>
+      <c r="A22" s="2"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="2" t="s">
-        <v>1960</v>
-      </c>
-      <c r="B23" s="44" t="s">
-        <v>1868</v>
-      </c>
+      <c r="A23" s="2"/>
+      <c r="B23" s="44"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="2" t="s">
-        <v>1961</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>1869</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>1962</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>1870</v>
-      </c>
+      <c r="A25" s="2"/>
+      <c r="B25" s="44"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
-        <v>1963</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>1871</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="2" t="s">
-        <v>1964</v>
-      </c>
-      <c r="B27" s="42" t="s">
-        <v>1872</v>
-      </c>
+      <c r="A27" s="2"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="2" t="s">
-        <v>1965</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>1873</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="2" t="s">
-        <v>1966</v>
-      </c>
-      <c r="B29" s="42" t="s">
-        <v>1874</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="2" t="s">
-        <v>1967</v>
-      </c>
-      <c r="B30" s="42" t="s">
-        <v>1875</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="2" t="s">
-        <v>1968</v>
-      </c>
-      <c r="B31" s="43" t="s">
-        <v>1876</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -15752,13 +15658,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="80.5" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15775,7 +15681,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1899</v>
+        <v>1886</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -15842,132 +15748,132 @@
     </row>
     <row r="10" spans="1:5" s="36" customFormat="1">
       <c r="A10" s="21" t="s">
-        <v>1900</v>
+        <v>1887</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1879</v>
+        <v>1866</v>
       </c>
       <c r="C10" s="49"/>
       <c r="D10" s="49"/>
       <c r="E10" s="21" t="s">
-        <v>1945</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="36" customFormat="1">
       <c r="A11" s="21" t="s">
-        <v>1901</v>
+        <v>1888</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1912</v>
+        <v>1899</v>
       </c>
       <c r="C11" s="49"/>
       <c r="D11" s="49"/>
       <c r="E11" s="21" t="s">
-        <v>1946</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="36" customFormat="1">
       <c r="A12" s="21" t="s">
-        <v>1902</v>
+        <v>1889</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1913</v>
+        <v>1900</v>
       </c>
       <c r="C12" s="49"/>
       <c r="D12" s="49"/>
       <c r="E12" s="21" t="s">
-        <v>1919</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="36" customFormat="1">
       <c r="A13" s="21" t="s">
-        <v>1903</v>
+        <v>1890</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1914</v>
+        <v>1901</v>
       </c>
       <c r="C13" s="49"/>
       <c r="D13" s="49"/>
       <c r="E13" s="21" t="s">
-        <v>1920</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="36" customFormat="1">
       <c r="A14" s="21" t="s">
-        <v>1904</v>
+        <v>1891</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>1915</v>
+        <v>1902</v>
       </c>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
       <c r="E14" s="21" t="s">
-        <v>1921</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="36" customFormat="1">
       <c r="A15" s="21" t="s">
-        <v>1905</v>
+        <v>1892</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>1916</v>
+        <v>1903</v>
       </c>
       <c r="C15" s="49"/>
       <c r="D15" s="49"/>
       <c r="E15" s="21" t="s">
-        <v>1922</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="36" customFormat="1">
       <c r="A16" s="21" t="s">
-        <v>1906</v>
+        <v>1893</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>1907</v>
+        <v>1894</v>
       </c>
       <c r="C16" s="49"/>
       <c r="D16" s="49"/>
       <c r="E16" s="21" t="s">
-        <v>1923</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="36" customFormat="1">
       <c r="A17" s="21" t="s">
-        <v>1908</v>
+        <v>1895</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>1917</v>
+        <v>1904</v>
       </c>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
       <c r="E17" s="21" t="s">
-        <v>1924</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="36" customFormat="1">
       <c r="A18" s="21" t="s">
-        <v>1909</v>
+        <v>1896</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>1918</v>
+        <v>1905</v>
       </c>
       <c r="C18" s="49"/>
       <c r="D18" s="49"/>
       <c r="E18" s="21" t="s">
-        <v>1925</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="36" customFormat="1">
       <c r="A19" s="21" t="s">
-        <v>1910</v>
+        <v>1897</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>1911</v>
+        <v>1898</v>
       </c>
       <c r="C19" s="49"/>
       <c r="D19" s="49"/>
       <c r="E19" s="21" t="s">
-        <v>1926</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -16241,13 +16147,13 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16264,7 +16170,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1877</v>
+        <v>1864</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -16331,171 +16237,171 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="21" t="s">
-        <v>1878</v>
+        <v>1865</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1879</v>
+        <v>1866</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="21" t="s">
-        <v>1895</v>
+        <v>1882</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="21" t="s">
-        <v>1880</v>
+        <v>1867</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1936</v>
+        <v>1923</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="21" t="s">
-        <v>1927</v>
+        <v>1914</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="21" t="s">
-        <v>1881</v>
+        <v>1868</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1937</v>
+        <v>1924</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="21" t="s">
-        <v>1928</v>
+        <v>1915</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="21" t="s">
-        <v>1882</v>
+        <v>1869</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1938</v>
+        <v>1925</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="21" t="s">
-        <v>1929</v>
+        <v>1916</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="21" t="s">
-        <v>1883</v>
+        <v>1870</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>1939</v>
+        <v>1926</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="21" t="s">
-        <v>1930</v>
+        <v>1917</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="21" t="s">
-        <v>1884</v>
+        <v>1871</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>1940</v>
+        <v>1927</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="21" t="s">
-        <v>1931</v>
+        <v>1918</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="21" t="s">
-        <v>1885</v>
+        <v>1872</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>1941</v>
+        <v>1928</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="21" t="s">
-        <v>1932</v>
+        <v>1919</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="21" t="s">
-        <v>1886</v>
+        <v>1873</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>1942</v>
+        <v>1929</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="21" t="s">
-        <v>1933</v>
+        <v>1920</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="21" t="s">
-        <v>1887</v>
+        <v>1874</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>1943</v>
+        <v>1930</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="21" t="s">
-        <v>1934</v>
+        <v>1921</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="21" t="s">
-        <v>1888</v>
+        <v>1875</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>1944</v>
+        <v>1931</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="21" t="s">
-        <v>1935</v>
+        <v>1922</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="21" t="s">
-        <v>1889</v>
+        <v>1876</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>1890</v>
+        <v>1877</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="21" t="s">
-        <v>1896</v>
+        <v>1883</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="21" t="s">
-        <v>1891</v>
+        <v>1878</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>1892</v>
+        <v>1879</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="21" t="s">
-        <v>1897</v>
+        <v>1884</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" s="48" customFormat="1">
       <c r="A22" s="46" t="s">
-        <v>1893</v>
+        <v>1880</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>1894</v>
+        <v>1881</v>
       </c>
       <c r="C22" s="47"/>
       <c r="D22" s="47"/>
       <c r="E22" s="46" t="s">
-        <v>1898</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -16741,18 +16647,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" customWidth="1"/>
-    <col min="5" max="5" width="47.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16835,7 +16741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60">
+    <row r="10" spans="1:6" ht="64.5">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -16861,7 +16767,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -16875,7 +16781,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -16889,7 +16795,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -16902,7 +16808,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -16930,7 +16836,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="26.25">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -16956,7 +16862,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="26.25">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -16971,7 +16877,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -16997,7 +16903,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6" ht="39">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -17011,7 +16917,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:6" ht="39">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -17035,7 +16941,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="30">
+    <row r="25" spans="1:6" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -17049,7 +16955,7 @@
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="30">
+    <row r="26" spans="1:6" ht="26.25">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -17063,7 +16969,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="30">
+    <row r="27" spans="1:6" ht="26.25">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -17077,7 +16983,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -17113,7 +17019,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:6" ht="60">
+    <row r="31" spans="1:6" ht="51.75">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -17127,7 +17033,7 @@
       </c>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
@@ -17166,7 +17072,7 @@
       </c>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="26.25">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -17192,7 +17098,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" ht="120">
+    <row r="37" spans="1:6" ht="102.75">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
@@ -17206,7 +17112,7 @@
       </c>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" ht="30">
+    <row r="38" spans="1:6" ht="26.25">
       <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
@@ -17220,7 +17126,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="30">
+    <row r="39" spans="1:6" ht="39">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -17245,7 +17151,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" ht="30">
+    <row r="41" spans="1:6" ht="39">
       <c r="A41" s="2" t="s">
         <v>116</v>
       </c>
@@ -17259,7 +17165,7 @@
       </c>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" ht="26.25">
       <c r="A42" s="2" t="s">
         <v>119</v>
       </c>
@@ -17273,7 +17179,7 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" ht="30">
+    <row r="43" spans="1:6" ht="39">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -17297,7 +17203,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" ht="45">
+    <row r="45" spans="1:6" ht="39">
       <c r="A45" s="2" t="s">
         <v>127</v>
       </c>
@@ -17396,7 +17302,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="26.25">
       <c r="A53" s="2" t="s">
         <v>145</v>
       </c>
@@ -17410,7 +17316,7 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="60">
+    <row r="54" spans="1:6" ht="64.5">
       <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
@@ -17781,7 +17687,7 @@
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="1:6" ht="45">
+    <row r="85" spans="1:6" ht="39">
       <c r="A85" s="2" t="s">
         <v>214</v>
       </c>
@@ -17807,7 +17713,7 @@
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:6" ht="135">
+    <row r="87" spans="1:6" ht="128.25">
       <c r="A87" s="2" t="s">
         <v>219</v>
       </c>
@@ -17833,7 +17739,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="60">
+    <row r="89" spans="1:6" ht="51.75">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
@@ -17846,7 +17752,7 @@
       </c>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" ht="26.25">
       <c r="A90" s="2" t="s">
         <v>214</v>
       </c>
@@ -17886,7 +17792,7 @@
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:6" ht="30">
+    <row r="93" spans="1:6" ht="26.25">
       <c r="A93" s="2" t="s">
         <v>230</v>
       </c>
@@ -18057,7 +17963,7 @@
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
     </row>
-    <row r="107" spans="1:6" ht="30">
+    <row r="107" spans="1:6" ht="26.25">
       <c r="A107" s="2" t="s">
         <v>261</v>
       </c>
@@ -18071,7 +17977,7 @@
       </c>
       <c r="F107" s="12"/>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" ht="26.25">
       <c r="A108" s="2" t="s">
         <v>264</v>
       </c>
@@ -18195,7 +18101,7 @@
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" ht="30">
+    <row r="118" spans="1:6" ht="26.25">
       <c r="A118" s="2" t="s">
         <v>287</v>
       </c>
@@ -18209,7 +18115,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" ht="26.25">
       <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
@@ -18222,7 +18128,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="45">
+    <row r="120" spans="1:6" ht="39">
       <c r="A120" s="2" t="s">
         <v>293</v>
       </c>
@@ -18260,7 +18166,7 @@
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" ht="45">
+    <row r="123" spans="1:6" ht="39">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -18321,7 +18227,7 @@
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" ht="45">
+    <row r="128" spans="1:6" ht="39">
       <c r="A128" s="2" t="s">
         <v>311</v>
       </c>
@@ -18455,7 +18361,7 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="30">
+    <row r="139" spans="1:6" ht="26.25">
       <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
@@ -18480,7 +18386,7 @@
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
     </row>
-    <row r="141" spans="1:6" ht="30">
+    <row r="141" spans="1:6" ht="26.25">
       <c r="A141" s="2" t="s">
         <v>341</v>
       </c>
@@ -18494,7 +18400,7 @@
       </c>
       <c r="F141" s="12"/>
     </row>
-    <row r="142" spans="1:6" ht="30">
+    <row r="142" spans="1:6" ht="26.25">
       <c r="A142" s="2" t="s">
         <v>342</v>
       </c>
@@ -18508,7 +18414,7 @@
       </c>
       <c r="F142" s="12"/>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" ht="26.25">
       <c r="A143" s="2" t="s">
         <v>343</v>
       </c>
@@ -18522,7 +18428,7 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="30">
+    <row r="144" spans="1:6" ht="26.25">
       <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
@@ -18551,7 +18457,7 @@
       </c>
       <c r="F145" s="12"/>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" ht="26.25">
       <c r="A146" s="2" t="s">
         <v>347</v>
       </c>
@@ -18565,7 +18471,7 @@
       </c>
       <c r="F146" s="12"/>
     </row>
-    <row r="147" spans="1:6" ht="30">
+    <row r="147" spans="1:6" ht="39">
       <c r="A147" s="2" t="s">
         <v>348</v>
       </c>
@@ -18579,7 +18485,7 @@
       </c>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" spans="1:6" ht="30">
+    <row r="148" spans="1:6" ht="39">
       <c r="A148" s="2" t="s">
         <v>349</v>
       </c>
@@ -18593,7 +18499,7 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="30">
+    <row r="149" spans="1:6" ht="26.25">
       <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
@@ -18606,7 +18512,7 @@
       </c>
       <c r="F149" s="12"/>
     </row>
-    <row r="150" spans="1:6" ht="30">
+    <row r="150" spans="1:6" ht="26.25">
       <c r="A150" s="2" t="s">
         <v>351</v>
       </c>
@@ -18620,7 +18526,7 @@
       </c>
       <c r="F150" s="12"/>
     </row>
-    <row r="151" spans="1:6" ht="30">
+    <row r="151" spans="1:6" ht="26.25">
       <c r="A151" s="2" t="s">
         <v>352</v>
       </c>
@@ -18752,7 +18658,7 @@
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
     </row>
-    <row r="162" spans="1:6" ht="30">
+    <row r="162" spans="1:6" ht="39">
       <c r="A162" s="2" t="s">
         <v>373</v>
       </c>
@@ -18766,7 +18672,7 @@
       </c>
       <c r="F162" s="12"/>
     </row>
-    <row r="163" spans="1:6" ht="45">
+    <row r="163" spans="1:6" ht="39">
       <c r="A163" s="2" t="s">
         <v>376</v>
       </c>
@@ -18780,7 +18686,7 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="45">
+    <row r="164" spans="1:6" ht="39">
       <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
@@ -18831,7 +18737,7 @@
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
     </row>
-    <row r="168" spans="1:6" ht="30">
+    <row r="168" spans="1:6" ht="26.25">
       <c r="A168" s="2" t="s">
         <v>389</v>
       </c>
@@ -19048,7 +18954,7 @@
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
     </row>
-    <row r="186" spans="1:6" ht="30">
+    <row r="186" spans="1:6" ht="26.25">
       <c r="A186" s="2" t="s">
         <v>426</v>
       </c>
@@ -19184,7 +19090,7 @@
       </c>
       <c r="F196" s="12"/>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" ht="26.25">
       <c r="A197" s="2" t="s">
         <v>451</v>
       </c>
@@ -19284,7 +19190,7 @@
       <c r="E204" s="12"/>
       <c r="F204" s="12"/>
     </row>
-    <row r="205" spans="1:6" ht="30">
+    <row r="205" spans="1:6" ht="26.25">
       <c r="A205" s="2" t="s">
         <v>470</v>
       </c>
@@ -19310,7 +19216,7 @@
       <c r="E206" s="12"/>
       <c r="F206" s="12"/>
     </row>
-    <row r="207" spans="1:6" ht="30">
+    <row r="207" spans="1:6" ht="26.25">
       <c r="A207" s="2" t="s">
         <v>475</v>
       </c>
@@ -19408,7 +19314,7 @@
       <c r="E214" s="12"/>
       <c r="F214" s="12"/>
     </row>
-    <row r="215" spans="1:6" ht="30">
+    <row r="215" spans="1:6" ht="26.25">
       <c r="A215" s="2" t="s">
         <v>493</v>
       </c>
@@ -20229,7 +20135,7 @@
       <c r="E282" s="12"/>
       <c r="F282" s="12"/>
     </row>
-    <row r="283" spans="1:6" ht="30">
+    <row r="283" spans="1:6" ht="26.25">
       <c r="A283" s="2" t="s">
         <v>638</v>
       </c>
@@ -20243,7 +20149,7 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="30">
+    <row r="284" spans="1:6" ht="26.25">
       <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
@@ -20592,12 +20498,12 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20754,12 +20660,12 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20936,14 +20842,14 @@
       <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -23655,12 +23561,12 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="26.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -23671,7 +23577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="24.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -23737,7 +23643,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="39">
       <c r="A10" s="2" t="s">
         <v>1082</v>
       </c>
@@ -23759,7 +23665,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>1087</v>
       </c>
@@ -23769,7 +23675,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="39">
       <c r="A13" s="2" t="s">
         <v>1089</v>
       </c>
@@ -23779,7 +23685,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>1091</v>
       </c>
@@ -23789,7 +23695,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1093</v>
       </c>
@@ -23799,7 +23705,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1095</v>
       </c>
@@ -23811,7 +23717,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="45">
+    <row r="17" spans="1:4" ht="39">
       <c r="A17" s="2" t="s">
         <v>1098</v>
       </c>
@@ -23823,7 +23729,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="30">
+    <row r="18" spans="1:4" ht="39">
       <c r="A18" s="2" t="s">
         <v>1101</v>
       </c>
@@ -23833,7 +23739,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:4" ht="39">
       <c r="A19" s="2" t="s">
         <v>1103</v>
       </c>
@@ -23843,7 +23749,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>1105</v>
       </c>
@@ -23853,7 +23759,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="26.25">
       <c r="A21" s="2" t="s">
         <v>1107</v>
       </c>
@@ -23863,7 +23769,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="26.25">
       <c r="A22" s="2" t="s">
         <v>1109</v>
       </c>
@@ -23893,7 +23799,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>1115</v>
       </c>
@@ -23923,7 +23829,7 @@
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="30">
+    <row r="28" spans="1:4" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>1120</v>
       </c>
@@ -23935,7 +23841,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="30">
+    <row r="29" spans="1:4" ht="26.25">
       <c r="A29" s="2" t="s">
         <v>1123</v>
       </c>
@@ -23947,7 +23853,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="30">
+    <row r="30" spans="1:4" ht="26.25">
       <c r="A30" s="2" t="s">
         <v>1126</v>
       </c>
@@ -23969,7 +23875,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="30">
+    <row r="32" spans="1:4" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1131</v>
       </c>
@@ -23981,7 +23887,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="30">
+    <row r="33" spans="1:4" ht="39">
       <c r="A33" s="2" t="s">
         <v>1134</v>
       </c>
@@ -23993,7 +23899,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="26.25">
       <c r="A34" s="2" t="s">
         <v>1137</v>
       </c>
@@ -24005,7 +23911,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="135">
+    <row r="35" spans="1:4" ht="128.25">
       <c r="A35" s="2" t="s">
         <v>1140</v>
       </c>
@@ -24017,7 +23923,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="135">
+    <row r="36" spans="1:4" ht="128.25">
       <c r="A36" s="2" t="s">
         <v>1143</v>
       </c>
@@ -24101,7 +24007,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="30">
+    <row r="44" spans="1:4" ht="26.25">
       <c r="A44" s="2" t="s">
         <v>1160</v>
       </c>
@@ -24113,7 +24019,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="30">
+    <row r="45" spans="1:4" ht="26.25">
       <c r="A45" s="2" t="s">
         <v>1163</v>
       </c>
@@ -24123,7 +24029,7 @@
       <c r="C45" s="12"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="75">
+    <row r="46" spans="1:4" ht="77.25">
       <c r="A46" s="2" t="s">
         <v>1165</v>
       </c>
@@ -24152,13 +24058,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="39.5" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -24273,7 +24179,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>1177</v>
       </c>
@@ -24297,7 +24203,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1182</v>
       </c>
@@ -24310,7 +24216,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1185</v>
       </c>
@@ -24334,7 +24240,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="40">
+    <row r="18" spans="1:5" ht="48.75">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -24347,7 +24253,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="64.5">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -24496,7 +24402,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1222</v>
       </c>
@@ -24509,7 +24415,7 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" ht="30">
+    <row r="33" spans="1:5" ht="26.25">
       <c r="A33" s="2" t="s">
         <v>1225</v>
       </c>
@@ -24596,7 +24502,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" ht="45">
+    <row r="40" spans="1:5" ht="51.75">
       <c r="A40" s="2" t="s">
         <v>1244</v>
       </c>
@@ -24633,7 +24539,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" ht="30">
+    <row r="43" spans="1:5" ht="26.25">
       <c r="A43" s="2" t="s">
         <v>1252</v>
       </c>
@@ -24646,7 +24552,7 @@
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5" ht="39">
       <c r="A44" s="2" t="s">
         <v>1253</v>
       </c>
@@ -24705,7 +24611,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="26.25">
       <c r="A49" s="2" t="s">
         <v>1265</v>
       </c>
@@ -24740,7 +24646,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5" ht="30">
+    <row r="52" spans="1:5" ht="26.25">
       <c r="A52" s="2" t="s">
         <v>1272</v>
       </c>
@@ -24834,7 +24740,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="39">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -24876,14 +24782,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.6640625" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25497,14 +25403,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25932,13 +25838,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26024,7 +25930,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32">
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="18" t="s">
         <v>1314</v>
       </c>
@@ -26037,7 +25943,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="32">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="18" t="s">
         <v>1317</v>
       </c>
@@ -26050,7 +25956,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="18" t="s">
         <v>1320</v>
       </c>
@@ -26063,7 +25969,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="32">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="18" t="s">
         <v>1323</v>
       </c>
@@ -26076,7 +25982,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="18" t="s">
         <v>1326</v>
       </c>
@@ -26089,7 +25995,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="32">
+    <row r="15" spans="1:5" ht="45">
       <c r="A15" s="18" t="s">
         <v>1329</v>
       </c>
@@ -26102,7 +26008,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="32">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="18" t="s">
         <v>1332</v>
       </c>
@@ -26115,7 +26021,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="32">
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="18" t="s">
         <v>1335</v>
       </c>
@@ -26128,7 +26034,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="48">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="18" t="s">
         <v>1338</v>
       </c>
@@ -26141,7 +26047,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="48">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="18" t="s">
         <v>1341</v>
       </c>
@@ -26154,7 +26060,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="32">
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="18" t="s">
         <v>1344</v>
       </c>
@@ -26167,7 +26073,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="32">
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="18" t="s">
         <v>1347</v>
       </c>
@@ -26180,7 +26086,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="32">
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="18" t="s">
         <v>1350</v>
       </c>
@@ -26193,7 +26099,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="32">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="18" t="s">
         <v>1353</v>
       </c>
@@ -26206,7 +26112,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="32">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="18" t="s">
         <v>1356</v>
       </c>
@@ -26219,7 +26125,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="32">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="18" t="s">
         <v>1359</v>
       </c>
@@ -26232,7 +26138,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="32">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="18" t="s">
         <v>1362</v>
       </c>
@@ -26245,7 +26151,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="16">
+    <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
         <v>1365</v>
       </c>
@@ -26258,7 +26164,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="32">
+    <row r="28" spans="1:5" ht="30">
       <c r="A28" s="18" t="s">
         <v>1367</v>
       </c>
@@ -26271,7 +26177,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="16">
+    <row r="29" spans="1:5">
       <c r="A29" s="18" t="s">
         <v>1370</v>
       </c>
@@ -26284,7 +26190,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="16">
+    <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
         <v>1373</v>
       </c>
@@ -26312,13 +26218,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26415,7 +26321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="18" t="s">
         <v>1378</v>
       </c>
@@ -26429,7 +26335,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="48">
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="18" t="s">
         <v>1381</v>
       </c>
@@ -26443,7 +26349,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="32">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="18" t="s">
         <v>1384</v>
       </c>
@@ -26457,7 +26363,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="32">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="18" t="s">
         <v>1387</v>
       </c>
@@ -26471,7 +26377,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="32">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="18" t="s">
         <v>1390</v>
       </c>
@@ -26485,7 +26391,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="32">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="18" t="s">
         <v>1393</v>
       </c>
@@ -26499,7 +26405,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="32">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="18" t="s">
         <v>1396</v>
       </c>
@@ -26513,7 +26419,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="48">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="18" t="s">
         <v>1370</v>
       </c>
@@ -26527,7 +26433,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="32">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="18" t="s">
         <v>1401</v>
       </c>
@@ -26647,69 +26553,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="4317e20fb51ec4e85b8666dabb09ede3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b908cdd69cb0859c51683a5db1834d0" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -26772,12 +26617,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -26890,7 +26735,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -26909,7 +26754,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -26982,7 +26827,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -27031,8 +26876,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -27121,22 +26966,69 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8EAFAAD-45BD-4A4A-9EC1-DDF1B9581D22}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27148,21 +27040,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32A1607C-5E5F-439E-B62E-A69106800C3A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.07.02 11:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1035" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C7BB4F8-520C-4D49-B69C-1057BCFDD770}"/>
+  <xr:revisionPtr revIDLastSave="1054" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A645E5-0C8D-4214-85A8-C0C88A86B91D}"/>
   <bookViews>
-    <workbookView xWindow="10050" yWindow="570" windowWidth="16500" windowHeight="13980" tabRatio="877" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="450" windowWidth="25455" windowHeight="13980" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <sheet name="#Informations sur le requérant" sheetId="4" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$4:$K$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$2:$K$18</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2515" uniqueCount="1947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="1949">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -6090,9 +6090,6 @@
     <t>Demander une prise en charge de médecine générale</t>
   </si>
   <si>
-    <t>Demander une prise en charge de nombreuses patients/victimes</t>
-  </si>
-  <si>
     <t>SAP</t>
   </si>
   <si>
@@ -6118,13 +6115,22 @@
   </si>
   <si>
     <t>BARIA</t>
+  </si>
+  <si>
+    <t>Détails à préciser dans le texte libre de la demande de ressources</t>
+  </si>
+  <si>
+    <t>Demander une prise en charge de nombreux patients/victimes</t>
+  </si>
+  <si>
+    <t>Pour obtenir une consultation ou une visite du MG (uniquement pour lien 15-15)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6226,12 +6232,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -6264,18 +6264,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -6311,6 +6299,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -6338,7 +6338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -6359,15 +6359,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -6416,9 +6407,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6477,68 +6468,62 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -8572,10 +8557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
-  <dimension ref="A1:K219"/>
+  <dimension ref="A1:K217"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -8590,73 +8575,122 @@
     <col min="12" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-    </row>
-    <row r="4" spans="1:11" s="30" customFormat="1" ht="15">
-      <c r="A4" s="29" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:11" s="30" customFormat="1" ht="15">
+      <c r="A2" s="29" t="s">
         <v>1850</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B2" s="29" t="s">
         <v>1827</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C2" s="29" t="s">
         <v>1828</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D2" s="29" t="s">
         <v>1819</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E2" s="29" t="s">
         <v>1820</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>1821</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G2" s="29" t="s">
         <v>1844</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H2" s="29" t="s">
         <v>1843</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I2" s="29" t="s">
         <v>1845</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J2" s="29" t="s">
         <v>1846</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>1847</v>
       </c>
+    </row>
+    <row r="3" spans="1:11" ht="15">
+      <c r="A3" s="31" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C3" s="31" t="str">
+        <f>'Nature de fait'!$B$1</f>
+        <v>CISU</v>
+      </c>
+      <c r="D3" s="32" t="str">
+        <f>'Nature de fait'!B2</f>
+        <v>Code_Nature_de_fait</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>1824</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>1840</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>1848</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>1848</v>
+      </c>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+    </row>
+    <row r="4" spans="1:11" ht="15">
+      <c r="A4" s="31" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C4" s="31" t="str">
+        <f>'Type de lieu'!$B$1</f>
+        <v>CISU</v>
+      </c>
+      <c r="D4" s="31" t="str">
+        <f>'Type de lieu'!B2</f>
+        <v>Code_Type_de_lieu</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>1824</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>1840</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>1848</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>1848</v>
+      </c>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" ht="15">
       <c r="A5" s="31" t="s">
         <v>1822</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>1823</v>
+      <c r="B5" s="38" t="s">
+        <v>1830</v>
       </c>
       <c r="C5" s="31" t="str">
-        <f>'Nature de fait'!$B$1</f>
+        <f>'Risque, menace et sensibilité'!$B$1</f>
         <v>CISU</v>
       </c>
-      <c r="D5" s="32" t="str">
-        <f>'Nature de fait'!B2</f>
-        <v>Code_Nature_de_fait</v>
+      <c r="D5" s="31" t="str">
+        <f>'Risque, menace et sensibilité'!$B$2</f>
+        <v>Code_Risque-Menace-Sensibilité</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>1824</v>
@@ -8678,16 +8712,16 @@
       <c r="A6" s="31" t="s">
         <v>1822</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>1829</v>
-      </c>
-      <c r="C6" s="31" t="str">
-        <f>'Type de lieu'!$B$1</f>
-        <v>CISU</v>
+      <c r="B6" s="38" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C6" s="54" t="str">
+        <f>'Motif de recours médico-secouri'!$B$1</f>
+        <v>SI-SAMU</v>
       </c>
       <c r="D6" s="31" t="str">
-        <f>'Type de lieu'!B2</f>
-        <v>Code_Type_de_lieu</v>
+        <f>'Motif de recours médico-secouri'!$B$2</f>
+        <v>Code_Motif_patient-victime</v>
       </c>
       <c r="E6" s="33" t="s">
         <v>1824</v>
@@ -8709,16 +8743,16 @@
       <c r="A7" s="31" t="s">
         <v>1822</v>
       </c>
-      <c r="B7" s="40" t="s">
-        <v>1830</v>
-      </c>
-      <c r="C7" s="31" t="str">
-        <f>'Risque, menace et sensibilité'!$B$1</f>
-        <v>CISU</v>
+      <c r="B7" s="38" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C7" s="54" t="str">
+        <f>'Attribution du dossier'!$B$1</f>
+        <v>SI-SAMU</v>
       </c>
       <c r="D7" s="31" t="str">
-        <f>'Risque, menace et sensibilité'!$B$2</f>
-        <v>Code_Risque-Menace-Sensibilité</v>
+        <f>'Attribution du dossier'!$B$2</f>
+        <v>DEVENIRD</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>1824</v>
@@ -8726,9 +8760,7 @@
       <c r="F7" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="G7" s="34"/>
       <c r="H7" s="34" t="s">
         <v>1848</v>
       </c>
@@ -8740,16 +8772,16 @@
       <c r="A8" s="31" t="s">
         <v>1822</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>1854</v>
-      </c>
-      <c r="C8" s="38" t="str">
-        <f>'Motif de recours médico-secouri'!$B$1</f>
+      <c r="B8" s="38" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C8" s="54" t="str">
+        <f>'Priorité de régulation médicale'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D8" s="31" t="str">
-        <f>'Motif de recours médico-secouri'!$B$2</f>
-        <v>Code_Motif_patient-victime</v>
+        <f>'Priorité de régulation médicale'!$B$2</f>
+        <v>PRIORITE</v>
       </c>
       <c r="E8" s="33" t="s">
         <v>1824</v>
@@ -8757,9 +8789,7 @@
       <c r="F8" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G8" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="G8" s="34"/>
       <c r="H8" s="34" t="s">
         <v>1848</v>
       </c>
@@ -8769,18 +8799,18 @@
     </row>
     <row r="9" spans="1:11" ht="15">
       <c r="A9" s="31" t="s">
-        <v>1822</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>1826</v>
-      </c>
-      <c r="C9" s="31" t="str">
-        <f>'Attribution du dossier'!$B$1</f>
+        <v>1825</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C9" s="54" t="str">
+        <f>'Type de requérant'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D9" s="31" t="str">
-        <f>'Attribution du dossier'!$B$2</f>
-        <v>DEVENIRD</v>
+        <f>'Type de requérant'!$B$2</f>
+        <v>TYPAPPLT</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>1824</v>
@@ -8788,7 +8818,9 @@
       <c r="F9" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G9" s="34"/>
+      <c r="G9" s="34" t="s">
+        <v>1848</v>
+      </c>
       <c r="H9" s="34" t="s">
         <v>1848</v>
       </c>
@@ -8798,18 +8830,18 @@
     </row>
     <row r="10" spans="1:11" ht="15">
       <c r="A10" s="31" t="s">
-        <v>1822</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>1834</v>
-      </c>
-      <c r="C10" s="31" t="str">
-        <f>'Priorité de régulation médicale'!$B$1</f>
+        <v>1825</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C10" s="54" t="str">
+        <f>'Difficultés de communication'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D10" s="31" t="str">
-        <f>'Priorité de régulation médicale'!$B$2</f>
-        <v>PRIORITE</v>
+        <f>'Difficultés de communication'!$B$2</f>
+        <v>PBAPL</v>
       </c>
       <c r="E10" s="33" t="s">
         <v>1824</v>
@@ -8817,7 +8849,9 @@
       <c r="F10" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G10" s="34"/>
+      <c r="G10" s="34" t="s">
+        <v>1848</v>
+      </c>
       <c r="H10" s="34" t="s">
         <v>1848</v>
       </c>
@@ -8826,19 +8860,19 @@
       <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:11" ht="15">
-      <c r="A11" s="31" t="s">
-        <v>1825</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>1831</v>
-      </c>
-      <c r="C11" s="31" t="str">
-        <f>'Type de requérant'!$B$1</f>
+      <c r="A11" s="32" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C11" s="54" t="str">
+        <f>Sexe!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D11" s="31" t="str">
-        <f>'Type de requérant'!$B$2</f>
-        <v>TYPAPPLT</v>
+        <f>Sexe!$B$2</f>
+        <v>NOMENC_SEXE</v>
       </c>
       <c r="E11" s="33" t="s">
         <v>1824</v>
@@ -8857,19 +8891,19 @@
       <c r="K11" s="34"/>
     </row>
     <row r="12" spans="1:11" ht="15">
-      <c r="A12" s="31" t="s">
-        <v>1825</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>1832</v>
-      </c>
-      <c r="C12" s="31" t="str">
-        <f>'Difficultés de communication'!$B$1</f>
+      <c r="A12" s="32" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>1836</v>
+      </c>
+      <c r="C12" s="54" t="str">
+        <f>'Niveau de soin'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D12" s="31" t="str">
-        <f>'Difficultés de communication'!$B$2</f>
-        <v>PBAPL</v>
+        <f>'Niveau de soin'!$B$2</f>
+        <v>GRAVITE</v>
       </c>
       <c r="E12" s="33" t="s">
         <v>1824</v>
@@ -8877,9 +8911,7 @@
       <c r="F12" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G12" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="G12" s="34"/>
       <c r="H12" s="34" t="s">
         <v>1848</v>
       </c>
@@ -8888,19 +8920,19 @@
       <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:11" ht="15">
-      <c r="A13" s="32" t="s">
-        <v>1841</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>1835</v>
-      </c>
-      <c r="C13" s="31" t="str">
-        <f>Sexe!$B$1</f>
+      <c r="A13" s="31" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C13" s="54" t="str">
+        <f>'Type de décision'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D13" s="31" t="str">
-        <f>Sexe!$B$2</f>
-        <v>NOMENC_SEXE</v>
+        <f>'Type de décision'!$B$2</f>
+        <v>TYPEDEC</v>
       </c>
       <c r="E13" s="33" t="s">
         <v>1824</v>
@@ -8919,19 +8951,19 @@
       <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="32" t="s">
-        <v>1841</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>1836</v>
-      </c>
-      <c r="C14" s="31" t="str">
-        <f>'Niveau de soin'!$B$1</f>
+      <c r="A14" s="31" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C14" s="54" t="str">
+        <f>'Type de ressource'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D14" s="31" t="str">
-        <f>'Niveau de soin'!$B$2</f>
-        <v>GRAVITE</v>
+        <f>'Type de ressource'!$B$2</f>
+        <v>TYPE_MOYEN</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>1824</v>
@@ -8943,24 +8975,28 @@
       <c r="H14" s="34" t="s">
         <v>1848</v>
       </c>
-      <c r="I14" s="34"/>
+      <c r="I14" s="34" t="s">
+        <v>1848</v>
+      </c>
       <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
+      <c r="K14" s="34" t="s">
+        <v>1848</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15">
-      <c r="A15" s="31" t="s">
-        <v>1842</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>1837</v>
-      </c>
-      <c r="C15" s="31" t="str">
-        <f>'Type de décision'!$B$1</f>
-        <v>SI-SAMU</v>
+      <c r="A15" s="32" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>1853</v>
+      </c>
+      <c r="C15" s="54" t="str">
+        <f>'Type de vecteurs'!$B$1</f>
+        <v>CISU</v>
       </c>
       <c r="D15" s="31" t="str">
-        <f>'Type de décision'!$B$2</f>
-        <v>TYPEDEC</v>
+        <f>'Type de vecteurs'!$B$2</f>
+        <v>TYPE_VECTEUR</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>1824</v>
@@ -8968,30 +9004,32 @@
       <c r="F15" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G15" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="G15" s="34"/>
       <c r="H15" s="34" t="s">
         <v>1848</v>
       </c>
-      <c r="I15" s="34"/>
+      <c r="I15" s="34" t="s">
+        <v>1848</v>
+      </c>
       <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
+      <c r="K15" s="34" t="s">
+        <v>1848</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="15">
       <c r="A16" s="31" t="s">
         <v>1851</v>
       </c>
-      <c r="B16" s="40" t="s">
-        <v>1839</v>
-      </c>
-      <c r="C16" s="37" t="str">
-        <f>'Type de ressource'!$B$1</f>
+      <c r="B16" s="38" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C16" s="31" t="str">
+        <f>'Niveau de prise en charge'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D16" s="31" t="str">
-        <f>'Type de ressource'!$B$2</f>
-        <v>TYPE_MOYEN</v>
+        <f>'Niveau de prise en charge'!$B$2</f>
+        <v>NIVSOIN</v>
       </c>
       <c r="E16" s="33" t="s">
         <v>1824</v>
@@ -8999,7 +9037,9 @@
       <c r="F16" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G16" s="34"/>
+      <c r="G16" s="34" t="s">
+        <v>1848</v>
+      </c>
       <c r="H16" s="34" t="s">
         <v>1848</v>
       </c>
@@ -9012,19 +9052,19 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15">
-      <c r="A17" s="32" t="s">
-        <v>1851</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>1853</v>
+      <c r="A17" s="31" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>1838</v>
       </c>
       <c r="C17" s="31" t="str">
-        <f>'Type de vecteurs'!$B$1</f>
-        <v>CISU</v>
+        <f>'Type de devenir du patient'!$B$1</f>
+        <v>SI-SAMU</v>
       </c>
       <c r="D17" s="31" t="str">
-        <f>'Type de vecteurs'!$B$2</f>
-        <v>TYPE_VECTEUR</v>
+        <f>'Type de devenir du patient'!$B$2</f>
+        <v>NOMENC_DEVENIR_PAT</v>
       </c>
       <c r="E17" s="33" t="s">
         <v>1824</v>
@@ -9032,32 +9072,30 @@
       <c r="F17" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G17" s="34"/>
+      <c r="G17" s="34" t="s">
+        <v>1848</v>
+      </c>
       <c r="H17" s="34" t="s">
         <v>1848</v>
       </c>
-      <c r="I17" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="I17" s="34"/>
       <c r="J17" s="34"/>
-      <c r="K17" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="K17" s="34"/>
     </row>
     <row r="18" spans="1:11" ht="15">
-      <c r="A18" s="31" t="s">
-        <v>1851</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>1849</v>
+      <c r="A18" s="32" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>1833</v>
       </c>
       <c r="C18" s="31" t="str">
-        <f>'Niveau de prise en charge'!$B$1</f>
-        <v>SI-SAMU</v>
+        <f>'Effet à obtenir'!$B$1</f>
+        <v>CISU</v>
       </c>
       <c r="D18" s="31" t="str">
-        <f>'Niveau de prise en charge'!$B$2</f>
-        <v>NIVSOIN</v>
+        <f>'Effet à obtenir'!$B$2</f>
+        <v>Code_Effet_a_obtenir</v>
       </c>
       <c r="E18" s="33" t="s">
         <v>1824</v>
@@ -9065,86 +9103,46 @@
       <c r="F18" s="32" t="s">
         <v>1840</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34" t="s">
         <v>1848</v>
       </c>
-      <c r="H18" s="34" t="s">
-        <v>1848</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>1848</v>
-      </c>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="K18" s="34"/>
     </row>
     <row r="19" spans="1:11" ht="15">
-      <c r="A19" s="31" t="s">
-        <v>1842</v>
-      </c>
-      <c r="B19" s="40" t="s">
-        <v>1838</v>
-      </c>
-      <c r="C19" s="31" t="str">
-        <f>'Type de devenir du patient'!$B$1</f>
-        <v>SI-SAMU</v>
-      </c>
-      <c r="D19" s="31" t="str">
-        <f>'Type de devenir du patient'!$B$2</f>
-        <v>NOMENC_DEVENIR_PAT</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>1824</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>1840</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>1848</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="A19" s="32"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
     </row>
-    <row r="20" spans="1:11" ht="15">
-      <c r="A20" s="32" t="s">
-        <v>1852</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>1833</v>
-      </c>
-      <c r="C20" s="31" t="str">
-        <f>'Effet à obtenir'!$B$1</f>
-        <v>CISU</v>
-      </c>
-      <c r="D20" s="31" t="str">
-        <f>'Effet à obtenir'!$B$2</f>
-        <v>Code_Effet_a_obtenir</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>1824</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>1840</v>
-      </c>
+    <row r="20" spans="1:11">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="34"/>
       <c r="H20" s="34"/>
       <c r="I20" s="34"/>
-      <c r="J20" s="34" t="s">
-        <v>1848</v>
-      </c>
+      <c r="J20" s="34"/>
       <c r="K20" s="34"/>
     </row>
-    <row r="21" spans="1:11" ht="15">
+    <row r="21" spans="1:11">
       <c r="A21" s="32"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="32"/>
-      <c r="E21" s="33"/>
+      <c r="E21" s="32"/>
       <c r="F21" s="32"/>
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
@@ -9419,11 +9417,11 @@
       <c r="D42" s="32"/>
       <c r="E42" s="32"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="32"/>
@@ -9432,11 +9430,11 @@
       <c r="D43" s="32"/>
       <c r="E43" s="32"/>
       <c r="F43" s="32"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
-      <c r="K43" s="34"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="32"/>
@@ -11700,38 +11698,9 @@
       <c r="J217" s="32"/>
       <c r="K217" s="32"/>
     </row>
-    <row r="218" spans="1:11">
-      <c r="A218" s="32"/>
-      <c r="B218" s="32"/>
-      <c r="C218" s="32"/>
-      <c r="D218" s="32"/>
-      <c r="E218" s="32"/>
-      <c r="F218" s="32"/>
-      <c r="G218" s="32"/>
-      <c r="H218" s="32"/>
-      <c r="I218" s="32"/>
-      <c r="J218" s="32"/>
-      <c r="K218" s="32"/>
-    </row>
-    <row r="219" spans="1:11">
-      <c r="A219" s="32"/>
-      <c r="B219" s="32"/>
-      <c r="C219" s="32"/>
-      <c r="D219" s="32"/>
-      <c r="E219" s="32"/>
-      <c r="F219" s="32"/>
-      <c r="G219" s="32"/>
-      <c r="H219" s="32"/>
-      <c r="I219" s="32"/>
-      <c r="J219" s="32"/>
-      <c r="K219" s="32"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A4:K20" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}"/>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A5:K219">
+  <autoFilter ref="A2:K18" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}"/>
+  <conditionalFormatting sqref="A3:K217">
     <cfRule type="expression" dxfId="2" priority="6">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
@@ -11739,32 +11708,32 @@
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:K20">
+  <conditionalFormatting sqref="G3:K18">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>G5=""</formula>
+      <formula>G3=""</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>G5="X"</formula>
+      <formula>G3="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E5" location="'Nature de fait'!A1" display="Lien nomenclature" xr:uid="{539BD578-8B92-438E-9797-279F8E85B856}"/>
-    <hyperlink ref="E6" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{83312ADE-108A-4D25-8BE7-27C9395C4886}"/>
-    <hyperlink ref="E7:E20" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{29712ED5-564A-4FD2-8437-4B4AE7679944}"/>
-    <hyperlink ref="E7" location="'Risque, menace et sensibilité'!A1" display="Lien nomenclature" xr:uid="{9F738CF9-B437-4A27-8CF2-C50C5C0734F4}"/>
-    <hyperlink ref="E8" location="'Motif de recours médico-secouri'!A1" display="Lien nomenclature" xr:uid="{34887817-DE20-4996-9B54-60201BD7BF6B}"/>
-    <hyperlink ref="E9" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{3EDF5532-205A-406E-822B-B79908DFAF6A}"/>
-    <hyperlink ref="E10" location="'Priorité de régulation médicale'!A1" display="Lien nomenclature" xr:uid="{D59E4120-4823-486C-9505-D44F77A631EC}"/>
-    <hyperlink ref="E11" location="'Type de requérant'!A1" display="Lien nomenclature" xr:uid="{379E2147-AD1C-464C-83FF-DA5B8754B9E0}"/>
-    <hyperlink ref="E12" location="'Difficultés de communication'!A1" display="Lien nomenclature" xr:uid="{178F7592-0B6B-4DA8-89F4-525A55C10FA0}"/>
-    <hyperlink ref="E13" location="Sexe!A1" display="Lien nomenclature" xr:uid="{65BDA639-D0DB-4DC1-8264-8E35FE3B2996}"/>
-    <hyperlink ref="E14" location="'Niveau de soin'!A1" display="Lien nomenclature" xr:uid="{30F27E7E-2FB0-4F79-A16D-620776E8FCF1}"/>
-    <hyperlink ref="E15" location="'Type de décision'!A1" display="Lien nomenclature" xr:uid="{4F195D5A-2BD1-4EA9-BE69-3011CC92C820}"/>
-    <hyperlink ref="E16" location="'Type de ressource'!A1" display="Lien nomenclature" xr:uid="{3CDD18B1-CEEB-4D52-9CB8-283B075579C8}"/>
-    <hyperlink ref="E17" location="'Type de vecteurs'!A1" display="Lien nomenclature" xr:uid="{4A249EF4-3DA2-4A6E-947A-08D74AFD0EF9}"/>
-    <hyperlink ref="E18" location="'Niveau de prise en charge'!A1" display="Lien nomenclature" xr:uid="{2154EBB7-71EE-44B5-BBEE-716579483CDC}"/>
-    <hyperlink ref="E19" location="'Type de devenir du patient'!A1" display="Lien nomenclature" xr:uid="{0E2A9314-0B8D-4156-A7C3-BC0E2885D9D2}"/>
-    <hyperlink ref="E20" location="'Effet à obtenir'!A1" display="Lien nomenclature" xr:uid="{F32B9CB2-26FC-4D51-B612-B9EB269DC3B1}"/>
+    <hyperlink ref="E3" location="'Nature de fait'!A1" display="Lien nomenclature" xr:uid="{539BD578-8B92-438E-9797-279F8E85B856}"/>
+    <hyperlink ref="E4" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{83312ADE-108A-4D25-8BE7-27C9395C4886}"/>
+    <hyperlink ref="E5:E18" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{29712ED5-564A-4FD2-8437-4B4AE7679944}"/>
+    <hyperlink ref="E5" location="'Risque, menace et sensibilité'!A1" display="Lien nomenclature" xr:uid="{9F738CF9-B437-4A27-8CF2-C50C5C0734F4}"/>
+    <hyperlink ref="E6" location="'Motif de recours médico-secouri'!A1" display="Lien nomenclature" xr:uid="{34887817-DE20-4996-9B54-60201BD7BF6B}"/>
+    <hyperlink ref="E7" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{3EDF5532-205A-406E-822B-B79908DFAF6A}"/>
+    <hyperlink ref="E8" location="'Priorité de régulation médicale'!A1" display="Lien nomenclature" xr:uid="{D59E4120-4823-486C-9505-D44F77A631EC}"/>
+    <hyperlink ref="E9" location="'Type de requérant'!A1" display="Lien nomenclature" xr:uid="{379E2147-AD1C-464C-83FF-DA5B8754B9E0}"/>
+    <hyperlink ref="E10" location="'Difficultés de communication'!A1" display="Lien nomenclature" xr:uid="{178F7592-0B6B-4DA8-89F4-525A55C10FA0}"/>
+    <hyperlink ref="E11" location="Sexe!A1" display="Lien nomenclature" xr:uid="{65BDA639-D0DB-4DC1-8264-8E35FE3B2996}"/>
+    <hyperlink ref="E12" location="'Niveau de soin'!A1" display="Lien nomenclature" xr:uid="{30F27E7E-2FB0-4F79-A16D-620776E8FCF1}"/>
+    <hyperlink ref="E13" location="'Type de décision'!A1" display="Lien nomenclature" xr:uid="{4F195D5A-2BD1-4EA9-BE69-3011CC92C820}"/>
+    <hyperlink ref="E14" location="'Type de ressource'!A1" display="Lien nomenclature" xr:uid="{3CDD18B1-CEEB-4D52-9CB8-283B075579C8}"/>
+    <hyperlink ref="E15" location="'Type de vecteurs'!A1" display="Lien nomenclature" xr:uid="{4A249EF4-3DA2-4A6E-947A-08D74AFD0EF9}"/>
+    <hyperlink ref="E16" location="'Niveau de prise en charge'!A1" display="Lien nomenclature" xr:uid="{2154EBB7-71EE-44B5-BBEE-716579483CDC}"/>
+    <hyperlink ref="E17" location="'Type de devenir du patient'!A1" display="Lien nomenclature" xr:uid="{0E2A9314-0B8D-4156-A7C3-BC0E2885D9D2}"/>
+    <hyperlink ref="E18" location="'Effet à obtenir'!A1" display="Lien nomenclature" xr:uid="{F32B9CB2-26FC-4D51-B612-B9EB269DC3B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15175,8 +15144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -15184,7 +15153,7 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="56.140625" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="61.5703125" customWidth="1"/>
     <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15268,203 +15237,207 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="52" t="s">
-        <v>1938</v>
-      </c>
-      <c r="B10" s="41" t="s">
+      <c r="A10" s="48" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B10" s="53" t="s">
         <v>1855</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="40"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="49" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="50" t="s">
         <v>1939</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>1856</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="54" t="s">
+      <c r="B12" s="39" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="50" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="50" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>1936</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40" t="s">
+        <v>1948</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="50" t="s">
+        <v>1573</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="50" t="s">
         <v>1940</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>1857</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="54" t="s">
-        <v>1580</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>1935</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="54" t="s">
-        <v>1444</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>1936</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="54" t="s">
-        <v>1573</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>1858</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="54" t="s">
+      <c r="B16" s="40" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40" t="s">
+        <v>1946</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="51" t="s">
         <v>1941</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>1859</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="55" t="s">
+      <c r="B17" s="39" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="52" t="s">
         <v>1942</v>
       </c>
-      <c r="B17" s="41" t="s">
-        <v>1860</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="56" t="s">
+      <c r="B18" s="39" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="50" t="s">
         <v>1943</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>1937</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="54" t="s">
+      <c r="B19" s="39" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="50" t="s">
         <v>1944</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>1861</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="54" t="s">
+      <c r="B20" s="39" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="50" t="s">
         <v>1945</v>
       </c>
-      <c r="B20" s="41" t="s">
-        <v>1862</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="54" t="s">
-        <v>1946</v>
-      </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="39" t="s">
         <v>1863</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="2"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="40"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="2"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="2"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="2"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2"/>
-      <c r="B29" s="42"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2"/>
-      <c r="B31" s="43"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -15753,8 +15726,8 @@
       <c r="B10" s="21" t="s">
         <v>1866</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="21" t="s">
         <v>1932</v>
       </c>
@@ -15766,8 +15739,8 @@
       <c r="B11" s="21" t="s">
         <v>1899</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="21" t="s">
         <v>1933</v>
       </c>
@@ -15779,8 +15752,8 @@
       <c r="B12" s="21" t="s">
         <v>1900</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="21" t="s">
         <v>1906</v>
       </c>
@@ -15792,8 +15765,8 @@
       <c r="B13" s="21" t="s">
         <v>1901</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="21" t="s">
         <v>1907</v>
       </c>
@@ -15805,8 +15778,8 @@
       <c r="B14" s="21" t="s">
         <v>1902</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="21" t="s">
         <v>1908</v>
       </c>
@@ -15818,8 +15791,8 @@
       <c r="B15" s="21" t="s">
         <v>1903</v>
       </c>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
       <c r="E15" s="21" t="s">
         <v>1909</v>
       </c>
@@ -15831,8 +15804,8 @@
       <c r="B16" s="21" t="s">
         <v>1894</v>
       </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="21" t="s">
         <v>1910</v>
       </c>
@@ -15844,8 +15817,8 @@
       <c r="B17" s="21" t="s">
         <v>1904</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="21" t="s">
         <v>1911</v>
       </c>
@@ -15857,8 +15830,8 @@
       <c r="B18" s="21" t="s">
         <v>1905</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="21" t="s">
         <v>1912</v>
       </c>
@@ -15870,8 +15843,8 @@
       <c r="B19" s="21" t="s">
         <v>1898</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="21" t="s">
         <v>1913</v>
       </c>
@@ -15888,74 +15861,74 @@
       <c r="B21" s="21"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="45"/>
-    </row>
-    <row r="22" spans="1:5" s="48" customFormat="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="46"/>
+      <c r="E21" s="43"/>
+    </row>
+    <row r="22" spans="1:5" s="46" customFormat="1">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="44"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2"/>
-      <c r="B23" s="44"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2"/>
-      <c r="B24" s="41"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2"/>
-      <c r="B25" s="44"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2"/>
-      <c r="B26" s="41"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2"/>
-      <c r="B27" s="42"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2"/>
-      <c r="B28" s="42"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2"/>
-      <c r="B29" s="42"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2"/>
-      <c r="B31" s="43"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -16391,78 +16364,78 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" s="48" customFormat="1">
-      <c r="A22" s="46" t="s">
+    <row r="22" spans="1:5" s="46" customFormat="1">
+      <c r="A22" s="44" t="s">
         <v>1880</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="44" t="s">
         <v>1881</v>
       </c>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="46" t="s">
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="44" t="s">
         <v>1885</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2"/>
-      <c r="B23" s="44"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2"/>
-      <c r="B24" s="41"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2"/>
-      <c r="B25" s="44"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2"/>
-      <c r="B26" s="41"/>
+      <c r="B26" s="39"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2"/>
-      <c r="B27" s="42"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2"/>
-      <c r="B28" s="42"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2"/>
-      <c r="B29" s="42"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2"/>
-      <c r="B30" s="42"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2"/>
-      <c r="B31" s="43"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -26967,15 +26940,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -27027,32 +26991,57 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8EAFAAD-45BD-4A4A-9EC1-DDF1B9581D22}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F317E4A3-C0C5-4204-BAF7-619A6A4AE4A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.07.03 09:43] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romainfouilland/Library/CloudStorage/OneDrive-SharedLibraries-ANS/Espace Projets - Espace Programme SI-SAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1054" documentId="11_D1219352A73AC3F06E4E08ED344B052DFE2EB084" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43A645E5-0C8D-4214-85A8-C0C88A86B91D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1890" yWindow="450" windowWidth="25455" windowHeight="13980" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="877" firstSheet="13" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <sheet name="#Delai de réponse" sheetId="39" r:id="rId19"/>
     <sheet name="#Nombre de patients-victimes" sheetId="2" r:id="rId20"/>
     <sheet name="#Informations sur le requérant" sheetId="4" r:id="rId21"/>
+    <sheet name="#Code Antares" sheetId="41" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$2:$K$18</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="1949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="2039">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -6124,6 +6125,276 @@
   </si>
   <si>
     <t>Pour obtenir une consultation ou une visite du MG (uniquement pour lien 15-15)</t>
+  </si>
+  <si>
+    <t>Code Antares</t>
+  </si>
+  <si>
+    <t>nexsis_code_situation</t>
+  </si>
+  <si>
+    <t>signification</t>
+  </si>
+  <si>
+    <t>Libelle_ long</t>
+  </si>
+  <si>
+    <t>Libelle_court</t>
+  </si>
+  <si>
+    <t>type_status</t>
+  </si>
+  <si>
+    <t>PARTI</t>
+  </si>
+  <si>
+    <t>Parti indisponible</t>
+  </si>
+  <si>
+    <t>mobilisation</t>
+  </si>
+  <si>
+    <t>SUR_LES_LIEUX</t>
+  </si>
+  <si>
+    <t>Sur les lieux indisponible</t>
+  </si>
+  <si>
+    <t>SUR LES LIEUX</t>
+  </si>
+  <si>
+    <t>SLL</t>
+  </si>
+  <si>
+    <t>Demande de parole pour message</t>
+  </si>
+  <si>
+    <t>MESSAGE</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Demande de parole pour message urgent</t>
+  </si>
+  <si>
+    <t>MESSAGE URGENT</t>
+  </si>
+  <si>
+    <t>MESS URG</t>
+  </si>
+  <si>
+    <t>EN_TRANSIT_HOPITAL</t>
+  </si>
+  <si>
+    <t>Transport au centre hospitalierindisponible</t>
+  </si>
+  <si>
+    <t>TRANSP. HOPITAL</t>
+  </si>
+  <si>
+    <t>TRANS HOP</t>
+  </si>
+  <si>
+    <t>ARRIVE_HOPITAL</t>
+  </si>
+  <si>
+    <t>ArrivÈe au centre hospitalierl indisponible</t>
+  </si>
+  <si>
+    <t>ARRIVEE HOPITAL</t>
+  </si>
+  <si>
+    <t>ARR HOP</t>
+  </si>
+  <si>
+    <t>Disponible</t>
+  </si>
+  <si>
+    <t>DISPONIBLE</t>
+  </si>
+  <si>
+    <t>DISPO</t>
+  </si>
+  <si>
+    <t>INDISPONIBLE</t>
+  </si>
+  <si>
+    <t>RENTRE_A_UF</t>
+  </si>
+  <si>
+    <t>RentrÈ indisponible</t>
+  </si>
+  <si>
+    <t>RENTRE</t>
+  </si>
+  <si>
+    <t>Reconnaissance en cours</t>
+  </si>
+  <si>
+    <t>REC. EN COURS</t>
+  </si>
+  <si>
+    <t>REC COURS</t>
+  </si>
+  <si>
+    <t>Feu circonscrit</t>
+  </si>
+  <si>
+    <t>FEU CIRCONSCRIT</t>
+  </si>
+  <si>
+    <t>FEU CIRC</t>
+  </si>
+  <si>
+    <t>Ma√Ætre du feu</t>
+  </si>
+  <si>
+    <t>MAITRE DU FEU</t>
+  </si>
+  <si>
+    <t>MTRE FEU</t>
+  </si>
+  <si>
+    <t>Feu Èteint</t>
+  </si>
+  <si>
+    <t>FEU ETEINT</t>
+  </si>
+  <si>
+    <t>F. ETEINT</t>
+  </si>
+  <si>
+    <t>RETOUR_VERS_UF</t>
+  </si>
+  <si>
+    <t>Quitte les lieux du sinistre indisponible</t>
+  </si>
+  <si>
+    <t>QUITTE LES LIEUX</t>
+  </si>
+  <si>
+    <t>QTTE LIEUX</t>
+  </si>
+  <si>
+    <t>Victime  refusant son transport</t>
+  </si>
+  <si>
+    <t>VIC REFUS. TRANSP</t>
+  </si>
+  <si>
+    <t>VIC REF T</t>
+  </si>
+  <si>
+    <t>Victime dÈcÈdÈe</t>
+  </si>
+  <si>
+    <t>VICTIME DECEDEE</t>
+  </si>
+  <si>
+    <t>VIC DCD</t>
+  </si>
+  <si>
+    <t>SMUR sur les lieux</t>
+  </si>
+  <si>
+    <t>SMUR SLL</t>
+  </si>
+  <si>
+    <t>Quitte le centre hospitalier indisponible</t>
+  </si>
+  <si>
+    <t>QUITTE HOP</t>
+  </si>
+  <si>
+    <t>QTTE HOP</t>
+  </si>
+  <si>
+    <t>Police sur les lieux</t>
+  </si>
+  <si>
+    <t>POLICE SLL</t>
+  </si>
+  <si>
+    <t>POL SLL</t>
+  </si>
+  <si>
+    <t>Gendarmerie sur les lieux</t>
+  </si>
+  <si>
+    <t>GENDARMERIE SLL</t>
+  </si>
+  <si>
+    <t>GEND SLL</t>
+  </si>
+  <si>
+    <t>EDF sur les lieux</t>
+  </si>
+  <si>
+    <t>EDF SLL</t>
+  </si>
+  <si>
+    <t>GDF sur les lieux</t>
+  </si>
+  <si>
+    <t>GDF SLL</t>
+  </si>
+  <si>
+    <t>DDT sur les lieux</t>
+  </si>
+  <si>
+    <t>DDT SLL</t>
+  </si>
+  <si>
+    <t>Accueil (inscription Flotte dÈpartement d'accueil)</t>
+  </si>
+  <si>
+    <t>ACCUEIL</t>
+  </si>
+  <si>
+    <t>inscription</t>
+  </si>
+  <si>
+    <t>Demande confirmation d'appel et d'adresse</t>
+  </si>
+  <si>
+    <t>DM CNF APP ET AD</t>
+  </si>
+  <si>
+    <t>DCAA</t>
+  </si>
+  <si>
+    <t>Demande Police ou Gendarmerie</t>
+  </si>
+  <si>
+    <t>DEM POLICE OU GEND</t>
+  </si>
+  <si>
+    <t>D. POL GEN</t>
+  </si>
+  <si>
+    <t>renfort</t>
+  </si>
+  <si>
+    <t>Demande SMUR</t>
+  </si>
+  <si>
+    <t>DEM SMUR</t>
+  </si>
+  <si>
+    <t>D. SMUR</t>
+  </si>
+  <si>
+    <t>DÈtresse d'un moyen</t>
+  </si>
+  <si>
+    <t>DETRESSE</t>
+  </si>
+  <si>
+    <t>SOS</t>
+  </si>
+  <si>
+    <t>sos</t>
   </si>
 </sst>
 </file>
@@ -6527,8 +6798,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
+    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
@@ -8559,20 +8830,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
   <dimension ref="A1:K217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="31" style="28" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="28" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="28" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="37.1640625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="28" customWidth="1"/>
     <col min="7" max="11" width="9" style="28" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="28"/>
+    <col min="12" max="16384" width="11.5" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -8580,7 +8851,7 @@
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:11" s="30" customFormat="1" ht="15">
+    <row r="2" spans="1:11" s="30" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>1850</v>
       </c>
@@ -8615,7 +8886,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15">
+    <row r="3" spans="1:11">
       <c r="A3" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8646,7 +8917,7 @@
       <c r="J3" s="34"/>
       <c r="K3" s="34"/>
     </row>
-    <row r="4" spans="1:11" ht="15">
+    <row r="4" spans="1:11">
       <c r="A4" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8677,7 +8948,7 @@
       <c r="J4" s="34"/>
       <c r="K4" s="34"/>
     </row>
-    <row r="5" spans="1:11" ht="15">
+    <row r="5" spans="1:11">
       <c r="A5" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8708,7 +8979,7 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:11">
       <c r="A6" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8739,7 +9010,7 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:11">
       <c r="A7" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8768,7 +9039,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:11">
       <c r="A8" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8797,7 +9068,7 @@
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:11">
       <c r="A9" s="31" t="s">
         <v>1825</v>
       </c>
@@ -8828,7 +9099,7 @@
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
     </row>
-    <row r="10" spans="1:11" ht="15">
+    <row r="10" spans="1:11">
       <c r="A10" s="31" t="s">
         <v>1825</v>
       </c>
@@ -8859,7 +9130,7 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
     </row>
-    <row r="11" spans="1:11" ht="15">
+    <row r="11" spans="1:11">
       <c r="A11" s="32" t="s">
         <v>1841</v>
       </c>
@@ -8890,7 +9161,7 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
     </row>
-    <row r="12" spans="1:11" ht="15">
+    <row r="12" spans="1:11">
       <c r="A12" s="32" t="s">
         <v>1841</v>
       </c>
@@ -8919,7 +9190,7 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
     </row>
-    <row r="13" spans="1:11" ht="15">
+    <row r="13" spans="1:11">
       <c r="A13" s="31" t="s">
         <v>1842</v>
       </c>
@@ -8950,7 +9221,7 @@
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
     </row>
-    <row r="14" spans="1:11" ht="15">
+    <row r="14" spans="1:11">
       <c r="A14" s="31" t="s">
         <v>1851</v>
       </c>
@@ -8983,7 +9254,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15">
+    <row r="15" spans="1:11">
       <c r="A15" s="32" t="s">
         <v>1851</v>
       </c>
@@ -9016,7 +9287,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15">
+    <row r="16" spans="1:11">
       <c r="A16" s="31" t="s">
         <v>1851</v>
       </c>
@@ -9051,7 +9322,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15">
+    <row r="17" spans="1:11">
       <c r="A17" s="31" t="s">
         <v>1842</v>
       </c>
@@ -9082,7 +9353,7 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
     </row>
-    <row r="18" spans="1:11" ht="15">
+    <row r="18" spans="1:11">
       <c r="A18" s="32" t="s">
         <v>1852</v>
       </c>
@@ -9111,7 +9382,7 @@
       </c>
       <c r="K18" s="34"/>
     </row>
-    <row r="19" spans="1:11" ht="15">
+    <row r="19" spans="1:11">
       <c r="A19" s="32"/>
       <c r="B19" s="35"/>
       <c r="C19" s="31"/>
@@ -11747,13 +12018,13 @@
       <selection activeCell="E9" sqref="E9:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
-    <col min="6" max="6" width="61.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="6" max="6" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -11907,14 +12178,14 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12336,14 +12607,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12781,13 +13052,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13231,12 +13502,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14212,13 +14483,13 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14634,13 +14905,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15148,13 +15419,13 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15236,7 +15507,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="48" t="s">
         <v>1937</v>
       </c>
@@ -15258,7 +15529,7 @@
       <c r="D11" s="40"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="50" t="s">
         <v>1939</v>
       </c>
@@ -15269,7 +15540,7 @@
       <c r="D12" s="40"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="16">
       <c r="A13" s="50" t="s">
         <v>1580</v>
       </c>
@@ -15280,7 +15551,7 @@
       <c r="D13" s="40"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" s="50" t="s">
         <v>1444</v>
       </c>
@@ -15293,7 +15564,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="16">
       <c r="A15" s="50" t="s">
         <v>1573</v>
       </c>
@@ -15304,7 +15575,7 @@
       <c r="D15" s="40"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="16">
       <c r="A16" s="50" t="s">
         <v>1940</v>
       </c>
@@ -15317,7 +15588,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="16">
       <c r="A17" s="51" t="s">
         <v>1941</v>
       </c>
@@ -15328,7 +15599,7 @@
       <c r="D17" s="40"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="16">
       <c r="A18" s="52" t="s">
         <v>1942</v>
       </c>
@@ -15339,7 +15610,7 @@
       <c r="D18" s="40"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="16">
       <c r="A19" s="50" t="s">
         <v>1943</v>
       </c>
@@ -15350,7 +15621,7 @@
       <c r="D19" s="40"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="16">
       <c r="A20" s="50" t="s">
         <v>1944</v>
       </c>
@@ -15361,7 +15632,7 @@
       <c r="D20" s="40"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="16">
       <c r="A21" s="50" t="s">
         <v>1945</v>
       </c>
@@ -15631,13 +15902,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="80.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="80.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16120,13 +16391,13 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16624,14 +16895,14 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" customWidth="1"/>
+    <col min="5" max="5" width="47.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16714,7 +16985,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="64.5">
+    <row r="10" spans="1:6" ht="60">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -16740,7 +17011,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -16754,7 +17025,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="26.25">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -16768,7 +17039,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -16781,7 +17052,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" ht="26.25">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -16809,7 +17080,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="26.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -16835,7 +17106,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -16850,7 +17121,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -16876,7 +17147,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="39">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -16890,7 +17161,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="39">
+    <row r="23" spans="1:6" ht="30">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -16914,7 +17185,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25">
+    <row r="25" spans="1:6" ht="30">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -16928,7 +17199,7 @@
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="26.25">
+    <row r="26" spans="1:6" ht="30">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -16942,7 +17213,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="26.25">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -16956,7 +17227,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6" ht="26.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -16992,7 +17263,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:6" ht="51.75">
+    <row r="31" spans="1:6" ht="60">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -17006,7 +17277,7 @@
       </c>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" ht="26.25">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
@@ -17045,7 +17316,7 @@
       </c>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25">
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -17071,7 +17342,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" ht="102.75">
+    <row r="37" spans="1:6" ht="120">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
@@ -17085,7 +17356,7 @@
       </c>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" ht="26.25">
+    <row r="38" spans="1:6" ht="30">
       <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
@@ -17099,7 +17370,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="39">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -17124,7 +17395,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" ht="39">
+    <row r="41" spans="1:6" ht="30">
       <c r="A41" s="2" t="s">
         <v>116</v>
       </c>
@@ -17138,7 +17409,7 @@
       </c>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>119</v>
       </c>
@@ -17152,7 +17423,7 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" ht="39">
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -17176,7 +17447,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" ht="39">
+    <row r="45" spans="1:6" ht="45">
       <c r="A45" s="2" t="s">
         <v>127</v>
       </c>
@@ -17275,7 +17546,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6" ht="26.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
         <v>145</v>
       </c>
@@ -17289,7 +17560,7 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="64.5">
+    <row r="54" spans="1:6" ht="60">
       <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
@@ -17660,7 +17931,7 @@
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="1:6" ht="39">
+    <row r="85" spans="1:6" ht="45">
       <c r="A85" s="2" t="s">
         <v>214</v>
       </c>
@@ -17686,7 +17957,7 @@
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:6" ht="128.25">
+    <row r="87" spans="1:6" ht="135">
       <c r="A87" s="2" t="s">
         <v>219</v>
       </c>
@@ -17712,7 +17983,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="51.75">
+    <row r="89" spans="1:6" ht="60">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
@@ -17725,7 +17996,7 @@
       </c>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
         <v>214</v>
       </c>
@@ -17765,7 +18036,7 @@
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25">
+    <row r="93" spans="1:6" ht="30">
       <c r="A93" s="2" t="s">
         <v>230</v>
       </c>
@@ -17936,7 +18207,7 @@
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
     </row>
-    <row r="107" spans="1:6" ht="26.25">
+    <row r="107" spans="1:6" ht="30">
       <c r="A107" s="2" t="s">
         <v>261</v>
       </c>
@@ -17950,7 +18221,7 @@
       </c>
       <c r="F107" s="12"/>
     </row>
-    <row r="108" spans="1:6" ht="26.25">
+    <row r="108" spans="1:6">
       <c r="A108" s="2" t="s">
         <v>264</v>
       </c>
@@ -18074,7 +18345,7 @@
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" ht="26.25">
+    <row r="118" spans="1:6" ht="30">
       <c r="A118" s="2" t="s">
         <v>287</v>
       </c>
@@ -18088,7 +18359,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="26.25">
+    <row r="119" spans="1:6">
       <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
@@ -18101,7 +18372,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="39">
+    <row r="120" spans="1:6" ht="45">
       <c r="A120" s="2" t="s">
         <v>293</v>
       </c>
@@ -18139,7 +18410,7 @@
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" ht="39">
+    <row r="123" spans="1:6" ht="45">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -18200,7 +18471,7 @@
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" ht="39">
+    <row r="128" spans="1:6" ht="45">
       <c r="A128" s="2" t="s">
         <v>311</v>
       </c>
@@ -18334,7 +18605,7 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="26.25">
+    <row r="139" spans="1:6" ht="30">
       <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
@@ -18359,7 +18630,7 @@
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
     </row>
-    <row r="141" spans="1:6" ht="26.25">
+    <row r="141" spans="1:6" ht="30">
       <c r="A141" s="2" t="s">
         <v>341</v>
       </c>
@@ -18373,7 +18644,7 @@
       </c>
       <c r="F141" s="12"/>
     </row>
-    <row r="142" spans="1:6" ht="26.25">
+    <row r="142" spans="1:6" ht="30">
       <c r="A142" s="2" t="s">
         <v>342</v>
       </c>
@@ -18387,7 +18658,7 @@
       </c>
       <c r="F142" s="12"/>
     </row>
-    <row r="143" spans="1:6" ht="26.25">
+    <row r="143" spans="1:6">
       <c r="A143" s="2" t="s">
         <v>343</v>
       </c>
@@ -18401,7 +18672,7 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="26.25">
+    <row r="144" spans="1:6" ht="30">
       <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
@@ -18430,7 +18701,7 @@
       </c>
       <c r="F145" s="12"/>
     </row>
-    <row r="146" spans="1:6" ht="26.25">
+    <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
         <v>347</v>
       </c>
@@ -18444,7 +18715,7 @@
       </c>
       <c r="F146" s="12"/>
     </row>
-    <row r="147" spans="1:6" ht="39">
+    <row r="147" spans="1:6" ht="30">
       <c r="A147" s="2" t="s">
         <v>348</v>
       </c>
@@ -18458,7 +18729,7 @@
       </c>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" spans="1:6" ht="39">
+    <row r="148" spans="1:6" ht="30">
       <c r="A148" s="2" t="s">
         <v>349</v>
       </c>
@@ -18472,7 +18743,7 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="26.25">
+    <row r="149" spans="1:6" ht="30">
       <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
@@ -18485,7 +18756,7 @@
       </c>
       <c r="F149" s="12"/>
     </row>
-    <row r="150" spans="1:6" ht="26.25">
+    <row r="150" spans="1:6" ht="30">
       <c r="A150" s="2" t="s">
         <v>351</v>
       </c>
@@ -18499,7 +18770,7 @@
       </c>
       <c r="F150" s="12"/>
     </row>
-    <row r="151" spans="1:6" ht="26.25">
+    <row r="151" spans="1:6" ht="30">
       <c r="A151" s="2" t="s">
         <v>352</v>
       </c>
@@ -18631,7 +18902,7 @@
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
     </row>
-    <row r="162" spans="1:6" ht="39">
+    <row r="162" spans="1:6" ht="30">
       <c r="A162" s="2" t="s">
         <v>373</v>
       </c>
@@ -18645,7 +18916,7 @@
       </c>
       <c r="F162" s="12"/>
     </row>
-    <row r="163" spans="1:6" ht="39">
+    <row r="163" spans="1:6" ht="45">
       <c r="A163" s="2" t="s">
         <v>376</v>
       </c>
@@ -18659,7 +18930,7 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="39">
+    <row r="164" spans="1:6" ht="45">
       <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
@@ -18710,7 +18981,7 @@
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
     </row>
-    <row r="168" spans="1:6" ht="26.25">
+    <row r="168" spans="1:6" ht="30">
       <c r="A168" s="2" t="s">
         <v>389</v>
       </c>
@@ -18927,7 +19198,7 @@
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
     </row>
-    <row r="186" spans="1:6" ht="26.25">
+    <row r="186" spans="1:6" ht="30">
       <c r="A186" s="2" t="s">
         <v>426</v>
       </c>
@@ -19063,7 +19334,7 @@
       </c>
       <c r="F196" s="12"/>
     </row>
-    <row r="197" spans="1:6" ht="26.25">
+    <row r="197" spans="1:6">
       <c r="A197" s="2" t="s">
         <v>451</v>
       </c>
@@ -19163,7 +19434,7 @@
       <c r="E204" s="12"/>
       <c r="F204" s="12"/>
     </row>
-    <row r="205" spans="1:6" ht="26.25">
+    <row r="205" spans="1:6" ht="30">
       <c r="A205" s="2" t="s">
         <v>470</v>
       </c>
@@ -19189,7 +19460,7 @@
       <c r="E206" s="12"/>
       <c r="F206" s="12"/>
     </row>
-    <row r="207" spans="1:6" ht="26.25">
+    <row r="207" spans="1:6" ht="30">
       <c r="A207" s="2" t="s">
         <v>475</v>
       </c>
@@ -19287,7 +19558,7 @@
       <c r="E214" s="12"/>
       <c r="F214" s="12"/>
     </row>
-    <row r="215" spans="1:6" ht="26.25">
+    <row r="215" spans="1:6" ht="30">
       <c r="A215" s="2" t="s">
         <v>493</v>
       </c>
@@ -20108,7 +20379,7 @@
       <c r="E282" s="12"/>
       <c r="F282" s="12"/>
     </row>
-    <row r="283" spans="1:6" ht="26.25">
+    <row r="283" spans="1:6" ht="30">
       <c r="A283" s="2" t="s">
         <v>638</v>
       </c>
@@ -20122,7 +20393,7 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="26.25">
+    <row r="284" spans="1:6" ht="30">
       <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
@@ -20471,12 +20742,12 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20633,12 +20904,12 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20804,6 +21075,548 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA591B4A-9FC5-C747-8937-BC88FF6AE57D}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1950</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1951</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1953</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1955</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1956</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1955</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1955</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1958</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1959</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1960</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1961</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1962</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1963</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1966</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1967</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1968</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1970</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1971</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1973</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1974</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1975</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1978</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1877</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1979</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1876</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1982</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1982</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1983</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1984</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1985</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1986</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1987</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1988</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1989</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1991</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1993</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1994</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1995</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1996</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1997</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1998</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1999</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2001</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2002</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2003</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2004</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2006</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2006</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1995</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2007</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2008</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2009</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2010</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2011</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2012</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2013</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2014</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2015</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2016</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2017</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2017</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2018</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2019</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2019</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2020</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2021</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2022</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2023</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2023</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2025</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2026</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2027</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2028</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2029</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2030</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>43</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2033</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2034</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>218</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2036</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2037</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -20815,14 +21628,14 @@
       <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -23534,12 +24347,12 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -23550,7 +24363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.75">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -23616,7 +24429,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="39">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="2" t="s">
         <v>1082</v>
       </c>
@@ -23638,7 +24451,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="26.25">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="2" t="s">
         <v>1087</v>
       </c>
@@ -23648,7 +24461,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="39">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="2" t="s">
         <v>1089</v>
       </c>
@@ -23658,7 +24471,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="26.25">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" s="2" t="s">
         <v>1091</v>
       </c>
@@ -23668,7 +24481,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="26.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>1093</v>
       </c>
@@ -23678,7 +24491,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="26.25">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" s="2" t="s">
         <v>1095</v>
       </c>
@@ -23690,7 +24503,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="39">
+    <row r="17" spans="1:4" ht="45">
       <c r="A17" s="2" t="s">
         <v>1098</v>
       </c>
@@ -23702,7 +24515,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="39">
+    <row r="18" spans="1:4" ht="30">
       <c r="A18" s="2" t="s">
         <v>1101</v>
       </c>
@@ -23712,7 +24525,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="39">
+    <row r="19" spans="1:4" ht="45">
       <c r="A19" s="2" t="s">
         <v>1103</v>
       </c>
@@ -23722,7 +24535,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="26.25">
+    <row r="20" spans="1:4" ht="30">
       <c r="A20" s="2" t="s">
         <v>1105</v>
       </c>
@@ -23732,7 +24545,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="26.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>1107</v>
       </c>
@@ -23742,7 +24555,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="26.25">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" s="2" t="s">
         <v>1109</v>
       </c>
@@ -23772,7 +24585,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="26.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>1115</v>
       </c>
@@ -23802,7 +24615,7 @@
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="26.25">
+    <row r="28" spans="1:4" ht="30">
       <c r="A28" s="2" t="s">
         <v>1120</v>
       </c>
@@ -23814,7 +24627,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="26.25">
+    <row r="29" spans="1:4" ht="30">
       <c r="A29" s="2" t="s">
         <v>1123</v>
       </c>
@@ -23826,7 +24639,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="26.25">
+    <row r="30" spans="1:4" ht="30">
       <c r="A30" s="2" t="s">
         <v>1126</v>
       </c>
@@ -23848,7 +24661,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="26.25">
+    <row r="32" spans="1:4" ht="30">
       <c r="A32" s="2" t="s">
         <v>1131</v>
       </c>
@@ -23860,7 +24673,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="39">
+    <row r="33" spans="1:4" ht="30">
       <c r="A33" s="2" t="s">
         <v>1134</v>
       </c>
@@ -23872,7 +24685,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="26.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>1137</v>
       </c>
@@ -23884,7 +24697,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="128.25">
+    <row r="35" spans="1:4" ht="135">
       <c r="A35" s="2" t="s">
         <v>1140</v>
       </c>
@@ -23896,7 +24709,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="128.25">
+    <row r="36" spans="1:4" ht="135">
       <c r="A36" s="2" t="s">
         <v>1143</v>
       </c>
@@ -23980,7 +24793,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="26.25">
+    <row r="44" spans="1:4" ht="30">
       <c r="A44" s="2" t="s">
         <v>1160</v>
       </c>
@@ -23992,7 +24805,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="26.25">
+    <row r="45" spans="1:4" ht="30">
       <c r="A45" s="2" t="s">
         <v>1163</v>
       </c>
@@ -24002,7 +24815,7 @@
       <c r="C45" s="12"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="77.25">
+    <row r="46" spans="1:4" ht="75">
       <c r="A46" s="2" t="s">
         <v>1165</v>
       </c>
@@ -24031,13 +24844,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -24152,7 +24965,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" ht="26.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>1177</v>
       </c>
@@ -24176,7 +24989,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" ht="26.25">
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="2" t="s">
         <v>1182</v>
       </c>
@@ -24189,7 +25002,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" ht="26.25">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="2" t="s">
         <v>1185</v>
       </c>
@@ -24213,7 +25026,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="48.75">
+    <row r="18" spans="1:5" ht="40">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -24226,7 +25039,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="64.5">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -24375,7 +25188,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="26.25">
+    <row r="32" spans="1:5" ht="30">
       <c r="A32" s="2" t="s">
         <v>1222</v>
       </c>
@@ -24388,7 +25201,7 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" ht="26.25">
+    <row r="33" spans="1:5" ht="30">
       <c r="A33" s="2" t="s">
         <v>1225</v>
       </c>
@@ -24475,7 +25288,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" ht="51.75">
+    <row r="40" spans="1:5" ht="45">
       <c r="A40" s="2" t="s">
         <v>1244</v>
       </c>
@@ -24512,7 +25325,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" ht="26.25">
+    <row r="43" spans="1:5" ht="30">
       <c r="A43" s="2" t="s">
         <v>1252</v>
       </c>
@@ -24525,7 +25338,7 @@
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5" ht="39">
+    <row r="44" spans="1:5" ht="30">
       <c r="A44" s="2" t="s">
         <v>1253</v>
       </c>
@@ -24584,7 +25397,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" ht="26.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="2" t="s">
         <v>1265</v>
       </c>
@@ -24619,7 +25432,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5" ht="26.25">
+    <row r="52" spans="1:5" ht="30">
       <c r="A52" s="2" t="s">
         <v>1272</v>
       </c>
@@ -24713,7 +25526,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="39">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -24755,14 +25568,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.7109375" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.6640625" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25376,14 +26189,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25811,13 +26624,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -25903,7 +26716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="32">
       <c r="A10" s="18" t="s">
         <v>1314</v>
       </c>
@@ -25916,7 +26729,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="32">
       <c r="A11" s="18" t="s">
         <v>1317</v>
       </c>
@@ -25929,7 +26742,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="18" t="s">
         <v>1320</v>
       </c>
@@ -25942,7 +26755,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="32">
       <c r="A13" s="18" t="s">
         <v>1323</v>
       </c>
@@ -25955,7 +26768,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" s="18" t="s">
         <v>1326</v>
       </c>
@@ -25968,7 +26781,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:5" ht="32">
       <c r="A15" s="18" t="s">
         <v>1329</v>
       </c>
@@ -25981,7 +26794,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="32">
       <c r="A16" s="18" t="s">
         <v>1332</v>
       </c>
@@ -25994,7 +26807,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="32">
       <c r="A17" s="18" t="s">
         <v>1335</v>
       </c>
@@ -26007,7 +26820,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="48">
       <c r="A18" s="18" t="s">
         <v>1338</v>
       </c>
@@ -26020,7 +26833,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="48">
       <c r="A19" s="18" t="s">
         <v>1341</v>
       </c>
@@ -26033,7 +26846,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" ht="32">
       <c r="A20" s="18" t="s">
         <v>1344</v>
       </c>
@@ -26046,7 +26859,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5" ht="32">
       <c r="A21" s="18" t="s">
         <v>1347</v>
       </c>
@@ -26059,7 +26872,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5" ht="32">
       <c r="A22" s="18" t="s">
         <v>1350</v>
       </c>
@@ -26072,7 +26885,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5" ht="32">
       <c r="A23" s="18" t="s">
         <v>1353</v>
       </c>
@@ -26085,7 +26898,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="32">
       <c r="A24" s="18" t="s">
         <v>1356</v>
       </c>
@@ -26098,7 +26911,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5" ht="32">
       <c r="A25" s="18" t="s">
         <v>1359</v>
       </c>
@@ -26111,7 +26924,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5" ht="32">
       <c r="A26" s="18" t="s">
         <v>1362</v>
       </c>
@@ -26124,7 +26937,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="16">
       <c r="A27" s="18" t="s">
         <v>1365</v>
       </c>
@@ -26137,7 +26950,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="30">
+    <row r="28" spans="1:5" ht="32">
       <c r="A28" s="18" t="s">
         <v>1367</v>
       </c>
@@ -26150,7 +26963,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="16">
       <c r="A29" s="18" t="s">
         <v>1370</v>
       </c>
@@ -26163,7 +26976,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="16">
       <c r="A30" s="18" t="s">
         <v>1373</v>
       </c>
@@ -26191,13 +27004,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26294,7 +27107,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="18" t="s">
         <v>1378</v>
       </c>
@@ -26308,7 +27121,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="48">
       <c r="A11" s="18" t="s">
         <v>1381</v>
       </c>
@@ -26322,7 +27135,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="45">
+    <row r="12" spans="1:6" ht="32">
       <c r="A12" s="18" t="s">
         <v>1384</v>
       </c>
@@ -26336,7 +27149,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="32">
       <c r="A13" s="18" t="s">
         <v>1387</v>
       </c>
@@ -26350,7 +27163,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:6" ht="32">
       <c r="A14" s="18" t="s">
         <v>1390</v>
       </c>
@@ -26364,7 +27177,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="32">
       <c r="A15" s="18" t="s">
         <v>1393</v>
       </c>
@@ -26378,7 +27191,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6" ht="32">
       <c r="A16" s="18" t="s">
         <v>1396</v>
       </c>
@@ -26392,7 +27205,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="45">
+    <row r="17" spans="1:6" ht="48">
       <c r="A17" s="18" t="s">
         <v>1370</v>
       </c>
@@ -26406,7 +27219,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="30">
+    <row r="18" spans="1:6" ht="32">
       <c r="A18" s="18" t="s">
         <v>1401</v>
       </c>
@@ -26526,8 +27339,69 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="b3317a165cd10de70dc68851db9884d1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b8430278eece82d06f551ff77398a68" ns1:_="" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="4317e20fb51ec4e85b8666dabb09ede3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b908cdd69cb0859c51683a5db1834d0" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -26590,12 +27464,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -26708,7 +27582,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -26727,7 +27601,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -26800,7 +27674,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -26849,8 +27723,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -26939,83 +27813,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F317E4A3-C0C5-4204-BAF7-619A6A4AE4A7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27039,9 +27840,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC150521-9E19-41EA-8AB8-73E22B400E61}"/>
 </file>
</xml_diff>

<commit_message>
[24.07.09 09:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romainfouilland/Library/CloudStorage/OneDrive-SharedLibraries-ANS/Espace Projets - Espace Programme SI-SAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC0CFD67-B7A4-4DC9-B092-41319B8D5E3A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="877" firstSheet="13" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="1380" windowWidth="22995" windowHeight="12330" tabRatio="877" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2642" uniqueCount="2039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="2045">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -6124,9 +6124,6 @@
     <t>Demander une prise en charge de nombreux patients/victimes</t>
   </si>
   <si>
-    <t>Pour obtenir une consultation ou une visite du MG (uniquement pour lien 15-15)</t>
-  </si>
-  <si>
     <t>Code Antares</t>
   </si>
   <si>
@@ -6395,13 +6392,34 @@
   </si>
   <si>
     <t>sos</t>
+  </si>
+  <si>
+    <t>changer nom pour type de moyen engagé</t>
+  </si>
+  <si>
+    <t>Demander l'intervention d'une équipe secouriste / ambulance privée</t>
+  </si>
+  <si>
+    <t>Demander la régulation médicale du dossier par un médecin régulateur (cas de partage d'activité - exemples : régulation spécialisée, régulation déportée la nuit, délestage, atypie locale )</t>
+  </si>
+  <si>
+    <t>Demander l'intervention de la CUMP</t>
+  </si>
+  <si>
+    <t>Demander l'intervention d'une équipe SMUR</t>
+  </si>
+  <si>
+    <t>Demander l'obtention d'une consultation ou une visite du MG (uniquement pour lien 15-15)</t>
+  </si>
+  <si>
+    <t>Demander l'intervention d'une équipe paramédicale (UMHP).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6572,13 +6590,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -6680,7 +6691,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6790,16 +6801,19 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
@@ -8831,19 +8845,19 @@
   <dimension ref="A1:K217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="31" style="28" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="28" customWidth="1"/>
-    <col min="4" max="4" width="37.1640625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="28" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="28" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="28" customWidth="1"/>
     <col min="7" max="11" width="9" style="28" customWidth="1"/>
-    <col min="12" max="16384" width="11.5" style="28"/>
+    <col min="12" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -8851,7 +8865,7 @@
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:11" s="30" customFormat="1">
+    <row r="2" spans="1:11" s="30" customFormat="1" ht="15">
       <c r="A2" s="29" t="s">
         <v>1850</v>
       </c>
@@ -8886,7 +8900,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8917,7 +8931,7 @@
       <c r="J3" s="34"/>
       <c r="K3" s="34"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8948,7 +8962,7 @@
       <c r="J4" s="34"/>
       <c r="K4" s="34"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="15">
       <c r="A5" s="31" t="s">
         <v>1822</v>
       </c>
@@ -8979,14 +8993,14 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="31" t="s">
         <v>1822</v>
       </c>
       <c r="B6" s="38" t="s">
         <v>1854</v>
       </c>
-      <c r="C6" s="54" t="str">
+      <c r="C6" s="53" t="str">
         <f>'Motif de recours médico-secouri'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9010,14 +9024,14 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" s="31" t="s">
         <v>1822</v>
       </c>
       <c r="B7" s="38" t="s">
         <v>1826</v>
       </c>
-      <c r="C7" s="54" t="str">
+      <c r="C7" s="53" t="str">
         <f>'Attribution du dossier'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9039,14 +9053,14 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" ht="15">
       <c r="A8" s="31" t="s">
         <v>1822</v>
       </c>
       <c r="B8" s="38" t="s">
         <v>1834</v>
       </c>
-      <c r="C8" s="54" t="str">
+      <c r="C8" s="53" t="str">
         <f>'Priorité de régulation médicale'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9068,14 +9082,14 @@
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="31" t="s">
         <v>1825</v>
       </c>
       <c r="B9" s="38" t="s">
         <v>1831</v>
       </c>
-      <c r="C9" s="54" t="str">
+      <c r="C9" s="53" t="str">
         <f>'Type de requérant'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9099,14 +9113,14 @@
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="31" t="s">
         <v>1825</v>
       </c>
       <c r="B10" s="38" t="s">
         <v>1832</v>
       </c>
-      <c r="C10" s="54" t="str">
+      <c r="C10" s="53" t="str">
         <f>'Difficultés de communication'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9130,14 +9144,14 @@
       <c r="J10" s="34"/>
       <c r="K10" s="34"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" s="32" t="s">
         <v>1841</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>1835</v>
       </c>
-      <c r="C11" s="54" t="str">
+      <c r="C11" s="53" t="str">
         <f>Sexe!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9161,14 +9175,14 @@
       <c r="J11" s="34"/>
       <c r="K11" s="34"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" s="32" t="s">
         <v>1841</v>
       </c>
       <c r="B12" s="38" t="s">
         <v>1836</v>
       </c>
-      <c r="C12" s="54" t="str">
+      <c r="C12" s="53" t="str">
         <f>'Niveau de soin'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9190,14 +9204,14 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="31" t="s">
         <v>1842</v>
       </c>
       <c r="B13" s="38" t="s">
         <v>1837</v>
       </c>
-      <c r="C13" s="54" t="str">
+      <c r="C13" s="53" t="str">
         <f>'Type de décision'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9221,14 +9235,14 @@
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="31" t="s">
         <v>1851</v>
       </c>
       <c r="B14" s="38" t="s">
         <v>1839</v>
       </c>
-      <c r="C14" s="54" t="str">
+      <c r="C14" s="53" t="str">
         <f>'Type de ressource'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
@@ -9254,14 +9268,14 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="32" t="s">
         <v>1851</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>1853</v>
       </c>
-      <c r="C15" s="54" t="str">
+      <c r="C15" s="53" t="str">
         <f>'Type de vecteurs'!$B$1</f>
         <v>CISU</v>
       </c>
@@ -9287,7 +9301,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="31" t="s">
         <v>1851</v>
       </c>
@@ -9322,7 +9336,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" ht="15">
       <c r="A17" s="31" t="s">
         <v>1842</v>
       </c>
@@ -9353,7 +9367,7 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="15">
       <c r="A18" s="32" t="s">
         <v>1852</v>
       </c>
@@ -9382,7 +9396,7 @@
       </c>
       <c r="K18" s="34"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="15">
       <c r="A19" s="32"/>
       <c r="B19" s="35"/>
       <c r="C19" s="31"/>
@@ -12018,13 +12032,13 @@
       <selection activeCell="E9" sqref="E9:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
-    <col min="6" max="6" width="61.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12178,14 +12192,14 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12607,14 +12621,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13049,16 +13063,16 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13078,7 +13092,9 @@
       <c r="B2" s="25" t="s">
         <v>1579</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>2038</v>
+      </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6">
@@ -13497,17 +13513,17 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14483,13 +14499,13 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14905,13 +14921,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15415,17 +15431,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15507,121 +15523,137 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
+    <row r="10" spans="1:5">
       <c r="A10" s="48" t="s">
         <v>1937</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="54" t="s">
         <v>1855</v>
       </c>
       <c r="C10" s="40"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="54" t="s">
+        <v>2039</v>
+      </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="49" t="s">
         <v>1938</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="54" t="s">
         <v>1856</v>
       </c>
       <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="D11" s="54" t="s">
+        <v>2040</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:5">
       <c r="A12" s="50" t="s">
         <v>1939</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="54" t="s">
         <v>1857</v>
       </c>
       <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
+      <c r="D12" s="54" t="s">
+        <v>2041</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="16">
+    <row r="13" spans="1:5">
       <c r="A13" s="50" t="s">
         <v>1580</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="54" t="s">
         <v>1935</v>
       </c>
       <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
+      <c r="D13" s="54" t="s">
+        <v>2042</v>
+      </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:5">
       <c r="A14" s="50" t="s">
         <v>1444</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="54" t="s">
         <v>1936</v>
       </c>
       <c r="C14" s="40"/>
-      <c r="D14" s="40" t="s">
-        <v>1948</v>
+      <c r="D14" s="54" t="s">
+        <v>2043</v>
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="16">
+    <row r="15" spans="1:5">
       <c r="A15" s="50" t="s">
         <v>1573</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="54" t="s">
         <v>1858</v>
       </c>
       <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
+      <c r="D15" s="54" t="s">
+        <v>2044</v>
+      </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="16">
+    <row r="16" spans="1:5">
       <c r="A16" s="50" t="s">
         <v>1940</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="55" t="s">
         <v>1859</v>
       </c>
       <c r="C16" s="40"/>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="54" t="s">
         <v>1946</v>
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="16">
+    <row r="17" spans="1:5">
       <c r="A17" s="51" t="s">
         <v>1941</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="54" t="s">
         <v>1860</v>
       </c>
       <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
+      <c r="D17" s="54" t="s">
+        <v>1860</v>
+      </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="16">
+    <row r="18" spans="1:5">
       <c r="A18" s="52" t="s">
         <v>1942</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="54" t="s">
         <v>1947</v>
       </c>
       <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
+      <c r="D18" s="54" t="s">
+        <v>1947</v>
+      </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="16">
+    <row r="19" spans="1:5">
       <c r="A19" s="50" t="s">
         <v>1943</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="54" t="s">
         <v>1861</v>
       </c>
       <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
+      <c r="D19" s="54" t="s">
+        <v>1861</v>
+      </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="16">
+    <row r="20" spans="1:5">
       <c r="A20" s="50" t="s">
         <v>1944</v>
       </c>
@@ -15629,10 +15661,12 @@
         <v>1862</v>
       </c>
       <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
+      <c r="D20" s="54" t="s">
+        <v>1862</v>
+      </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="16">
+    <row r="21" spans="1:5">
       <c r="A21" s="50" t="s">
         <v>1945</v>
       </c>
@@ -15640,7 +15674,9 @@
         <v>1863</v>
       </c>
       <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
+      <c r="D21" s="54" t="s">
+        <v>1863</v>
+      </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
@@ -15902,13 +15938,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="80.5" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16391,13 +16427,13 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16895,14 +16931,14 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" customWidth="1"/>
-    <col min="5" max="5" width="47.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16985,7 +17021,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60">
+    <row r="10" spans="1:6" ht="64.5">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -17011,7 +17047,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -17025,7 +17061,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -17039,7 +17075,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -17052,7 +17088,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -17080,7 +17116,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="26.25">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -17106,7 +17142,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="26.25">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -17121,7 +17157,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -17147,7 +17183,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6" ht="39">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -17161,7 +17197,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:6" ht="39">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -17185,7 +17221,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="30">
+    <row r="25" spans="1:6" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -17199,7 +17235,7 @@
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="30">
+    <row r="26" spans="1:6" ht="26.25">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -17213,7 +17249,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="30">
+    <row r="27" spans="1:6" ht="26.25">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -17227,7 +17263,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -17263,7 +17299,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:6" ht="60">
+    <row r="31" spans="1:6" ht="51.75">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -17277,7 +17313,7 @@
       </c>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
@@ -17316,7 +17352,7 @@
       </c>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="26.25">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -17342,7 +17378,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" ht="120">
+    <row r="37" spans="1:6" ht="102.75">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
@@ -17356,7 +17392,7 @@
       </c>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" ht="30">
+    <row r="38" spans="1:6" ht="26.25">
       <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
@@ -17370,7 +17406,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="30">
+    <row r="39" spans="1:6" ht="39">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -17395,7 +17431,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" ht="30">
+    <row r="41" spans="1:6" ht="39">
       <c r="A41" s="2" t="s">
         <v>116</v>
       </c>
@@ -17409,7 +17445,7 @@
       </c>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" ht="26.25">
       <c r="A42" s="2" t="s">
         <v>119</v>
       </c>
@@ -17423,7 +17459,7 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" ht="30">
+    <row r="43" spans="1:6" ht="39">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -17447,7 +17483,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" ht="45">
+    <row r="45" spans="1:6" ht="39">
       <c r="A45" s="2" t="s">
         <v>127</v>
       </c>
@@ -17546,7 +17582,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="26.25">
       <c r="A53" s="2" t="s">
         <v>145</v>
       </c>
@@ -17560,7 +17596,7 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="60">
+    <row r="54" spans="1:6" ht="64.5">
       <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
@@ -17931,7 +17967,7 @@
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="1:6" ht="45">
+    <row r="85" spans="1:6" ht="39">
       <c r="A85" s="2" t="s">
         <v>214</v>
       </c>
@@ -17957,7 +17993,7 @@
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:6" ht="135">
+    <row r="87" spans="1:6" ht="128.25">
       <c r="A87" s="2" t="s">
         <v>219</v>
       </c>
@@ -17983,7 +18019,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="60">
+    <row r="89" spans="1:6" ht="51.75">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
@@ -17996,7 +18032,7 @@
       </c>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" ht="26.25">
       <c r="A90" s="2" t="s">
         <v>214</v>
       </c>
@@ -18036,7 +18072,7 @@
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:6" ht="30">
+    <row r="93" spans="1:6" ht="26.25">
       <c r="A93" s="2" t="s">
         <v>230</v>
       </c>
@@ -18207,7 +18243,7 @@
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
     </row>
-    <row r="107" spans="1:6" ht="30">
+    <row r="107" spans="1:6" ht="26.25">
       <c r="A107" s="2" t="s">
         <v>261</v>
       </c>
@@ -18221,7 +18257,7 @@
       </c>
       <c r="F107" s="12"/>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" ht="26.25">
       <c r="A108" s="2" t="s">
         <v>264</v>
       </c>
@@ -18345,7 +18381,7 @@
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" ht="30">
+    <row r="118" spans="1:6" ht="26.25">
       <c r="A118" s="2" t="s">
         <v>287</v>
       </c>
@@ -18359,7 +18395,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" ht="26.25">
       <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
@@ -18372,7 +18408,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="45">
+    <row r="120" spans="1:6" ht="39">
       <c r="A120" s="2" t="s">
         <v>293</v>
       </c>
@@ -18410,7 +18446,7 @@
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" ht="45">
+    <row r="123" spans="1:6" ht="39">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -18471,7 +18507,7 @@
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" ht="45">
+    <row r="128" spans="1:6" ht="39">
       <c r="A128" s="2" t="s">
         <v>311</v>
       </c>
@@ -18605,7 +18641,7 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="30">
+    <row r="139" spans="1:6" ht="26.25">
       <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
@@ -18630,7 +18666,7 @@
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
     </row>
-    <row r="141" spans="1:6" ht="30">
+    <row r="141" spans="1:6" ht="26.25">
       <c r="A141" s="2" t="s">
         <v>341</v>
       </c>
@@ -18644,7 +18680,7 @@
       </c>
       <c r="F141" s="12"/>
     </row>
-    <row r="142" spans="1:6" ht="30">
+    <row r="142" spans="1:6" ht="26.25">
       <c r="A142" s="2" t="s">
         <v>342</v>
       </c>
@@ -18658,7 +18694,7 @@
       </c>
       <c r="F142" s="12"/>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" ht="26.25">
       <c r="A143" s="2" t="s">
         <v>343</v>
       </c>
@@ -18672,7 +18708,7 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="30">
+    <row r="144" spans="1:6" ht="26.25">
       <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
@@ -18701,7 +18737,7 @@
       </c>
       <c r="F145" s="12"/>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" ht="26.25">
       <c r="A146" s="2" t="s">
         <v>347</v>
       </c>
@@ -18715,7 +18751,7 @@
       </c>
       <c r="F146" s="12"/>
     </row>
-    <row r="147" spans="1:6" ht="30">
+    <row r="147" spans="1:6" ht="39">
       <c r="A147" s="2" t="s">
         <v>348</v>
       </c>
@@ -18729,7 +18765,7 @@
       </c>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" spans="1:6" ht="30">
+    <row r="148" spans="1:6" ht="39">
       <c r="A148" s="2" t="s">
         <v>349</v>
       </c>
@@ -18743,7 +18779,7 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="30">
+    <row r="149" spans="1:6" ht="26.25">
       <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
@@ -18756,7 +18792,7 @@
       </c>
       <c r="F149" s="12"/>
     </row>
-    <row r="150" spans="1:6" ht="30">
+    <row r="150" spans="1:6" ht="26.25">
       <c r="A150" s="2" t="s">
         <v>351</v>
       </c>
@@ -18770,7 +18806,7 @@
       </c>
       <c r="F150" s="12"/>
     </row>
-    <row r="151" spans="1:6" ht="30">
+    <row r="151" spans="1:6" ht="26.25">
       <c r="A151" s="2" t="s">
         <v>352</v>
       </c>
@@ -18902,7 +18938,7 @@
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
     </row>
-    <row r="162" spans="1:6" ht="30">
+    <row r="162" spans="1:6" ht="39">
       <c r="A162" s="2" t="s">
         <v>373</v>
       </c>
@@ -18916,7 +18952,7 @@
       </c>
       <c r="F162" s="12"/>
     </row>
-    <row r="163" spans="1:6" ht="45">
+    <row r="163" spans="1:6" ht="39">
       <c r="A163" s="2" t="s">
         <v>376</v>
       </c>
@@ -18930,7 +18966,7 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="45">
+    <row r="164" spans="1:6" ht="39">
       <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
@@ -18981,7 +19017,7 @@
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
     </row>
-    <row r="168" spans="1:6" ht="30">
+    <row r="168" spans="1:6" ht="26.25">
       <c r="A168" s="2" t="s">
         <v>389</v>
       </c>
@@ -19198,7 +19234,7 @@
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
     </row>
-    <row r="186" spans="1:6" ht="30">
+    <row r="186" spans="1:6" ht="26.25">
       <c r="A186" s="2" t="s">
         <v>426</v>
       </c>
@@ -19334,7 +19370,7 @@
       </c>
       <c r="F196" s="12"/>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" ht="26.25">
       <c r="A197" s="2" t="s">
         <v>451</v>
       </c>
@@ -19434,7 +19470,7 @@
       <c r="E204" s="12"/>
       <c r="F204" s="12"/>
     </row>
-    <row r="205" spans="1:6" ht="30">
+    <row r="205" spans="1:6" ht="26.25">
       <c r="A205" s="2" t="s">
         <v>470</v>
       </c>
@@ -19460,7 +19496,7 @@
       <c r="E206" s="12"/>
       <c r="F206" s="12"/>
     </row>
-    <row r="207" spans="1:6" ht="30">
+    <row r="207" spans="1:6" ht="26.25">
       <c r="A207" s="2" t="s">
         <v>475</v>
       </c>
@@ -19558,7 +19594,7 @@
       <c r="E214" s="12"/>
       <c r="F214" s="12"/>
     </row>
-    <row r="215" spans="1:6" ht="30">
+    <row r="215" spans="1:6" ht="26.25">
       <c r="A215" s="2" t="s">
         <v>493</v>
       </c>
@@ -20379,7 +20415,7 @@
       <c r="E282" s="12"/>
       <c r="F282" s="12"/>
     </row>
-    <row r="283" spans="1:6" ht="30">
+    <row r="283" spans="1:6" ht="26.25">
       <c r="A283" s="2" t="s">
         <v>638</v>
       </c>
@@ -20393,7 +20429,7 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="30">
+    <row r="284" spans="1:6" ht="26.25">
       <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
@@ -20742,12 +20778,12 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20904,12 +20940,12 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -21085,7 +21121,7 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -21093,29 +21129,29 @@
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B1" t="s">
         <v>1949</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1950</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1951</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1952</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1953</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1954</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -21123,19 +21159,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="C2" t="s">
         <v>1955</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1954</v>
+      </c>
+      <c r="F2" t="s">
         <v>1956</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1955</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1955</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1957</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -21143,19 +21179,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>1957</v>
+      </c>
+      <c r="C3" t="s">
         <v>1958</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1959</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>1960</v>
       </c>
-      <c r="E3" t="s">
-        <v>1961</v>
-      </c>
       <c r="F3" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -21163,16 +21199,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>1961</v>
+      </c>
+      <c r="D4" t="s">
         <v>1962</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>1962</v>
+      </c>
+      <c r="F4" t="s">
         <v>1963</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1963</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1964</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -21180,16 +21216,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>1964</v>
+      </c>
+      <c r="D5" t="s">
         <v>1965</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>1966</v>
       </c>
-      <c r="E5" t="s">
-        <v>1967</v>
-      </c>
       <c r="F5" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -21197,19 +21233,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>1967</v>
+      </c>
+      <c r="C6" t="s">
         <v>1968</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>1969</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>1970</v>
       </c>
-      <c r="E6" t="s">
-        <v>1971</v>
-      </c>
       <c r="F6" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -21217,19 +21253,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C7" t="s">
         <v>1972</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>1973</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>1974</v>
       </c>
-      <c r="E7" t="s">
-        <v>1975</v>
-      </c>
       <c r="F7" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -21237,16 +21273,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>1975</v>
+      </c>
+      <c r="D8" t="s">
         <v>1976</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>1977</v>
       </c>
-      <c r="E8" t="s">
-        <v>1978</v>
-      </c>
       <c r="F8" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -21257,13 +21293,13 @@
         <v>1877</v>
       </c>
       <c r="D9" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="E9" t="s">
         <v>1876</v>
       </c>
       <c r="F9" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -21271,19 +21307,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>1979</v>
+      </c>
+      <c r="C10" t="s">
         <v>1980</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>1981</v>
       </c>
-      <c r="D10" t="s">
-        <v>1982</v>
-      </c>
       <c r="E10" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="F10" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -21291,16 +21327,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>1982</v>
+      </c>
+      <c r="D11" t="s">
         <v>1983</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>1984</v>
       </c>
-      <c r="E11" t="s">
-        <v>1985</v>
-      </c>
       <c r="F11" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -21308,16 +21344,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>1985</v>
+      </c>
+      <c r="D12" t="s">
         <v>1986</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>1987</v>
       </c>
-      <c r="E12" t="s">
-        <v>1988</v>
-      </c>
       <c r="F12" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -21325,16 +21361,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
+        <v>1988</v>
+      </c>
+      <c r="D13" t="s">
         <v>1989</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>1990</v>
       </c>
-      <c r="E13" t="s">
-        <v>1991</v>
-      </c>
       <c r="F13" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -21342,16 +21378,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
+        <v>1991</v>
+      </c>
+      <c r="D14" t="s">
         <v>1992</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>1993</v>
       </c>
-      <c r="E14" t="s">
-        <v>1994</v>
-      </c>
       <c r="F14" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -21359,19 +21395,19 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>1994</v>
+      </c>
+      <c r="C15" t="s">
         <v>1995</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>1996</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>1997</v>
       </c>
-      <c r="E15" t="s">
-        <v>1998</v>
-      </c>
       <c r="F15" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -21379,16 +21415,16 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
+        <v>1998</v>
+      </c>
+      <c r="D16" t="s">
         <v>1999</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>2000</v>
       </c>
-      <c r="E16" t="s">
-        <v>2001</v>
-      </c>
       <c r="F16" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -21396,16 +21432,16 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
+        <v>2001</v>
+      </c>
+      <c r="D17" t="s">
         <v>2002</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>2003</v>
       </c>
-      <c r="E17" t="s">
-        <v>2004</v>
-      </c>
       <c r="F17" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -21413,16 +21449,16 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
+        <v>2004</v>
+      </c>
+      <c r="D18" t="s">
         <v>2005</v>
       </c>
-      <c r="D18" t="s">
-        <v>2006</v>
-      </c>
       <c r="E18" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="F18" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -21430,19 +21466,19 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="C19" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D19" t="s">
         <v>2007</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>2008</v>
       </c>
-      <c r="E19" t="s">
-        <v>2009</v>
-      </c>
       <c r="F19" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -21450,16 +21486,16 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
+        <v>2009</v>
+      </c>
+      <c r="D20" t="s">
         <v>2010</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>2011</v>
       </c>
-      <c r="E20" t="s">
-        <v>2012</v>
-      </c>
       <c r="F20" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -21467,16 +21503,16 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
+        <v>2012</v>
+      </c>
+      <c r="D21" t="s">
         <v>2013</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>2014</v>
       </c>
-      <c r="E21" t="s">
-        <v>2015</v>
-      </c>
       <c r="F21" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -21484,16 +21520,16 @@
         <v>32</v>
       </c>
       <c r="C22" t="s">
+        <v>2015</v>
+      </c>
+      <c r="D22" t="s">
         <v>2016</v>
       </c>
-      <c r="D22" t="s">
-        <v>2017</v>
-      </c>
       <c r="E22" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F22" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -21501,16 +21537,16 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
+        <v>2017</v>
+      </c>
+      <c r="D23" t="s">
         <v>2018</v>
       </c>
-      <c r="D23" t="s">
-        <v>2019</v>
-      </c>
       <c r="E23" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F23" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -21518,16 +21554,16 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
+        <v>2019</v>
+      </c>
+      <c r="D24" t="s">
         <v>2020</v>
       </c>
-      <c r="D24" t="s">
-        <v>2021</v>
-      </c>
       <c r="E24" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="F24" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -21535,16 +21571,16 @@
         <v>40</v>
       </c>
       <c r="C25" t="s">
+        <v>2021</v>
+      </c>
+      <c r="D25" t="s">
         <v>2022</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>2022</v>
+      </c>
+      <c r="F25" t="s">
         <v>2023</v>
-      </c>
-      <c r="E25" t="s">
-        <v>2023</v>
-      </c>
-      <c r="F25" t="s">
-        <v>2024</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -21552,16 +21588,16 @@
         <v>41</v>
       </c>
       <c r="C26" t="s">
+        <v>2024</v>
+      </c>
+      <c r="D26" t="s">
         <v>2025</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>2026</v>
       </c>
-      <c r="E26" t="s">
-        <v>2027</v>
-      </c>
       <c r="F26" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -21569,16 +21605,16 @@
         <v>42</v>
       </c>
       <c r="C27" t="s">
+        <v>2027</v>
+      </c>
+      <c r="D27" t="s">
         <v>2028</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>2029</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>2030</v>
-      </c>
-      <c r="F27" t="s">
-        <v>2031</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -21586,16 +21622,16 @@
         <v>43</v>
       </c>
       <c r="C28" t="s">
+        <v>2031</v>
+      </c>
+      <c r="D28" t="s">
         <v>2032</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>2033</v>
       </c>
-      <c r="E28" t="s">
-        <v>2034</v>
-      </c>
       <c r="F28" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -21603,16 +21639,16 @@
         <v>218</v>
       </c>
       <c r="C29" t="s">
+        <v>2034</v>
+      </c>
+      <c r="D29" t="s">
         <v>2035</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>2036</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>2037</v>
-      </c>
-      <c r="F29" t="s">
-        <v>2038</v>
       </c>
     </row>
   </sheetData>
@@ -21624,18 +21660,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F144" sqref="F144"/>
+    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -24347,12 +24383,12 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="26.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -24363,7 +24399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="24.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -24429,7 +24465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="39">
       <c r="A10" s="2" t="s">
         <v>1082</v>
       </c>
@@ -24451,7 +24487,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>1087</v>
       </c>
@@ -24461,7 +24497,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="39">
       <c r="A13" s="2" t="s">
         <v>1089</v>
       </c>
@@ -24471,7 +24507,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>1091</v>
       </c>
@@ -24481,7 +24517,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1093</v>
       </c>
@@ -24491,7 +24527,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1095</v>
       </c>
@@ -24503,7 +24539,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="45">
+    <row r="17" spans="1:4" ht="39">
       <c r="A17" s="2" t="s">
         <v>1098</v>
       </c>
@@ -24515,7 +24551,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="30">
+    <row r="18" spans="1:4" ht="39">
       <c r="A18" s="2" t="s">
         <v>1101</v>
       </c>
@@ -24525,7 +24561,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:4" ht="39">
       <c r="A19" s="2" t="s">
         <v>1103</v>
       </c>
@@ -24535,7 +24571,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>1105</v>
       </c>
@@ -24545,7 +24581,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="26.25">
       <c r="A21" s="2" t="s">
         <v>1107</v>
       </c>
@@ -24555,7 +24591,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="26.25">
       <c r="A22" s="2" t="s">
         <v>1109</v>
       </c>
@@ -24585,7 +24621,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>1115</v>
       </c>
@@ -24615,7 +24651,7 @@
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="30">
+    <row r="28" spans="1:4" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>1120</v>
       </c>
@@ -24627,7 +24663,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="30">
+    <row r="29" spans="1:4" ht="26.25">
       <c r="A29" s="2" t="s">
         <v>1123</v>
       </c>
@@ -24639,7 +24675,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="30">
+    <row r="30" spans="1:4" ht="26.25">
       <c r="A30" s="2" t="s">
         <v>1126</v>
       </c>
@@ -24661,7 +24697,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="30">
+    <row r="32" spans="1:4" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1131</v>
       </c>
@@ -24673,7 +24709,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="30">
+    <row r="33" spans="1:4" ht="39">
       <c r="A33" s="2" t="s">
         <v>1134</v>
       </c>
@@ -24685,7 +24721,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="26.25">
       <c r="A34" s="2" t="s">
         <v>1137</v>
       </c>
@@ -24697,7 +24733,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="135">
+    <row r="35" spans="1:4" ht="128.25">
       <c r="A35" s="2" t="s">
         <v>1140</v>
       </c>
@@ -24709,7 +24745,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="135">
+    <row r="36" spans="1:4" ht="128.25">
       <c r="A36" s="2" t="s">
         <v>1143</v>
       </c>
@@ -24793,7 +24829,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="30">
+    <row r="44" spans="1:4" ht="26.25">
       <c r="A44" s="2" t="s">
         <v>1160</v>
       </c>
@@ -24805,7 +24841,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="30">
+    <row r="45" spans="1:4" ht="26.25">
       <c r="A45" s="2" t="s">
         <v>1163</v>
       </c>
@@ -24815,7 +24851,7 @@
       <c r="C45" s="12"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="75">
+    <row r="46" spans="1:4" ht="77.25">
       <c r="A46" s="2" t="s">
         <v>1165</v>
       </c>
@@ -24844,13 +24880,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="39.5" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -24965,7 +25001,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>1177</v>
       </c>
@@ -24989,7 +25025,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1182</v>
       </c>
@@ -25002,7 +25038,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1185</v>
       </c>
@@ -25026,7 +25062,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="40">
+    <row r="18" spans="1:5" ht="48.75">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -25039,7 +25075,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="64.5">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -25188,7 +25224,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1222</v>
       </c>
@@ -25201,7 +25237,7 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" ht="30">
+    <row r="33" spans="1:5" ht="26.25">
       <c r="A33" s="2" t="s">
         <v>1225</v>
       </c>
@@ -25288,7 +25324,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" ht="45">
+    <row r="40" spans="1:5" ht="51.75">
       <c r="A40" s="2" t="s">
         <v>1244</v>
       </c>
@@ -25325,7 +25361,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" ht="30">
+    <row r="43" spans="1:5" ht="26.25">
       <c r="A43" s="2" t="s">
         <v>1252</v>
       </c>
@@ -25338,7 +25374,7 @@
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5" ht="39">
       <c r="A44" s="2" t="s">
         <v>1253</v>
       </c>
@@ -25397,7 +25433,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="26.25">
       <c r="A49" s="2" t="s">
         <v>1265</v>
       </c>
@@ -25432,7 +25468,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5" ht="30">
+    <row r="52" spans="1:5" ht="26.25">
       <c r="A52" s="2" t="s">
         <v>1272</v>
       </c>
@@ -25526,7 +25562,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="39">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -25568,14 +25604,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.6640625" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26189,14 +26225,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26624,13 +26660,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26716,7 +26752,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32">
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="18" t="s">
         <v>1314</v>
       </c>
@@ -26729,7 +26765,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="32">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="18" t="s">
         <v>1317</v>
       </c>
@@ -26742,7 +26778,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="18" t="s">
         <v>1320</v>
       </c>
@@ -26755,7 +26791,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="32">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="18" t="s">
         <v>1323</v>
       </c>
@@ -26768,7 +26804,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="18" t="s">
         <v>1326</v>
       </c>
@@ -26781,7 +26817,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="32">
+    <row r="15" spans="1:5" ht="45">
       <c r="A15" s="18" t="s">
         <v>1329</v>
       </c>
@@ -26794,7 +26830,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="32">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="18" t="s">
         <v>1332</v>
       </c>
@@ -26807,7 +26843,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="32">
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="18" t="s">
         <v>1335</v>
       </c>
@@ -26820,7 +26856,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="48">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="18" t="s">
         <v>1338</v>
       </c>
@@ -26833,7 +26869,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="48">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="18" t="s">
         <v>1341</v>
       </c>
@@ -26846,7 +26882,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="32">
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="18" t="s">
         <v>1344</v>
       </c>
@@ -26859,7 +26895,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="32">
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="18" t="s">
         <v>1347</v>
       </c>
@@ -26872,7 +26908,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="32">
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="18" t="s">
         <v>1350</v>
       </c>
@@ -26885,7 +26921,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="32">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="18" t="s">
         <v>1353</v>
       </c>
@@ -26898,7 +26934,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="32">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="18" t="s">
         <v>1356</v>
       </c>
@@ -26911,7 +26947,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="32">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="18" t="s">
         <v>1359</v>
       </c>
@@ -26924,7 +26960,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="32">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="18" t="s">
         <v>1362</v>
       </c>
@@ -26937,7 +26973,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="16">
+    <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
         <v>1365</v>
       </c>
@@ -26950,7 +26986,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="32">
+    <row r="28" spans="1:5" ht="30">
       <c r="A28" s="18" t="s">
         <v>1367</v>
       </c>
@@ -26963,7 +26999,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="16">
+    <row r="29" spans="1:5">
       <c r="A29" s="18" t="s">
         <v>1370</v>
       </c>
@@ -26976,7 +27012,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="16">
+    <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
         <v>1373</v>
       </c>
@@ -27004,13 +27040,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27107,7 +27143,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="18" t="s">
         <v>1378</v>
       </c>
@@ -27121,7 +27157,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="48">
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="18" t="s">
         <v>1381</v>
       </c>
@@ -27135,7 +27171,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="32">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="18" t="s">
         <v>1384</v>
       </c>
@@ -27149,7 +27185,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="32">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="18" t="s">
         <v>1387</v>
       </c>
@@ -27163,7 +27199,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="32">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="18" t="s">
         <v>1390</v>
       </c>
@@ -27177,7 +27213,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="32">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="18" t="s">
         <v>1393</v>
       </c>
@@ -27191,7 +27227,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="32">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="18" t="s">
         <v>1396</v>
       </c>
@@ -27205,7 +27241,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="48">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="18" t="s">
         <v>1370</v>
       </c>
@@ -27219,7 +27255,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="32">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="18" t="s">
         <v>1401</v>
       </c>
@@ -27400,8 +27436,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="4317e20fb51ec4e85b8666dabb09ede3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b908cdd69cb0859c51683a5db1834d0" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -27464,12 +27500,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -27582,7 +27618,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -27601,7 +27637,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -27674,7 +27710,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -27723,8 +27759,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -27824,21 +27860,37 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC150521-9E19-41EA-8AB8-73E22B400E61}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059494DF-AC78-4572-AFB9-E7754F64CB4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.07.17 15:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC0CFD67-B7A4-4DC9-B092-41319B8D5E3A}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D96BE2AE-D72E-4509-8C7E-D69CD3AE4562}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="1380" windowWidth="22995" windowHeight="12330" tabRatio="877" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5595" yWindow="75" windowWidth="22800" windowHeight="14460" tabRatio="877" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="2045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2611" uniqueCount="2009">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -5248,15 +5248,9 @@
     <t>Vehicule Leger de Sécurité Civile</t>
   </si>
   <si>
-    <t>VL SC</t>
-  </si>
-  <si>
     <t>Autre vecteur de Sécurité Civile</t>
   </si>
   <si>
-    <t>VH SC</t>
-  </si>
-  <si>
     <t>Taxi et assimilés</t>
   </si>
   <si>
@@ -5266,15 +5260,9 @@
     <t>Transports en commun</t>
   </si>
   <si>
-    <t>BUS TRAM</t>
-  </si>
-  <si>
     <t>Autre vecteur</t>
   </si>
   <si>
-    <t>VH</t>
-  </si>
-  <si>
     <t>Train</t>
   </si>
   <si>
@@ -5290,105 +5278,54 @@
     <t>Moyen personnel sans précsion</t>
   </si>
   <si>
-    <t>VH PERSO</t>
-  </si>
-  <si>
     <t>A pied</t>
   </si>
   <si>
-    <t>A PIED</t>
-  </si>
-  <si>
     <t>Moyen inconnu</t>
   </si>
   <si>
     <t>Conseil médical</t>
   </si>
   <si>
-    <t>CONSEIL MED</t>
-  </si>
-  <si>
     <t>Défibrillateur Automatique externe</t>
   </si>
   <si>
     <t>Hélicoptère Forces de l’Ordre</t>
   </si>
   <si>
-    <t>HELICO FSI</t>
-  </si>
-  <si>
     <t>VL des FSI</t>
   </si>
   <si>
-    <t>VL FSI</t>
-  </si>
-  <si>
     <t>Fourgon des FSI</t>
   </si>
   <si>
-    <t>FOURGON FSI</t>
-  </si>
-  <si>
     <t>Autre vecteur des FSI</t>
   </si>
   <si>
-    <t>AUTRE VH FSI</t>
-  </si>
-  <si>
     <t>Consultation de Médicale Générale</t>
   </si>
   <si>
-    <t>CONSULT MG</t>
-  </si>
-  <si>
     <t>Visite de Médicale Générale</t>
   </si>
   <si>
-    <t>VISITE MG</t>
-  </si>
-  <si>
     <t>Recours au pharmacien</t>
   </si>
   <si>
-    <t>PHARMACIE</t>
-  </si>
-  <si>
     <t>Recours à un infirmier</t>
   </si>
   <si>
-    <t>INFIRMIER</t>
-  </si>
-  <si>
     <t>Recours à un médecin autre spécialité</t>
   </si>
   <si>
-    <t>MED AUTRE SPE</t>
-  </si>
-  <si>
     <t>Recours à un dentiste</t>
   </si>
   <si>
-    <t>DENTISTE</t>
-  </si>
-  <si>
-    <t>Autre professionnel de santé</t>
-  </si>
-  <si>
-    <t>AUTRE PRO</t>
-  </si>
-  <si>
     <t>Hélicoptère sécurité civile</t>
   </si>
   <si>
-    <t>HELICO SC</t>
-  </si>
-  <si>
     <t>Avion sécurité civile</t>
   </si>
   <si>
-    <t>AVION SC</t>
-  </si>
-  <si>
     <t>Véhicule de secours et d'assistance aux victimes</t>
   </si>
   <si>
@@ -5404,81 +5341,42 @@
     <t>Véhicule plongeurs</t>
   </si>
   <si>
-    <t>PLONGEURS</t>
-  </si>
-  <si>
     <t>Moyens de secours routiers du SIS</t>
   </si>
   <si>
-    <t>SECOURS ROUTIER</t>
-  </si>
-  <si>
     <t>Moyens incendie du SIS</t>
   </si>
   <si>
-    <t>MOYEN INCENDIE</t>
-  </si>
-  <si>
     <t>Véhicule du Poste Médical Avancé</t>
   </si>
   <si>
-    <t>PMA</t>
-  </si>
-  <si>
     <t>Véhicule intervention chimique</t>
   </si>
   <si>
-    <t>VH inter chimique</t>
-  </si>
-  <si>
     <t>Véhicule intervention radioactivité</t>
   </si>
   <si>
-    <t>VH inter radio</t>
-  </si>
-  <si>
     <t>Poste de commandement</t>
   </si>
   <si>
-    <t>PC SIS</t>
-  </si>
-  <si>
     <t>Véhicule léger infirmier SP</t>
   </si>
   <si>
-    <t>VL-ISP</t>
-  </si>
-  <si>
     <t>Véhicule léger Médecin SP</t>
   </si>
   <si>
-    <t>VL-MSP</t>
-  </si>
-  <si>
     <t>Véhicule léger chef de groupe</t>
   </si>
   <si>
-    <t>VL CHEF</t>
-  </si>
-  <si>
     <t>Véhicule léger autre usage</t>
   </si>
   <si>
-    <t>VL SIS</t>
-  </si>
-  <si>
     <t>Autre moyen SSE</t>
   </si>
   <si>
-    <t>MOYEN SSE</t>
-  </si>
-  <si>
     <t>Autre moyen du SIS</t>
   </si>
   <si>
-    <t>MOYEN SIS</t>
-  </si>
-  <si>
     <t>Véhicule Léger Médicalisé</t>
   </si>
   <si>
@@ -5494,21 +5392,12 @@
     <t>Ambulance de réanimation Bariatrique</t>
   </si>
   <si>
-    <t>AR BARIA</t>
-  </si>
-  <si>
     <t>Ambulance de réanimation Pédiatrique</t>
   </si>
   <si>
-    <t>AR PEDIA</t>
-  </si>
-  <si>
     <t>Véhicule de liaison Smur</t>
   </si>
   <si>
-    <t>VL SMUR</t>
-  </si>
-  <si>
     <t>HéliSmur</t>
   </si>
   <si>
@@ -5518,21 +5407,12 @@
     <t>Hélicoptère de transport sanitaire</t>
   </si>
   <si>
-    <t>HELICO SAN</t>
-  </si>
-  <si>
     <t>Avion Smur</t>
   </si>
   <si>
-    <t>AVIONSMUR</t>
-  </si>
-  <si>
     <t>Avion de transport sanitaire</t>
   </si>
   <si>
-    <t>AVION SAN</t>
-  </si>
-  <si>
     <t>NaviSmur</t>
   </si>
   <si>
@@ -5560,39 +5440,21 @@
     <t>Véhicule logistique transport PSM pédiatrique</t>
   </si>
   <si>
-    <t>PSM PEDIA</t>
-  </si>
-  <si>
     <t>Véhicule Poste de Commandement et ou d’évacuation SAMU</t>
   </si>
   <si>
-    <t>PC SAMU</t>
-  </si>
-  <si>
     <t>Ambulance privée grand contenant - type A</t>
   </si>
   <si>
-    <t>AP GRAND V3</t>
-  </si>
-  <si>
     <t>Ambulance privée petit contenant - type C</t>
   </si>
   <si>
-    <t>AP PETIT V3</t>
-  </si>
-  <si>
     <t>Ambulance privée grand contenant - type bariatrique</t>
   </si>
   <si>
-    <t>AP BARIA</t>
-  </si>
-  <si>
     <t>Ambulance de catégorie non définie</t>
   </si>
   <si>
-    <t>AP</t>
-  </si>
-  <si>
     <t>Véhicule Sanitaire Léger</t>
   </si>
   <si>
@@ -6413,13 +6275,44 @@
   </si>
   <si>
     <t>Demander l'intervention d'une équipe paramédicale (UMHP).</t>
+  </si>
+  <si>
+    <t>Ne transporte pas</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Hybride</t>
+  </si>
+  <si>
+    <t>AUTREVECT</t>
+  </si>
+  <si>
+    <t>AUTRETRANS</t>
+  </si>
+  <si>
+    <t>Autre vecteur de transport</t>
+  </si>
+  <si>
+    <t>DEFIB</t>
+  </si>
+  <si>
+    <t>Défibrillateur</t>
+  </si>
+  <si>
+    <t>Recours à autre professionnel de santé</t>
+  </si>
+  <si>
+    <t>Utilisée exclusivement en inter-santé
+A garder pour échanger : EMSI  (dans OPG) - dans le sens type de moyen/ressource, plus large que le type de vecteur/véhicule</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6593,6 +6486,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -6691,7 +6589,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -6809,6 +6707,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -8867,45 +8769,45 @@
     </row>
     <row r="2" spans="1:11" s="30" customFormat="1" ht="15">
       <c r="A2" s="29" t="s">
-        <v>1850</v>
+        <v>1804</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>1827</v>
+        <v>1781</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>1828</v>
+        <v>1782</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>1819</v>
+        <v>1773</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>1820</v>
+        <v>1774</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>1821</v>
+        <v>1775</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>1844</v>
+        <v>1798</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>1843</v>
+        <v>1797</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>1845</v>
+        <v>1799</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>1846</v>
+        <v>1800</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>1847</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15">
       <c r="A3" s="31" t="s">
-        <v>1822</v>
+        <v>1776</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>1823</v>
+        <v>1777</v>
       </c>
       <c r="C3" s="31" t="str">
         <f>'Nature de fait'!$B$1</f>
@@ -8916,16 +8818,16 @@
         <v>Code_Nature_de_fait</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
@@ -8933,10 +8835,10 @@
     </row>
     <row r="4" spans="1:11" ht="15">
       <c r="A4" s="31" t="s">
-        <v>1822</v>
+        <v>1776</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1829</v>
+        <v>1783</v>
       </c>
       <c r="C4" s="31" t="str">
         <f>'Type de lieu'!$B$1</f>
@@ -8947,16 +8849,16 @@
         <v>Code_Type_de_lieu</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
@@ -8964,10 +8866,10 @@
     </row>
     <row r="5" spans="1:11" ht="15">
       <c r="A5" s="31" t="s">
-        <v>1822</v>
+        <v>1776</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1830</v>
+        <v>1784</v>
       </c>
       <c r="C5" s="31" t="str">
         <f>'Risque, menace et sensibilité'!$B$1</f>
@@ -8978,16 +8880,16 @@
         <v>Code_Risque-Menace-Sensibilité</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I5" s="34"/>
       <c r="J5" s="34"/>
@@ -8995,10 +8897,10 @@
     </row>
     <row r="6" spans="1:11" ht="15">
       <c r="A6" s="31" t="s">
-        <v>1822</v>
+        <v>1776</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>1854</v>
+        <v>1808</v>
       </c>
       <c r="C6" s="53" t="str">
         <f>'Motif de recours médico-secouri'!$B$1</f>
@@ -9009,16 +8911,16 @@
         <v>Code_Motif_patient-victime</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
@@ -9026,10 +8928,10 @@
     </row>
     <row r="7" spans="1:11" ht="15">
       <c r="A7" s="31" t="s">
-        <v>1822</v>
+        <v>1776</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>1826</v>
+        <v>1780</v>
       </c>
       <c r="C7" s="53" t="str">
         <f>'Attribution du dossier'!$B$1</f>
@@ -9040,14 +8942,14 @@
         <v>DEVENIRD</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G7" s="34"/>
       <c r="H7" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
@@ -9055,10 +8957,10 @@
     </row>
     <row r="8" spans="1:11" ht="15">
       <c r="A8" s="31" t="s">
-        <v>1822</v>
+        <v>1776</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>1834</v>
+        <v>1788</v>
       </c>
       <c r="C8" s="53" t="str">
         <f>'Priorité de régulation médicale'!$B$1</f>
@@ -9069,14 +8971,14 @@
         <v>PRIORITE</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
@@ -9084,10 +8986,10 @@
     </row>
     <row r="9" spans="1:11" ht="15">
       <c r="A9" s="31" t="s">
-        <v>1825</v>
+        <v>1779</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>1831</v>
+        <v>1785</v>
       </c>
       <c r="C9" s="53" t="str">
         <f>'Type de requérant'!$B$1</f>
@@ -9098,16 +9000,16 @@
         <v>TYPAPPLT</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -9115,10 +9017,10 @@
     </row>
     <row r="10" spans="1:11" ht="15">
       <c r="A10" s="31" t="s">
-        <v>1825</v>
+        <v>1779</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>1832</v>
+        <v>1786</v>
       </c>
       <c r="C10" s="53" t="str">
         <f>'Difficultés de communication'!$B$1</f>
@@ -9129,16 +9031,16 @@
         <v>PBAPL</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -9146,10 +9048,10 @@
     </row>
     <row r="11" spans="1:11" ht="15">
       <c r="A11" s="32" t="s">
-        <v>1841</v>
+        <v>1795</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>1835</v>
+        <v>1789</v>
       </c>
       <c r="C11" s="53" t="str">
         <f>Sexe!$B$1</f>
@@ -9160,16 +9062,16 @@
         <v>NOMENC_SEXE</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
@@ -9177,10 +9079,10 @@
     </row>
     <row r="12" spans="1:11" ht="15">
       <c r="A12" s="32" t="s">
-        <v>1841</v>
+        <v>1795</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>1836</v>
+        <v>1790</v>
       </c>
       <c r="C12" s="53" t="str">
         <f>'Niveau de soin'!$B$1</f>
@@ -9191,14 +9093,14 @@
         <v>GRAVITE</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -9206,10 +9108,10 @@
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="A13" s="31" t="s">
-        <v>1842</v>
+        <v>1796</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>1837</v>
+        <v>1791</v>
       </c>
       <c r="C13" s="53" t="str">
         <f>'Type de décision'!$B$1</f>
@@ -9220,16 +9122,16 @@
         <v>TYPEDEC</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
@@ -9237,10 +9139,10 @@
     </row>
     <row r="14" spans="1:11" ht="15">
       <c r="A14" s="31" t="s">
-        <v>1851</v>
+        <v>1805</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>1839</v>
+        <v>1793</v>
       </c>
       <c r="C14" s="53" t="str">
         <f>'Type de ressource'!$B$1</f>
@@ -9251,29 +9153,29 @@
         <v>TYPE_MOYEN</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G14" s="34"/>
       <c r="H14" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="J14" s="34"/>
       <c r="K14" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15">
       <c r="A15" s="32" t="s">
-        <v>1851</v>
+        <v>1805</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>1853</v>
+        <v>1807</v>
       </c>
       <c r="C15" s="53" t="str">
         <f>'Type de vecteurs'!$B$1</f>
@@ -9284,29 +9186,29 @@
         <v>TYPE_VECTEUR</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="J15" s="34"/>
       <c r="K15" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15">
       <c r="A16" s="31" t="s">
-        <v>1851</v>
+        <v>1805</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>1849</v>
+        <v>1803</v>
       </c>
       <c r="C16" s="31" t="str">
         <f>'Niveau de prise en charge'!$B$1</f>
@@ -9317,31 +9219,31 @@
         <v>NIVSOIN</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I16" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="J16" s="34"/>
       <c r="K16" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15">
       <c r="A17" s="31" t="s">
-        <v>1842</v>
+        <v>1796</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>1838</v>
+        <v>1792</v>
       </c>
       <c r="C17" s="31" t="str">
         <f>'Type de devenir du patient'!$B$1</f>
@@ -9352,16 +9254,16 @@
         <v>NOMENC_DEVENIR_PAT</v>
       </c>
       <c r="E17" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F17" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
@@ -9369,10 +9271,10 @@
     </row>
     <row r="18" spans="1:11" ht="15">
       <c r="A18" s="32" t="s">
-        <v>1852</v>
+        <v>1806</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>1833</v>
+        <v>1787</v>
       </c>
       <c r="C18" s="31" t="str">
         <f>'Effet à obtenir'!$B$1</f>
@@ -9383,16 +9285,16 @@
         <v>Code_Effet_a_obtenir</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>1824</v>
+        <v>1778</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>1840</v>
+        <v>1794</v>
       </c>
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
       <c r="J18" s="34" t="s">
-        <v>1848</v>
+        <v>1802</v>
       </c>
       <c r="K18" s="34"/>
     </row>
@@ -13093,7 +12995,7 @@
         <v>1579</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2038</v>
+        <v>1992</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -13234,7 +13136,7 @@
     </row>
     <row r="15" spans="1:6" s="36" customFormat="1">
       <c r="A15" s="21" t="s">
-        <v>1815</v>
+        <v>1769</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>1597</v>
@@ -13510,23 +13412,24 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EE5AD-9985-4D20-8EAC-8B61AD8038D6}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="36" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="36" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13536,7 +13439,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -13546,7 +13449,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -13554,7 +13457,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" customFormat="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -13562,7 +13465,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" customFormat="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -13570,7 +13473,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" customFormat="1">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -13578,27 +13481,27 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" customFormat="1">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>1081</v>
+        <v>1169</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" customFormat="1" ht="36.75">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>1608</v>
+      <c r="B8" s="57" t="s">
+        <v>2008</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" customFormat="1">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -13619,871 +13522,912 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="A10" s="56" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>1769</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="56" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="56" t="s">
         <v>1654</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" s="56"/>
+      <c r="C12" s="56" t="s">
         <v>1653</v>
       </c>
-      <c r="C10" t="s">
-        <v>1654</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1815</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>1775</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1655</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D12" s="56"/>
+      <c r="E12" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="56" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56" t="s">
         <v>1656</v>
       </c>
-      <c r="F11" t="s">
-        <v>1815</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>1776</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D13" s="56"/>
+      <c r="E13" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="56" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B14" s="56" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="56" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="56" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B16" s="56"/>
+      <c r="C16" s="56" t="s">
         <v>1657</v>
       </c>
-      <c r="C12" t="s">
-        <v>1658</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1815</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="D16" s="56"/>
+      <c r="E16" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="56" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="56" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="56" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56" t="s">
+        <v>1663</v>
+      </c>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="56" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56" t="s">
+        <v>1665</v>
+      </c>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="56" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="56" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56" t="s">
         <v>1660</v>
       </c>
-      <c r="B13" t="s">
-        <v>1659</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1660</v>
-      </c>
-      <c r="F13" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>1777</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1661</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1662</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>1370</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1663</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1664</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>1666</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1665</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1666</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>1668</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D22" s="56"/>
+      <c r="E22" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="56" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56" t="s">
+        <v>2004</v>
+      </c>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="56" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56" t="s">
         <v>1667</v>
       </c>
-      <c r="C17" t="s">
-        <v>1668</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>1504</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D24" s="56"/>
+      <c r="E24" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="56" t="s">
+        <v>2005</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>2005</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>2006</v>
+      </c>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="56" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56" t="s">
         <v>1669</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D26" s="56"/>
+      <c r="E26" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="56" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B27" s="56" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="56" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56" t="s">
         <v>1670</v>
       </c>
-      <c r="F18" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D28" s="56"/>
+      <c r="E28" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="56" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56" t="s">
         <v>1671</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D29" s="56"/>
+      <c r="E29" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="56" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56" t="s">
         <v>1672</v>
       </c>
-      <c r="F19" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D30" s="56"/>
+      <c r="E30" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="56" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56" t="s">
         <v>1673</v>
       </c>
-      <c r="C20" t="s">
-        <v>1373</v>
-      </c>
-      <c r="F20" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>1550</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D31" s="56"/>
+      <c r="E31" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="56" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B32" s="56" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="56" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56" t="s">
         <v>1674</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D33" s="56"/>
+      <c r="E33" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="56" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56" t="s">
         <v>1675</v>
       </c>
-      <c r="F21" t="s">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>1594</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D34" s="56"/>
+      <c r="E34" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="56" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56" t="s">
         <v>1676</v>
       </c>
-      <c r="C22" t="s">
-        <v>1594</v>
-      </c>
-      <c r="F22" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>1779</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D35" s="56"/>
+      <c r="E35" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="56" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56" t="s">
         <v>1677</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D36" s="56"/>
+      <c r="E36" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="56" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56" t="s">
         <v>1678</v>
       </c>
-      <c r="F23" t="s">
-        <v>1816</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>1780</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="D37" s="56"/>
+      <c r="E37" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="56" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56" t="s">
         <v>1679</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D38" s="56"/>
+      <c r="E38" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="56" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56" t="s">
+        <v>2007</v>
+      </c>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="56" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B40" s="56" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="56" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="56" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56" t="s">
+        <v>1684</v>
+      </c>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="56" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B43" s="56"/>
+      <c r="C43" s="56" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D43" s="56"/>
+      <c r="E43" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="56" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="56" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="56" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="56" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B47" s="56"/>
+      <c r="C47" s="56" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="56" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B48" s="56"/>
+      <c r="C48" s="56" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="56" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B49" s="56"/>
+      <c r="C49" s="56" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="56" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="56" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="56" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B52" s="56"/>
+      <c r="C52" s="56" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="56" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="56" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56" t="s">
         <v>1680</v>
       </c>
-      <c r="F24" t="s">
-        <v>1816</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
-        <v>1781</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D54" s="56"/>
+      <c r="E54" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="56" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B55" s="56"/>
+      <c r="C55" s="56" t="s">
         <v>1681</v>
       </c>
-      <c r="C25" t="s">
-        <v>1682</v>
-      </c>
-      <c r="F25" t="s">
-        <v>1816</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>1782</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1683</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1684</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1816</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>1783</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1686</v>
-      </c>
-      <c r="F27" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>1784</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1687</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1688</v>
-      </c>
-      <c r="F28" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>1785</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1690</v>
-      </c>
-      <c r="F29" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1691</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1692</v>
-      </c>
-      <c r="F30" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>1786</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1693</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1694</v>
-      </c>
-      <c r="F31" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>1414</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1695</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1696</v>
-      </c>
-      <c r="F32" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>1787</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="D55" s="56"/>
+      <c r="E55" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="56" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B56" s="56"/>
+      <c r="C56" s="56" t="s">
         <v>1697</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D56" s="56"/>
+      <c r="E56" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="56" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B57" s="56"/>
+      <c r="C57" s="56" t="s">
         <v>1698</v>
       </c>
-      <c r="F33" t="s">
-        <v>1584</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>1788</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D57" s="56"/>
+      <c r="E57" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="56" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B58" s="56"/>
+      <c r="C58" s="56" t="s">
+        <v>1727</v>
+      </c>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56" t="s">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="56" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B59" s="56" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C59" s="56"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="56" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B60" s="56"/>
+      <c r="C60" s="56" t="s">
         <v>1699</v>
       </c>
-      <c r="C34" t="s">
-        <v>1700</v>
-      </c>
-      <c r="F34" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>1789</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D60" s="56"/>
+      <c r="E60" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="56" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B61" s="56"/>
+      <c r="C61" s="56" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D61" s="56"/>
+      <c r="E61" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="56" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B62" s="56"/>
+      <c r="C62" s="56" t="s">
+        <v>1713</v>
+      </c>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="56" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B63" s="56"/>
+      <c r="C63" s="56" t="s">
+        <v>1715</v>
+      </c>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="56" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B64" s="56"/>
+      <c r="C64" s="56" t="s">
+        <v>1717</v>
+      </c>
+      <c r="D64" s="56"/>
+      <c r="E64" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="56" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B65" s="56"/>
+      <c r="C65" s="56" t="s">
+        <v>1719</v>
+      </c>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="56" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B66" s="56"/>
+      <c r="C66" s="56" t="s">
+        <v>1720</v>
+      </c>
+      <c r="D66" s="56"/>
+      <c r="E66" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="56" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B67" s="56"/>
+      <c r="C67" s="56" t="s">
         <v>1701</v>
       </c>
-      <c r="C35" t="s">
-        <v>1702</v>
-      </c>
-      <c r="F35" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
+      <c r="D67" s="56"/>
+      <c r="E67" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="56" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B68" s="56"/>
+      <c r="C68" s="56" t="s">
+        <v>1703</v>
+      </c>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="56" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B69" s="56"/>
+      <c r="C69" s="56" t="s">
         <v>1704</v>
       </c>
-      <c r="B36" t="s">
-        <v>1703</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1704</v>
-      </c>
-      <c r="F36" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
+      <c r="D69" s="56"/>
+      <c r="E69" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="56" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B70" s="56"/>
+      <c r="C70" s="56" t="s">
         <v>1706</v>
       </c>
-      <c r="B37" t="s">
-        <v>1705</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1706</v>
-      </c>
-      <c r="F37" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
-        <v>1790</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D70" s="56"/>
+      <c r="E70" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="56" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B71" s="56"/>
+      <c r="C71" s="56" t="s">
         <v>1708</v>
       </c>
-      <c r="F38" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>1791</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D71" s="56"/>
+      <c r="E71" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="56" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B72" s="56"/>
+      <c r="C72" s="56" t="s">
         <v>1709</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D72" s="56"/>
+      <c r="E72" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="56" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B73" s="56"/>
+      <c r="C73" s="56" t="s">
         <v>1710</v>
       </c>
-      <c r="F39" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
-        <v>1792</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="D73" s="56"/>
+      <c r="E73" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="56" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B74" s="56"/>
+      <c r="C74" s="56" t="s">
         <v>1711</v>
       </c>
-      <c r="C40" t="s">
-        <v>1712</v>
-      </c>
-      <c r="F40" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>1793</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1714</v>
-      </c>
-      <c r="F41" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>1794</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1716</v>
-      </c>
-      <c r="F42" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>1795</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1717</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1718</v>
-      </c>
-      <c r="F43" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>1796</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1719</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1720</v>
-      </c>
-      <c r="F44" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>1797</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="D74" s="56"/>
+      <c r="E74" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="56" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B75" s="56" t="s">
+        <v>1771</v>
+      </c>
+      <c r="C75" s="56"/>
+      <c r="D75" s="56"/>
+      <c r="E75" s="56"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="56" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B76" s="56"/>
+      <c r="C76" s="56" t="s">
+        <v>1725</v>
+      </c>
+      <c r="D76" s="56"/>
+      <c r="E76" s="56" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="56" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B77" s="56"/>
+      <c r="C77" s="56" t="s">
         <v>1721</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D77" s="56"/>
+      <c r="E77" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="56" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B78" s="56"/>
+      <c r="C78" s="56" t="s">
         <v>1722</v>
       </c>
-      <c r="F45" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>1798</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="D78" s="56"/>
+      <c r="E78" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="56" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B79" s="56"/>
+      <c r="C79" s="56" t="s">
         <v>1723</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D79" s="56"/>
+      <c r="E79" s="56" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="56" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B80" s="56"/>
+      <c r="C80" s="56" t="s">
         <v>1724</v>
       </c>
-      <c r="F46" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>1799</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1725</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1726</v>
-      </c>
-      <c r="F47" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" t="s">
-        <v>1800</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1727</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1728</v>
-      </c>
-      <c r="F48" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>1801</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1729</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1730</v>
-      </c>
-      <c r="F49" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" t="s">
-        <v>1802</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1731</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1732</v>
-      </c>
-      <c r="F50" t="s">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1733</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1734</v>
-      </c>
-      <c r="F51" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
-        <v>1736</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1735</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1736</v>
-      </c>
-      <c r="F52" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>1803</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1737</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1738</v>
-      </c>
-      <c r="F53" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" t="s">
-        <v>1804</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1740</v>
-      </c>
-      <c r="F54" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" t="s">
-        <v>1805</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1741</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1742</v>
-      </c>
-      <c r="F55" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" t="s">
-        <v>1744</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1743</v>
-      </c>
-      <c r="C56" t="s">
-        <v>1744</v>
-      </c>
-      <c r="F56" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" t="s">
-        <v>1806</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C57" t="s">
-        <v>1746</v>
-      </c>
-      <c r="F57" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" t="s">
-        <v>1807</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1747</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1748</v>
-      </c>
-      <c r="F58" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" t="s">
-        <v>1808</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1749</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1750</v>
-      </c>
-      <c r="F59" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" t="s">
-        <v>1752</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1751</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1752</v>
-      </c>
-      <c r="F60" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1753</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1754</v>
-      </c>
-      <c r="F61" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1755</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1756</v>
-      </c>
-      <c r="F62" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1757</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1758</v>
-      </c>
-      <c r="F63" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
-        <v>1809</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1759</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1760</v>
-      </c>
-      <c r="F64" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" t="s">
-        <v>1810</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1761</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1762</v>
-      </c>
-      <c r="F65" t="s">
-        <v>1580</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1763</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1764</v>
-      </c>
-      <c r="F66" t="s">
-        <v>1817</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" t="s">
-        <v>1812</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1765</v>
-      </c>
-      <c r="C67" t="s">
-        <v>1766</v>
-      </c>
-      <c r="F67" t="s">
-        <v>1817</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" t="s">
-        <v>1813</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1767</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1768</v>
-      </c>
-      <c r="F68" t="s">
-        <v>1817</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" t="s">
-        <v>1814</v>
-      </c>
-      <c r="B69" t="s">
-        <v>1769</v>
-      </c>
-      <c r="C69" t="s">
-        <v>1770</v>
-      </c>
-      <c r="F69" t="s">
-        <v>1817</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
-        <v>1772</v>
-      </c>
-      <c r="B70" t="s">
-        <v>1771</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1772</v>
-      </c>
-      <c r="F70" t="s">
-        <v>1817</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" t="s">
-        <v>1774</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1773</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1774</v>
-      </c>
-      <c r="F71" t="s">
-        <v>1588</v>
+      <c r="D80" s="56"/>
+      <c r="E80" s="56" t="s">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -15431,7 +15375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3700FB-CD0A-4D38-965B-161A1B9D93F3}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -15458,7 +15402,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1934</v>
+        <v>1888</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -15525,40 +15469,40 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="48" t="s">
-        <v>1937</v>
+        <v>1891</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>1855</v>
+        <v>1809</v>
       </c>
       <c r="C10" s="40"/>
       <c r="D10" s="54" t="s">
-        <v>2039</v>
+        <v>1993</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="49" t="s">
-        <v>1938</v>
+        <v>1892</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>1856</v>
+        <v>1810</v>
       </c>
       <c r="C11" s="40"/>
       <c r="D11" s="54" t="s">
-        <v>2040</v>
+        <v>1994</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="50" t="s">
-        <v>1939</v>
+        <v>1893</v>
       </c>
       <c r="B12" s="54" t="s">
-        <v>1857</v>
+        <v>1811</v>
       </c>
       <c r="C12" s="40"/>
       <c r="D12" s="54" t="s">
-        <v>2041</v>
+        <v>1995</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -15567,11 +15511,11 @@
         <v>1580</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>1935</v>
+        <v>1889</v>
       </c>
       <c r="C13" s="40"/>
       <c r="D13" s="54" t="s">
-        <v>2042</v>
+        <v>1996</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -15580,11 +15524,11 @@
         <v>1444</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>1936</v>
+        <v>1890</v>
       </c>
       <c r="C14" s="40"/>
       <c r="D14" s="54" t="s">
-        <v>2043</v>
+        <v>1997</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -15593,89 +15537,89 @@
         <v>1573</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>1858</v>
+        <v>1812</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="54" t="s">
-        <v>2044</v>
+        <v>1998</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="50" t="s">
-        <v>1940</v>
+        <v>1894</v>
       </c>
       <c r="B16" s="55" t="s">
-        <v>1859</v>
+        <v>1813</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="54" t="s">
-        <v>1946</v>
+        <v>1900</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="51" t="s">
-        <v>1941</v>
+        <v>1895</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>1860</v>
+        <v>1814</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="54" t="s">
-        <v>1860</v>
+        <v>1814</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="52" t="s">
-        <v>1942</v>
+        <v>1896</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>1947</v>
+        <v>1901</v>
       </c>
       <c r="C18" s="40"/>
       <c r="D18" s="54" t="s">
-        <v>1947</v>
+        <v>1901</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="50" t="s">
-        <v>1943</v>
+        <v>1897</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>1861</v>
+        <v>1815</v>
       </c>
       <c r="C19" s="40"/>
       <c r="D19" s="54" t="s">
-        <v>1861</v>
+        <v>1815</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="50" t="s">
-        <v>1944</v>
+        <v>1898</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>1862</v>
+        <v>1816</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="54" t="s">
-        <v>1862</v>
+        <v>1816</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="50" t="s">
-        <v>1945</v>
+        <v>1899</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>1863</v>
+        <v>1817</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="54" t="s">
-        <v>1863</v>
+        <v>1817</v>
       </c>
       <c r="E21" s="2"/>
     </row>
@@ -15961,7 +15905,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1886</v>
+        <v>1840</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -16028,132 +15972,132 @@
     </row>
     <row r="10" spans="1:5" s="36" customFormat="1">
       <c r="A10" s="21" t="s">
-        <v>1887</v>
+        <v>1841</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1866</v>
+        <v>1820</v>
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="47"/>
       <c r="E10" s="21" t="s">
-        <v>1932</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="36" customFormat="1">
       <c r="A11" s="21" t="s">
-        <v>1888</v>
+        <v>1842</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1899</v>
+        <v>1853</v>
       </c>
       <c r="C11" s="47"/>
       <c r="D11" s="47"/>
       <c r="E11" s="21" t="s">
-        <v>1933</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="36" customFormat="1">
       <c r="A12" s="21" t="s">
-        <v>1889</v>
+        <v>1843</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1900</v>
+        <v>1854</v>
       </c>
       <c r="C12" s="47"/>
       <c r="D12" s="47"/>
       <c r="E12" s="21" t="s">
-        <v>1906</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="36" customFormat="1">
       <c r="A13" s="21" t="s">
-        <v>1890</v>
+        <v>1844</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1901</v>
+        <v>1855</v>
       </c>
       <c r="C13" s="47"/>
       <c r="D13" s="47"/>
       <c r="E13" s="21" t="s">
-        <v>1907</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="36" customFormat="1">
       <c r="A14" s="21" t="s">
-        <v>1891</v>
+        <v>1845</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>1902</v>
+        <v>1856</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
       <c r="E14" s="21" t="s">
-        <v>1908</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="36" customFormat="1">
       <c r="A15" s="21" t="s">
-        <v>1892</v>
+        <v>1846</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>1903</v>
+        <v>1857</v>
       </c>
       <c r="C15" s="47"/>
       <c r="D15" s="47"/>
       <c r="E15" s="21" t="s">
-        <v>1909</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="36" customFormat="1">
       <c r="A16" s="21" t="s">
-        <v>1893</v>
+        <v>1847</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>1894</v>
+        <v>1848</v>
       </c>
       <c r="C16" s="47"/>
       <c r="D16" s="47"/>
       <c r="E16" s="21" t="s">
-        <v>1910</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="36" customFormat="1">
       <c r="A17" s="21" t="s">
-        <v>1895</v>
+        <v>1849</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>1904</v>
+        <v>1858</v>
       </c>
       <c r="C17" s="47"/>
       <c r="D17" s="47"/>
       <c r="E17" s="21" t="s">
-        <v>1911</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="36" customFormat="1">
       <c r="A18" s="21" t="s">
-        <v>1896</v>
+        <v>1850</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>1905</v>
+        <v>1859</v>
       </c>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
       <c r="E18" s="21" t="s">
-        <v>1912</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="36" customFormat="1">
       <c r="A19" s="21" t="s">
-        <v>1897</v>
+        <v>1851</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>1898</v>
+        <v>1852</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
       <c r="E19" s="21" t="s">
-        <v>1913</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -16450,7 +16394,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1864</v>
+        <v>1818</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -16517,171 +16461,171 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="21" t="s">
-        <v>1865</v>
+        <v>1819</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>1866</v>
+        <v>1820</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="21" t="s">
-        <v>1882</v>
+        <v>1836</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="21" t="s">
-        <v>1867</v>
+        <v>1821</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>1923</v>
+        <v>1877</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="21" t="s">
-        <v>1914</v>
+        <v>1868</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="21" t="s">
-        <v>1868</v>
+        <v>1822</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>1924</v>
+        <v>1878</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="21" t="s">
-        <v>1915</v>
+        <v>1869</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="21" t="s">
-        <v>1869</v>
+        <v>1823</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>1925</v>
+        <v>1879</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="21" t="s">
-        <v>1916</v>
+        <v>1870</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="21" t="s">
-        <v>1870</v>
+        <v>1824</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>1926</v>
+        <v>1880</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="21" t="s">
-        <v>1917</v>
+        <v>1871</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="21" t="s">
-        <v>1871</v>
+        <v>1825</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>1927</v>
+        <v>1881</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="21" t="s">
-        <v>1918</v>
+        <v>1872</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="21" t="s">
-        <v>1872</v>
+        <v>1826</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>1928</v>
+        <v>1882</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="21" t="s">
-        <v>1919</v>
+        <v>1873</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="21" t="s">
-        <v>1873</v>
+        <v>1827</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>1929</v>
+        <v>1883</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="21" t="s">
-        <v>1920</v>
+        <v>1874</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="21" t="s">
-        <v>1874</v>
+        <v>1828</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>1930</v>
+        <v>1884</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="21" t="s">
-        <v>1921</v>
+        <v>1875</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="21" t="s">
-        <v>1875</v>
+        <v>1829</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>1931</v>
+        <v>1885</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="21" t="s">
-        <v>1922</v>
+        <v>1876</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="21" t="s">
-        <v>1876</v>
+        <v>1830</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>1877</v>
+        <v>1831</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="21" t="s">
-        <v>1883</v>
+        <v>1837</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="21" t="s">
-        <v>1878</v>
+        <v>1832</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>1879</v>
+        <v>1833</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="21" t="s">
-        <v>1884</v>
+        <v>1838</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" s="46" customFormat="1">
       <c r="A22" s="44" t="s">
-        <v>1880</v>
+        <v>1834</v>
       </c>
       <c r="B22" s="44" t="s">
-        <v>1881</v>
+        <v>1835</v>
       </c>
       <c r="C22" s="45"/>
       <c r="D22" s="45"/>
       <c r="E22" s="44" t="s">
-        <v>1885</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -21136,22 +21080,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>1948</v>
+        <v>1902</v>
       </c>
       <c r="B1" t="s">
-        <v>1949</v>
+        <v>1903</v>
       </c>
       <c r="C1" t="s">
-        <v>1950</v>
+        <v>1904</v>
       </c>
       <c r="D1" t="s">
-        <v>1951</v>
+        <v>1905</v>
       </c>
       <c r="E1" t="s">
-        <v>1952</v>
+        <v>1906</v>
       </c>
       <c r="F1" t="s">
-        <v>1953</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -21159,19 +21103,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1954</v>
+        <v>1908</v>
       </c>
       <c r="C2" t="s">
-        <v>1955</v>
+        <v>1909</v>
       </c>
       <c r="D2" t="s">
-        <v>1954</v>
+        <v>1908</v>
       </c>
       <c r="E2" t="s">
-        <v>1954</v>
+        <v>1908</v>
       </c>
       <c r="F2" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -21179,19 +21123,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1957</v>
+        <v>1911</v>
       </c>
       <c r="C3" t="s">
-        <v>1958</v>
+        <v>1912</v>
       </c>
       <c r="D3" t="s">
-        <v>1959</v>
+        <v>1913</v>
       </c>
       <c r="E3" t="s">
-        <v>1960</v>
+        <v>1914</v>
       </c>
       <c r="F3" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -21199,16 +21143,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>1961</v>
+        <v>1915</v>
       </c>
       <c r="D4" t="s">
-        <v>1962</v>
+        <v>1916</v>
       </c>
       <c r="E4" t="s">
-        <v>1962</v>
+        <v>1916</v>
       </c>
       <c r="F4" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -21216,16 +21160,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>1964</v>
+        <v>1918</v>
       </c>
       <c r="D5" t="s">
-        <v>1965</v>
+        <v>1919</v>
       </c>
       <c r="E5" t="s">
-        <v>1966</v>
+        <v>1920</v>
       </c>
       <c r="F5" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -21233,19 +21177,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1967</v>
+        <v>1921</v>
       </c>
       <c r="C6" t="s">
-        <v>1968</v>
+        <v>1922</v>
       </c>
       <c r="D6" t="s">
-        <v>1969</v>
+        <v>1923</v>
       </c>
       <c r="E6" t="s">
-        <v>1970</v>
+        <v>1924</v>
       </c>
       <c r="F6" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -21253,19 +21197,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1971</v>
+        <v>1925</v>
       </c>
       <c r="C7" t="s">
-        <v>1972</v>
+        <v>1926</v>
       </c>
       <c r="D7" t="s">
-        <v>1973</v>
+        <v>1927</v>
       </c>
       <c r="E7" t="s">
-        <v>1974</v>
+        <v>1928</v>
       </c>
       <c r="F7" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -21273,16 +21217,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>1975</v>
+        <v>1929</v>
       </c>
       <c r="D8" t="s">
-        <v>1976</v>
+        <v>1930</v>
       </c>
       <c r="E8" t="s">
-        <v>1977</v>
+        <v>1931</v>
       </c>
       <c r="F8" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -21290,16 +21234,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>1877</v>
+        <v>1831</v>
       </c>
       <c r="D9" t="s">
-        <v>1978</v>
+        <v>1932</v>
       </c>
       <c r="E9" t="s">
-        <v>1876</v>
+        <v>1830</v>
       </c>
       <c r="F9" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -21307,19 +21251,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1979</v>
+        <v>1933</v>
       </c>
       <c r="C10" t="s">
-        <v>1980</v>
+        <v>1934</v>
       </c>
       <c r="D10" t="s">
-        <v>1981</v>
+        <v>1935</v>
       </c>
       <c r="E10" t="s">
-        <v>1981</v>
+        <v>1935</v>
       </c>
       <c r="F10" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -21327,16 +21271,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>1982</v>
+        <v>1936</v>
       </c>
       <c r="D11" t="s">
-        <v>1983</v>
+        <v>1937</v>
       </c>
       <c r="E11" t="s">
-        <v>1984</v>
+        <v>1938</v>
       </c>
       <c r="F11" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -21344,16 +21288,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>1985</v>
+        <v>1939</v>
       </c>
       <c r="D12" t="s">
-        <v>1986</v>
+        <v>1940</v>
       </c>
       <c r="E12" t="s">
-        <v>1987</v>
+        <v>1941</v>
       </c>
       <c r="F12" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -21361,16 +21305,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>1988</v>
+        <v>1942</v>
       </c>
       <c r="D13" t="s">
-        <v>1989</v>
+        <v>1943</v>
       </c>
       <c r="E13" t="s">
-        <v>1990</v>
+        <v>1944</v>
       </c>
       <c r="F13" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -21378,16 +21322,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>1991</v>
+        <v>1945</v>
       </c>
       <c r="D14" t="s">
-        <v>1992</v>
+        <v>1946</v>
       </c>
       <c r="E14" t="s">
-        <v>1993</v>
+        <v>1947</v>
       </c>
       <c r="F14" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -21395,19 +21339,19 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>1994</v>
+        <v>1948</v>
       </c>
       <c r="C15" t="s">
-        <v>1995</v>
+        <v>1949</v>
       </c>
       <c r="D15" t="s">
-        <v>1996</v>
+        <v>1950</v>
       </c>
       <c r="E15" t="s">
-        <v>1997</v>
+        <v>1951</v>
       </c>
       <c r="F15" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -21415,16 +21359,16 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>1998</v>
+        <v>1952</v>
       </c>
       <c r="D16" t="s">
-        <v>1999</v>
+        <v>1953</v>
       </c>
       <c r="E16" t="s">
-        <v>2000</v>
+        <v>1954</v>
       </c>
       <c r="F16" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -21432,16 +21376,16 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>2001</v>
+        <v>1955</v>
       </c>
       <c r="D17" t="s">
-        <v>2002</v>
+        <v>1956</v>
       </c>
       <c r="E17" t="s">
-        <v>2003</v>
+        <v>1957</v>
       </c>
       <c r="F17" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -21449,16 +21393,16 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>2004</v>
+        <v>1958</v>
       </c>
       <c r="D18" t="s">
-        <v>2005</v>
+        <v>1959</v>
       </c>
       <c r="E18" t="s">
-        <v>2005</v>
+        <v>1959</v>
       </c>
       <c r="F18" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -21466,19 +21410,19 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>1994</v>
+        <v>1948</v>
       </c>
       <c r="C19" t="s">
-        <v>2006</v>
+        <v>1960</v>
       </c>
       <c r="D19" t="s">
-        <v>2007</v>
+        <v>1961</v>
       </c>
       <c r="E19" t="s">
-        <v>2008</v>
+        <v>1962</v>
       </c>
       <c r="F19" t="s">
-        <v>1956</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -21486,16 +21430,16 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>2009</v>
+        <v>1963</v>
       </c>
       <c r="D20" t="s">
-        <v>2010</v>
+        <v>1964</v>
       </c>
       <c r="E20" t="s">
-        <v>2011</v>
+        <v>1965</v>
       </c>
       <c r="F20" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -21503,16 +21447,16 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>2012</v>
+        <v>1966</v>
       </c>
       <c r="D21" t="s">
-        <v>2013</v>
+        <v>1967</v>
       </c>
       <c r="E21" t="s">
-        <v>2014</v>
+        <v>1968</v>
       </c>
       <c r="F21" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -21520,16 +21464,16 @@
         <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>2015</v>
+        <v>1969</v>
       </c>
       <c r="D22" t="s">
-        <v>2016</v>
+        <v>1970</v>
       </c>
       <c r="E22" t="s">
-        <v>2016</v>
+        <v>1970</v>
       </c>
       <c r="F22" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -21537,16 +21481,16 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>2017</v>
+        <v>1971</v>
       </c>
       <c r="D23" t="s">
-        <v>2018</v>
+        <v>1972</v>
       </c>
       <c r="E23" t="s">
-        <v>2018</v>
+        <v>1972</v>
       </c>
       <c r="F23" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -21554,16 +21498,16 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>2019</v>
+        <v>1973</v>
       </c>
       <c r="D24" t="s">
-        <v>2020</v>
+        <v>1974</v>
       </c>
       <c r="E24" t="s">
-        <v>2020</v>
+        <v>1974</v>
       </c>
       <c r="F24" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -21571,16 +21515,16 @@
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>2021</v>
+        <v>1975</v>
       </c>
       <c r="D25" t="s">
-        <v>2022</v>
+        <v>1976</v>
       </c>
       <c r="E25" t="s">
-        <v>2022</v>
+        <v>1976</v>
       </c>
       <c r="F25" t="s">
-        <v>2023</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -21588,16 +21532,16 @@
         <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>2024</v>
+        <v>1978</v>
       </c>
       <c r="D26" t="s">
-        <v>2025</v>
+        <v>1979</v>
       </c>
       <c r="E26" t="s">
-        <v>2026</v>
+        <v>1980</v>
       </c>
       <c r="F26" t="s">
-        <v>1963</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -21605,16 +21549,16 @@
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>2027</v>
+        <v>1981</v>
       </c>
       <c r="D27" t="s">
-        <v>2028</v>
+        <v>1982</v>
       </c>
       <c r="E27" t="s">
-        <v>2029</v>
+        <v>1983</v>
       </c>
       <c r="F27" t="s">
-        <v>2030</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -21622,16 +21566,16 @@
         <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>2031</v>
+        <v>1985</v>
       </c>
       <c r="D28" t="s">
-        <v>2032</v>
+        <v>1986</v>
       </c>
       <c r="E28" t="s">
-        <v>2033</v>
+        <v>1987</v>
       </c>
       <c r="F28" t="s">
-        <v>2030</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -21639,16 +21583,16 @@
         <v>218</v>
       </c>
       <c r="C29" t="s">
-        <v>2034</v>
+        <v>1988</v>
       </c>
       <c r="D29" t="s">
-        <v>2035</v>
+        <v>1989</v>
       </c>
       <c r="E29" t="s">
-        <v>2036</v>
+        <v>1990</v>
       </c>
       <c r="F29" t="s">
-        <v>2037</v>
+        <v>1991</v>
       </c>
     </row>
   </sheetData>
@@ -25741,7 +25685,7 @@
         <v>1411</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>1818</v>
+        <v>1772</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18" t="s">
@@ -27375,67 +27319,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -27849,33 +27732,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059494DF-AC78-4572-AFB9-E7754F64CB4B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27893,4 +27811,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.07.18 15:39] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E3AE2A9-48E6-4275-8143-3511AF03FE6C}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BB02A10-B2DF-4A05-9415-EC4F0022A4C9}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="0" windowWidth="25635" windowHeight="14460" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3930" yWindow="345" windowWidth="23385" windowHeight="13110" tabRatio="877" firstSheet="13" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Type de devenir du patient" sheetId="35" r:id="rId16"/>
     <sheet name="Effet à obtenir" sheetId="10" r:id="rId17"/>
     <sheet name="Cadre conventionnel" sheetId="43" r:id="rId18"/>
-    <sheet name="Status du vecteur" sheetId="42" r:id="rId19"/>
+    <sheet name="Statut du vecteur" sheetId="42" r:id="rId19"/>
     <sheet name="#Delai d'intervention demande" sheetId="40" r:id="rId20"/>
     <sheet name="#Delai de réponse" sheetId="39" r:id="rId21"/>
     <sheet name="#Nombre de patients-victimes" sheetId="2" r:id="rId22"/>
@@ -6313,9 +6313,6 @@
     <t>RS-RR</t>
   </si>
   <si>
-    <t>Status du vecteur</t>
-  </si>
-  <si>
     <t>DECISION</t>
   </si>
   <si>
@@ -6569,6 +6566,9 @@
   </si>
   <si>
     <t>Ressource engagée / resourcesStatus</t>
+  </si>
+  <si>
+    <t>Statut du vecteur</t>
   </si>
 </sst>
 </file>
@@ -6903,7 +6903,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7038,7 +7038,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -7046,28 +7045,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
-  <dxfs count="81">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="79">
     <dxf>
       <fill>
         <patternFill>
@@ -7093,6 +7071,13 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8690,154 +8675,154 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A9:F308" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="74"/>
+    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8BF6ADF-B677-473E-8ABE-51264084FE99}" name="Table13" displayName="Table13" ref="A9:D14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A9:D14" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{98FD5D52-1BC0-4054-8358-F924F6A4BAB5}" name="Code" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{09CB4271-3531-437E-96F1-FF338E0F430E}" name="Libellé niveau 1" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{2E9B13FA-3333-42A6-BF3A-F3B7AD42D98A}" name="Description" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{EBA22499-7DD5-405F-82CA-7058FFC1AB2F}" name="Commentaire" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D27" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A9:D27" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
   <autoFilter ref="A9:F188" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A9:D46" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A9:E61" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A9:E30" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{865D8B57-135B-4BFA-938D-B62BC39AC970}" name="Code"/>
     <tableColumn id="2" xr3:uid="{E07D1CE2-997E-4A59-9869-D1EFB60F0809}" name="Libellé niveau 1"/>
     <tableColumn id="5" xr3:uid="{A8693491-C517-461F-B62C-F068AE507B25}" name="Libellé niveau 2"/>
-    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A9:F30" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9B470DB1-BD5A-4D37-B9A2-613B4968664F}" name="Code"/>
-    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A9:E55" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A9:E55" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}" name="Table13611" displayName="Table13611" ref="A9:E55" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}" name="Table13611" displayName="Table13611" ref="A9:E55" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="A9:E55" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE27AEC6-A24C-4178-99A7-1B2812152DC5}" name="Code" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{EB0C358C-6506-4607-BF79-8A517F8D75A1}" name="Libellé niveau 1" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{6068A160-E74F-4F9B-B66D-B8B2A21807F0}" name="Libellé niveau 2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{F5E953CB-171A-4B76-B54B-CA690E7F0F8D}" name="Description" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{7CB61F33-9B59-4443-8AA1-CF748FC4482A}" name="Commentaire" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{FE27AEC6-A24C-4178-99A7-1B2812152DC5}" name="Code" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{EB0C358C-6506-4607-BF79-8A517F8D75A1}" name="Libellé niveau 1" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{6068A160-E74F-4F9B-B66D-B8B2A21807F0}" name="Libellé niveau 2" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{F5E953CB-171A-4B76-B54B-CA690E7F0F8D}" name="Description" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{7CB61F33-9B59-4443-8AA1-CF748FC4482A}" name="Commentaire" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9108,8 +9093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
   <dimension ref="A1:L216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -9684,7 +9669,7 @@
         <v>1803</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="C19" s="31" t="str">
         <f>'Cadre conventionnel'!$B$1</f>
@@ -9709,17 +9694,17 @@
     </row>
     <row r="20" spans="1:12" ht="15">
       <c r="A20" s="32" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B20" s="35" t="s">
         <v>2095</v>
       </c>
-      <c r="B20" s="35" t="s">
-        <v>2010</v>
-      </c>
       <c r="C20" s="31" t="str">
-        <f>'Status du vecteur'!$B$1</f>
+        <f>'Statut du vecteur'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="D20" s="31" t="str">
-        <f>'Status du vecteur'!$B$2</f>
+        <f>'Statut du vecteur'!$B$2</f>
         <v>STATUS_VECTEUR</v>
       </c>
       <c r="E20" s="33" t="s">
@@ -12485,36 +12470,28 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:K18" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}"/>
+  <conditionalFormatting sqref="A19">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+    <cfRule type="expression" priority="4">
+      <formula>ISODD(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A3:L216">
-    <cfRule type="expression" dxfId="7" priority="16">
+    <cfRule type="expression" dxfId="4" priority="16">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
     <cfRule type="expression" priority="18">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:L37 G3:K19">
-    <cfRule type="expression" dxfId="6" priority="11">
+  <conditionalFormatting sqref="G3:L37">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>G3=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>G3="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L19">
-    <cfRule type="expression" dxfId="4" priority="7">
-      <formula>L3=""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
-      <formula>L3="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-    <cfRule type="expression" priority="4">
-      <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
@@ -13589,9 +13566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9407A0FF-6A83-4239-B794-9A5636395AD1}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
@@ -16526,7 +16501,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="61"/>
@@ -16602,113 +16577,113 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="68" t="s">
+      <c r="A10" t="s">
+        <v>2064</v>
+      </c>
+      <c r="B10" t="s">
         <v>2065</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="F10" t="s">
         <v>2066</v>
       </c>
-      <c r="F10" s="68" t="s">
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
         <v>2067</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="68" t="s">
+      <c r="B11" t="s">
         <v>2068</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="F11" t="s">
         <v>2069</v>
       </c>
-      <c r="F11" s="68" t="s">
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>2070</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="68" t="s">
+      <c r="B12" t="s">
         <v>2071</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="F12" t="s">
         <v>2072</v>
       </c>
-      <c r="F12" s="68" t="s">
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>2073</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="68" t="s">
+      <c r="B13" t="s">
         <v>2074</v>
       </c>
-      <c r="B13" s="68" t="s">
+      <c r="F13" t="s">
         <v>2075</v>
       </c>
-      <c r="F13" s="68" t="s">
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>2076</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="68" t="s">
+      <c r="B14" t="s">
         <v>2077</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="F14" t="s">
         <v>2078</v>
       </c>
-      <c r="F14" s="68" t="s">
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
         <v>2079</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="68" t="s">
+      <c r="B15" t="s">
         <v>2080</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="F15" t="s">
         <v>2081</v>
       </c>
-      <c r="F15" s="68" t="s">
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>2082</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="68" t="s">
+      <c r="B16" t="s">
         <v>2083</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="F16" t="s">
         <v>2084</v>
       </c>
-      <c r="F16" s="68" t="s">
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>2085</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="68" t="s">
+      <c r="B17" t="s">
         <v>2086</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="F17" t="s">
         <v>2087</v>
       </c>
-      <c r="F17" s="68" t="s">
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>2088</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="68" t="s">
+      <c r="B18" t="s">
         <v>2089</v>
       </c>
-      <c r="B18" s="68" t="s">
+      <c r="F18" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
         <v>2090</v>
       </c>
-      <c r="F18" s="68" t="s">
-        <v>2088</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="68" t="s">
+      <c r="B19" t="s">
         <v>2091</v>
       </c>
-      <c r="B19" s="68" t="s">
-        <v>2092</v>
-      </c>
-      <c r="F19" s="68" t="s">
-        <v>2088</v>
+      <c r="F19" t="s">
+        <v>2087</v>
       </c>
     </row>
   </sheetData>
@@ -16720,7 +16695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B730C132-AF0D-4124-AB29-0565D21E3ED1}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -16748,7 +16725,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="61"/>
@@ -16825,92 +16802,92 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="66" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B10" s="54" t="s">
         <v>2011</v>
-      </c>
-      <c r="B10" s="54" t="s">
-        <v>2012</v>
       </c>
       <c r="C10" s="67"/>
       <c r="E10" s="67" t="s">
+        <v>2012</v>
+      </c>
+      <c r="F10" s="56" t="s">
         <v>2013</v>
-      </c>
-      <c r="F10" s="56" t="s">
-        <v>2014</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="50" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B11" s="39" t="s">
         <v>2015</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="E11" s="56" t="s">
         <v>2016</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>2017</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="50" t="s">
+        <v>2017</v>
+      </c>
+      <c r="B12" s="39" t="s">
         <v>2018</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="E12" s="56" t="s">
         <v>2019</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="F12" s="56" t="s">
         <v>2020</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>2021</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="50" t="s">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="39" t="s">
         <v>2022</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>2023</v>
       </c>
       <c r="C13"/>
       <c r="E13" s="56" t="s">
+        <v>2023</v>
+      </c>
+      <c r="F13" s="56" t="s">
         <v>2024</v>
-      </c>
-      <c r="F13" s="56" t="s">
-        <v>2025</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="66" t="s">
+        <v>2025</v>
+      </c>
+      <c r="C14" s="54" t="s">
         <v>2026</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="E14" s="56" t="s">
         <v>2027</v>
-      </c>
-      <c r="E14" s="56" t="s">
-        <v>2028</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="50" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B15" s="56" t="s">
         <v>2029</v>
-      </c>
-      <c r="B15" s="56" t="s">
-        <v>2030</v>
       </c>
       <c r="C15"/>
       <c r="E15" s="56" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="66" t="s">
+        <v>2031</v>
+      </c>
+      <c r="B16" s="56" t="s">
         <v>2032</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>2033</v>
       </c>
       <c r="C16" s="54"/>
       <c r="F16" s="56" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -16918,113 +16895,113 @@
         <v>1624</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="C17" s="67"/>
       <c r="E17" s="56" t="s">
+        <v>2035</v>
+      </c>
+      <c r="F17" s="56" t="s">
         <v>2036</v>
-      </c>
-      <c r="F17" s="56" t="s">
-        <v>2037</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="66" t="s">
+        <v>2037</v>
+      </c>
+      <c r="C18" s="54" t="s">
         <v>2038</v>
-      </c>
-      <c r="C18" s="54" t="s">
-        <v>2039</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="66" t="s">
+        <v>2039</v>
+      </c>
+      <c r="C19" s="54" t="s">
         <v>2040</v>
-      </c>
-      <c r="C19" s="54" t="s">
-        <v>2041</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="66" t="s">
+        <v>2041</v>
+      </c>
+      <c r="C20" s="54" t="s">
         <v>2042</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>2043</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="66" t="s">
+        <v>2043</v>
+      </c>
+      <c r="C21" s="54" t="s">
         <v>2044</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>2045</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="50" t="s">
+        <v>2045</v>
+      </c>
+      <c r="B22" s="39" t="s">
         <v>2046</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>2047</v>
       </c>
       <c r="C22"/>
       <c r="E22" s="56" t="s">
+        <v>2047</v>
+      </c>
+      <c r="F22" s="56" t="s">
         <v>2048</v>
-      </c>
-      <c r="F22" s="56" t="s">
-        <v>2049</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="50" t="s">
+        <v>2049</v>
+      </c>
+      <c r="B23" s="39" t="s">
         <v>2050</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>2051</v>
       </c>
       <c r="C23"/>
       <c r="E23" s="56" t="s">
+        <v>2051</v>
+      </c>
+      <c r="F23" s="56" t="s">
         <v>2052</v>
-      </c>
-      <c r="F23" s="56" t="s">
-        <v>2053</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="50" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B24" s="39" t="s">
         <v>2054</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>2055</v>
       </c>
       <c r="C24"/>
       <c r="E24" s="56" t="s">
+        <v>2055</v>
+      </c>
+      <c r="F24" s="56" t="s">
         <v>2056</v>
-      </c>
-      <c r="F24" s="56" t="s">
-        <v>2057</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="66" t="s">
+        <v>2057</v>
+      </c>
+      <c r="C25" s="39" t="s">
         <v>2058</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="E25" s="56" t="s">
         <v>2059</v>
-      </c>
-      <c r="E25" s="56" t="s">
-        <v>2060</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="66" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B26" s="56" t="s">
         <v>2061</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="E26" s="56" t="s">
         <v>2062</v>
-      </c>
-      <c r="E26" s="56" t="s">
-        <v>2063</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -29042,6 +29019,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -29093,15 +29079,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059494DF-AC78-4572-AFB9-E7754F64CB4B}">
   <ds:schemaRefs>
@@ -29123,27 +29100,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.07.18 17:49] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BB02A10-B2DF-4A05-9415-EC4F0022A4C9}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3930" yWindow="345" windowWidth="23385" windowHeight="13110" tabRatio="877" firstSheet="13" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -7040,8 +7040,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
+    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
@@ -7049,14 +7049,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9097,16 +9097,16 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" style="28" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="28" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="28" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="28" customWidth="1"/>
-    <col min="7" max="12" width="12.7109375" style="28" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="28"/>
+    <col min="4" max="4" width="37.1640625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="28" customWidth="1"/>
+    <col min="7" max="12" width="12.6640625" style="28" customWidth="1"/>
+    <col min="13" max="16384" width="11.5" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -9114,7 +9114,7 @@
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:12" s="30" customFormat="1" ht="15">
+    <row r="2" spans="1:12" s="30" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>1801</v>
       </c>
@@ -9152,7 +9152,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15">
+    <row r="3" spans="1:12">
       <c r="A3" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9184,7 +9184,7 @@
       <c r="K3" s="34"/>
       <c r="L3" s="34"/>
     </row>
-    <row r="4" spans="1:12" ht="15">
+    <row r="4" spans="1:12">
       <c r="A4" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9216,7 +9216,7 @@
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
     </row>
-    <row r="5" spans="1:12" ht="15">
+    <row r="5" spans="1:12">
       <c r="A5" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9248,7 +9248,7 @@
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
     </row>
-    <row r="6" spans="1:12" ht="15">
+    <row r="6" spans="1:12">
       <c r="A6" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9280,7 +9280,7 @@
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
     </row>
-    <row r="7" spans="1:12" ht="15">
+    <row r="7" spans="1:12">
       <c r="A7" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9310,7 +9310,7 @@
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
     </row>
-    <row r="8" spans="1:12" ht="15">
+    <row r="8" spans="1:12">
       <c r="A8" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9340,7 +9340,7 @@
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
     </row>
-    <row r="9" spans="1:12" ht="15">
+    <row r="9" spans="1:12">
       <c r="A9" s="31" t="s">
         <v>1779</v>
       </c>
@@ -9372,7 +9372,7 @@
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
     </row>
-    <row r="10" spans="1:12" ht="15">
+    <row r="10" spans="1:12">
       <c r="A10" s="31" t="s">
         <v>1779</v>
       </c>
@@ -9404,7 +9404,7 @@
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
     </row>
-    <row r="11" spans="1:12" ht="15">
+    <row r="11" spans="1:12">
       <c r="A11" s="32" t="s">
         <v>1795</v>
       </c>
@@ -9436,7 +9436,7 @@
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
     </row>
-    <row r="12" spans="1:12" ht="15">
+    <row r="12" spans="1:12">
       <c r="A12" s="32" t="s">
         <v>1795</v>
       </c>
@@ -9466,7 +9466,7 @@
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
     </row>
-    <row r="13" spans="1:12" ht="15">
+    <row r="13" spans="1:12">
       <c r="A13" s="31" t="s">
         <v>1796</v>
       </c>
@@ -9498,7 +9498,7 @@
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
     </row>
-    <row r="14" spans="1:12" ht="15">
+    <row r="14" spans="1:12">
       <c r="A14" s="31" t="s">
         <v>1802</v>
       </c>
@@ -9532,7 +9532,7 @@
       </c>
       <c r="L14" s="34"/>
     </row>
-    <row r="15" spans="1:12" ht="15">
+    <row r="15" spans="1:12">
       <c r="A15" s="32" t="s">
         <v>1802</v>
       </c>
@@ -9566,7 +9566,7 @@
       </c>
       <c r="L15" s="34"/>
     </row>
-    <row r="16" spans="1:12" ht="15">
+    <row r="16" spans="1:12">
       <c r="A16" s="31" t="s">
         <v>1802</v>
       </c>
@@ -9602,7 +9602,7 @@
       </c>
       <c r="L16" s="34"/>
     </row>
-    <row r="17" spans="1:12" ht="15">
+    <row r="17" spans="1:12">
       <c r="A17" s="31" t="s">
         <v>1796</v>
       </c>
@@ -9634,7 +9634,7 @@
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
     </row>
-    <row r="18" spans="1:12" ht="15">
+    <row r="18" spans="1:12">
       <c r="A18" s="32" t="s">
         <v>1803</v>
       </c>
@@ -9664,7 +9664,7 @@
       <c r="K18" s="34"/>
       <c r="L18" s="34"/>
     </row>
-    <row r="19" spans="1:12" ht="15">
+    <row r="19" spans="1:12">
       <c r="A19" s="32" t="s">
         <v>1803</v>
       </c>
@@ -9692,7 +9692,7 @@
       </c>
       <c r="L19" s="34"/>
     </row>
-    <row r="20" spans="1:12" ht="15">
+    <row r="20" spans="1:12">
       <c r="A20" s="32" t="s">
         <v>2094</v>
       </c>
@@ -9724,7 +9724,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15">
+    <row r="21" spans="1:12">
       <c r="A21" s="32"/>
       <c r="B21" s="35"/>
       <c r="C21" s="32"/>
@@ -9738,7 +9738,7 @@
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>
     </row>
-    <row r="22" spans="1:12" ht="15">
+    <row r="22" spans="1:12">
       <c r="A22" s="32"/>
       <c r="B22" s="35"/>
       <c r="C22" s="32"/>
@@ -9752,7 +9752,7 @@
       <c r="K22" s="34"/>
       <c r="L22" s="34"/>
     </row>
-    <row r="23" spans="1:12" ht="15">
+    <row r="23" spans="1:12">
       <c r="A23" s="32"/>
       <c r="B23" s="35"/>
       <c r="C23" s="32"/>
@@ -9766,7 +9766,7 @@
       <c r="K23" s="34"/>
       <c r="L23" s="34"/>
     </row>
-    <row r="24" spans="1:12" ht="15">
+    <row r="24" spans="1:12">
       <c r="A24" s="32"/>
       <c r="B24" s="35"/>
       <c r="C24" s="32"/>
@@ -9780,7 +9780,7 @@
       <c r="K24" s="34"/>
       <c r="L24" s="34"/>
     </row>
-    <row r="25" spans="1:12" ht="15">
+    <row r="25" spans="1:12">
       <c r="A25" s="32"/>
       <c r="B25" s="35"/>
       <c r="C25" s="32"/>
@@ -12479,11 +12479,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:L216">
+    <cfRule type="expression" priority="18">
+      <formula>ISODD(ROW())</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="4" priority="16">
       <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-    <cfRule type="expression" priority="18">
-      <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:L37">
@@ -12495,11 +12495,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>L19="X"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>L19=""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>L19="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -12536,13 +12536,13 @@
       <selection activeCell="E9" sqref="E9:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
-    <col min="6" max="6" width="61.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="6" max="6" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12696,14 +12696,14 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13125,14 +13125,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13568,13 +13568,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14018,15 +14018,15 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="36" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="36" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="36" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="36"/>
+    <col min="1" max="1" width="21.5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.1640625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="36" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="36" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1">
@@ -14091,7 +14091,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:6" customFormat="1" ht="36.75">
+    <row r="8" spans="1:6" customFormat="1" ht="40">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -15043,13 +15043,13 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15465,13 +15465,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15977,13 +15977,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16065,7 +16065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="48" t="s">
         <v>1888</v>
       </c>
@@ -16091,7 +16091,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="50" t="s">
         <v>1890</v>
       </c>
@@ -16104,7 +16104,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="16">
       <c r="A13" s="50" t="s">
         <v>1580</v>
       </c>
@@ -16117,7 +16117,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" s="50" t="s">
         <v>1444</v>
       </c>
@@ -16130,7 +16130,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="16">
       <c r="A15" s="50" t="s">
         <v>1573</v>
       </c>
@@ -16143,7 +16143,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="16">
       <c r="A16" s="50" t="s">
         <v>1891</v>
       </c>
@@ -16156,7 +16156,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="16">
       <c r="A17" s="51" t="s">
         <v>1892</v>
       </c>
@@ -16169,7 +16169,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="16">
       <c r="A18" s="52" t="s">
         <v>1893</v>
       </c>
@@ -16182,7 +16182,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="16">
       <c r="A19" s="50" t="s">
         <v>1894</v>
       </c>
@@ -16195,7 +16195,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="16">
       <c r="A20" s="50" t="s">
         <v>1895</v>
       </c>
@@ -16208,7 +16208,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="16">
       <c r="A21" s="50" t="s">
         <v>1896</v>
       </c>
@@ -16479,11 +16479,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="95.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="95.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="56" customFormat="1">
@@ -16695,19 +16695,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B730C132-AF0D-4124-AB29-0565D21E3ED1}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" style="56" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="56" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" style="56" customWidth="1"/>
-    <col min="5" max="5" width="88.7109375" style="56" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="56" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="56"/>
+    <col min="1" max="1" width="21.5" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" style="56" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="56" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="56" customWidth="1"/>
+    <col min="5" max="5" width="88.6640625" style="56" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="56" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16800,7 +16800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="66" t="s">
         <v>2010</v>
       </c>
@@ -16815,7 +16815,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="50" t="s">
         <v>2014</v>
       </c>
@@ -16826,7 +16826,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="50" t="s">
         <v>2017</v>
       </c>
@@ -16840,7 +16840,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="50" t="s">
         <v>2021</v>
       </c>
@@ -16855,7 +16855,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="66" t="s">
         <v>2025</v>
       </c>
@@ -16866,7 +16866,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="50" t="s">
         <v>2028</v>
       </c>
@@ -16878,7 +16878,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="66" t="s">
         <v>2031</v>
       </c>
@@ -16890,7 +16890,7 @@
         <v>2033</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="16">
       <c r="A17" s="66" t="s">
         <v>1624</v>
       </c>
@@ -16905,7 +16905,7 @@
         <v>2036</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="16">
       <c r="A18" s="66" t="s">
         <v>2037</v>
       </c>
@@ -16913,7 +16913,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="16">
       <c r="A19" s="66" t="s">
         <v>2039</v>
       </c>
@@ -16921,7 +16921,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="16">
       <c r="A20" s="66" t="s">
         <v>2041</v>
       </c>
@@ -16929,7 +16929,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="16">
       <c r="A21" s="66" t="s">
         <v>2043</v>
       </c>
@@ -16937,7 +16937,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="16">
       <c r="A22" s="50" t="s">
         <v>2045</v>
       </c>
@@ -16952,7 +16952,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="16">
       <c r="A23" s="50" t="s">
         <v>2049</v>
       </c>
@@ -16967,7 +16967,7 @@
         <v>2052</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="16">
       <c r="A24" s="50" t="s">
         <v>2053</v>
       </c>
@@ -16982,7 +16982,7 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="16">
       <c r="A25" s="66" t="s">
         <v>2057</v>
       </c>
@@ -16993,7 +16993,7 @@
         <v>2059</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="16">
       <c r="A26" s="66" t="s">
         <v>2060</v>
       </c>
@@ -17165,14 +17165,14 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" customWidth="1"/>
+    <col min="5" max="5" width="47.83203125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17255,7 +17255,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="64.5">
+    <row r="10" spans="1:6" ht="60">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -17281,7 +17281,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -17295,7 +17295,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="26.25">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -17309,7 +17309,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -17322,7 +17322,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" ht="26.25">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -17350,7 +17350,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="26.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -17376,7 +17376,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -17391,7 +17391,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -17417,7 +17417,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="39">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -17431,7 +17431,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="39">
+    <row r="23" spans="1:6" ht="30">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -17455,7 +17455,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25">
+    <row r="25" spans="1:6" ht="30">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -17469,7 +17469,7 @@
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="26.25">
+    <row r="26" spans="1:6" ht="30">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -17483,7 +17483,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="26.25">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -17497,7 +17497,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6" ht="26.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -17533,7 +17533,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:6" ht="51.75">
+    <row r="31" spans="1:6" ht="60">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -17547,7 +17547,7 @@
       </c>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" ht="26.25">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
@@ -17586,7 +17586,7 @@
       </c>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25">
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -17612,7 +17612,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" ht="102.75">
+    <row r="37" spans="1:6" ht="120">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
@@ -17626,7 +17626,7 @@
       </c>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" ht="26.25">
+    <row r="38" spans="1:6" ht="30">
       <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
@@ -17640,7 +17640,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="39">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -17665,7 +17665,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" ht="39">
+    <row r="41" spans="1:6" ht="30">
       <c r="A41" s="2" t="s">
         <v>116</v>
       </c>
@@ -17679,7 +17679,7 @@
       </c>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>119</v>
       </c>
@@ -17693,7 +17693,7 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" ht="39">
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -17717,7 +17717,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" ht="39">
+    <row r="45" spans="1:6" ht="45">
       <c r="A45" s="2" t="s">
         <v>127</v>
       </c>
@@ -17816,7 +17816,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6" ht="26.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
         <v>145</v>
       </c>
@@ -17830,7 +17830,7 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="64.5">
+    <row r="54" spans="1:6" ht="60">
       <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
@@ -18201,7 +18201,7 @@
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="1:6" ht="39">
+    <row r="85" spans="1:6" ht="45">
       <c r="A85" s="2" t="s">
         <v>214</v>
       </c>
@@ -18227,7 +18227,7 @@
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:6" ht="128.25">
+    <row r="87" spans="1:6" ht="135">
       <c r="A87" s="2" t="s">
         <v>219</v>
       </c>
@@ -18253,7 +18253,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="51.75">
+    <row r="89" spans="1:6" ht="60">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
@@ -18266,7 +18266,7 @@
       </c>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
         <v>214</v>
       </c>
@@ -18306,7 +18306,7 @@
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25">
+    <row r="93" spans="1:6" ht="30">
       <c r="A93" s="2" t="s">
         <v>230</v>
       </c>
@@ -18477,7 +18477,7 @@
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
     </row>
-    <row r="107" spans="1:6" ht="26.25">
+    <row r="107" spans="1:6" ht="30">
       <c r="A107" s="2" t="s">
         <v>261</v>
       </c>
@@ -18491,7 +18491,7 @@
       </c>
       <c r="F107" s="12"/>
     </row>
-    <row r="108" spans="1:6" ht="26.25">
+    <row r="108" spans="1:6">
       <c r="A108" s="2" t="s">
         <v>264</v>
       </c>
@@ -18615,7 +18615,7 @@
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" ht="26.25">
+    <row r="118" spans="1:6" ht="30">
       <c r="A118" s="2" t="s">
         <v>287</v>
       </c>
@@ -18629,7 +18629,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="26.25">
+    <row r="119" spans="1:6">
       <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
@@ -18642,7 +18642,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="39">
+    <row r="120" spans="1:6" ht="45">
       <c r="A120" s="2" t="s">
         <v>293</v>
       </c>
@@ -18680,7 +18680,7 @@
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" ht="39">
+    <row r="123" spans="1:6" ht="45">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -18741,7 +18741,7 @@
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" ht="39">
+    <row r="128" spans="1:6" ht="45">
       <c r="A128" s="2" t="s">
         <v>311</v>
       </c>
@@ -18875,7 +18875,7 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="26.25">
+    <row r="139" spans="1:6" ht="30">
       <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
@@ -18900,7 +18900,7 @@
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
     </row>
-    <row r="141" spans="1:6" ht="26.25">
+    <row r="141" spans="1:6" ht="30">
       <c r="A141" s="2" t="s">
         <v>341</v>
       </c>
@@ -18914,7 +18914,7 @@
       </c>
       <c r="F141" s="12"/>
     </row>
-    <row r="142" spans="1:6" ht="26.25">
+    <row r="142" spans="1:6" ht="30">
       <c r="A142" s="2" t="s">
         <v>342</v>
       </c>
@@ -18928,7 +18928,7 @@
       </c>
       <c r="F142" s="12"/>
     </row>
-    <row r="143" spans="1:6" ht="26.25">
+    <row r="143" spans="1:6">
       <c r="A143" s="2" t="s">
         <v>343</v>
       </c>
@@ -18942,7 +18942,7 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="26.25">
+    <row r="144" spans="1:6" ht="30">
       <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
@@ -18971,7 +18971,7 @@
       </c>
       <c r="F145" s="12"/>
     </row>
-    <row r="146" spans="1:6" ht="26.25">
+    <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
         <v>347</v>
       </c>
@@ -18985,7 +18985,7 @@
       </c>
       <c r="F146" s="12"/>
     </row>
-    <row r="147" spans="1:6" ht="39">
+    <row r="147" spans="1:6" ht="30">
       <c r="A147" s="2" t="s">
         <v>348</v>
       </c>
@@ -18999,7 +18999,7 @@
       </c>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" spans="1:6" ht="39">
+    <row r="148" spans="1:6" ht="30">
       <c r="A148" s="2" t="s">
         <v>349</v>
       </c>
@@ -19013,7 +19013,7 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="26.25">
+    <row r="149" spans="1:6" ht="30">
       <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
@@ -19026,7 +19026,7 @@
       </c>
       <c r="F149" s="12"/>
     </row>
-    <row r="150" spans="1:6" ht="26.25">
+    <row r="150" spans="1:6" ht="30">
       <c r="A150" s="2" t="s">
         <v>351</v>
       </c>
@@ -19040,7 +19040,7 @@
       </c>
       <c r="F150" s="12"/>
     </row>
-    <row r="151" spans="1:6" ht="26.25">
+    <row r="151" spans="1:6" ht="30">
       <c r="A151" s="2" t="s">
         <v>352</v>
       </c>
@@ -19172,7 +19172,7 @@
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
     </row>
-    <row r="162" spans="1:6" ht="39">
+    <row r="162" spans="1:6" ht="30">
       <c r="A162" s="2" t="s">
         <v>373</v>
       </c>
@@ -19186,7 +19186,7 @@
       </c>
       <c r="F162" s="12"/>
     </row>
-    <row r="163" spans="1:6" ht="39">
+    <row r="163" spans="1:6" ht="45">
       <c r="A163" s="2" t="s">
         <v>376</v>
       </c>
@@ -19200,7 +19200,7 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="39">
+    <row r="164" spans="1:6" ht="45">
       <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
@@ -19251,7 +19251,7 @@
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
     </row>
-    <row r="168" spans="1:6" ht="26.25">
+    <row r="168" spans="1:6" ht="30">
       <c r="A168" s="2" t="s">
         <v>389</v>
       </c>
@@ -19468,7 +19468,7 @@
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
     </row>
-    <row r="186" spans="1:6" ht="26.25">
+    <row r="186" spans="1:6" ht="30">
       <c r="A186" s="2" t="s">
         <v>426</v>
       </c>
@@ -19604,7 +19604,7 @@
       </c>
       <c r="F196" s="12"/>
     </row>
-    <row r="197" spans="1:6" ht="26.25">
+    <row r="197" spans="1:6">
       <c r="A197" s="2" t="s">
         <v>451</v>
       </c>
@@ -19704,7 +19704,7 @@
       <c r="E204" s="12"/>
       <c r="F204" s="12"/>
     </row>
-    <row r="205" spans="1:6" ht="26.25">
+    <row r="205" spans="1:6" ht="30">
       <c r="A205" s="2" t="s">
         <v>470</v>
       </c>
@@ -19730,7 +19730,7 @@
       <c r="E206" s="12"/>
       <c r="F206" s="12"/>
     </row>
-    <row r="207" spans="1:6" ht="26.25">
+    <row r="207" spans="1:6" ht="30">
       <c r="A207" s="2" t="s">
         <v>475</v>
       </c>
@@ -19828,7 +19828,7 @@
       <c r="E214" s="12"/>
       <c r="F214" s="12"/>
     </row>
-    <row r="215" spans="1:6" ht="26.25">
+    <row r="215" spans="1:6" ht="30">
       <c r="A215" s="2" t="s">
         <v>493</v>
       </c>
@@ -20649,7 +20649,7 @@
       <c r="E282" s="12"/>
       <c r="F282" s="12"/>
     </row>
-    <row r="283" spans="1:6" ht="26.25">
+    <row r="283" spans="1:6" ht="30">
       <c r="A283" s="2" t="s">
         <v>638</v>
       </c>
@@ -20663,7 +20663,7 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="26.25">
+    <row r="284" spans="1:6" ht="30">
       <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
@@ -21012,13 +21012,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="80.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="80.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -21501,13 +21501,13 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22008,12 +22008,12 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -22170,12 +22170,12 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -22359,9 +22359,9 @@
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22894,14 +22894,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -25609,16 +25609,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -25629,7 +25629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.75">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -25695,7 +25695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="39">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="2" t="s">
         <v>1082</v>
       </c>
@@ -25717,7 +25717,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="26.25">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="2" t="s">
         <v>1087</v>
       </c>
@@ -25727,7 +25727,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="39">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="2" t="s">
         <v>1089</v>
       </c>
@@ -25737,7 +25737,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="26.25">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" s="2" t="s">
         <v>1091</v>
       </c>
@@ -25747,7 +25747,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="26.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>1093</v>
       </c>
@@ -25757,7 +25757,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="26.25">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" s="2" t="s">
         <v>1095</v>
       </c>
@@ -25769,7 +25769,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="39">
+    <row r="17" spans="1:4" ht="45">
       <c r="A17" s="2" t="s">
         <v>1098</v>
       </c>
@@ -25781,7 +25781,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="39">
+    <row r="18" spans="1:4" ht="30">
       <c r="A18" s="2" t="s">
         <v>1101</v>
       </c>
@@ -25791,7 +25791,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="39">
+    <row r="19" spans="1:4" ht="45">
       <c r="A19" s="2" t="s">
         <v>1103</v>
       </c>
@@ -25801,7 +25801,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="26.25">
+    <row r="20" spans="1:4" ht="30">
       <c r="A20" s="2" t="s">
         <v>1105</v>
       </c>
@@ -25811,7 +25811,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="26.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>1107</v>
       </c>
@@ -25821,7 +25821,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="26.25">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" s="2" t="s">
         <v>1109</v>
       </c>
@@ -25851,7 +25851,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="26.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>1115</v>
       </c>
@@ -25881,7 +25881,7 @@
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="26.25">
+    <row r="28" spans="1:4" ht="30">
       <c r="A28" s="2" t="s">
         <v>1120</v>
       </c>
@@ -25893,7 +25893,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="26.25">
+    <row r="29" spans="1:4" ht="30">
       <c r="A29" s="2" t="s">
         <v>1123</v>
       </c>
@@ -25905,7 +25905,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="26.25">
+    <row r="30" spans="1:4" ht="30">
       <c r="A30" s="2" t="s">
         <v>1126</v>
       </c>
@@ -25927,7 +25927,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="26.25">
+    <row r="32" spans="1:4" ht="30">
       <c r="A32" s="2" t="s">
         <v>1131</v>
       </c>
@@ -25939,7 +25939,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="39">
+    <row r="33" spans="1:4" ht="30">
       <c r="A33" s="2" t="s">
         <v>1134</v>
       </c>
@@ -25951,7 +25951,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="26.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>1137</v>
       </c>
@@ -25963,7 +25963,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="128.25">
+    <row r="35" spans="1:4" ht="135">
       <c r="A35" s="2" t="s">
         <v>1140</v>
       </c>
@@ -25975,7 +25975,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="128.25">
+    <row r="36" spans="1:4" ht="135">
       <c r="A36" s="2" t="s">
         <v>1143</v>
       </c>
@@ -26059,7 +26059,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="26.25">
+    <row r="44" spans="1:4" ht="30">
       <c r="A44" s="2" t="s">
         <v>1160</v>
       </c>
@@ -26071,7 +26071,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="26.25">
+    <row r="45" spans="1:4" ht="30">
       <c r="A45" s="2" t="s">
         <v>1163</v>
       </c>
@@ -26081,7 +26081,7 @@
       <c r="C45" s="12"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="77.25">
+    <row r="46" spans="1:4" ht="75">
       <c r="A46" s="2" t="s">
         <v>1165</v>
       </c>
@@ -26110,13 +26110,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26231,7 +26231,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5" ht="26.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>1177</v>
       </c>
@@ -26255,7 +26255,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" ht="26.25">
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="2" t="s">
         <v>1182</v>
       </c>
@@ -26268,7 +26268,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" ht="26.25">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="2" t="s">
         <v>1185</v>
       </c>
@@ -26292,7 +26292,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="48.75">
+    <row r="18" spans="1:5" ht="40">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -26305,7 +26305,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="64.5">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -26454,7 +26454,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="26.25">
+    <row r="32" spans="1:5" ht="30">
       <c r="A32" s="2" t="s">
         <v>1222</v>
       </c>
@@ -26467,7 +26467,7 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" ht="26.25">
+    <row r="33" spans="1:5" ht="30">
       <c r="A33" s="2" t="s">
         <v>1225</v>
       </c>
@@ -26554,7 +26554,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" ht="51.75">
+    <row r="40" spans="1:5" ht="45">
       <c r="A40" s="2" t="s">
         <v>1244</v>
       </c>
@@ -26591,7 +26591,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" ht="26.25">
+    <row r="43" spans="1:5" ht="30">
       <c r="A43" s="2" t="s">
         <v>1252</v>
       </c>
@@ -26604,7 +26604,7 @@
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5" ht="39">
+    <row r="44" spans="1:5" ht="30">
       <c r="A44" s="2" t="s">
         <v>1253</v>
       </c>
@@ -26663,7 +26663,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" ht="26.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="2" t="s">
         <v>1265</v>
       </c>
@@ -26698,7 +26698,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5" ht="26.25">
+    <row r="52" spans="1:5" ht="30">
       <c r="A52" s="2" t="s">
         <v>1272</v>
       </c>
@@ -26792,7 +26792,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="39">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -26834,14 +26834,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.7109375" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.6640625" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27455,14 +27455,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27890,13 +27890,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -27982,7 +27982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="32">
       <c r="A10" s="18" t="s">
         <v>1314</v>
       </c>
@@ -27995,7 +27995,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="32">
       <c r="A11" s="18" t="s">
         <v>1317</v>
       </c>
@@ -28008,7 +28008,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="18" t="s">
         <v>1320</v>
       </c>
@@ -28021,7 +28021,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="32">
       <c r="A13" s="18" t="s">
         <v>1323</v>
       </c>
@@ -28034,7 +28034,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" s="18" t="s">
         <v>1326</v>
       </c>
@@ -28047,7 +28047,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:5" ht="32">
       <c r="A15" s="18" t="s">
         <v>1329</v>
       </c>
@@ -28060,7 +28060,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="32">
       <c r="A16" s="18" t="s">
         <v>1332</v>
       </c>
@@ -28073,7 +28073,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="32">
       <c r="A17" s="18" t="s">
         <v>1335</v>
       </c>
@@ -28086,7 +28086,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="48">
       <c r="A18" s="18" t="s">
         <v>1338</v>
       </c>
@@ -28099,7 +28099,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="48">
       <c r="A19" s="18" t="s">
         <v>1341</v>
       </c>
@@ -28112,7 +28112,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" ht="32">
       <c r="A20" s="18" t="s">
         <v>1344</v>
       </c>
@@ -28125,7 +28125,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5" ht="32">
       <c r="A21" s="18" t="s">
         <v>1347</v>
       </c>
@@ -28138,7 +28138,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5" ht="32">
       <c r="A22" s="18" t="s">
         <v>1350</v>
       </c>
@@ -28151,7 +28151,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5" ht="32">
       <c r="A23" s="18" t="s">
         <v>1353</v>
       </c>
@@ -28164,7 +28164,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="32">
       <c r="A24" s="18" t="s">
         <v>1356</v>
       </c>
@@ -28177,7 +28177,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5" ht="32">
       <c r="A25" s="18" t="s">
         <v>1359</v>
       </c>
@@ -28190,7 +28190,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5" ht="32">
       <c r="A26" s="18" t="s">
         <v>1362</v>
       </c>
@@ -28203,7 +28203,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="16">
       <c r="A27" s="18" t="s">
         <v>1365</v>
       </c>
@@ -28216,7 +28216,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="30">
+    <row r="28" spans="1:5" ht="32">
       <c r="A28" s="18" t="s">
         <v>1367</v>
       </c>
@@ -28229,7 +28229,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="16">
       <c r="A29" s="18" t="s">
         <v>1370</v>
       </c>
@@ -28242,7 +28242,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="16">
       <c r="A30" s="18" t="s">
         <v>1373</v>
       </c>
@@ -28270,13 +28270,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -28373,7 +28373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="18" t="s">
         <v>1378</v>
       </c>
@@ -28387,7 +28387,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="48">
       <c r="A11" s="18" t="s">
         <v>1381</v>
       </c>
@@ -28401,7 +28401,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="45">
+    <row r="12" spans="1:6" ht="32">
       <c r="A12" s="18" t="s">
         <v>1384</v>
       </c>
@@ -28415,7 +28415,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="32">
       <c r="A13" s="18" t="s">
         <v>1387</v>
       </c>
@@ -28429,7 +28429,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:6" ht="32">
       <c r="A14" s="18" t="s">
         <v>1390</v>
       </c>
@@ -28443,7 +28443,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="32">
       <c r="A15" s="18" t="s">
         <v>1393</v>
       </c>
@@ -28457,7 +28457,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6" ht="32">
       <c r="A16" s="18" t="s">
         <v>1396</v>
       </c>
@@ -28471,7 +28471,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="45">
+    <row r="17" spans="1:6" ht="48">
       <c r="A17" s="18" t="s">
         <v>1370</v>
       </c>
@@ -28485,7 +28485,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="30">
+    <row r="18" spans="1:6" ht="32">
       <c r="A18" s="18" t="s">
         <v>1401</v>
       </c>
@@ -29019,15 +29019,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -29079,6 +29070,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059494DF-AC78-4572-AFB9-E7754F64CB4B}">
   <ds:schemaRefs>
@@ -29100,27 +29100,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.07.19 09:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -28605,8 +28605,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="5a233c5be867259e7f523794110a7773">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71fc54e2a62b1985aea6da9d2195ce0c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -28669,12 +28669,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -28787,7 +28787,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -28806,7 +28806,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -28879,7 +28879,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -28928,8 +28928,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -29080,23 +29080,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059494DF-AC78-4572-AFB9-E7754F64CB4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ECB47E9-2B60-4219-92DB-621EC7B64685}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
[24.07.19 17:39] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BB02A10-B2DF-4A05-9415-EC4F0022A4C9}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35A5D8E9-2519-457B-9EB1-2338627C3F4B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="877" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -6373,9 +6373,6 @@
     <t>Annulation  de l’intervention</t>
   </si>
   <si>
-    <t>La ressource engagée a été annulée : heure d'annulation de la ressource</t>
-  </si>
-  <si>
     <t>BILAN</t>
   </si>
   <si>
@@ -6569,6 +6566,9 @@
   </si>
   <si>
     <t>Statut du vecteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La ressource engagée a été annulée </t>
   </si>
 </sst>
 </file>
@@ -7040,8 +7040,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
@@ -7049,14 +7049,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9097,16 +9097,16 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="32.5" style="28" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="28" customWidth="1"/>
-    <col min="4" max="4" width="37.1640625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="28" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="28" customWidth="1"/>
-    <col min="7" max="12" width="12.6640625" style="28" customWidth="1"/>
-    <col min="13" max="16384" width="11.5" style="28"/>
+    <col min="4" max="4" width="37.140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="28" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="28" customWidth="1"/>
+    <col min="7" max="12" width="12.7109375" style="28" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -9114,7 +9114,7 @@
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:12" s="30" customFormat="1">
+    <row r="2" spans="1:12" s="30" customFormat="1" ht="15">
       <c r="A2" s="29" t="s">
         <v>1801</v>
       </c>
@@ -9152,7 +9152,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="15">
       <c r="A3" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9184,7 +9184,7 @@
       <c r="K3" s="34"/>
       <c r="L3" s="34"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="15">
       <c r="A4" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9216,7 +9216,7 @@
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" ht="15">
       <c r="A5" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9248,7 +9248,7 @@
       <c r="K5" s="34"/>
       <c r="L5" s="34"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" ht="15">
       <c r="A6" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9280,7 +9280,7 @@
       <c r="K6" s="34"/>
       <c r="L6" s="34"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" ht="15">
       <c r="A7" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9310,7 +9310,7 @@
       <c r="K7" s="34"/>
       <c r="L7" s="34"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" ht="15">
       <c r="A8" s="31" t="s">
         <v>1776</v>
       </c>
@@ -9340,7 +9340,7 @@
       <c r="K8" s="34"/>
       <c r="L8" s="34"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" ht="15">
       <c r="A9" s="31" t="s">
         <v>1779</v>
       </c>
@@ -9372,7 +9372,7 @@
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" ht="15">
       <c r="A10" s="31" t="s">
         <v>1779</v>
       </c>
@@ -9404,7 +9404,7 @@
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" ht="15">
       <c r="A11" s="32" t="s">
         <v>1795</v>
       </c>
@@ -9436,7 +9436,7 @@
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" ht="15">
       <c r="A12" s="32" t="s">
         <v>1795</v>
       </c>
@@ -9466,7 +9466,7 @@
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" ht="15">
       <c r="A13" s="31" t="s">
         <v>1796</v>
       </c>
@@ -9498,7 +9498,7 @@
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" ht="15">
       <c r="A14" s="31" t="s">
         <v>1802</v>
       </c>
@@ -9532,7 +9532,7 @@
       </c>
       <c r="L14" s="34"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" ht="15">
       <c r="A15" s="32" t="s">
         <v>1802</v>
       </c>
@@ -9566,7 +9566,7 @@
       </c>
       <c r="L15" s="34"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" ht="15">
       <c r="A16" s="31" t="s">
         <v>1802</v>
       </c>
@@ -9602,7 +9602,7 @@
       </c>
       <c r="L16" s="34"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="15">
       <c r="A17" s="31" t="s">
         <v>1796</v>
       </c>
@@ -9634,7 +9634,7 @@
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="15">
       <c r="A18" s="32" t="s">
         <v>1803</v>
       </c>
@@ -9664,12 +9664,12 @@
       <c r="K18" s="34"/>
       <c r="L18" s="34"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="15">
       <c r="A19" s="32" t="s">
         <v>1803</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="C19" s="31" t="str">
         <f>'Cadre conventionnel'!$B$1</f>
@@ -9692,12 +9692,12 @@
       </c>
       <c r="L19" s="34"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" ht="15">
       <c r="A20" s="32" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B20" s="35" t="s">
         <v>2094</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>2095</v>
       </c>
       <c r="C20" s="31" t="str">
         <f>'Statut du vecteur'!$B$1</f>
@@ -9724,7 +9724,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" ht="15">
       <c r="A21" s="32"/>
       <c r="B21" s="35"/>
       <c r="C21" s="32"/>
@@ -9738,7 +9738,7 @@
       <c r="K21" s="34"/>
       <c r="L21" s="34"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="15">
       <c r="A22" s="32"/>
       <c r="B22" s="35"/>
       <c r="C22" s="32"/>
@@ -9752,7 +9752,7 @@
       <c r="K22" s="34"/>
       <c r="L22" s="34"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="15">
       <c r="A23" s="32"/>
       <c r="B23" s="35"/>
       <c r="C23" s="32"/>
@@ -9766,7 +9766,7 @@
       <c r="K23" s="34"/>
       <c r="L23" s="34"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" ht="15">
       <c r="A24" s="32"/>
       <c r="B24" s="35"/>
       <c r="C24" s="32"/>
@@ -9780,7 +9780,7 @@
       <c r="K24" s="34"/>
       <c r="L24" s="34"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="15">
       <c r="A25" s="32"/>
       <c r="B25" s="35"/>
       <c r="C25" s="32"/>
@@ -12479,11 +12479,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:L216">
+    <cfRule type="expression" dxfId="4" priority="16">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
     <cfRule type="expression" priority="18">
       <formula>ISODD(ROW())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="16">
-      <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:L37">
@@ -12495,11 +12495,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>L19=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>L19="X"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>L19=""</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -12536,13 +12536,13 @@
       <selection activeCell="E9" sqref="E9:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
-    <col min="6" max="6" width="61.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12696,14 +12696,14 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13125,14 +13125,14 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13568,13 +13568,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14014,19 +14014,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EE5AD-9985-4D20-8EAC-8B61AD8038D6}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.1640625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="36" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="36" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" style="36" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" style="36"/>
+    <col min="1" max="1" width="21.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="36" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="36" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="36" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1">
@@ -14091,7 +14091,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:6" customFormat="1" ht="40">
+    <row r="8" spans="1:6" customFormat="1" ht="36.75">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -15040,16 +15040,16 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15465,13 +15465,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15977,13 +15977,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16065,7 +16065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
+    <row r="10" spans="1:5">
       <c r="A10" s="48" t="s">
         <v>1888</v>
       </c>
@@ -16091,7 +16091,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:5">
       <c r="A12" s="50" t="s">
         <v>1890</v>
       </c>
@@ -16104,7 +16104,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="16">
+    <row r="13" spans="1:5">
       <c r="A13" s="50" t="s">
         <v>1580</v>
       </c>
@@ -16117,7 +16117,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:5">
       <c r="A14" s="50" t="s">
         <v>1444</v>
       </c>
@@ -16130,7 +16130,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="16">
+    <row r="15" spans="1:5">
       <c r="A15" s="50" t="s">
         <v>1573</v>
       </c>
@@ -16143,7 +16143,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="16">
+    <row r="16" spans="1:5">
       <c r="A16" s="50" t="s">
         <v>1891</v>
       </c>
@@ -16156,7 +16156,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="16">
+    <row r="17" spans="1:5">
       <c r="A17" s="51" t="s">
         <v>1892</v>
       </c>
@@ -16169,7 +16169,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="16">
+    <row r="18" spans="1:5">
       <c r="A18" s="52" t="s">
         <v>1893</v>
       </c>
@@ -16182,7 +16182,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="16">
+    <row r="19" spans="1:5">
       <c r="A19" s="50" t="s">
         <v>1894</v>
       </c>
@@ -16195,7 +16195,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="16">
+    <row r="20" spans="1:5">
       <c r="A20" s="50" t="s">
         <v>1895</v>
       </c>
@@ -16208,7 +16208,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="16">
+    <row r="21" spans="1:5">
       <c r="A21" s="50" t="s">
         <v>1896</v>
       </c>
@@ -16479,11 +16479,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="95.5" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="95.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="56" customFormat="1">
@@ -16501,7 +16501,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="61"/>
@@ -16578,112 +16578,112 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B10" t="s">
         <v>2064</v>
       </c>
-      <c r="B10" t="s">
+      <c r="F10" t="s">
         <v>2065</v>
-      </c>
-      <c r="F10" t="s">
-        <v>2066</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>2066</v>
+      </c>
+      <c r="B11" t="s">
         <v>2067</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F11" t="s">
         <v>2068</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2069</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B12" t="s">
         <v>2070</v>
       </c>
-      <c r="B12" t="s">
+      <c r="F12" t="s">
         <v>2071</v>
-      </c>
-      <c r="F12" t="s">
-        <v>2072</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B13" t="s">
         <v>2073</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F13" t="s">
         <v>2074</v>
-      </c>
-      <c r="F13" t="s">
-        <v>2075</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B14" t="s">
         <v>2076</v>
       </c>
-      <c r="B14" t="s">
+      <c r="F14" t="s">
         <v>2077</v>
-      </c>
-      <c r="F14" t="s">
-        <v>2078</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
+        <v>2078</v>
+      </c>
+      <c r="B15" t="s">
         <v>2079</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F15" t="s">
         <v>2080</v>
-      </c>
-      <c r="F15" t="s">
-        <v>2081</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B16" t="s">
         <v>2082</v>
       </c>
-      <c r="B16" t="s">
+      <c r="F16" t="s">
         <v>2083</v>
-      </c>
-      <c r="F16" t="s">
-        <v>2084</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B17" t="s">
         <v>2085</v>
       </c>
-      <c r="B17" t="s">
+      <c r="F17" t="s">
         <v>2086</v>
-      </c>
-      <c r="F17" t="s">
-        <v>2087</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
+        <v>2087</v>
+      </c>
+      <c r="B18" t="s">
         <v>2088</v>
       </c>
-      <c r="B18" t="s">
-        <v>2089</v>
-      </c>
       <c r="F18" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
+        <v>2089</v>
+      </c>
+      <c r="B19" t="s">
         <v>2090</v>
       </c>
-      <c r="B19" t="s">
-        <v>2091</v>
-      </c>
       <c r="F19" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
   </sheetData>
@@ -16696,18 +16696,18 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" style="56" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="56" customWidth="1"/>
-    <col min="4" max="4" width="39.5" style="56" customWidth="1"/>
-    <col min="5" max="5" width="88.6640625" style="56" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" style="56" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" style="56"/>
+    <col min="1" max="1" width="21.42578125" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="56" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="56" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="56" customWidth="1"/>
+    <col min="5" max="5" width="88.7109375" style="56" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" style="56" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16725,7 +16725,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="61"/>
@@ -16800,7 +16800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6">
       <c r="A10" s="66" t="s">
         <v>2010</v>
       </c>
@@ -16815,7 +16815,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16">
+    <row r="11" spans="1:6">
       <c r="A11" s="50" t="s">
         <v>2014</v>
       </c>
@@ -16826,7 +16826,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16">
+    <row r="12" spans="1:6">
       <c r="A12" s="50" t="s">
         <v>2017</v>
       </c>
@@ -16840,7 +16840,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16">
+    <row r="13" spans="1:6">
       <c r="A13" s="50" t="s">
         <v>2021</v>
       </c>
@@ -16855,7 +16855,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16">
+    <row r="14" spans="1:6">
       <c r="A14" s="66" t="s">
         <v>2025</v>
       </c>
@@ -16866,7 +16866,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16">
+    <row r="15" spans="1:6">
       <c r="A15" s="50" t="s">
         <v>2028</v>
       </c>
@@ -16875,133 +16875,133 @@
       </c>
       <c r="C15"/>
       <c r="E15" s="56" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="66" t="s">
         <v>2030</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="16">
-      <c r="A16" s="66" t="s">
+      <c r="B16" s="56" t="s">
         <v>2031</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>2032</v>
       </c>
       <c r="C16" s="54"/>
       <c r="F16" s="56" t="s">
-        <v>2033</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="66" t="s">
         <v>1624</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="C17" s="67"/>
       <c r="E17" s="56" t="s">
+        <v>2034</v>
+      </c>
+      <c r="F17" s="56" t="s">
         <v>2035</v>
       </c>
-      <c r="F17" s="56" t="s">
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="66" t="s">
         <v>2036</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="16">
-      <c r="A18" s="66" t="s">
+      <c r="C18" s="54" t="s">
         <v>2037</v>
       </c>
-      <c r="C18" s="54" t="s">
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="66" t="s">
         <v>2038</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="16">
-      <c r="A19" s="66" t="s">
+      <c r="C19" s="54" t="s">
         <v>2039</v>
       </c>
-      <c r="C19" s="54" t="s">
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="66" t="s">
         <v>2040</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="16">
-      <c r="A20" s="66" t="s">
+      <c r="C20" s="54" t="s">
         <v>2041</v>
       </c>
-      <c r="C20" s="54" t="s">
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="66" t="s">
         <v>2042</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="16">
-      <c r="A21" s="66" t="s">
+      <c r="C21" s="54" t="s">
         <v>2043</v>
       </c>
-      <c r="C21" s="54" t="s">
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="50" t="s">
         <v>2044</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="16">
-      <c r="A22" s="50" t="s">
+      <c r="B22" s="39" t="s">
         <v>2045</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>2046</v>
       </c>
       <c r="C22"/>
       <c r="E22" s="56" t="s">
+        <v>2046</v>
+      </c>
+      <c r="F22" s="56" t="s">
         <v>2047</v>
       </c>
-      <c r="F22" s="56" t="s">
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="50" t="s">
         <v>2048</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="16">
-      <c r="A23" s="50" t="s">
+      <c r="B23" s="39" t="s">
         <v>2049</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>2050</v>
       </c>
       <c r="C23"/>
       <c r="E23" s="56" t="s">
+        <v>2050</v>
+      </c>
+      <c r="F23" s="56" t="s">
         <v>2051</v>
       </c>
-      <c r="F23" s="56" t="s">
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="50" t="s">
         <v>2052</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="16">
-      <c r="A24" s="50" t="s">
+      <c r="B24" s="39" t="s">
         <v>2053</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>2054</v>
       </c>
       <c r="C24"/>
       <c r="E24" s="56" t="s">
+        <v>2054</v>
+      </c>
+      <c r="F24" s="56" t="s">
         <v>2055</v>
       </c>
-      <c r="F24" s="56" t="s">
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="66" t="s">
         <v>2056</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="16">
-      <c r="A25" s="66" t="s">
+      <c r="C25" s="39" t="s">
         <v>2057</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="E25" s="56" t="s">
         <v>2058</v>
       </c>
-      <c r="E25" s="56" t="s">
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="66" t="s">
         <v>2059</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="16">
-      <c r="A26" s="66" t="s">
+      <c r="B26" s="56" t="s">
         <v>2060</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="E26" s="56" t="s">
         <v>2061</v>
-      </c>
-      <c r="E26" s="56" t="s">
-        <v>2062</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -17165,14 +17165,14 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" customWidth="1"/>
-    <col min="5" max="5" width="47.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17255,7 +17255,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60">
+    <row r="10" spans="1:6" ht="64.5">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -17281,7 +17281,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -17295,7 +17295,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -17309,7 +17309,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -17322,7 +17322,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -17350,7 +17350,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="26.25">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
@@ -17376,7 +17376,7 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="26.25">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -17391,7 +17391,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>60</v>
       </c>
@@ -17417,7 +17417,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6" ht="39">
       <c r="A22" s="2" t="s">
         <v>65</v>
       </c>
@@ -17431,7 +17431,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:6" ht="39">
       <c r="A23" s="2" t="s">
         <v>68</v>
       </c>
@@ -17455,7 +17455,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="30">
+    <row r="25" spans="1:6" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -17469,7 +17469,7 @@
       </c>
       <c r="F25" s="12"/>
     </row>
-    <row r="26" spans="1:6" ht="30">
+    <row r="26" spans="1:6" ht="26.25">
       <c r="A26" s="2" t="s">
         <v>76</v>
       </c>
@@ -17483,7 +17483,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" spans="1:6" ht="30">
+    <row r="27" spans="1:6" ht="26.25">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -17497,7 +17497,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -17533,7 +17533,7 @@
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
     </row>
-    <row r="31" spans="1:6" ht="60">
+    <row r="31" spans="1:6" ht="51.75">
       <c r="A31" s="2" t="s">
         <v>89</v>
       </c>
@@ -17547,7 +17547,7 @@
       </c>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>92</v>
       </c>
@@ -17586,7 +17586,7 @@
       </c>
       <c r="F34" s="12"/>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="26.25">
       <c r="A35" s="2" t="s">
         <v>100</v>
       </c>
@@ -17612,7 +17612,7 @@
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:6" ht="120">
+    <row r="37" spans="1:6" ht="102.75">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
@@ -17626,7 +17626,7 @@
       </c>
       <c r="F37" s="12"/>
     </row>
-    <row r="38" spans="1:6" ht="30">
+    <row r="38" spans="1:6" ht="26.25">
       <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
@@ -17640,7 +17640,7 @@
       </c>
       <c r="F38" s="12"/>
     </row>
-    <row r="39" spans="1:6" ht="30">
+    <row r="39" spans="1:6" ht="39">
       <c r="A39" s="2" t="s">
         <v>111</v>
       </c>
@@ -17665,7 +17665,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
     </row>
-    <row r="41" spans="1:6" ht="30">
+    <row r="41" spans="1:6" ht="39">
       <c r="A41" s="2" t="s">
         <v>116</v>
       </c>
@@ -17679,7 +17679,7 @@
       </c>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" ht="26.25">
       <c r="A42" s="2" t="s">
         <v>119</v>
       </c>
@@ -17693,7 +17693,7 @@
       </c>
       <c r="F42" s="12"/>
     </row>
-    <row r="43" spans="1:6" ht="30">
+    <row r="43" spans="1:6" ht="39">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -17717,7 +17717,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" ht="45">
+    <row r="45" spans="1:6" ht="39">
       <c r="A45" s="2" t="s">
         <v>127</v>
       </c>
@@ -17816,7 +17816,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="26.25">
       <c r="A53" s="2" t="s">
         <v>145</v>
       </c>
@@ -17830,7 +17830,7 @@
       </c>
       <c r="F53" s="12"/>
     </row>
-    <row r="54" spans="1:6" ht="60">
+    <row r="54" spans="1:6" ht="64.5">
       <c r="A54" s="2" t="s">
         <v>148</v>
       </c>
@@ -18201,7 +18201,7 @@
       <c r="E84" s="12"/>
       <c r="F84" s="12"/>
     </row>
-    <row r="85" spans="1:6" ht="45">
+    <row r="85" spans="1:6" ht="39">
       <c r="A85" s="2" t="s">
         <v>214</v>
       </c>
@@ -18227,7 +18227,7 @@
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
     </row>
-    <row r="87" spans="1:6" ht="135">
+    <row r="87" spans="1:6" ht="128.25">
       <c r="A87" s="2" t="s">
         <v>219</v>
       </c>
@@ -18253,7 +18253,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
     </row>
-    <row r="89" spans="1:6" ht="60">
+    <row r="89" spans="1:6" ht="51.75">
       <c r="A89" s="2" t="s">
         <v>212</v>
       </c>
@@ -18266,7 +18266,7 @@
       </c>
       <c r="F89" s="12"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" ht="26.25">
       <c r="A90" s="2" t="s">
         <v>214</v>
       </c>
@@ -18306,7 +18306,7 @@
       <c r="E92" s="12"/>
       <c r="F92" s="12"/>
     </row>
-    <row r="93" spans="1:6" ht="30">
+    <row r="93" spans="1:6" ht="26.25">
       <c r="A93" s="2" t="s">
         <v>230</v>
       </c>
@@ -18477,7 +18477,7 @@
       <c r="E106" s="12"/>
       <c r="F106" s="12"/>
     </row>
-    <row r="107" spans="1:6" ht="30">
+    <row r="107" spans="1:6" ht="26.25">
       <c r="A107" s="2" t="s">
         <v>261</v>
       </c>
@@ -18491,7 +18491,7 @@
       </c>
       <c r="F107" s="12"/>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" ht="26.25">
       <c r="A108" s="2" t="s">
         <v>264</v>
       </c>
@@ -18615,7 +18615,7 @@
       <c r="E117" s="12"/>
       <c r="F117" s="12"/>
     </row>
-    <row r="118" spans="1:6" ht="30">
+    <row r="118" spans="1:6" ht="26.25">
       <c r="A118" s="2" t="s">
         <v>287</v>
       </c>
@@ -18629,7 +18629,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" ht="26.25">
       <c r="A119" s="2" t="s">
         <v>290</v>
       </c>
@@ -18642,7 +18642,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="45">
+    <row r="120" spans="1:6" ht="39">
       <c r="A120" s="2" t="s">
         <v>293</v>
       </c>
@@ -18680,7 +18680,7 @@
       <c r="E122" s="12"/>
       <c r="F122" s="12"/>
     </row>
-    <row r="123" spans="1:6" ht="45">
+    <row r="123" spans="1:6" ht="39">
       <c r="A123" s="2" t="s">
         <v>300</v>
       </c>
@@ -18741,7 +18741,7 @@
       <c r="E127" s="12"/>
       <c r="F127" s="12"/>
     </row>
-    <row r="128" spans="1:6" ht="45">
+    <row r="128" spans="1:6" ht="39">
       <c r="A128" s="2" t="s">
         <v>311</v>
       </c>
@@ -18875,7 +18875,7 @@
       <c r="E138" s="12"/>
       <c r="F138" s="12"/>
     </row>
-    <row r="139" spans="1:6" ht="30">
+    <row r="139" spans="1:6" ht="26.25">
       <c r="A139" s="2" t="s">
         <v>336</v>
       </c>
@@ -18900,7 +18900,7 @@
       <c r="E140" s="12"/>
       <c r="F140" s="12"/>
     </row>
-    <row r="141" spans="1:6" ht="30">
+    <row r="141" spans="1:6" ht="26.25">
       <c r="A141" s="2" t="s">
         <v>341</v>
       </c>
@@ -18914,7 +18914,7 @@
       </c>
       <c r="F141" s="12"/>
     </row>
-    <row r="142" spans="1:6" ht="30">
+    <row r="142" spans="1:6" ht="26.25">
       <c r="A142" s="2" t="s">
         <v>342</v>
       </c>
@@ -18928,7 +18928,7 @@
       </c>
       <c r="F142" s="12"/>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" ht="26.25">
       <c r="A143" s="2" t="s">
         <v>343</v>
       </c>
@@ -18942,7 +18942,7 @@
       </c>
       <c r="F143" s="12"/>
     </row>
-    <row r="144" spans="1:6" ht="30">
+    <row r="144" spans="1:6" ht="26.25">
       <c r="A144" s="2" t="s">
         <v>344</v>
       </c>
@@ -18971,7 +18971,7 @@
       </c>
       <c r="F145" s="12"/>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" ht="26.25">
       <c r="A146" s="2" t="s">
         <v>347</v>
       </c>
@@ -18985,7 +18985,7 @@
       </c>
       <c r="F146" s="12"/>
     </row>
-    <row r="147" spans="1:6" ht="30">
+    <row r="147" spans="1:6" ht="39">
       <c r="A147" s="2" t="s">
         <v>348</v>
       </c>
@@ -18999,7 +18999,7 @@
       </c>
       <c r="F147" s="12"/>
     </row>
-    <row r="148" spans="1:6" ht="30">
+    <row r="148" spans="1:6" ht="39">
       <c r="A148" s="2" t="s">
         <v>349</v>
       </c>
@@ -19013,7 +19013,7 @@
       </c>
       <c r="F148" s="12"/>
     </row>
-    <row r="149" spans="1:6" ht="30">
+    <row r="149" spans="1:6" ht="26.25">
       <c r="A149" s="2" t="s">
         <v>350</v>
       </c>
@@ -19026,7 +19026,7 @@
       </c>
       <c r="F149" s="12"/>
     </row>
-    <row r="150" spans="1:6" ht="30">
+    <row r="150" spans="1:6" ht="26.25">
       <c r="A150" s="2" t="s">
         <v>351</v>
       </c>
@@ -19040,7 +19040,7 @@
       </c>
       <c r="F150" s="12"/>
     </row>
-    <row r="151" spans="1:6" ht="30">
+    <row r="151" spans="1:6" ht="26.25">
       <c r="A151" s="2" t="s">
         <v>352</v>
       </c>
@@ -19172,7 +19172,7 @@
       <c r="E161" s="12"/>
       <c r="F161" s="12"/>
     </row>
-    <row r="162" spans="1:6" ht="30">
+    <row r="162" spans="1:6" ht="39">
       <c r="A162" s="2" t="s">
         <v>373</v>
       </c>
@@ -19186,7 +19186,7 @@
       </c>
       <c r="F162" s="12"/>
     </row>
-    <row r="163" spans="1:6" ht="45">
+    <row r="163" spans="1:6" ht="39">
       <c r="A163" s="2" t="s">
         <v>376</v>
       </c>
@@ -19200,7 +19200,7 @@
       </c>
       <c r="F163" s="12"/>
     </row>
-    <row r="164" spans="1:6" ht="45">
+    <row r="164" spans="1:6" ht="39">
       <c r="A164" s="2" t="s">
         <v>379</v>
       </c>
@@ -19251,7 +19251,7 @@
       <c r="E167" s="12"/>
       <c r="F167" s="12"/>
     </row>
-    <row r="168" spans="1:6" ht="30">
+    <row r="168" spans="1:6" ht="26.25">
       <c r="A168" s="2" t="s">
         <v>389</v>
       </c>
@@ -19468,7 +19468,7 @@
       <c r="E185" s="12"/>
       <c r="F185" s="12"/>
     </row>
-    <row r="186" spans="1:6" ht="30">
+    <row r="186" spans="1:6" ht="26.25">
       <c r="A186" s="2" t="s">
         <v>426</v>
       </c>
@@ -19604,7 +19604,7 @@
       </c>
       <c r="F196" s="12"/>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" ht="26.25">
       <c r="A197" s="2" t="s">
         <v>451</v>
       </c>
@@ -19704,7 +19704,7 @@
       <c r="E204" s="12"/>
       <c r="F204" s="12"/>
     </row>
-    <row r="205" spans="1:6" ht="30">
+    <row r="205" spans="1:6" ht="26.25">
       <c r="A205" s="2" t="s">
         <v>470</v>
       </c>
@@ -19730,7 +19730,7 @@
       <c r="E206" s="12"/>
       <c r="F206" s="12"/>
     </row>
-    <row r="207" spans="1:6" ht="30">
+    <row r="207" spans="1:6" ht="26.25">
       <c r="A207" s="2" t="s">
         <v>475</v>
       </c>
@@ -19828,7 +19828,7 @@
       <c r="E214" s="12"/>
       <c r="F214" s="12"/>
     </row>
-    <row r="215" spans="1:6" ht="30">
+    <row r="215" spans="1:6" ht="26.25">
       <c r="A215" s="2" t="s">
         <v>493</v>
       </c>
@@ -20649,7 +20649,7 @@
       <c r="E282" s="12"/>
       <c r="F282" s="12"/>
     </row>
-    <row r="283" spans="1:6" ht="30">
+    <row r="283" spans="1:6" ht="26.25">
       <c r="A283" s="2" t="s">
         <v>638</v>
       </c>
@@ -20663,7 +20663,7 @@
       </c>
       <c r="F283" s="12"/>
     </row>
-    <row r="284" spans="1:6" ht="30">
+    <row r="284" spans="1:6" ht="26.25">
       <c r="A284" s="2" t="s">
         <v>641</v>
       </c>
@@ -21012,13 +21012,13 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="80.5" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -21501,13 +21501,13 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22008,12 +22008,12 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -22170,12 +22170,12 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -22359,9 +22359,9 @@
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22894,14 +22894,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -25609,16 +25609,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="26.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -25629,7 +25629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="24.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -25695,7 +25695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="39">
       <c r="A10" s="2" t="s">
         <v>1082</v>
       </c>
@@ -25717,7 +25717,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>1087</v>
       </c>
@@ -25727,7 +25727,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="39">
       <c r="A13" s="2" t="s">
         <v>1089</v>
       </c>
@@ -25737,7 +25737,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>1091</v>
       </c>
@@ -25747,7 +25747,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1093</v>
       </c>
@@ -25757,7 +25757,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1095</v>
       </c>
@@ -25769,7 +25769,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="45">
+    <row r="17" spans="1:4" ht="39">
       <c r="A17" s="2" t="s">
         <v>1098</v>
       </c>
@@ -25781,7 +25781,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="30">
+    <row r="18" spans="1:4" ht="39">
       <c r="A18" s="2" t="s">
         <v>1101</v>
       </c>
@@ -25791,7 +25791,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:4" ht="39">
       <c r="A19" s="2" t="s">
         <v>1103</v>
       </c>
@@ -25801,7 +25801,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>1105</v>
       </c>
@@ -25811,7 +25811,7 @@
       <c r="C20" s="12"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="26.25">
       <c r="A21" s="2" t="s">
         <v>1107</v>
       </c>
@@ -25821,7 +25821,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="26.25">
       <c r="A22" s="2" t="s">
         <v>1109</v>
       </c>
@@ -25851,7 +25851,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>1115</v>
       </c>
@@ -25881,7 +25881,7 @@
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="30">
+    <row r="28" spans="1:4" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>1120</v>
       </c>
@@ -25893,7 +25893,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="30">
+    <row r="29" spans="1:4" ht="26.25">
       <c r="A29" s="2" t="s">
         <v>1123</v>
       </c>
@@ -25905,7 +25905,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="30">
+    <row r="30" spans="1:4" ht="26.25">
       <c r="A30" s="2" t="s">
         <v>1126</v>
       </c>
@@ -25927,7 +25927,7 @@
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="30">
+    <row r="32" spans="1:4" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1131</v>
       </c>
@@ -25939,7 +25939,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="30">
+    <row r="33" spans="1:4" ht="39">
       <c r="A33" s="2" t="s">
         <v>1134</v>
       </c>
@@ -25951,7 +25951,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="26.25">
       <c r="A34" s="2" t="s">
         <v>1137</v>
       </c>
@@ -25963,7 +25963,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="135">
+    <row r="35" spans="1:4" ht="128.25">
       <c r="A35" s="2" t="s">
         <v>1140</v>
       </c>
@@ -25975,7 +25975,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="135">
+    <row r="36" spans="1:4" ht="128.25">
       <c r="A36" s="2" t="s">
         <v>1143</v>
       </c>
@@ -26059,7 +26059,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="30">
+    <row r="44" spans="1:4" ht="26.25">
       <c r="A44" s="2" t="s">
         <v>1160</v>
       </c>
@@ -26071,7 +26071,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="30">
+    <row r="45" spans="1:4" ht="26.25">
       <c r="A45" s="2" t="s">
         <v>1163</v>
       </c>
@@ -26081,7 +26081,7 @@
       <c r="C45" s="12"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="75">
+    <row r="46" spans="1:4" ht="77.25">
       <c r="A46" s="2" t="s">
         <v>1165</v>
       </c>
@@ -26110,13 +26110,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="39.5" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.1640625" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26231,7 +26231,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>1177</v>
       </c>
@@ -26255,7 +26255,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1182</v>
       </c>
@@ -26268,7 +26268,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1185</v>
       </c>
@@ -26292,7 +26292,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="40">
+    <row r="18" spans="1:5" ht="48.75">
       <c r="A18" s="2" t="s">
         <v>1190</v>
       </c>
@@ -26305,7 +26305,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="64.5">
       <c r="A19" s="2" t="s">
         <v>1193</v>
       </c>
@@ -26454,7 +26454,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1222</v>
       </c>
@@ -26467,7 +26467,7 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5" ht="30">
+    <row r="33" spans="1:5" ht="26.25">
       <c r="A33" s="2" t="s">
         <v>1225</v>
       </c>
@@ -26554,7 +26554,7 @@
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5" ht="45">
+    <row r="40" spans="1:5" ht="51.75">
       <c r="A40" s="2" t="s">
         <v>1244</v>
       </c>
@@ -26591,7 +26591,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5" ht="30">
+    <row r="43" spans="1:5" ht="26.25">
       <c r="A43" s="2" t="s">
         <v>1252</v>
       </c>
@@ -26604,7 +26604,7 @@
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5" ht="39">
       <c r="A44" s="2" t="s">
         <v>1253</v>
       </c>
@@ -26663,7 +26663,7 @@
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="26.25">
       <c r="A49" s="2" t="s">
         <v>1265</v>
       </c>
@@ -26698,7 +26698,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5" ht="30">
+    <row r="52" spans="1:5" ht="26.25">
       <c r="A52" s="2" t="s">
         <v>1272</v>
       </c>
@@ -26792,7 +26792,7 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="39">
       <c r="A60" s="2" t="s">
         <v>1291</v>
       </c>
@@ -26834,14 +26834,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.6640625" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27455,14 +27455,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27890,13 +27890,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -27982,7 +27982,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32">
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="18" t="s">
         <v>1314</v>
       </c>
@@ -27995,7 +27995,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="32">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="18" t="s">
         <v>1317</v>
       </c>
@@ -28008,7 +28008,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="18" t="s">
         <v>1320</v>
       </c>
@@ -28021,7 +28021,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="32">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="18" t="s">
         <v>1323</v>
       </c>
@@ -28034,7 +28034,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="18" t="s">
         <v>1326</v>
       </c>
@@ -28047,7 +28047,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="32">
+    <row r="15" spans="1:5" ht="45">
       <c r="A15" s="18" t="s">
         <v>1329</v>
       </c>
@@ -28060,7 +28060,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="32">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="18" t="s">
         <v>1332</v>
       </c>
@@ -28073,7 +28073,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="32">
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="18" t="s">
         <v>1335</v>
       </c>
@@ -28086,7 +28086,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="48">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="18" t="s">
         <v>1338</v>
       </c>
@@ -28099,7 +28099,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="48">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="18" t="s">
         <v>1341</v>
       </c>
@@ -28112,7 +28112,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="32">
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="18" t="s">
         <v>1344</v>
       </c>
@@ -28125,7 +28125,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="32">
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="18" t="s">
         <v>1347</v>
       </c>
@@ -28138,7 +28138,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="32">
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="18" t="s">
         <v>1350</v>
       </c>
@@ -28151,7 +28151,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="32">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="18" t="s">
         <v>1353</v>
       </c>
@@ -28164,7 +28164,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="32">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="18" t="s">
         <v>1356</v>
       </c>
@@ -28177,7 +28177,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="32">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="18" t="s">
         <v>1359</v>
       </c>
@@ -28190,7 +28190,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="32">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="18" t="s">
         <v>1362</v>
       </c>
@@ -28203,7 +28203,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="16">
+    <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
         <v>1365</v>
       </c>
@@ -28216,7 +28216,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="32">
+    <row r="28" spans="1:5" ht="30">
       <c r="A28" s="18" t="s">
         <v>1367</v>
       </c>
@@ -28229,7 +28229,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="16">
+    <row r="29" spans="1:5">
       <c r="A29" s="18" t="s">
         <v>1370</v>
       </c>
@@ -28242,7 +28242,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="16">
+    <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
         <v>1373</v>
       </c>
@@ -28270,13 +28270,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -28373,7 +28373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="18" t="s">
         <v>1378</v>
       </c>
@@ -28387,7 +28387,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="48">
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="18" t="s">
         <v>1381</v>
       </c>
@@ -28401,7 +28401,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="32">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="18" t="s">
         <v>1384</v>
       </c>
@@ -28415,7 +28415,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="32">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="18" t="s">
         <v>1387</v>
       </c>
@@ -28429,7 +28429,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="32">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="18" t="s">
         <v>1390</v>
       </c>
@@ -28443,7 +28443,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="32">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="18" t="s">
         <v>1393</v>
       </c>
@@ -28457,7 +28457,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="32">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="18" t="s">
         <v>1396</v>
       </c>
@@ -28471,7 +28471,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="48">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="18" t="s">
         <v>1370</v>
       </c>
@@ -28485,7 +28485,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="32">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="18" t="s">
         <v>1401</v>
       </c>
@@ -28605,8 +28605,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="5a233c5be867259e7f523794110a7773">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71fc54e2a62b1985aea6da9d2195ce0c" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -28669,12 +28669,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -28787,7 +28787,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -28806,7 +28806,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -28879,7 +28879,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -28928,8 +28928,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -29019,6 +29019,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -29070,41 +29079,32 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ECB47E9-2B60-4219-92DB-621EC7B64685}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42E5C9F3-538C-4D41-BA64-EAC55C1DE6EB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.07.30 15:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="985" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D858164C-96BA-4E56-96B6-D31AD34B2945}"/>
+  <xr:revisionPtr revIDLastSave="987" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7A42EB2-F1A1-42DF-A36B-FDCA7278AF85}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3165" yWindow="1170" windowWidth="25410" windowHeight="14145" tabRatio="877" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31140" yWindow="810" windowWidth="21930" windowHeight="14145" tabRatio="877" firstSheet="28" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -10919,8 +10919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
   <dimension ref="A1:L222"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -14716,7 +14716,7 @@
     <hyperlink ref="E31" location="'Type de devenir du patient'!A1" display="Lien nomenclature" xr:uid="{0E2A9314-0B8D-4156-A7C3-BC0E2885D9D2}"/>
     <hyperlink ref="E32" location="'Effet à obtenir'!A1" display="Lien nomenclature" xr:uid="{F32B9CB2-26FC-4D51-B612-B9EB269DC3B1}"/>
     <hyperlink ref="E36" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{9DFDDF82-C842-46CA-9B9A-3545027D4646}"/>
-    <hyperlink ref="E36" location="'Status du vecteur'!A1" display="Lien nomenclature" xr:uid="{CBB6C543-B740-4053-95FD-E8C10E8B561C}"/>
+    <hyperlink ref="E36" location="'Statut du vecteur'!A1" display="Lien nomenclature" xr:uid="{CBB6C543-B740-4053-95FD-E8C10E8B561C}"/>
     <hyperlink ref="E33" location="'Cadre conventionnel'!A1" display="Lien nomenclature" xr:uid="{018B40BB-963F-4A1C-AF4F-5EA9FD5F329B}"/>
     <hyperlink ref="E34" location="'Delai d''intervention souhaite'!A1" display="Lien nomenclature" xr:uid="{FA2A5069-90AE-4459-B4C7-F1CDCCD8EAB0}"/>
     <hyperlink ref="E10" location="'Nombre de patients-victimes'!A1" display="Lien nomenclature" xr:uid="{6309BD82-9F33-4F60-88D8-A0006F1258C1}"/>
@@ -21257,9 +21257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2B8C8C-87E7-449D-BC82-028AFFEC58AC}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
@@ -22602,7 +22600,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -23026,8 +23024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EE5AD-9985-4D20-8EAC-8B61AD8038D6}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -24011,7 +24009,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -26632,9 +26630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B730C132-AF0D-4124-AB29-0565D21E3ED1}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -27526,7 +27522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244BE68D-3EF4-4212-8122-4351014F1789}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -36746,7 +36742,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A24BC060-E3AE-4C00-A658-3FA30565C89A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37CEB336-22C7-4193-AADF-B99C7A8D0B12}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
[24.08.06 15:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1093" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D61D2A5-ADF7-4233-A025-ED1AE91240F4}"/>
+  <xr:revisionPtr revIDLastSave="1095" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA2406AC-B24B-40E7-A40C-28431DA35A4B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3450" yWindow="105" windowWidth="24975" windowHeight="14370" tabRatio="877" firstSheet="26" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="150" yWindow="30" windowWidth="24975" windowHeight="14370" tabRatio="877" firstSheet="26" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -6511,9 +6511,6 @@
     <t>La demande est refusée, le motif de refus est à préciser dans le freetext</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Qualification / Patient</t>
   </si>
   <si>
@@ -6578,6 +6575,9 @@
   </si>
   <si>
     <t>VECTEUR</t>
+  </si>
+  <si>
+    <t>Ambulance sans précision</t>
   </si>
 </sst>
 </file>
@@ -11507,7 +11507,7 @@
         <v>1726</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="C10" s="49" t="str">
         <f>'Etats du dossier'!B1</f>
@@ -12002,7 +12002,7 @@
     </row>
     <row r="26" spans="1:12" ht="15">
       <c r="A26" s="28" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>1740</v>
@@ -12233,7 +12233,7 @@
         <v>1745</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="C33" s="27" t="str">
         <f>'Type de destination'!B1</f>
@@ -23798,8 +23798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EE5AD-9985-4D20-8EAC-8B61AD8038D6}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -24710,7 +24710,7 @@
       </c>
       <c r="B72" s="52"/>
       <c r="C72" s="52" t="s">
-        <v>2078</v>
+        <v>2100</v>
       </c>
       <c r="D72" s="52"/>
       <c r="E72" s="52" t="s">
@@ -25644,7 +25644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84808B80-6F52-46A5-8814-B228DDBE2F0A}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -25863,7 +25863,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="79" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>1601</v>
@@ -26187,7 +26187,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -26256,10 +26256,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="71" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="B10" s="78" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -26270,7 +26270,7 @@
         <v>1317</v>
       </c>
       <c r="B11" s="78" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -26278,10 +26278,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="B12" s="78" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -26289,7 +26289,7 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="B13" s="78" t="s">
         <v>683</v>
@@ -26300,10 +26300,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="B14" s="78" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -26314,7 +26314,7 @@
         <v>1343</v>
       </c>
       <c r="B15" s="78" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52"/>
@@ -37065,7 +37065,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -37134,10 +37134,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="71" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B10" s="71" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -37145,10 +37145,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -37156,10 +37156,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -37167,10 +37167,10 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52"/>
@@ -37178,10 +37178,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -37189,10 +37189,10 @@
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1">
       <c r="A15" s="52" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52"/>
@@ -37200,10 +37200,10 @@
     </row>
     <row r="16" spans="1:5" s="32" customFormat="1">
       <c r="A16" s="52" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="52"/>

</xml_diff>

<commit_message>
[24.08.06 17:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1095" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA2406AC-B24B-40E7-A40C-28431DA35A4B}"/>
+  <xr:revisionPtr revIDLastSave="1098" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB5DA4E4-B74F-E247-87E7-5E3544E7E0AB}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="150" yWindow="30" windowWidth="24975" windowHeight="14370" tabRatio="877" firstSheet="26" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="760" windowWidth="24980" windowHeight="14380" tabRatio="877" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -52,7 +52,7 @@
     <sheet name="Reponse demande ressources" sheetId="59" r:id="rId37"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$2:$K$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$2:$K$38</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3049" uniqueCount="2101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3047" uniqueCount="2100">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -6293,9 +6293,6 @@
   </si>
   <si>
     <t>Delai d'intervention souhaité</t>
-  </si>
-  <si>
-    <t>Filière</t>
   </si>
   <si>
     <t>Type d'intervention</t>
@@ -6828,7 +6825,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6863,12 +6860,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF8EA9DB"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -6963,7 +6954,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7098,12 +7089,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -7132,47 +7117,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
+    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
-  <dxfs count="186">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF58383"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="181">
     <dxf>
       <fill>
         <patternFill>
@@ -10617,341 +10567,341 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8CBD23D8-3CB7-491B-B00E-5486B907388F}" name="Table13611123111813" displayName="Table13611123111813" ref="A9:E55" totalsRowShown="0" headerRowDxfId="185" dataDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8CBD23D8-3CB7-491B-B00E-5486B907388F}" name="Table13611123111813" displayName="Table13611123111813" ref="A9:E55" totalsRowShown="0" headerRowDxfId="180" dataDxfId="179">
   <autoFilter ref="A9:E55" xr:uid="{8CBD23D8-3CB7-491B-B00E-5486B907388F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E0E4BEF8-D213-4F3F-97E1-4EF95756B90E}" name="Code" dataDxfId="183"/>
-    <tableColumn id="2" xr3:uid="{3431D095-AE1F-4ABA-9D63-EC4DB501B423}" name="Libellé niveau 1" dataDxfId="182"/>
-    <tableColumn id="5" xr3:uid="{97BD8D92-80A6-4F7F-9379-59C2B46726A3}" name="Libellé niveau 2" dataDxfId="181"/>
-    <tableColumn id="3" xr3:uid="{127B5052-742A-4FFC-ABFE-8F7750C796F5}" name="Description" dataDxfId="180"/>
-    <tableColumn id="4" xr3:uid="{166EA99C-D40A-41CA-8E35-76670A47C2FF}" name="Commentaire" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{E0E4BEF8-D213-4F3F-97E1-4EF95756B90E}" name="Code" dataDxfId="178"/>
+    <tableColumn id="2" xr3:uid="{3431D095-AE1F-4ABA-9D63-EC4DB501B423}" name="Libellé niveau 1" dataDxfId="177"/>
+    <tableColumn id="5" xr3:uid="{97BD8D92-80A6-4F7F-9379-59C2B46726A3}" name="Libellé niveau 2" dataDxfId="176"/>
+    <tableColumn id="3" xr3:uid="{127B5052-742A-4FFC-ABFE-8F7750C796F5}" name="Description" dataDxfId="175"/>
+    <tableColumn id="4" xr3:uid="{166EA99C-D40A-41CA-8E35-76670A47C2FF}" name="Commentaire" dataDxfId="174"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{823C2F13-948D-4974-9C9C-1AD390776B68}" name="Table136111235" displayName="Table136111235" ref="A9:E55" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{823C2F13-948D-4974-9C9C-1AD390776B68}" name="Table136111235" displayName="Table136111235" ref="A9:E55" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115">
   <autoFilter ref="A9:E55" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C65B8274-E954-4CBF-8B3B-6DACFEF3D09F}" name="Code" dataDxfId="119"/>
-    <tableColumn id="2" xr3:uid="{84ACD83D-893A-4B00-89F4-93AEE374E815}" name="Libellé niveau 1" dataDxfId="118"/>
-    <tableColumn id="5" xr3:uid="{E64A61DE-4BB8-4C3E-B7B9-726F1A447BD7}" name="Libellé niveau 2" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{B1043381-4D28-4782-8747-DA98FAFD4504}" name="Description" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{DF53D3E2-A057-4D40-BE92-9E7F311D817E}" name="Commentaire" dataDxfId="115"/>
+    <tableColumn id="1" xr3:uid="{C65B8274-E954-4CBF-8B3B-6DACFEF3D09F}" name="Code" dataDxfId="114"/>
+    <tableColumn id="2" xr3:uid="{84ACD83D-893A-4B00-89F4-93AEE374E815}" name="Libellé niveau 1" dataDxfId="113"/>
+    <tableColumn id="5" xr3:uid="{E64A61DE-4BB8-4C3E-B7B9-726F1A447BD7}" name="Libellé niveau 2" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{B1043381-4D28-4782-8747-DA98FAFD4504}" name="Description" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{DF53D3E2-A057-4D40-BE92-9E7F311D817E}" name="Commentaire" dataDxfId="110"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C3C96985-E377-4F48-BA27-F14A223DCC95}" name="Table1361112311" displayName="Table1361112311" ref="A9:E55" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C3C96985-E377-4F48-BA27-F14A223DCC95}" name="Table1361112311" displayName="Table1361112311" ref="A9:E55" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108">
   <autoFilter ref="A9:E55" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{888FD29E-2275-4F75-ADD9-E04935713E5C}" name="Code" dataDxfId="112"/>
-    <tableColumn id="2" xr3:uid="{49B955E3-E63C-42E4-A3D1-7E9F8878B275}" name="Libellé niveau 1" dataDxfId="111"/>
-    <tableColumn id="5" xr3:uid="{C2281989-9EA7-462C-90E1-C689C38F32FC}" name="Libellé niveau 2" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{693429A6-E746-47FF-A745-B1D8AFE53E56}" name="Description" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{91A2BB1F-5F3A-47DF-86F4-E97AB53ADD89}" name="Commentaire" dataDxfId="108"/>
+    <tableColumn id="1" xr3:uid="{888FD29E-2275-4F75-ADD9-E04935713E5C}" name="Code" dataDxfId="107"/>
+    <tableColumn id="2" xr3:uid="{49B955E3-E63C-42E4-A3D1-7E9F8878B275}" name="Libellé niveau 1" dataDxfId="106"/>
+    <tableColumn id="5" xr3:uid="{C2281989-9EA7-462C-90E1-C689C38F32FC}" name="Libellé niveau 2" dataDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{693429A6-E746-47FF-A745-B1D8AFE53E56}" name="Description" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{91A2BB1F-5F3A-47DF-86F4-E97AB53ADD89}" name="Commentaire" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FCFF9977-C677-479A-85FC-B06533A394C5}" name="Table136111231115" displayName="Table136111231115" ref="A9:E55" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FCFF9977-C677-479A-85FC-B06533A394C5}" name="Table136111231115" displayName="Table136111231115" ref="A9:E55" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
   <autoFilter ref="A9:E55" xr:uid="{FCFF9977-C677-479A-85FC-B06533A394C5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A576D64-7823-4B55-BF7E-F5CB76EA3E3E}" name="Code" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{CBBE7E46-1033-4C8A-AE13-078E2F5F30BD}" name="Libellé niveau 1" dataDxfId="104"/>
-    <tableColumn id="5" xr3:uid="{294792C7-CE9D-42DF-96E0-1035ACCFF003}" name="Libellé niveau 2" dataDxfId="103"/>
-    <tableColumn id="3" xr3:uid="{CA095527-FAAE-4845-8EC8-35CF34674BD1}" name="Description" dataDxfId="102"/>
-    <tableColumn id="4" xr3:uid="{D599D956-3DCB-49BC-91E2-9495FEFE3A0D}" name="Commentaire" dataDxfId="101"/>
+    <tableColumn id="1" xr3:uid="{4A576D64-7823-4B55-BF7E-F5CB76EA3E3E}" name="Code" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{CBBE7E46-1033-4C8A-AE13-078E2F5F30BD}" name="Libellé niveau 1" dataDxfId="99"/>
+    <tableColumn id="5" xr3:uid="{294792C7-CE9D-42DF-96E0-1035ACCFF003}" name="Libellé niveau 2" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{CA095527-FAAE-4845-8EC8-35CF34674BD1}" name="Description" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{D599D956-3DCB-49BC-91E2-9495FEFE3A0D}" name="Commentaire" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{2A2AD6DF-70D1-4862-8B6B-3EA16EA226E8}" name="Table136111231116" displayName="Table136111231116" ref="A9:E55" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{2A2AD6DF-70D1-4862-8B6B-3EA16EA226E8}" name="Table136111231116" displayName="Table136111231116" ref="A9:E55" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A9:E55" xr:uid="{2A2AD6DF-70D1-4862-8B6B-3EA16EA226E8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DAD71D71-B89C-4E24-B32B-350EE5ECD2D7}" name="Code" dataDxfId="98"/>
-    <tableColumn id="2" xr3:uid="{9814D279-C1B5-40C4-8A18-1E240B57B85C}" name="Libellé niveau 1" dataDxfId="97"/>
-    <tableColumn id="5" xr3:uid="{4BFAD3EE-A659-4BE0-8AAB-3469FECB5643}" name="Libellé niveau 2" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{96657DDA-8D57-40A2-B54B-E4AC1B489A0D}" name="Description" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{12AB4119-159D-434F-85AA-2B89F1A63856}" name="Commentaire" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{DAD71D71-B89C-4E24-B32B-350EE5ECD2D7}" name="Code" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{9814D279-C1B5-40C4-8A18-1E240B57B85C}" name="Libellé niveau 1" dataDxfId="92"/>
+    <tableColumn id="5" xr3:uid="{4BFAD3EE-A659-4BE0-8AAB-3469FECB5643}" name="Libellé niveau 2" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{96657DDA-8D57-40A2-B54B-E4AC1B489A0D}" name="Description" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{12AB4119-159D-434F-85AA-2B89F1A63856}" name="Commentaire" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{4D2E6F8C-DACC-4A26-AF1C-27A96B5B0CEB}" name="Table136111231117" displayName="Table136111231117" ref="A9:E55" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{4D2E6F8C-DACC-4A26-AF1C-27A96B5B0CEB}" name="Table136111231117" displayName="Table136111231117" ref="A9:E55" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87">
   <autoFilter ref="A9:E55" xr:uid="{4D2E6F8C-DACC-4A26-AF1C-27A96B5B0CEB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{73A28F86-A0B9-4591-B8D2-0160E457A112}" name="Code" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{F7506F92-2DA9-4093-9FDA-9893B7117480}" name="Libellé niveau 1" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{87CA381F-E725-4FBA-9AD1-5C61C6B110A7}" name="Libellé niveau 2" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{39D920FE-DBE6-4BFE-9670-1D3E45145CF4}" name="Description" dataDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{6A637CD0-E4AE-4CBB-B448-5134035C720F}" name="Commentaire" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{73A28F86-A0B9-4591-B8D2-0160E457A112}" name="Code" dataDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{F7506F92-2DA9-4093-9FDA-9893B7117480}" name="Libellé niveau 1" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{87CA381F-E725-4FBA-9AD1-5C61C6B110A7}" name="Libellé niveau 2" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{39D920FE-DBE6-4BFE-9670-1D3E45145CF4}" name="Description" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{6A637CD0-E4AE-4CBB-B448-5134035C720F}" name="Commentaire" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{E64CCCB9-2511-4EC1-8A5A-FF1038C81F09}" name="Table136111231118" displayName="Table136111231118" ref="A9:E55" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{E64CCCB9-2511-4EC1-8A5A-FF1038C81F09}" name="Table136111231118" displayName="Table136111231118" ref="A9:E55" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
   <autoFilter ref="A9:E55" xr:uid="{E64CCCB9-2511-4EC1-8A5A-FF1038C81F09}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{09E6D0E8-8FB6-4435-A553-92417353F896}" name="Code" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{A213C1A0-1722-4289-A2D1-5A6EB30EA09B}" name="Libellé niveau 1" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{53CF9BCE-0E7D-4BDE-B31F-55A8819FC0A0}" name="Libellé niveau 2" dataDxfId="82"/>
-    <tableColumn id="3" xr3:uid="{514C1BC9-9ADF-4004-BAB2-15D24A3A1D09}" name="Description" dataDxfId="81"/>
-    <tableColumn id="4" xr3:uid="{B12E6EEC-3F2C-407F-9AA7-389D7A17FCF7}" name="Commentaire" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{09E6D0E8-8FB6-4435-A553-92417353F896}" name="Code" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{A213C1A0-1722-4289-A2D1-5A6EB30EA09B}" name="Libellé niveau 1" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{53CF9BCE-0E7D-4BDE-B31F-55A8819FC0A0}" name="Libellé niveau 2" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{514C1BC9-9ADF-4004-BAB2-15D24A3A1D09}" name="Description" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{B12E6EEC-3F2C-407F-9AA7-389D7A17FCF7}" name="Commentaire" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{E49A72A2-799E-4EB5-A633-DA9AD17ABED3}" name="Table136111231119" displayName="Table136111231119" ref="A9:E55" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{E49A72A2-799E-4EB5-A633-DA9AD17ABED3}" name="Table136111231119" displayName="Table136111231119" ref="A9:E55" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <autoFilter ref="A9:E55" xr:uid="{E49A72A2-799E-4EB5-A633-DA9AD17ABED3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:E55">
     <sortCondition ref="A10:A55"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7BFF7477-5274-4DF2-96EF-E56B7D69958A}" name="Code" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{FA4C3FFB-F1E7-4D2E-A4DD-0D3DF4405172}" name="Libellé niveau 1" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{A8127A8F-6B34-448D-A889-6BE2CE9E132C}" name="Libellé niveau 2" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{7B4AEDBA-3677-4E04-9052-1F30AB73A25F}" name="Description" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{9F627AE1-28AD-49D7-815A-4D3C089B24ED}" name="Commentaire" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{7BFF7477-5274-4DF2-96EF-E56B7D69958A}" name="Code" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{FA4C3FFB-F1E7-4D2E-A4DD-0D3DF4405172}" name="Libellé niveau 1" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{A8127A8F-6B34-448D-A889-6BE2CE9E132C}" name="Libellé niveau 2" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{7B4AEDBA-3677-4E04-9052-1F30AB73A25F}" name="Description" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{9F627AE1-28AD-49D7-815A-4D3C089B24ED}" name="Commentaire" dataDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{4B4CDC31-DA4C-4411-9B0D-8DA3539A0493}" name="Table136111231120" displayName="Table136111231120" ref="A9:E55" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{4B4CDC31-DA4C-4411-9B0D-8DA3539A0493}" name="Table136111231120" displayName="Table136111231120" ref="A9:E55" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="A9:E55" xr:uid="{4B4CDC31-DA4C-4411-9B0D-8DA3539A0493}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{317D1C42-0F4B-4773-8F99-F1B182F45481}" name="Code" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{77113B58-1151-4391-BEF5-DB56D3F4E4D5}" name="Libellé niveau 1" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{1CB9B5EC-80A3-4CA4-A035-92C9648D737A}" name="Libellé niveau 2" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{5FD1FD14-CDEB-40D4-9245-CD50BA9263BB}" name="Description" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{84BF17F5-072D-4227-B551-BE57A4509B17}" name="Commentaire" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{317D1C42-0F4B-4773-8F99-F1B182F45481}" name="Code" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{77113B58-1151-4391-BEF5-DB56D3F4E4D5}" name="Libellé niveau 1" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{1CB9B5EC-80A3-4CA4-A035-92C9648D737A}" name="Libellé niveau 2" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{5FD1FD14-CDEB-40D4-9245-CD50BA9263BB}" name="Description" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{84BF17F5-072D-4227-B551-BE57A4509B17}" name="Commentaire" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A9:E30" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{865D8B57-135B-4BFA-938D-B62BC39AC970}" name="Code"/>
     <tableColumn id="2" xr3:uid="{E07D1CE2-997E-4A59-9869-D1EFB60F0809}" name="Libellé niveau 1"/>
     <tableColumn id="5" xr3:uid="{A8693491-C517-461F-B62C-F068AE507B25}" name="Libellé niveau 2"/>
-    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <autoFilter ref="A9:F30" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9B470DB1-BD5A-4D37-B9A2-613B4968664F}" name="Code"/>
-    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3B0BCC87-0508-4B50-B37F-D0A3A984A79D}" name="Table13611123111814" displayName="Table13611123111814" ref="A9:E55" totalsRowShown="0" headerRowDxfId="178" dataDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3B0BCC87-0508-4B50-B37F-D0A3A984A79D}" name="Table13611123111814" displayName="Table13611123111814" ref="A9:E55" totalsRowShown="0" headerRowDxfId="173" dataDxfId="172">
   <autoFilter ref="A9:E55" xr:uid="{3B0BCC87-0508-4B50-B37F-D0A3A984A79D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{526E210B-F075-426E-960B-2873C3BD0C3B}" name="Code" dataDxfId="176"/>
-    <tableColumn id="2" xr3:uid="{2DA7E824-8886-4D58-ADE6-5377ED969D2A}" name="Libellé niveau 1" dataDxfId="175"/>
-    <tableColumn id="5" xr3:uid="{5D94993D-C9B5-47AD-AE15-32C420404C57}" name="Libellé niveau 2" dataDxfId="174"/>
-    <tableColumn id="3" xr3:uid="{436A1EAF-13B2-4CB3-9DDA-971E988E804D}" name="Description" dataDxfId="173"/>
-    <tableColumn id="4" xr3:uid="{82927005-4386-4694-9FA0-CF3D6DDB541C}" name="Commentaire" dataDxfId="172"/>
+    <tableColumn id="1" xr3:uid="{526E210B-F075-426E-960B-2873C3BD0C3B}" name="Code" dataDxfId="171"/>
+    <tableColumn id="2" xr3:uid="{2DA7E824-8886-4D58-ADE6-5377ED969D2A}" name="Libellé niveau 1" dataDxfId="170"/>
+    <tableColumn id="5" xr3:uid="{5D94993D-C9B5-47AD-AE15-32C420404C57}" name="Libellé niveau 2" dataDxfId="169"/>
+    <tableColumn id="3" xr3:uid="{436A1EAF-13B2-4CB3-9DDA-971E988E804D}" name="Description" dataDxfId="168"/>
+    <tableColumn id="4" xr3:uid="{82927005-4386-4694-9FA0-CF3D6DDB541C}" name="Commentaire" dataDxfId="167"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{53E2508C-FDA4-492A-BCC5-54C2C9927701}" name="Table1361112311182122" displayName="Table1361112311182122" ref="A9:E55" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{53E2508C-FDA4-492A-BCC5-54C2C9927701}" name="Table1361112311182122" displayName="Table1361112311182122" ref="A9:E55" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A9:E55" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{61EFFEA6-F404-4D86-AF5A-470909BE208C}" name="Code" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{03E7B1DA-4913-4752-81D9-0DC5A650C798}" name="Libellé niveau 1" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{37E58575-3D14-49D7-8CD2-5DBE167C1AB2}" name="Libellé niveau 2" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{A2966C92-9801-4F74-B82F-3949B0B677E2}" name="Description" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{024E1FD3-4136-4C4D-9326-7EB1C41CE3F6}" name="Commentaire" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{61EFFEA6-F404-4D86-AF5A-470909BE208C}" name="Code" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{03E7B1DA-4913-4752-81D9-0DC5A650C798}" name="Libellé niveau 1" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{37E58575-3D14-49D7-8CD2-5DBE167C1AB2}" name="Libellé niveau 2" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{A2966C92-9801-4F74-B82F-3949B0B677E2}" name="Description" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{024E1FD3-4136-4C4D-9326-7EB1C41CE3F6}" name="Commentaire" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B9D58545-FB9E-446E-B811-6132BB1C3102}" name="Table136111231118212223" displayName="Table136111231118212223" ref="A9:E56" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B9D58545-FB9E-446E-B811-6132BB1C3102}" name="Table136111231118212223" displayName="Table136111231118212223" ref="A9:E56" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A9:E56" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E024BFB1-D7BC-4643-A173-73487B8EA76A}" name="Code" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{1FF3D037-3DC1-4032-AEEC-DB4E0FB2E125}" name="Libellé niveau 1" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{62B7E7BB-D7DB-42E9-9D6E-BCC352A62FAB}" name="Libellé niveau 2" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{D76DC12D-18A0-4B2C-9CCF-77E99D26B9F8}" name="Description" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{76F1640A-E1D7-412F-8753-57C0DE81055A}" name="Commentaire" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{E024BFB1-D7BC-4643-A173-73487B8EA76A}" name="Code" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{1FF3D037-3DC1-4032-AEEC-DB4E0FB2E125}" name="Libellé niveau 1" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{62B7E7BB-D7DB-42E9-9D6E-BCC352A62FAB}" name="Libellé niveau 2" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{D76DC12D-18A0-4B2C-9CCF-77E99D26B9F8}" name="Description" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{76F1640A-E1D7-412F-8753-57C0DE81055A}" name="Commentaire" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{02356107-77B0-4BE5-BEAF-E473DB32590C}" name="Table1361112311181325" displayName="Table1361112311181325" ref="A9:E55" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{02356107-77B0-4BE5-BEAF-E473DB32590C}" name="Table1361112311181325" displayName="Table1361112311181325" ref="A9:E55" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A9:E55" xr:uid="{02356107-77B0-4BE5-BEAF-E473DB32590C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A3539628-1B96-4BB4-8A92-807D3B263DB7}" name="Code" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{AB8BA679-7023-4CF4-9883-6EE0FCD762F0}" name="Libellé niveau 1" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{5539128F-5313-4E5E-9C65-3502BDA2C44F}" name="Libellé niveau 2" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{D014B530-2E82-44D4-8C35-E5E40F3B9E3F}" name="Description" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{70515DEB-B1E5-4074-8DF3-44DBE6841499}" name="Commentaire" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{A3539628-1B96-4BB4-8A92-807D3B263DB7}" name="Code" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{AB8BA679-7023-4CF4-9883-6EE0FCD762F0}" name="Libellé niveau 1" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{5539128F-5313-4E5E-9C65-3502BDA2C44F}" name="Libellé niveau 2" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{D014B530-2E82-44D4-8C35-E5E40F3B9E3F}" name="Description" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{70515DEB-B1E5-4074-8DF3-44DBE6841499}" name="Commentaire" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A9:E55" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A9:E55" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}" name="Table13611123111821" displayName="Table13611123111821" ref="A9:E55" totalsRowShown="0" headerRowDxfId="171" dataDxfId="170">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}" name="Table13611123111821" displayName="Table13611123111821" ref="A9:E55" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165">
   <autoFilter ref="A9:E55" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E79380D3-D068-423A-A034-02D5BAD28B34}" name="Code" dataDxfId="169"/>
-    <tableColumn id="2" xr3:uid="{38AD2FF1-8A7F-4689-AF86-3D0B5B4171F9}" name="Libellé niveau 1" dataDxfId="168"/>
-    <tableColumn id="5" xr3:uid="{F5EB8D60-F8AE-488C-8A75-B040D771B063}" name="Libellé niveau 2" dataDxfId="167"/>
-    <tableColumn id="3" xr3:uid="{1346777B-B4B8-4C5A-A2A0-C55CA418799A}" name="Description" dataDxfId="166"/>
-    <tableColumn id="4" xr3:uid="{7565A967-B560-4204-9869-CC57B1587900}" name="Commentaire" dataDxfId="165"/>
+    <tableColumn id="1" xr3:uid="{E79380D3-D068-423A-A034-02D5BAD28B34}" name="Code" dataDxfId="164"/>
+    <tableColumn id="2" xr3:uid="{38AD2FF1-8A7F-4689-AF86-3D0B5B4171F9}" name="Libellé niveau 1" dataDxfId="163"/>
+    <tableColumn id="5" xr3:uid="{F5EB8D60-F8AE-488C-8A75-B040D771B063}" name="Libellé niveau 2" dataDxfId="162"/>
+    <tableColumn id="3" xr3:uid="{1346777B-B4B8-4C5A-A2A0-C55CA418799A}" name="Description" dataDxfId="161"/>
+    <tableColumn id="4" xr3:uid="{7565A967-B560-4204-9869-CC57B1587900}" name="Commentaire" dataDxfId="160"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="164" dataDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="159" dataDxfId="158">
   <autoFilter ref="A9:F308" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="161"/>
-    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="160"/>
-    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="159"/>
-    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="158"/>
-    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="157"/>
+    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="157"/>
+    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="156"/>
+    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="155"/>
+    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="154"/>
+    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="153"/>
+    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="152"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="156" dataDxfId="155">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="151" dataDxfId="150">
   <autoFilter ref="A9:F188" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="154"/>
-    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="153"/>
-    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="152"/>
-    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="151"/>
-    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="149"/>
+    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="149"/>
+    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="148"/>
+    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="147"/>
+    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="146"/>
+    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="145"/>
+    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="144"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="148" dataDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
   <autoFilter ref="A9:D46" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="146"/>
-    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="145"/>
-    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="144"/>
-    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="143"/>
+    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="140"/>
+    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="137" dataDxfId="136">
   <autoFilter ref="A9:E61" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="140"/>
-    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="139"/>
-    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="138"/>
-    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="137"/>
-    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="136"/>
+    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="135"/>
+    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="134"/>
+    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="133"/>
+    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="132"/>
+    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="131"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B4F34E16-6907-43F3-BE39-7236A5E958C1}" name="Table1361112311181324" displayName="Table1361112311181324" ref="A9:E55" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B4F34E16-6907-43F3-BE39-7236A5E958C1}" name="Table1361112311181324" displayName="Table1361112311181324" ref="A9:E55" totalsRowShown="0" headerRowDxfId="130" dataDxfId="129">
   <autoFilter ref="A9:E55" xr:uid="{B4F34E16-6907-43F3-BE39-7236A5E958C1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E04E8FE3-37D1-4BCD-B413-743E4DC4D779}" name="Code" dataDxfId="133"/>
-    <tableColumn id="2" xr3:uid="{AD3A7356-1689-4604-9ECC-BE119363210C}" name="Libellé niveau 1" dataDxfId="132"/>
-    <tableColumn id="5" xr3:uid="{2348B431-9FD0-4141-896C-0D101A9A5F99}" name="Libellé niveau 2" dataDxfId="131"/>
-    <tableColumn id="3" xr3:uid="{4B8B8570-D8A1-4AEA-90A5-8E0E9C6DD58C}" name="Description" dataDxfId="130"/>
-    <tableColumn id="4" xr3:uid="{B436BE35-AE75-458E-BF9D-1A1F55295033}" name="Commentaire" dataDxfId="129"/>
+    <tableColumn id="1" xr3:uid="{E04E8FE3-37D1-4BCD-B413-743E4DC4D779}" name="Code" dataDxfId="128"/>
+    <tableColumn id="2" xr3:uid="{AD3A7356-1689-4604-9ECC-BE119363210C}" name="Libellé niveau 1" dataDxfId="127"/>
+    <tableColumn id="5" xr3:uid="{2348B431-9FD0-4141-896C-0D101A9A5F99}" name="Libellé niveau 2" dataDxfId="126"/>
+    <tableColumn id="3" xr3:uid="{4B8B8570-D8A1-4AEA-90A5-8E0E9C6DD58C}" name="Description" dataDxfId="125"/>
+    <tableColumn id="4" xr3:uid="{B436BE35-AE75-458E-BF9D-1A1F55295033}" name="Commentaire" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}" name="Table13611123" displayName="Table13611123" ref="A9:E55" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}" name="Table13611123" displayName="Table13611123" ref="A9:E55" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="A9:E55" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A5D7830D-ADAE-49D1-AC01-5A1DFA001520}" name="Code" dataDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{314EEFD1-40EA-4FC8-B871-E91D87553FAE}" name="Libellé niveau 1" dataDxfId="125"/>
-    <tableColumn id="5" xr3:uid="{2A634FA7-602A-4CA9-B5C2-AF22E2C2C4B5}" name="Libellé niveau 2" dataDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{110DEB60-AD15-400E-BCE9-BFB19B19C22B}" name="Description" dataDxfId="123"/>
-    <tableColumn id="4" xr3:uid="{946798AA-F310-452C-873A-8DEE9082FA3D}" name="Commentaire" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{A5D7830D-ADAE-49D1-AC01-5A1DFA001520}" name="Code" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{314EEFD1-40EA-4FC8-B871-E91D87553FAE}" name="Libellé niveau 1" dataDxfId="120"/>
+    <tableColumn id="5" xr3:uid="{2A634FA7-602A-4CA9-B5C2-AF22E2C2C4B5}" name="Libellé niveau 2" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{110DEB60-AD15-400E-BCE9-BFB19B19C22B}" name="Description" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{946798AA-F310-452C-873A-8DEE9082FA3D}" name="Commentaire" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11220,25 +11170,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" style="24" customWidth="1"/>
+    <col min="2" max="2" width="43.83203125" style="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="24" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="24" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" style="24" customWidth="1"/>
-    <col min="7" max="12" width="12.7109375" style="24" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="24"/>
+    <col min="4" max="4" width="37.1640625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="24" customWidth="1"/>
+    <col min="7" max="12" width="12.6640625" style="24" customWidth="1"/>
+    <col min="13" max="16384" width="11.5" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -11246,7 +11197,7 @@
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:12" s="26" customFormat="1" ht="15">
+    <row r="2" spans="1:12" s="26" customFormat="1">
       <c r="A2" s="25" t="s">
         <v>1750</v>
       </c>
@@ -11284,12 +11235,12 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15">
+    <row r="3" spans="1:12" hidden="1">
       <c r="A3" s="27" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="C3" s="27" t="str">
         <f>Filiere!$B$1</f>
@@ -11314,12 +11265,12 @@
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
     </row>
-    <row r="4" spans="1:12" ht="15">
+    <row r="4" spans="1:12" hidden="1">
       <c r="A4" s="27" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="C4" s="27" t="str">
         <f>'Type d''intervention'!$B$1</f>
@@ -11344,12 +11295,12 @@
       <c r="K4" s="30"/>
       <c r="L4" s="30"/>
     </row>
-    <row r="5" spans="1:12" ht="15">
+    <row r="5" spans="1:12" hidden="1">
       <c r="A5" s="27" t="s">
         <v>1726</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="C5" s="27" t="str">
         <f>'Origine de l''appel'!$B$1</f>
@@ -11374,7 +11325,7 @@
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
     </row>
-    <row r="6" spans="1:12" ht="15">
+    <row r="6" spans="1:12">
       <c r="A6" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11406,7 +11357,7 @@
       <c r="K6" s="30"/>
       <c r="L6" s="30"/>
     </row>
-    <row r="7" spans="1:12" ht="15">
+    <row r="7" spans="1:12">
       <c r="A7" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11438,7 +11389,7 @@
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
     </row>
-    <row r="8" spans="1:12" ht="15">
+    <row r="8" spans="1:12">
       <c r="A8" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11470,7 +11421,7 @@
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
     </row>
-    <row r="9" spans="1:12" ht="15">
+    <row r="9" spans="1:12">
       <c r="A9" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11502,12 +11453,12 @@
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
     </row>
-    <row r="10" spans="1:12" ht="15">
+    <row r="10" spans="1:12" ht="15" hidden="1">
       <c r="A10" s="27" t="s">
         <v>1726</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="C10" s="49" t="str">
         <f>'Etats du dossier'!B1</f>
@@ -11517,7 +11468,7 @@
         <f>'Etats du dossier'!B2</f>
         <v>Etats_Dossier</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="68" t="s">
         <v>1728</v>
       </c>
       <c r="F10" s="28" t="s">
@@ -11532,7 +11483,7 @@
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
     </row>
-    <row r="11" spans="1:12" ht="15">
+    <row r="11" spans="1:12">
       <c r="A11" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11562,7 +11513,7 @@
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
     </row>
-    <row r="12" spans="1:12" ht="15">
+    <row r="12" spans="1:12">
       <c r="A12" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11592,7 +11543,7 @@
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
     </row>
-    <row r="13" spans="1:12" ht="15">
+    <row r="13" spans="1:12" hidden="1">
       <c r="A13" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11622,7 +11573,7 @@
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
     </row>
-    <row r="14" spans="1:12" ht="15">
+    <row r="14" spans="1:12" hidden="1">
       <c r="A14" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11657,7 +11608,7 @@
         <v>2004</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C15" s="28" t="str">
         <f>'Lieu - Source ou type d''id'!$B$1</f>
@@ -11667,7 +11618,7 @@
         <f>'Lieu - Source ou type d''id'!$B2</f>
         <v>SOURCE_Id_Lieu</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="68" t="s">
         <v>1728</v>
       </c>
       <c r="F15" s="28" t="s">
@@ -11684,7 +11635,7 @@
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
     </row>
-    <row r="16" spans="1:12" ht="15">
+    <row r="16" spans="1:12">
       <c r="A16" s="27" t="s">
         <v>2004</v>
       </c>
@@ -11716,7 +11667,7 @@
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
     </row>
-    <row r="17" spans="1:12" ht="15">
+    <row r="17" spans="1:12">
       <c r="A17" s="27" t="s">
         <v>2004</v>
       </c>
@@ -11748,7 +11699,7 @@
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
     </row>
-    <row r="18" spans="1:12" ht="15">
+    <row r="18" spans="1:12">
       <c r="A18" s="27" t="s">
         <v>2004</v>
       </c>
@@ -11780,7 +11731,7 @@
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
     </row>
-    <row r="19" spans="1:12" ht="15">
+    <row r="19" spans="1:12">
       <c r="A19" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11810,7 +11761,7 @@
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
     </row>
-    <row r="20" spans="1:12" ht="15">
+    <row r="20" spans="1:12">
       <c r="A20" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11842,7 +11793,7 @@
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
     </row>
-    <row r="21" spans="1:12" ht="15">
+    <row r="21" spans="1:12">
       <c r="A21" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11874,7 +11825,7 @@
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
     </row>
-    <row r="22" spans="1:12" ht="15">
+    <row r="22" spans="1:12">
       <c r="A22" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11906,7 +11857,7 @@
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
     </row>
-    <row r="23" spans="1:12" ht="15">
+    <row r="23" spans="1:12">
       <c r="A23" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11938,12 +11889,12 @@
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
     </row>
-    <row r="24" spans="1:12" ht="15">
+    <row r="24" spans="1:12" hidden="1">
       <c r="A24" s="28" t="s">
         <v>1744</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="C24" s="49" t="str">
         <f>'Patient - type d''Id'!$B$1</f>
@@ -11968,7 +11919,7 @@
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
     </row>
-    <row r="25" spans="1:12" ht="15">
+    <row r="25" spans="1:12">
       <c r="A25" s="28" t="s">
         <v>1744</v>
       </c>
@@ -12000,9 +11951,9 @@
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
     </row>
-    <row r="26" spans="1:12" ht="15">
+    <row r="26" spans="1:12" hidden="1">
       <c r="A26" s="28" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>1740</v>
@@ -12030,12 +11981,12 @@
       <c r="K26" s="30"/>
       <c r="L26" s="30"/>
     </row>
-    <row r="27" spans="1:12" ht="15">
+    <row r="27" spans="1:12" hidden="1">
       <c r="A27" s="28" t="s">
+        <v>2059</v>
+      </c>
+      <c r="B27" s="34" t="s">
         <v>2060</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>2061</v>
       </c>
       <c r="C27" s="49" t="str">
         <f>Role!$B$1</f>
@@ -12060,12 +12011,12 @@
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
     </row>
-    <row r="28" spans="1:12" ht="15">
+    <row r="28" spans="1:12">
       <c r="A28" s="27" t="s">
         <v>1745</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="C28" s="49" t="str">
         <f>'Type de decision'!$B$1</f>
@@ -12081,10 +12032,10 @@
       <c r="F28" s="28" t="s">
         <v>1743</v>
       </c>
-      <c r="G28" s="72" t="s">
+      <c r="G28" s="70" t="s">
         <v>1748</v>
       </c>
-      <c r="H28" s="72" t="s">
+      <c r="H28" s="70" t="s">
         <v>1748</v>
       </c>
       <c r="I28" s="30"/>
@@ -12092,7 +12043,7 @@
       <c r="K28" s="30"/>
       <c r="L28" s="30"/>
     </row>
-    <row r="29" spans="1:12" ht="15">
+    <row r="29" spans="1:12" hidden="1">
       <c r="A29" s="27" t="s">
         <v>1751</v>
       </c>
@@ -12126,7 +12077,7 @@
       </c>
       <c r="L29" s="30"/>
     </row>
-    <row r="30" spans="1:12" ht="15">
+    <row r="30" spans="1:12" hidden="1">
       <c r="A30" s="28" t="s">
         <v>1751</v>
       </c>
@@ -12160,7 +12111,7 @@
       </c>
       <c r="L30" s="30"/>
     </row>
-    <row r="31" spans="1:12" ht="15">
+    <row r="31" spans="1:12">
       <c r="A31" s="27" t="s">
         <v>1751</v>
       </c>
@@ -12196,7 +12147,7 @@
       </c>
       <c r="L31" s="30"/>
     </row>
-    <row r="32" spans="1:12" ht="15">
+    <row r="32" spans="1:12">
       <c r="A32" s="27" t="s">
         <v>1745</v>
       </c>
@@ -12228,12 +12179,12 @@
       <c r="K32" s="30"/>
       <c r="L32" s="30"/>
     </row>
-    <row r="33" spans="1:12" ht="15">
+    <row r="33" spans="1:12" ht="15" hidden="1">
       <c r="A33" s="27" t="s">
         <v>1745</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="C33" s="27" t="str">
         <f>'Type de destination'!B1</f>
@@ -12243,7 +12194,7 @@
         <f>'Type de destination'!B2</f>
         <v>TYPE_Destination</v>
       </c>
-      <c r="E33" s="70" t="s">
+      <c r="E33" s="68" t="s">
         <v>1728</v>
       </c>
       <c r="F33" s="28" t="s">
@@ -12258,7 +12209,7 @@
       <c r="K33" s="30"/>
       <c r="L33" s="30"/>
     </row>
-    <row r="34" spans="1:12" ht="15">
+    <row r="34" spans="1:12" hidden="1">
       <c r="A34" s="28" t="s">
         <v>1752</v>
       </c>
@@ -12288,7 +12239,7 @@
       <c r="K34" s="30"/>
       <c r="L34" s="30"/>
     </row>
-    <row r="35" spans="1:12" ht="15">
+    <row r="35" spans="1:12" hidden="1">
       <c r="A35" s="28" t="s">
         <v>1752</v>
       </c>
@@ -12316,7 +12267,7 @@
       </c>
       <c r="L35" s="30"/>
     </row>
-    <row r="36" spans="1:12" ht="15">
+    <row r="36" spans="1:12" hidden="1">
       <c r="A36" s="28" t="s">
         <v>1752</v>
       </c>
@@ -12346,12 +12297,12 @@
       <c r="K36" s="30"/>
       <c r="L36" s="30"/>
     </row>
-    <row r="37" spans="1:12" ht="15">
+    <row r="37" spans="1:12" hidden="1">
       <c r="A37" s="28" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="C37" s="27" t="str">
         <f>'Reponse demande ressources'!$B$1</f>
@@ -12376,7 +12327,7 @@
       </c>
       <c r="L37" s="30"/>
     </row>
-    <row r="38" spans="1:12" ht="15">
+    <row r="38" spans="1:12" hidden="1">
       <c r="A38" s="28" t="s">
         <v>1883</v>
       </c>
@@ -12408,7 +12359,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15">
+    <row r="39" spans="1:12">
       <c r="B39" s="31"/>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>
@@ -12421,7 +12372,7 @@
       <c r="K39" s="30"/>
       <c r="L39" s="30"/>
     </row>
-    <row r="40" spans="1:12" ht="15">
+    <row r="40" spans="1:12">
       <c r="A40" s="28"/>
       <c r="B40" s="31"/>
       <c r="C40" s="28"/>
@@ -12435,7 +12386,7 @@
       <c r="K40" s="30"/>
       <c r="L40" s="30"/>
     </row>
-    <row r="41" spans="1:12" ht="15">
+    <row r="41" spans="1:12">
       <c r="A41" s="28"/>
       <c r="B41" s="31"/>
       <c r="C41" s="28"/>
@@ -15012,9 +14963,15 @@
       <c r="L224" s="28"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:K34" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}"/>
+  <autoFilter ref="A2:K38" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="A19:E21">
-    <cfRule type="expression" dxfId="19" priority="31">
+    <cfRule type="expression" dxfId="14" priority="31">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
     <cfRule type="expression" priority="32">
@@ -15022,7 +14979,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:L5">
-    <cfRule type="expression" dxfId="18" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15032,7 +14989,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:L38 B39:L39 A40:L224">
-    <cfRule type="expression" dxfId="17" priority="58">
+    <cfRule type="expression" dxfId="12" priority="58">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15042,26 +14999,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:L5">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>G3=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>G3="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:L45">
-    <cfRule type="expression" dxfId="14" priority="54">
+    <cfRule type="expression" dxfId="9" priority="54">
       <formula>G6=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="55">
+    <cfRule type="expression" dxfId="8" priority="55">
       <formula>G6="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35:L37">
-    <cfRule type="expression" dxfId="12" priority="52">
+    <cfRule type="expression" dxfId="7" priority="52">
       <formula>L35=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="53">
+    <cfRule type="expression" dxfId="6" priority="53">
       <formula>L35="X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15116,12 +15073,12 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15568,12 +15525,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16012,18 +15969,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE40BA41-A85C-4FB9-AA6F-684436E03697}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.7109375" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.6640625" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16641,14 +16598,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17078,12 +17035,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17101,7 +17058,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -17526,12 +17483,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="154.83203125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17982,12 +17939,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18421,13 +18378,13 @@
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18863,18 +18820,18 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C5FB96-59E0-48E6-B04E-97CCEBD7B1B7}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22:M23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19015,118 +18972,112 @@
       <c r="D16" s="52"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:13" s="32" customFormat="1">
+    <row r="17" spans="1:5" s="32" customFormat="1">
       <c r="A17" s="52"/>
       <c r="B17" s="52"/>
       <c r="C17" s="43"/>
       <c r="D17" s="52"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:13" s="32" customFormat="1">
+    <row r="18" spans="1:5" s="32" customFormat="1">
       <c r="A18" s="52"/>
       <c r="B18" s="52"/>
       <c r="C18" s="43"/>
       <c r="D18" s="52"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:13" s="32" customFormat="1">
+    <row r="19" spans="1:5" s="32" customFormat="1">
       <c r="A19" s="52"/>
       <c r="B19" s="52"/>
       <c r="C19" s="43"/>
       <c r="D19" s="52"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:5">
       <c r="A20" s="52"/>
       <c r="B20" s="52"/>
       <c r="C20" s="2"/>
       <c r="D20" s="52"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:5">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="39"/>
     </row>
-    <row r="22" spans="1:13" s="42" customFormat="1">
+    <row r="22" spans="1:5" s="42" customFormat="1">
       <c r="A22" s="40"/>
       <c r="B22" s="40"/>
       <c r="C22" s="41"/>
       <c r="D22" s="41"/>
       <c r="E22" s="40"/>
-      <c r="M22" s="68" t="s">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="2"/>
       <c r="B23" s="38"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="M23" s="69" t="s">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="2"/>
       <c r="B24" s="35"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:5">
       <c r="A25" s="2"/>
       <c r="B25" s="38"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:5">
       <c r="A26" s="2"/>
       <c r="B26" s="35"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:5">
       <c r="A27" s="2"/>
       <c r="B27" s="36"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:5">
       <c r="A28" s="2"/>
       <c r="B28" s="36"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:5">
       <c r="A29" s="2"/>
       <c r="B29" s="36"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:5">
       <c r="A30" s="2"/>
       <c r="B30" s="36"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:5">
       <c r="A31" s="2"/>
       <c r="B31" s="37"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:5">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -19295,23 +19246,6 @@
       <c r="E55" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M22:M23">
-    <cfRule type="expression" dxfId="4" priority="1">
-      <formula>OR($AD22="X",$AC22="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>AND($AD22=1,$AC22=1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$AD22=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
-      <formula>$AC22=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
-      <formula>AND(NOT(ISBLANK($V22)),ISBLANK($AC22),ISBLANK($AD22))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -19327,13 +19261,13 @@
       <selection activeCell="M22" sqref="M22:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19779,13 +19713,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19802,7 +19736,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -19848,7 +19782,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -19869,29 +19803,29 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1">
-      <c r="A10" s="71" t="s">
-        <v>2010</v>
+    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+      <c r="A10" s="69" t="s">
+        <v>2009</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>2011</v>
-      </c>
-      <c r="B11" s="52" t="s">
-        <v>2012</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -19900,24 +19834,24 @@
         <v>1396</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -20239,11 +20173,11 @@
       <selection activeCell="M22" sqref="M22:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20686,17 +20620,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29F356B-BB22-47DE-A619-877383F0285B}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -20784,7 +20716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="32">
       <c r="A10" s="16" t="s">
         <v>1287</v>
       </c>
@@ -20797,7 +20729,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="32">
       <c r="A11" s="16" t="s">
         <v>1290</v>
       </c>
@@ -20810,7 +20742,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="16" t="s">
         <v>1293</v>
       </c>
@@ -20823,7 +20755,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="30">
+    <row r="13" spans="1:5" ht="32">
       <c r="A13" s="16" t="s">
         <v>1296</v>
       </c>
@@ -20836,7 +20768,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" s="16" t="s">
         <v>1299</v>
       </c>
@@ -20849,7 +20781,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="45">
+    <row r="15" spans="1:5" ht="32">
       <c r="A15" s="16" t="s">
         <v>1302</v>
       </c>
@@ -20862,7 +20794,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="32">
       <c r="A16" s="16" t="s">
         <v>1305</v>
       </c>
@@ -20875,7 +20807,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="32">
       <c r="A17" s="16" t="s">
         <v>1308</v>
       </c>
@@ -20888,7 +20820,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="45">
+    <row r="18" spans="1:5" ht="48">
       <c r="A18" s="16" t="s">
         <v>1311</v>
       </c>
@@ -20901,7 +20833,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="48">
       <c r="A19" s="16" t="s">
         <v>1314</v>
       </c>
@@ -20914,7 +20846,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="45">
+    <row r="20" spans="1:5" ht="32">
       <c r="A20" s="16" t="s">
         <v>1317</v>
       </c>
@@ -20927,7 +20859,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5" ht="32">
       <c r="A21" s="16" t="s">
         <v>1320</v>
       </c>
@@ -20940,7 +20872,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5" ht="32">
       <c r="A22" s="16" t="s">
         <v>1323</v>
       </c>
@@ -20953,7 +20885,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5" ht="32">
       <c r="A23" s="16" t="s">
         <v>1326</v>
       </c>
@@ -20966,7 +20898,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="30">
+    <row r="24" spans="1:5" ht="32">
       <c r="A24" s="16" t="s">
         <v>1329</v>
       </c>
@@ -20979,7 +20911,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5" ht="32">
       <c r="A25" s="16" t="s">
         <v>1332</v>
       </c>
@@ -20992,7 +20924,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5" ht="32">
       <c r="A26" s="16" t="s">
         <v>1335</v>
       </c>
@@ -21005,7 +20937,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="16">
       <c r="A27" s="16" t="s">
         <v>1338</v>
       </c>
@@ -21018,7 +20950,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="30">
+    <row r="28" spans="1:5" ht="32">
       <c r="A28" s="16" t="s">
         <v>1340</v>
       </c>
@@ -21031,7 +20963,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="16">
       <c r="A29" s="16" t="s">
         <v>1343</v>
       </c>
@@ -21044,7 +20976,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="16">
       <c r="A30" s="16" t="s">
         <v>1346</v>
       </c>
@@ -21074,13 +21006,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -21179,7 +21111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="16" t="s">
         <v>1351</v>
       </c>
@@ -21193,7 +21125,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="48">
       <c r="A11" s="16" t="s">
         <v>1354</v>
       </c>
@@ -21207,7 +21139,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="45">
+    <row r="12" spans="1:6" ht="32">
       <c r="A12" s="16" t="s">
         <v>1357</v>
       </c>
@@ -21221,7 +21153,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="32">
       <c r="A13" s="16" t="s">
         <v>1360</v>
       </c>
@@ -21235,7 +21167,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:6" ht="32">
       <c r="A14" s="16" t="s">
         <v>1363</v>
       </c>
@@ -21249,7 +21181,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="32">
       <c r="A15" s="16" t="s">
         <v>1366</v>
       </c>
@@ -21263,7 +21195,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="30">
+    <row r="16" spans="1:6" ht="32">
       <c r="A16" s="16" t="s">
         <v>1369</v>
       </c>
@@ -21277,7 +21209,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="45">
+    <row r="17" spans="1:6" ht="48">
       <c r="A17" s="16" t="s">
         <v>1343</v>
       </c>
@@ -21291,7 +21223,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="30">
+    <row r="18" spans="1:6" ht="32">
       <c r="A18" s="16" t="s">
         <v>1374</v>
       </c>
@@ -21418,12 +21350,12 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -21440,7 +21372,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -21507,66 +21439,66 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="52" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="2" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="2" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="2" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="2" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="2" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -21873,13 +21805,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
-    <col min="6" max="6" width="61.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="6" max="6" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22033,14 +21965,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22462,12 +22394,12 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22484,7 +22416,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -22530,7 +22462,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -22551,81 +22483,81 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1">
-      <c r="A10" s="74" t="s">
-        <v>2046</v>
-      </c>
-      <c r="B10" s="74" t="s">
-        <v>2046</v>
+    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+      <c r="A10" s="72" t="s">
+        <v>2045</v>
+      </c>
+      <c r="B10" s="72" t="s">
+        <v>2045</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="73" t="s">
+        <v>2046</v>
+      </c>
+      <c r="B11" s="73" t="s">
+        <v>2046</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="74" t="s">
+        <v>2052</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" s="32" customFormat="1">
+      <c r="A12" s="73" t="s">
         <v>2047</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B12" s="73" t="s">
         <v>2047</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="76" t="s">
-        <v>2053</v>
-      </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" s="32" customFormat="1">
-      <c r="A12" s="75" t="s">
-        <v>2048</v>
-      </c>
-      <c r="B12" s="75" t="s">
-        <v>2048</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
-      <c r="A13" s="75" t="s">
-        <v>2049</v>
-      </c>
-      <c r="B13" s="75" t="s">
-        <v>2049</v>
+      <c r="A13" s="73" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B13" s="73" t="s">
+        <v>2048</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="73" t="s">
         <v>1343</v>
       </c>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="73" t="s">
         <v>1343</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1">
-      <c r="A15" s="75" t="s">
+      <c r="A15" s="73" t="s">
         <v>1346</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="73" t="s">
         <v>1346</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -22930,14 +22862,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -23377,13 +23309,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -23404,7 +23336,7 @@
         <v>1552</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -23450,8 +23382,8 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="48.75">
-      <c r="A8" s="77" t="s">
+    <row r="8" spans="1:6" ht="40">
+      <c r="A8" s="75" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="66" t="s">
@@ -23798,19 +23730,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55EE5AD-9985-4D20-8EAC-8B61AD8038D6}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.1640625" style="32" customWidth="1"/>
     <col min="3" max="3" width="56" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="32" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="32" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="32"/>
+    <col min="4" max="4" width="17.6640625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="32" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="32" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1">
@@ -24057,7 +23989,7 @@
       </c>
       <c r="B21" s="53"/>
       <c r="C21" s="53" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="D21" s="53"/>
       <c r="E21" s="52" t="s">
@@ -24183,7 +24115,7 @@
       </c>
       <c r="B31" s="52"/>
       <c r="C31" s="52" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="D31" s="52"/>
       <c r="E31" s="52" t="s">
@@ -24710,7 +24642,7 @@
       </c>
       <c r="B72" s="52"/>
       <c r="C72" s="52" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="D72" s="52"/>
       <c r="E72" s="52" t="s">
@@ -24786,13 +24718,13 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -24809,7 +24741,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -24874,12 +24806,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1">
-      <c r="A10" s="71" t="s">
-        <v>2024</v>
-      </c>
-      <c r="B10" s="71" t="s">
-        <v>2024</v>
+    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+      <c r="A10" s="69" t="s">
+        <v>2023</v>
+      </c>
+      <c r="B10" s="69" t="s">
+        <v>2023</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -24887,10 +24819,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -24898,10 +24830,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -25224,13 +25156,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25648,13 +25580,13 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25862,8 +25794,8 @@
       <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="79" t="s">
-        <v>2099</v>
+      <c r="A18" s="77" t="s">
+        <v>2098</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>1601</v>
@@ -26164,13 +26096,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26187,7 +26119,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -26233,7 +26165,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -26254,12 +26186,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1">
-      <c r="A10" s="71" t="s">
-        <v>2096</v>
-      </c>
-      <c r="B10" s="78" t="s">
-        <v>2091</v>
+    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+      <c r="A10" s="69" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>2090</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -26269,8 +26201,8 @@
       <c r="A11" s="52" t="s">
         <v>1317</v>
       </c>
-      <c r="B11" s="78" t="s">
-        <v>2092</v>
+      <c r="B11" s="76" t="s">
+        <v>2091</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -26278,10 +26210,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2097</v>
-      </c>
-      <c r="B12" s="78" t="s">
-        <v>2093</v>
+        <v>2096</v>
+      </c>
+      <c r="B12" s="76" t="s">
+        <v>2092</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -26289,9 +26221,9 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2090</v>
-      </c>
-      <c r="B13" s="78" t="s">
+        <v>2089</v>
+      </c>
+      <c r="B13" s="76" t="s">
         <v>683</v>
       </c>
       <c r="C13" s="43"/>
@@ -26300,10 +26232,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2098</v>
-      </c>
-      <c r="B14" s="78" t="s">
-        <v>2094</v>
+        <v>2097</v>
+      </c>
+      <c r="B14" s="76" t="s">
+        <v>2093</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -26313,8 +26245,8 @@
       <c r="A15" s="52" t="s">
         <v>1343</v>
       </c>
-      <c r="B15" s="78" t="s">
-        <v>2095</v>
+      <c r="B15" s="76" t="s">
+        <v>2094</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52"/>
@@ -26624,13 +26556,13 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26714,7 +26646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="44" t="s">
         <v>1775</v>
       </c>
@@ -26740,7 +26672,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="46" t="s">
         <v>1777</v>
       </c>
@@ -26753,7 +26685,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="16">
       <c r="A13" s="46" t="s">
         <v>1553</v>
       </c>
@@ -26766,7 +26698,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" s="46" t="s">
         <v>1417</v>
       </c>
@@ -26779,7 +26711,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="16">
       <c r="A15" s="46" t="s">
         <v>1546</v>
       </c>
@@ -26792,7 +26724,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="16">
       <c r="A16" s="46" t="s">
         <v>1778</v>
       </c>
@@ -26805,7 +26737,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="16">
       <c r="A17" s="47" t="s">
         <v>1779</v>
       </c>
@@ -26818,7 +26750,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="16">
       <c r="A18" s="48" t="s">
         <v>1780</v>
       </c>
@@ -26831,7 +26763,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="16">
       <c r="A19" s="46" t="s">
         <v>1781</v>
       </c>
@@ -26844,7 +26776,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="16">
       <c r="A20" s="46" t="s">
         <v>1782</v>
       </c>
@@ -26857,7 +26789,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="16">
       <c r="A21" s="46" t="s">
         <v>1783</v>
       </c>
@@ -27128,12 +27060,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="163.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="163.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="52" customFormat="1">
@@ -27354,12 +27286,12 @@
       <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="154.83203125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -27870,15 +27802,15 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" style="52" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="52" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" style="52" customWidth="1"/>
-    <col min="5" max="5" width="88.7109375" style="52" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="52" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="52"/>
+    <col min="1" max="1" width="21.5" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" style="52" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="52" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="52" customWidth="1"/>
+    <col min="5" max="5" width="88.6640625" style="52" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="52" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27973,7 +27905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="60" t="s">
         <v>1800</v>
       </c>
@@ -27988,7 +27920,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="46" t="s">
         <v>1804</v>
       </c>
@@ -27999,7 +27931,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="46" t="s">
         <v>1807</v>
       </c>
@@ -28013,7 +27945,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="46" t="s">
         <v>1811</v>
       </c>
@@ -28028,7 +27960,7 @@
         <v>1814</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="16">
       <c r="A14" s="60" t="s">
         <v>1815</v>
       </c>
@@ -28039,7 +27971,7 @@
         <v>1817</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="16">
       <c r="A15" s="46" t="s">
         <v>1818</v>
       </c>
@@ -28051,7 +27983,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="16">
       <c r="A16" s="60" t="s">
         <v>1820</v>
       </c>
@@ -28063,7 +27995,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="16">
       <c r="A17" s="60" t="s">
         <v>1589</v>
       </c>
@@ -28078,7 +28010,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="16">
       <c r="A18" s="60" t="s">
         <v>1826</v>
       </c>
@@ -28086,7 +28018,7 @@
         <v>1827</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="16">
       <c r="A19" s="60" t="s">
         <v>1828</v>
       </c>
@@ -28094,7 +28026,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="16">
       <c r="A20" s="60" t="s">
         <v>1830</v>
       </c>
@@ -28102,7 +28034,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="16">
       <c r="A21" s="60" t="s">
         <v>1832</v>
       </c>
@@ -28110,7 +28042,7 @@
         <v>1833</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="16">
       <c r="A22" s="46" t="s">
         <v>1834</v>
       </c>
@@ -28125,7 +28057,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="16">
       <c r="A23" s="46" t="s">
         <v>1838</v>
       </c>
@@ -28140,7 +28072,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="16">
       <c r="A24" s="46" t="s">
         <v>1842</v>
       </c>
@@ -28155,7 +28087,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="16">
       <c r="A25" s="60" t="s">
         <v>1846</v>
       </c>
@@ -28166,7 +28098,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="16">
       <c r="A26" s="60" t="s">
         <v>1849</v>
       </c>
@@ -28338,13 +28270,13 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="74" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -28362,7 +28294,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -28414,7 +28346,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -28439,59 +28371,59 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="60" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="19" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="16">
       <c r="A11" s="46" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="19" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="16">
       <c r="A12" s="46" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="19" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="16">
       <c r="A13" s="46" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="19" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="F13" s="16"/>
     </row>
@@ -28764,11 +28696,11 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -28786,7 +28718,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -28832,7 +28764,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -28854,15 +28786,15 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
-      <c r="A10" s="73">
+      <c r="A10" s="71">
         <v>15</v>
       </c>
-      <c r="B10" s="73">
+      <c r="B10" s="71">
         <v>15</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="2" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -28875,7 +28807,7 @@
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="2" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -28888,7 +28820,7 @@
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="2" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -28901,7 +28833,7 @@
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="2" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -28914,7 +28846,7 @@
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="2" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -29209,22 +29141,22 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="O27">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>OR($AD27="X",$AC27="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>AND($AD27=1,$AC27=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$AD27=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$AC27=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>AND(NOT(ISBLANK($V27)),ISBLANK($AC27),ISBLANK($AD27))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>AND($Q27="X",OR($B27&lt;&gt;"",$C27&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29243,14 +29175,14 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" customWidth="1"/>
+    <col min="5" max="5" width="47.83203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -29335,7 +29267,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="64.5">
+    <row r="10" spans="1:6" ht="60">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -29361,7 +29293,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -29375,7 +29307,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="26.25">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -29389,7 +29321,7 @@
       </c>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -29402,7 +29334,7 @@
       </c>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:6" ht="26.25">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -29430,7 +29362,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="26.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -29456,7 +29388,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" ht="26.25">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="2" t="s">
         <v>43</v>
       </c>
@@ -29471,7 +29403,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
@@ -29497,7 +29429,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="39">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
@@ -29511,7 +29443,7 @@
       </c>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" ht="39">
+    <row r="23" spans="1:6" ht="30">
       <c r="A23" s="2" t="s">
         <v>55</v>
       </c>
@@ -29536,7 +29468,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25">
+    <row r="25" spans="1:6" ht="30">
       <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
@@ -29550,7 +29482,7 @@
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" ht="26.25">
+    <row r="26" spans="1:6" ht="30">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -29564,7 +29496,7 @@
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="26.25">
+    <row r="27" spans="1:6" ht="30">
       <c r="A27" s="2" t="s">
         <v>66</v>
       </c>
@@ -29578,7 +29510,7 @@
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:6" ht="26.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
         <v>69</v>
       </c>
@@ -29615,7 +29547,7 @@
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:6" ht="51.75">
+    <row r="31" spans="1:6" ht="60">
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>
@@ -29629,7 +29561,7 @@
       </c>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:6" ht="26.25">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="2" t="s">
         <v>79</v>
       </c>
@@ -29668,7 +29600,7 @@
       </c>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25">
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="2" t="s">
         <v>87</v>
       </c>
@@ -29694,7 +29626,7 @@
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" ht="102.75">
+    <row r="37" spans="1:6" ht="120">
       <c r="A37" s="2" t="s">
         <v>92</v>
       </c>
@@ -29708,7 +29640,7 @@
       </c>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" ht="26.25">
+    <row r="38" spans="1:6" ht="30">
       <c r="A38" s="2" t="s">
         <v>95</v>
       </c>
@@ -29722,7 +29654,7 @@
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" ht="39">
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="2" t="s">
         <v>98</v>
       </c>
@@ -29747,7 +29679,7 @@
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" ht="39">
+    <row r="41" spans="1:6" ht="30">
       <c r="A41" s="2" t="s">
         <v>103</v>
       </c>
@@ -29761,7 +29693,7 @@
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" ht="26.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>106</v>
       </c>
@@ -29775,7 +29707,7 @@
       </c>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" ht="39">
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="2" t="s">
         <v>109</v>
       </c>
@@ -29800,7 +29732,7 @@
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:6" ht="39">
+    <row r="45" spans="1:6" ht="45">
       <c r="A45" s="2" t="s">
         <v>114</v>
       </c>
@@ -29899,7 +29831,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:6" ht="26.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
         <v>132</v>
       </c>
@@ -29913,7 +29845,7 @@
       </c>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" spans="1:6" ht="64.5">
+    <row r="54" spans="1:6" ht="60">
       <c r="A54" s="2" t="s">
         <v>135</v>
       </c>
@@ -30286,7 +30218,7 @@
       <c r="E84" s="10"/>
       <c r="F84" s="10"/>
     </row>
-    <row r="85" spans="1:6" ht="39">
+    <row r="85" spans="1:6" ht="45">
       <c r="A85" s="2" t="s">
         <v>201</v>
       </c>
@@ -30312,7 +30244,7 @@
       <c r="E86" s="10"/>
       <c r="F86" s="10"/>
     </row>
-    <row r="87" spans="1:6" ht="128.25">
+    <row r="87" spans="1:6" ht="135">
       <c r="A87" s="2" t="s">
         <v>206</v>
       </c>
@@ -30338,7 +30270,7 @@
       <c r="E88" s="10"/>
       <c r="F88" s="10"/>
     </row>
-    <row r="89" spans="1:6" ht="51.75">
+    <row r="89" spans="1:6" ht="60">
       <c r="A89" s="2" t="s">
         <v>199</v>
       </c>
@@ -30351,7 +30283,7 @@
       </c>
       <c r="F89" s="10"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25">
+    <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
         <v>201</v>
       </c>
@@ -30391,7 +30323,7 @@
       <c r="E92" s="10"/>
       <c r="F92" s="10"/>
     </row>
-    <row r="93" spans="1:6" ht="26.25">
+    <row r="93" spans="1:6" ht="30">
       <c r="A93" s="2" t="s">
         <v>217</v>
       </c>
@@ -30563,7 +30495,7 @@
       <c r="E106" s="10"/>
       <c r="F106" s="10"/>
     </row>
-    <row r="107" spans="1:6" ht="26.25">
+    <row r="107" spans="1:6" ht="30">
       <c r="A107" s="2" t="s">
         <v>248</v>
       </c>
@@ -30577,7 +30509,7 @@
       </c>
       <c r="F107" s="10"/>
     </row>
-    <row r="108" spans="1:6" ht="26.25">
+    <row r="108" spans="1:6">
       <c r="A108" s="2" t="s">
         <v>251</v>
       </c>
@@ -30701,7 +30633,7 @@
       <c r="E117" s="10"/>
       <c r="F117" s="10"/>
     </row>
-    <row r="118" spans="1:6" ht="26.25">
+    <row r="118" spans="1:6" ht="30">
       <c r="A118" s="2" t="s">
         <v>274</v>
       </c>
@@ -30715,7 +30647,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="26.25">
+    <row r="119" spans="1:6">
       <c r="A119" s="2" t="s">
         <v>277</v>
       </c>
@@ -30728,7 +30660,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="39">
+    <row r="120" spans="1:6" ht="45">
       <c r="A120" s="2" t="s">
         <v>280</v>
       </c>
@@ -30766,7 +30698,7 @@
       <c r="E122" s="10"/>
       <c r="F122" s="10"/>
     </row>
-    <row r="123" spans="1:6" ht="39">
+    <row r="123" spans="1:6" ht="45">
       <c r="A123" s="2" t="s">
         <v>287</v>
       </c>
@@ -30827,7 +30759,7 @@
       <c r="E127" s="10"/>
       <c r="F127" s="10"/>
     </row>
-    <row r="128" spans="1:6" ht="39">
+    <row r="128" spans="1:6" ht="45">
       <c r="A128" s="2" t="s">
         <v>298</v>
       </c>
@@ -30963,7 +30895,7 @@
       <c r="E138" s="10"/>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" spans="1:6" ht="26.25">
+    <row r="139" spans="1:6" ht="30">
       <c r="A139" s="2" t="s">
         <v>323</v>
       </c>
@@ -30989,7 +30921,7 @@
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" spans="1:6" ht="26.25">
+    <row r="141" spans="1:6" ht="30">
       <c r="A141" s="2" t="s">
         <v>328</v>
       </c>
@@ -31003,7 +30935,7 @@
       </c>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" spans="1:6" ht="26.25">
+    <row r="142" spans="1:6" ht="30">
       <c r="A142" s="2" t="s">
         <v>329</v>
       </c>
@@ -31017,7 +30949,7 @@
       </c>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" spans="1:6" ht="26.25">
+    <row r="143" spans="1:6">
       <c r="A143" s="2" t="s">
         <v>330</v>
       </c>
@@ -31031,7 +30963,7 @@
       </c>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" spans="1:6" ht="26.25">
+    <row r="144" spans="1:6" ht="30">
       <c r="A144" s="2" t="s">
         <v>331</v>
       </c>
@@ -31060,7 +30992,7 @@
       </c>
       <c r="F145" s="10"/>
     </row>
-    <row r="146" spans="1:6" ht="26.25">
+    <row r="146" spans="1:6">
       <c r="A146" s="2" t="s">
         <v>334</v>
       </c>
@@ -31074,7 +31006,7 @@
       </c>
       <c r="F146" s="10"/>
     </row>
-    <row r="147" spans="1:6" ht="39">
+    <row r="147" spans="1:6" ht="30">
       <c r="A147" s="2" t="s">
         <v>335</v>
       </c>
@@ -31088,7 +31020,7 @@
       </c>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" spans="1:6" ht="39">
+    <row r="148" spans="1:6" ht="30">
       <c r="A148" s="2" t="s">
         <v>336</v>
       </c>
@@ -31102,7 +31034,7 @@
       </c>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" spans="1:6" ht="26.25">
+    <row r="149" spans="1:6" ht="30">
       <c r="A149" s="2" t="s">
         <v>337</v>
       </c>
@@ -31115,7 +31047,7 @@
       </c>
       <c r="F149" s="10"/>
     </row>
-    <row r="150" spans="1:6" ht="26.25">
+    <row r="150" spans="1:6" ht="30">
       <c r="A150" s="2" t="s">
         <v>338</v>
       </c>
@@ -31129,7 +31061,7 @@
       </c>
       <c r="F150" s="10"/>
     </row>
-    <row r="151" spans="1:6" ht="26.25">
+    <row r="151" spans="1:6" ht="30">
       <c r="A151" s="2" t="s">
         <v>339</v>
       </c>
@@ -31261,7 +31193,7 @@
       <c r="E161" s="10"/>
       <c r="F161" s="10"/>
     </row>
-    <row r="162" spans="1:6" ht="39">
+    <row r="162" spans="1:6" ht="30">
       <c r="A162" s="2" t="s">
         <v>360</v>
       </c>
@@ -31275,7 +31207,7 @@
       </c>
       <c r="F162" s="10"/>
     </row>
-    <row r="163" spans="1:6" ht="39">
+    <row r="163" spans="1:6" ht="45">
       <c r="A163" s="2" t="s">
         <v>363</v>
       </c>
@@ -31289,7 +31221,7 @@
       </c>
       <c r="F163" s="10"/>
     </row>
-    <row r="164" spans="1:6" ht="39">
+    <row r="164" spans="1:6" ht="45">
       <c r="A164" s="2" t="s">
         <v>366</v>
       </c>
@@ -31340,7 +31272,7 @@
       <c r="E167" s="10"/>
       <c r="F167" s="10"/>
     </row>
-    <row r="168" spans="1:6" ht="26.25">
+    <row r="168" spans="1:6" ht="30">
       <c r="A168" s="2" t="s">
         <v>376</v>
       </c>
@@ -31557,7 +31489,7 @@
       <c r="E185" s="10"/>
       <c r="F185" s="10"/>
     </row>
-    <row r="186" spans="1:6" ht="26.25">
+    <row r="186" spans="1:6" ht="30">
       <c r="A186" s="2" t="s">
         <v>413</v>
       </c>
@@ -31693,7 +31625,7 @@
       </c>
       <c r="F196" s="10"/>
     </row>
-    <row r="197" spans="1:6" ht="26.25">
+    <row r="197" spans="1:6">
       <c r="A197" s="2" t="s">
         <v>438</v>
       </c>
@@ -31793,7 +31725,7 @@
       <c r="E204" s="10"/>
       <c r="F204" s="10"/>
     </row>
-    <row r="205" spans="1:6" ht="26.25">
+    <row r="205" spans="1:6" ht="30">
       <c r="A205" s="2" t="s">
         <v>457</v>
       </c>
@@ -31819,7 +31751,7 @@
       <c r="E206" s="10"/>
       <c r="F206" s="10"/>
     </row>
-    <row r="207" spans="1:6" ht="26.25">
+    <row r="207" spans="1:6" ht="30">
       <c r="A207" s="2" t="s">
         <v>462</v>
       </c>
@@ -31917,7 +31849,7 @@
       <c r="E214" s="10"/>
       <c r="F214" s="10"/>
     </row>
-    <row r="215" spans="1:6" ht="26.25">
+    <row r="215" spans="1:6" ht="30">
       <c r="A215" s="2" t="s">
         <v>480</v>
       </c>
@@ -32738,7 +32670,7 @@
       <c r="E282" s="10"/>
       <c r="F282" s="10"/>
     </row>
-    <row r="283" spans="1:6" ht="26.25">
+    <row r="283" spans="1:6" ht="30">
       <c r="A283" s="2" t="s">
         <v>625</v>
       </c>
@@ -32752,7 +32684,7 @@
       </c>
       <c r="F283" s="10"/>
     </row>
-    <row r="284" spans="1:6" ht="26.25">
+    <row r="284" spans="1:6" ht="30">
       <c r="A284" s="2" t="s">
         <v>628</v>
       </c>
@@ -33098,14 +33030,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -35819,12 +35751,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="8" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -35835,7 +35767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.75">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -35903,7 +35835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="39">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="2" t="s">
         <v>1069</v>
       </c>
@@ -35925,7 +35857,7 @@
       <c r="C11" s="10"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="26.25">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="2" t="s">
         <v>1074</v>
       </c>
@@ -35935,7 +35867,7 @@
       <c r="C12" s="10"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="39">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="2" t="s">
         <v>1076</v>
       </c>
@@ -35945,7 +35877,7 @@
       <c r="C13" s="10"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="26.25">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" s="2" t="s">
         <v>1078</v>
       </c>
@@ -35955,7 +35887,7 @@
       <c r="C14" s="10"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="26.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>1080</v>
       </c>
@@ -35965,7 +35897,7 @@
       <c r="C15" s="10"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="26.25">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" s="2" t="s">
         <v>1082</v>
       </c>
@@ -35977,7 +35909,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="39">
+    <row r="17" spans="1:4" ht="45">
       <c r="A17" s="2" t="s">
         <v>1085</v>
       </c>
@@ -35989,7 +35921,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="39">
+    <row r="18" spans="1:4" ht="30">
       <c r="A18" s="2" t="s">
         <v>1088</v>
       </c>
@@ -35999,7 +35931,7 @@
       <c r="C18" s="10"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="39">
+    <row r="19" spans="1:4" ht="45">
       <c r="A19" s="2" t="s">
         <v>1090</v>
       </c>
@@ -36009,7 +35941,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="26.25">
+    <row r="20" spans="1:4" ht="30">
       <c r="A20" s="2" t="s">
         <v>1092</v>
       </c>
@@ -36019,7 +35951,7 @@
       <c r="C20" s="10"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="26.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>1094</v>
       </c>
@@ -36029,7 +35961,7 @@
       <c r="C21" s="10"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="26.25">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" s="2" t="s">
         <v>1096</v>
       </c>
@@ -36059,7 +35991,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="26.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>1102</v>
       </c>
@@ -36089,7 +36021,7 @@
       <c r="C27" s="10"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="26.25">
+    <row r="28" spans="1:4" ht="30">
       <c r="A28" s="2" t="s">
         <v>1107</v>
       </c>
@@ -36101,7 +36033,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="26.25">
+    <row r="29" spans="1:4" ht="30">
       <c r="A29" s="2" t="s">
         <v>1110</v>
       </c>
@@ -36113,7 +36045,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="26.25">
+    <row r="30" spans="1:4" ht="30">
       <c r="A30" s="2" t="s">
         <v>1113</v>
       </c>
@@ -36135,7 +36067,7 @@
       <c r="C31" s="10"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="26.25">
+    <row r="32" spans="1:4" ht="30">
       <c r="A32" s="2" t="s">
         <v>1118</v>
       </c>
@@ -36147,7 +36079,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="39">
+    <row r="33" spans="1:4" ht="30">
       <c r="A33" s="2" t="s">
         <v>1121</v>
       </c>
@@ -36159,7 +36091,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="26.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>1124</v>
       </c>
@@ -36171,7 +36103,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="128.25">
+    <row r="35" spans="1:4" ht="135">
       <c r="A35" s="2" t="s">
         <v>1127</v>
       </c>
@@ -36183,7 +36115,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="128.25">
+    <row r="36" spans="1:4" ht="135">
       <c r="A36" s="2" t="s">
         <v>1130</v>
       </c>
@@ -36267,7 +36199,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="26.25">
+    <row r="44" spans="1:4" ht="30">
       <c r="A44" s="2" t="s">
         <v>1147</v>
       </c>
@@ -36279,7 +36211,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="26.25">
+    <row r="45" spans="1:4" ht="30">
       <c r="A45" s="2" t="s">
         <v>1150</v>
       </c>
@@ -36289,7 +36221,7 @@
       <c r="C45" s="10"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="77.25">
+    <row r="46" spans="1:4" ht="75">
       <c r="A46" s="2" t="s">
         <v>1152</v>
       </c>
@@ -36316,13 +36248,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -36439,7 +36371,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5" ht="26.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>1164</v>
       </c>
@@ -36463,7 +36395,7 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:5" ht="26.25">
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="2" t="s">
         <v>1169</v>
       </c>
@@ -36476,7 +36408,7 @@
       </c>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="1:5" ht="26.25">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="2" t="s">
         <v>1172</v>
       </c>
@@ -36500,7 +36432,7 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" ht="48.75">
+    <row r="18" spans="1:5" ht="40">
       <c r="A18" s="2" t="s">
         <v>1177</v>
       </c>
@@ -36513,7 +36445,7 @@
       </c>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" ht="64.5">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="2" t="s">
         <v>1180</v>
       </c>
@@ -36662,7 +36594,7 @@
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:5" ht="26.25">
+    <row r="32" spans="1:5" ht="30">
       <c r="A32" s="2" t="s">
         <v>1209</v>
       </c>
@@ -36675,7 +36607,7 @@
       </c>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" spans="1:5" ht="26.25">
+    <row r="33" spans="1:5" ht="30">
       <c r="A33" s="2" t="s">
         <v>1212</v>
       </c>
@@ -36762,7 +36694,7 @@
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
     </row>
-    <row r="40" spans="1:5" ht="51.75">
+    <row r="40" spans="1:5" ht="45">
       <c r="A40" s="2" t="s">
         <v>1231</v>
       </c>
@@ -36799,7 +36731,7 @@
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
     </row>
-    <row r="43" spans="1:5" ht="26.25">
+    <row r="43" spans="1:5" ht="30">
       <c r="A43" s="2" t="s">
         <v>1239</v>
       </c>
@@ -36812,7 +36744,7 @@
       </c>
       <c r="E43" s="10"/>
     </row>
-    <row r="44" spans="1:5" ht="39">
+    <row r="44" spans="1:5" ht="30">
       <c r="A44" s="2" t="s">
         <v>1240</v>
       </c>
@@ -36871,7 +36803,7 @@
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
     </row>
-    <row r="49" spans="1:5" ht="26.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="2" t="s">
         <v>1252</v>
       </c>
@@ -36906,7 +36838,7 @@
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
     </row>
-    <row r="52" spans="1:5" ht="26.25">
+    <row r="52" spans="1:5" ht="30">
       <c r="A52" s="2" t="s">
         <v>1259</v>
       </c>
@@ -37000,7 +36932,7 @@
       </c>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:5" ht="39">
+    <row r="60" spans="1:5" ht="45">
       <c r="A60" s="2" t="s">
         <v>1278</v>
       </c>
@@ -37042,13 +36974,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -37065,7 +36997,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -37111,7 +37043,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -37132,12 +37064,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1">
-      <c r="A10" s="71" t="s">
-        <v>2083</v>
-      </c>
-      <c r="B10" s="71" t="s">
-        <v>2083</v>
+    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+      <c r="A10" s="69" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B10" s="69" t="s">
+        <v>2082</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -37145,10 +37077,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -37156,10 +37088,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -37167,10 +37099,10 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52"/>
@@ -37178,10 +37110,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -37189,10 +37121,10 @@
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1">
       <c r="A15" s="52" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52"/>
@@ -37200,10 +37132,10 @@
     </row>
     <row r="16" spans="1:5" s="32" customFormat="1">
       <c r="A16" s="52" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="52"/>
@@ -37499,67 +37431,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -37973,33 +37844,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1BDBD4-E316-45AC-920A-A6692C88096C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -38017,4 +37923,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.08.07 11:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1098" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB5DA4E4-B74F-E247-87E7-5E3544E7E0AB}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="760" windowWidth="24980" windowHeight="14380" tabRatio="877" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="42600" yWindow="1560" windowWidth="3075" windowHeight="11295" tabRatio="877" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -7117,8 +7117,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
@@ -11180,16 +11180,16 @@
       <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="32.5" style="24" customWidth="1"/>
-    <col min="2" max="2" width="43.83203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="24" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="24" customWidth="1"/>
-    <col min="4" max="4" width="37.1640625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="24" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="24" customWidth="1"/>
-    <col min="7" max="12" width="12.6640625" style="24" customWidth="1"/>
-    <col min="13" max="16384" width="11.5" style="24"/>
+    <col min="4" max="4" width="37.140625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="24" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="24" customWidth="1"/>
+    <col min="7" max="12" width="12.7109375" style="24" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -11197,7 +11197,7 @@
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:12" s="26" customFormat="1">
+    <row r="2" spans="1:12" s="26" customFormat="1" ht="15">
       <c r="A2" s="25" t="s">
         <v>1750</v>
       </c>
@@ -11235,7 +11235,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1">
+    <row r="3" spans="1:12" ht="15" hidden="1">
       <c r="A3" s="27" t="s">
         <v>2025</v>
       </c>
@@ -11265,7 +11265,7 @@
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
     </row>
-    <row r="4" spans="1:12" hidden="1">
+    <row r="4" spans="1:12" ht="15" hidden="1">
       <c r="A4" s="27" t="s">
         <v>2006</v>
       </c>
@@ -11295,7 +11295,7 @@
       <c r="K4" s="30"/>
       <c r="L4" s="30"/>
     </row>
-    <row r="5" spans="1:12" hidden="1">
+    <row r="5" spans="1:12" ht="15" hidden="1">
       <c r="A5" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11325,7 +11325,7 @@
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" ht="15">
       <c r="A6" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11357,7 +11357,7 @@
       <c r="K6" s="30"/>
       <c r="L6" s="30"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" ht="15">
       <c r="A7" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11389,7 +11389,7 @@
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" ht="15">
       <c r="A8" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11421,7 +11421,7 @@
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" ht="15">
       <c r="A9" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11483,7 +11483,7 @@
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" ht="15">
       <c r="A11" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11513,7 +11513,7 @@
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" ht="15">
       <c r="A12" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11543,7 +11543,7 @@
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
     </row>
-    <row r="13" spans="1:12" hidden="1">
+    <row r="13" spans="1:12" ht="15" hidden="1">
       <c r="A13" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11573,7 +11573,7 @@
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
     </row>
-    <row r="14" spans="1:12" hidden="1">
+    <row r="14" spans="1:12" ht="15" hidden="1">
       <c r="A14" s="27" t="s">
         <v>1726</v>
       </c>
@@ -11635,7 +11635,7 @@
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" ht="15">
       <c r="A16" s="27" t="s">
         <v>2004</v>
       </c>
@@ -11667,7 +11667,7 @@
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" ht="15">
       <c r="A17" s="27" t="s">
         <v>2004</v>
       </c>
@@ -11699,7 +11699,7 @@
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" ht="15">
       <c r="A18" s="27" t="s">
         <v>2004</v>
       </c>
@@ -11731,7 +11731,7 @@
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" ht="15">
       <c r="A19" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11761,7 +11761,7 @@
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" ht="15">
       <c r="A20" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11793,7 +11793,7 @@
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" ht="15">
       <c r="A21" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11825,7 +11825,7 @@
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" ht="15">
       <c r="A22" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11857,7 +11857,7 @@
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="15">
       <c r="A23" s="27" t="s">
         <v>1729</v>
       </c>
@@ -11889,7 +11889,7 @@
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
     </row>
-    <row r="24" spans="1:12" hidden="1">
+    <row r="24" spans="1:12" ht="15" hidden="1">
       <c r="A24" s="28" t="s">
         <v>1744</v>
       </c>
@@ -11919,7 +11919,7 @@
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" ht="15">
       <c r="A25" s="28" t="s">
         <v>1744</v>
       </c>
@@ -11951,7 +11951,7 @@
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
     </row>
-    <row r="26" spans="1:12" hidden="1">
+    <row r="26" spans="1:12" ht="15" hidden="1">
       <c r="A26" s="28" t="s">
         <v>2077</v>
       </c>
@@ -11981,7 +11981,7 @@
       <c r="K26" s="30"/>
       <c r="L26" s="30"/>
     </row>
-    <row r="27" spans="1:12" hidden="1">
+    <row r="27" spans="1:12" ht="15" hidden="1">
       <c r="A27" s="28" t="s">
         <v>2059</v>
       </c>
@@ -12011,7 +12011,7 @@
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" ht="15">
       <c r="A28" s="27" t="s">
         <v>1745</v>
       </c>
@@ -12043,7 +12043,7 @@
       <c r="K28" s="30"/>
       <c r="L28" s="30"/>
     </row>
-    <row r="29" spans="1:12" hidden="1">
+    <row r="29" spans="1:12" ht="15" hidden="1">
       <c r="A29" s="27" t="s">
         <v>1751</v>
       </c>
@@ -12077,7 +12077,7 @@
       </c>
       <c r="L29" s="30"/>
     </row>
-    <row r="30" spans="1:12" hidden="1">
+    <row r="30" spans="1:12" ht="15" hidden="1">
       <c r="A30" s="28" t="s">
         <v>1751</v>
       </c>
@@ -12111,7 +12111,7 @@
       </c>
       <c r="L30" s="30"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" ht="15">
       <c r="A31" s="27" t="s">
         <v>1751</v>
       </c>
@@ -12147,7 +12147,7 @@
       </c>
       <c r="L31" s="30"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" ht="15">
       <c r="A32" s="27" t="s">
         <v>1745</v>
       </c>
@@ -12209,7 +12209,7 @@
       <c r="K33" s="30"/>
       <c r="L33" s="30"/>
     </row>
-    <row r="34" spans="1:12" hidden="1">
+    <row r="34" spans="1:12" ht="15" hidden="1">
       <c r="A34" s="28" t="s">
         <v>1752</v>
       </c>
@@ -12239,7 +12239,7 @@
       <c r="K34" s="30"/>
       <c r="L34" s="30"/>
     </row>
-    <row r="35" spans="1:12" hidden="1">
+    <row r="35" spans="1:12" ht="15" hidden="1">
       <c r="A35" s="28" t="s">
         <v>1752</v>
       </c>
@@ -12267,7 +12267,7 @@
       </c>
       <c r="L35" s="30"/>
     </row>
-    <row r="36" spans="1:12" hidden="1">
+    <row r="36" spans="1:12" ht="15" hidden="1">
       <c r="A36" s="28" t="s">
         <v>1752</v>
       </c>
@@ -12297,7 +12297,7 @@
       <c r="K36" s="30"/>
       <c r="L36" s="30"/>
     </row>
-    <row r="37" spans="1:12" hidden="1">
+    <row r="37" spans="1:12" ht="15" hidden="1">
       <c r="A37" s="28" t="s">
         <v>2071</v>
       </c>
@@ -12327,7 +12327,7 @@
       </c>
       <c r="L37" s="30"/>
     </row>
-    <row r="38" spans="1:12" hidden="1">
+    <row r="38" spans="1:12" ht="15" hidden="1">
       <c r="A38" s="28" t="s">
         <v>1883</v>
       </c>
@@ -12359,7 +12359,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" ht="15">
       <c r="B39" s="31"/>
       <c r="C39" s="28"/>
       <c r="D39" s="28"/>
@@ -12372,7 +12372,7 @@
       <c r="K39" s="30"/>
       <c r="L39" s="30"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" ht="15">
       <c r="A40" s="28"/>
       <c r="B40" s="31"/>
       <c r="C40" s="28"/>
@@ -12386,7 +12386,7 @@
       <c r="K40" s="30"/>
       <c r="L40" s="30"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" ht="15">
       <c r="A41" s="28"/>
       <c r="B41" s="31"/>
       <c r="C41" s="28"/>
@@ -15073,12 +15073,12 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15525,12 +15525,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15973,14 +15973,14 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="91.6640625" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.7109375" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -16598,14 +16598,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17035,12 +17035,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17483,12 +17483,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="154.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="154.85546875" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17939,12 +17939,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18378,13 +18378,13 @@
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18822,16 +18822,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C5FB96-59E0-48E6-B04E-97CCEBD7B1B7}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19261,13 +19261,13 @@
       <selection activeCell="M22" sqref="M22:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19713,13 +19713,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19803,7 +19803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+    <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="69" t="s">
         <v>2009</v>
       </c>
@@ -20173,11 +20173,11 @@
       <selection activeCell="M22" sqref="M22:M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20622,13 +20622,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -20716,7 +20716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32">
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="16" t="s">
         <v>1287</v>
       </c>
@@ -20729,7 +20729,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="32">
+    <row r="11" spans="1:5" ht="45">
       <c r="A11" s="16" t="s">
         <v>1290</v>
       </c>
@@ -20742,7 +20742,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="16" t="s">
         <v>1293</v>
       </c>
@@ -20755,7 +20755,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="32">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="16" t="s">
         <v>1296</v>
       </c>
@@ -20768,7 +20768,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="16" t="s">
         <v>1299</v>
       </c>
@@ -20781,7 +20781,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="32">
+    <row r="15" spans="1:5" ht="45">
       <c r="A15" s="16" t="s">
         <v>1302</v>
       </c>
@@ -20794,7 +20794,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="32">
+    <row r="16" spans="1:5" ht="30">
       <c r="A16" s="16" t="s">
         <v>1305</v>
       </c>
@@ -20807,7 +20807,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="32">
+    <row r="17" spans="1:5" ht="30">
       <c r="A17" s="16" t="s">
         <v>1308</v>
       </c>
@@ -20820,7 +20820,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="48">
+    <row r="18" spans="1:5" ht="45">
       <c r="A18" s="16" t="s">
         <v>1311</v>
       </c>
@@ -20833,7 +20833,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="48">
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="16" t="s">
         <v>1314</v>
       </c>
@@ -20846,7 +20846,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="32">
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="16" t="s">
         <v>1317</v>
       </c>
@@ -20859,7 +20859,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="32">
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="16" t="s">
         <v>1320</v>
       </c>
@@ -20872,7 +20872,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="32">
+    <row r="22" spans="1:5" ht="30">
       <c r="A22" s="16" t="s">
         <v>1323</v>
       </c>
@@ -20885,7 +20885,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="32">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="16" t="s">
         <v>1326</v>
       </c>
@@ -20898,7 +20898,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="32">
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="16" t="s">
         <v>1329</v>
       </c>
@@ -20911,7 +20911,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="32">
+    <row r="25" spans="1:5" ht="30">
       <c r="A25" s="16" t="s">
         <v>1332</v>
       </c>
@@ -20924,7 +20924,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="32">
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="16" t="s">
         <v>1335</v>
       </c>
@@ -20937,7 +20937,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="16">
+    <row r="27" spans="1:5">
       <c r="A27" s="16" t="s">
         <v>1338</v>
       </c>
@@ -20950,7 +20950,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="32">
+    <row r="28" spans="1:5" ht="30">
       <c r="A28" s="16" t="s">
         <v>1340</v>
       </c>
@@ -20963,7 +20963,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="16">
+    <row r="29" spans="1:5">
       <c r="A29" s="16" t="s">
         <v>1343</v>
       </c>
@@ -20976,7 +20976,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="16">
+    <row r="30" spans="1:5">
       <c r="A30" s="16" t="s">
         <v>1346</v>
       </c>
@@ -21006,13 +21006,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -21111,7 +21111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="16" t="s">
         <v>1351</v>
       </c>
@@ -21125,7 +21125,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="48">
+    <row r="11" spans="1:6" ht="45">
       <c r="A11" s="16" t="s">
         <v>1354</v>
       </c>
@@ -21139,7 +21139,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="32">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="16" t="s">
         <v>1357</v>
       </c>
@@ -21153,7 +21153,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" ht="32">
+    <row r="13" spans="1:6" ht="30">
       <c r="A13" s="16" t="s">
         <v>1360</v>
       </c>
@@ -21167,7 +21167,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" ht="32">
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="16" t="s">
         <v>1363</v>
       </c>
@@ -21181,7 +21181,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="32">
+    <row r="15" spans="1:6" ht="30">
       <c r="A15" s="16" t="s">
         <v>1366</v>
       </c>
@@ -21195,7 +21195,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="32">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="16" t="s">
         <v>1369</v>
       </c>
@@ -21209,7 +21209,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="48">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="16" t="s">
         <v>1343</v>
       </c>
@@ -21223,7 +21223,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="32">
+    <row r="18" spans="1:6" ht="30">
       <c r="A18" s="16" t="s">
         <v>1374</v>
       </c>
@@ -21350,12 +21350,12 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.5" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -21805,13 +21805,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
-    <col min="6" max="6" width="61.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" customWidth="1"/>
+    <col min="6" max="6" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -21965,14 +21965,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22394,12 +22394,12 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22483,7 +22483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+    <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="72" t="s">
         <v>2045</v>
       </c>
@@ -22862,14 +22862,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.5" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="170.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="170.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -23309,13 +23309,13 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -23382,7 +23382,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="40">
+    <row r="8" spans="1:6" ht="48.75">
       <c r="A8" s="75" t="s">
         <v>10</v>
       </c>
@@ -23734,15 +23734,15 @@
       <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.1640625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" style="32" customWidth="1"/>
     <col min="3" max="3" width="56" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="32" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" style="32" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" style="32" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" style="32"/>
+    <col min="4" max="4" width="17.7109375" style="32" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="32" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="32" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1">
@@ -24718,13 +24718,13 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -24806,7 +24806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+    <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="69" t="s">
         <v>2023</v>
       </c>
@@ -25156,13 +25156,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -25580,13 +25580,13 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26096,13 +26096,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26186,7 +26186,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+    <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="69" t="s">
         <v>2095</v>
       </c>
@@ -26556,13 +26556,13 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="61.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26646,7 +26646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16">
+    <row r="10" spans="1:5">
       <c r="A10" s="44" t="s">
         <v>1775</v>
       </c>
@@ -26672,7 +26672,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="16">
+    <row r="12" spans="1:5">
       <c r="A12" s="46" t="s">
         <v>1777</v>
       </c>
@@ -26685,7 +26685,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="16">
+    <row r="13" spans="1:5">
       <c r="A13" s="46" t="s">
         <v>1553</v>
       </c>
@@ -26698,7 +26698,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="16">
+    <row r="14" spans="1:5">
       <c r="A14" s="46" t="s">
         <v>1417</v>
       </c>
@@ -26711,7 +26711,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="16">
+    <row r="15" spans="1:5">
       <c r="A15" s="46" t="s">
         <v>1546</v>
       </c>
@@ -26724,7 +26724,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="16">
+    <row r="16" spans="1:5">
       <c r="A16" s="46" t="s">
         <v>1778</v>
       </c>
@@ -26737,7 +26737,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="16">
+    <row r="17" spans="1:5">
       <c r="A17" s="47" t="s">
         <v>1779</v>
       </c>
@@ -26750,7 +26750,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="16">
+    <row r="18" spans="1:5">
       <c r="A18" s="48" t="s">
         <v>1780</v>
       </c>
@@ -26763,7 +26763,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="16">
+    <row r="19" spans="1:5">
       <c r="A19" s="46" t="s">
         <v>1781</v>
       </c>
@@ -26776,7 +26776,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="16">
+    <row r="20" spans="1:5">
       <c r="A20" s="46" t="s">
         <v>1782</v>
       </c>
@@ -26789,7 +26789,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="16">
+    <row r="21" spans="1:5">
       <c r="A21" s="46" t="s">
         <v>1783</v>
       </c>
@@ -27060,12 +27060,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="163.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="163.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="52" customFormat="1">
@@ -27286,12 +27286,12 @@
       <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="154.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="154.85546875" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -27802,15 +27802,15 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" style="52" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="52" customWidth="1"/>
-    <col min="4" max="4" width="39.5" style="52" customWidth="1"/>
-    <col min="5" max="5" width="88.6640625" style="52" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" style="52" customWidth="1"/>
-    <col min="7" max="16384" width="11.5" style="52"/>
+    <col min="1" max="1" width="21.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="52" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="52" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="52" customWidth="1"/>
+    <col min="5" max="5" width="88.7109375" style="52" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" style="52" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27905,7 +27905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6">
       <c r="A10" s="60" t="s">
         <v>1800</v>
       </c>
@@ -27920,7 +27920,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16">
+    <row r="11" spans="1:6">
       <c r="A11" s="46" t="s">
         <v>1804</v>
       </c>
@@ -27931,7 +27931,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16">
+    <row r="12" spans="1:6">
       <c r="A12" s="46" t="s">
         <v>1807</v>
       </c>
@@ -27945,7 +27945,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16">
+    <row r="13" spans="1:6">
       <c r="A13" s="46" t="s">
         <v>1811</v>
       </c>
@@ -27960,7 +27960,7 @@
         <v>1814</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16">
+    <row r="14" spans="1:6">
       <c r="A14" s="60" t="s">
         <v>1815</v>
       </c>
@@ -27971,7 +27971,7 @@
         <v>1817</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16">
+    <row r="15" spans="1:6">
       <c r="A15" s="46" t="s">
         <v>1818</v>
       </c>
@@ -27983,7 +27983,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16">
+    <row r="16" spans="1:6">
       <c r="A16" s="60" t="s">
         <v>1820</v>
       </c>
@@ -27995,7 +27995,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16">
+    <row r="17" spans="1:6">
       <c r="A17" s="60" t="s">
         <v>1589</v>
       </c>
@@ -28010,7 +28010,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16">
+    <row r="18" spans="1:6">
       <c r="A18" s="60" t="s">
         <v>1826</v>
       </c>
@@ -28018,7 +28018,7 @@
         <v>1827</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16">
+    <row r="19" spans="1:6">
       <c r="A19" s="60" t="s">
         <v>1828</v>
       </c>
@@ -28026,7 +28026,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16">
+    <row r="20" spans="1:6">
       <c r="A20" s="60" t="s">
         <v>1830</v>
       </c>
@@ -28034,7 +28034,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16">
+    <row r="21" spans="1:6">
       <c r="A21" s="60" t="s">
         <v>1832</v>
       </c>
@@ -28042,7 +28042,7 @@
         <v>1833</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16">
+    <row r="22" spans="1:6">
       <c r="A22" s="46" t="s">
         <v>1834</v>
       </c>
@@ -28057,7 +28057,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16">
+    <row r="23" spans="1:6">
       <c r="A23" s="46" t="s">
         <v>1838</v>
       </c>
@@ -28072,7 +28072,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16">
+    <row r="24" spans="1:6">
       <c r="A24" s="46" t="s">
         <v>1842</v>
       </c>
@@ -28087,7 +28087,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16">
+    <row r="25" spans="1:6">
       <c r="A25" s="60" t="s">
         <v>1846</v>
       </c>
@@ -28098,7 +28098,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16">
+    <row r="26" spans="1:6">
       <c r="A26" s="60" t="s">
         <v>1849</v>
       </c>
@@ -28270,13 +28270,13 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="74" customWidth="1"/>
-    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -28371,7 +28371,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16">
+    <row r="10" spans="1:6">
       <c r="A10" s="60" t="s">
         <v>2063</v>
       </c>
@@ -28385,7 +28385,7 @@
       </c>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" ht="16">
+    <row r="11" spans="1:6">
       <c r="A11" s="46" t="s">
         <v>2064</v>
       </c>
@@ -28399,7 +28399,7 @@
       </c>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" ht="16">
+    <row r="12" spans="1:6">
       <c r="A12" s="46" t="s">
         <v>2065</v>
       </c>
@@ -28413,7 +28413,7 @@
       </c>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" ht="16">
+    <row r="13" spans="1:6">
       <c r="A13" s="46" t="s">
         <v>2066</v>
       </c>
@@ -28696,11 +28696,11 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29175,14 +29175,14 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" customWidth="1"/>
-    <col min="5" max="5" width="47.83203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -29267,7 +29267,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60">
+    <row r="10" spans="1:6" ht="64.5">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -29293,7 +29293,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -29307,7 +29307,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -29321,7 +29321,7 @@
       </c>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -29334,7 +29334,7 @@
       </c>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -29362,7 +29362,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="26.25">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -29388,7 +29388,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="26.25">
       <c r="A19" s="2" t="s">
         <v>43</v>
       </c>
@@ -29403,7 +29403,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
@@ -29429,7 +29429,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6" ht="39">
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
@@ -29443,7 +29443,7 @@
       </c>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6" ht="30">
+    <row r="23" spans="1:6" ht="39">
       <c r="A23" s="2" t="s">
         <v>55</v>
       </c>
@@ -29468,7 +29468,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" ht="30">
+    <row r="25" spans="1:6" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>60</v>
       </c>
@@ -29482,7 +29482,7 @@
       </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" ht="30">
+    <row r="26" spans="1:6" ht="26.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -29496,7 +29496,7 @@
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="30">
+    <row r="27" spans="1:6" ht="26.25">
       <c r="A27" s="2" t="s">
         <v>66</v>
       </c>
@@ -29510,7 +29510,7 @@
       </c>
       <c r="F27" s="10"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>69</v>
       </c>
@@ -29547,7 +29547,7 @@
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:6" ht="60">
+    <row r="31" spans="1:6" ht="51.75">
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>
@@ -29561,7 +29561,7 @@
       </c>
       <c r="F31" s="10"/>
     </row>
-    <row r="32" spans="1:6" ht="30">
+    <row r="32" spans="1:6" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>79</v>
       </c>
@@ -29600,7 +29600,7 @@
       </c>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="26.25">
       <c r="A35" s="2" t="s">
         <v>87</v>
       </c>
@@ -29626,7 +29626,7 @@
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" ht="120">
+    <row r="37" spans="1:6" ht="102.75">
       <c r="A37" s="2" t="s">
         <v>92</v>
       </c>
@@ -29640,7 +29640,7 @@
       </c>
       <c r="F37" s="10"/>
     </row>
-    <row r="38" spans="1:6" ht="30">
+    <row r="38" spans="1:6" ht="26.25">
       <c r="A38" s="2" t="s">
         <v>95</v>
       </c>
@@ -29654,7 +29654,7 @@
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" ht="30">
+    <row r="39" spans="1:6" ht="39">
       <c r="A39" s="2" t="s">
         <v>98</v>
       </c>
@@ -29679,7 +29679,7 @@
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" ht="30">
+    <row r="41" spans="1:6" ht="39">
       <c r="A41" s="2" t="s">
         <v>103</v>
       </c>
@@ -29693,7 +29693,7 @@
       </c>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" ht="26.25">
       <c r="A42" s="2" t="s">
         <v>106</v>
       </c>
@@ -29707,7 +29707,7 @@
       </c>
       <c r="F42" s="10"/>
     </row>
-    <row r="43" spans="1:6" ht="30">
+    <row r="43" spans="1:6" ht="39">
       <c r="A43" s="2" t="s">
         <v>109</v>
       </c>
@@ -29732,7 +29732,7 @@
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:6" ht="45">
+    <row r="45" spans="1:6" ht="39">
       <c r="A45" s="2" t="s">
         <v>114</v>
       </c>
@@ -29831,7 +29831,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="26.25">
       <c r="A53" s="2" t="s">
         <v>132</v>
       </c>
@@ -29845,7 +29845,7 @@
       </c>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" spans="1:6" ht="60">
+    <row r="54" spans="1:6" ht="64.5">
       <c r="A54" s="2" t="s">
         <v>135</v>
       </c>
@@ -30218,7 +30218,7 @@
       <c r="E84" s="10"/>
       <c r="F84" s="10"/>
     </row>
-    <row r="85" spans="1:6" ht="45">
+    <row r="85" spans="1:6" ht="39">
       <c r="A85" s="2" t="s">
         <v>201</v>
       </c>
@@ -30244,7 +30244,7 @@
       <c r="E86" s="10"/>
       <c r="F86" s="10"/>
     </row>
-    <row r="87" spans="1:6" ht="135">
+    <row r="87" spans="1:6" ht="128.25">
       <c r="A87" s="2" t="s">
         <v>206</v>
       </c>
@@ -30270,7 +30270,7 @@
       <c r="E88" s="10"/>
       <c r="F88" s="10"/>
     </row>
-    <row r="89" spans="1:6" ht="60">
+    <row r="89" spans="1:6" ht="51.75">
       <c r="A89" s="2" t="s">
         <v>199</v>
       </c>
@@ -30283,7 +30283,7 @@
       </c>
       <c r="F89" s="10"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" ht="26.25">
       <c r="A90" s="2" t="s">
         <v>201</v>
       </c>
@@ -30323,7 +30323,7 @@
       <c r="E92" s="10"/>
       <c r="F92" s="10"/>
     </row>
-    <row r="93" spans="1:6" ht="30">
+    <row r="93" spans="1:6" ht="26.25">
       <c r="A93" s="2" t="s">
         <v>217</v>
       </c>
@@ -30495,7 +30495,7 @@
       <c r="E106" s="10"/>
       <c r="F106" s="10"/>
     </row>
-    <row r="107" spans="1:6" ht="30">
+    <row r="107" spans="1:6" ht="26.25">
       <c r="A107" s="2" t="s">
         <v>248</v>
       </c>
@@ -30509,7 +30509,7 @@
       </c>
       <c r="F107" s="10"/>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" ht="26.25">
       <c r="A108" s="2" t="s">
         <v>251</v>
       </c>
@@ -30633,7 +30633,7 @@
       <c r="E117" s="10"/>
       <c r="F117" s="10"/>
     </row>
-    <row r="118" spans="1:6" ht="30">
+    <row r="118" spans="1:6" ht="26.25">
       <c r="A118" s="2" t="s">
         <v>274</v>
       </c>
@@ -30647,7 +30647,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" ht="26.25">
       <c r="A119" s="2" t="s">
         <v>277</v>
       </c>
@@ -30660,7 +30660,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="45">
+    <row r="120" spans="1:6" ht="39">
       <c r="A120" s="2" t="s">
         <v>280</v>
       </c>
@@ -30698,7 +30698,7 @@
       <c r="E122" s="10"/>
       <c r="F122" s="10"/>
     </row>
-    <row r="123" spans="1:6" ht="45">
+    <row r="123" spans="1:6" ht="39">
       <c r="A123" s="2" t="s">
         <v>287</v>
       </c>
@@ -30759,7 +30759,7 @@
       <c r="E127" s="10"/>
       <c r="F127" s="10"/>
     </row>
-    <row r="128" spans="1:6" ht="45">
+    <row r="128" spans="1:6" ht="39">
       <c r="A128" s="2" t="s">
         <v>298</v>
       </c>
@@ -30895,7 +30895,7 @@
       <c r="E138" s="10"/>
       <c r="F138" s="10"/>
     </row>
-    <row r="139" spans="1:6" ht="30">
+    <row r="139" spans="1:6" ht="26.25">
       <c r="A139" s="2" t="s">
         <v>323</v>
       </c>
@@ -30921,7 +30921,7 @@
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
     </row>
-    <row r="141" spans="1:6" ht="30">
+    <row r="141" spans="1:6" ht="26.25">
       <c r="A141" s="2" t="s">
         <v>328</v>
       </c>
@@ -30935,7 +30935,7 @@
       </c>
       <c r="F141" s="10"/>
     </row>
-    <row r="142" spans="1:6" ht="30">
+    <row r="142" spans="1:6" ht="26.25">
       <c r="A142" s="2" t="s">
         <v>329</v>
       </c>
@@ -30949,7 +30949,7 @@
       </c>
       <c r="F142" s="10"/>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" ht="26.25">
       <c r="A143" s="2" t="s">
         <v>330</v>
       </c>
@@ -30963,7 +30963,7 @@
       </c>
       <c r="F143" s="10"/>
     </row>
-    <row r="144" spans="1:6" ht="30">
+    <row r="144" spans="1:6" ht="26.25">
       <c r="A144" s="2" t="s">
         <v>331</v>
       </c>
@@ -30992,7 +30992,7 @@
       </c>
       <c r="F145" s="10"/>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" ht="26.25">
       <c r="A146" s="2" t="s">
         <v>334</v>
       </c>
@@ -31006,7 +31006,7 @@
       </c>
       <c r="F146" s="10"/>
     </row>
-    <row r="147" spans="1:6" ht="30">
+    <row r="147" spans="1:6" ht="39">
       <c r="A147" s="2" t="s">
         <v>335</v>
       </c>
@@ -31020,7 +31020,7 @@
       </c>
       <c r="F147" s="10"/>
     </row>
-    <row r="148" spans="1:6" ht="30">
+    <row r="148" spans="1:6" ht="39">
       <c r="A148" s="2" t="s">
         <v>336</v>
       </c>
@@ -31034,7 +31034,7 @@
       </c>
       <c r="F148" s="10"/>
     </row>
-    <row r="149" spans="1:6" ht="30">
+    <row r="149" spans="1:6" ht="26.25">
       <c r="A149" s="2" t="s">
         <v>337</v>
       </c>
@@ -31047,7 +31047,7 @@
       </c>
       <c r="F149" s="10"/>
     </row>
-    <row r="150" spans="1:6" ht="30">
+    <row r="150" spans="1:6" ht="26.25">
       <c r="A150" s="2" t="s">
         <v>338</v>
       </c>
@@ -31061,7 +31061,7 @@
       </c>
       <c r="F150" s="10"/>
     </row>
-    <row r="151" spans="1:6" ht="30">
+    <row r="151" spans="1:6" ht="26.25">
       <c r="A151" s="2" t="s">
         <v>339</v>
       </c>
@@ -31193,7 +31193,7 @@
       <c r="E161" s="10"/>
       <c r="F161" s="10"/>
     </row>
-    <row r="162" spans="1:6" ht="30">
+    <row r="162" spans="1:6" ht="39">
       <c r="A162" s="2" t="s">
         <v>360</v>
       </c>
@@ -31207,7 +31207,7 @@
       </c>
       <c r="F162" s="10"/>
     </row>
-    <row r="163" spans="1:6" ht="45">
+    <row r="163" spans="1:6" ht="39">
       <c r="A163" s="2" t="s">
         <v>363</v>
       </c>
@@ -31221,7 +31221,7 @@
       </c>
       <c r="F163" s="10"/>
     </row>
-    <row r="164" spans="1:6" ht="45">
+    <row r="164" spans="1:6" ht="39">
       <c r="A164" s="2" t="s">
         <v>366</v>
       </c>
@@ -31272,7 +31272,7 @@
       <c r="E167" s="10"/>
       <c r="F167" s="10"/>
     </row>
-    <row r="168" spans="1:6" ht="30">
+    <row r="168" spans="1:6" ht="26.25">
       <c r="A168" s="2" t="s">
         <v>376</v>
       </c>
@@ -31489,7 +31489,7 @@
       <c r="E185" s="10"/>
       <c r="F185" s="10"/>
     </row>
-    <row r="186" spans="1:6" ht="30">
+    <row r="186" spans="1:6" ht="26.25">
       <c r="A186" s="2" t="s">
         <v>413</v>
       </c>
@@ -31625,7 +31625,7 @@
       </c>
       <c r="F196" s="10"/>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:6" ht="26.25">
       <c r="A197" s="2" t="s">
         <v>438</v>
       </c>
@@ -31725,7 +31725,7 @@
       <c r="E204" s="10"/>
       <c r="F204" s="10"/>
     </row>
-    <row r="205" spans="1:6" ht="30">
+    <row r="205" spans="1:6" ht="26.25">
       <c r="A205" s="2" t="s">
         <v>457</v>
       </c>
@@ -31751,7 +31751,7 @@
       <c r="E206" s="10"/>
       <c r="F206" s="10"/>
     </row>
-    <row r="207" spans="1:6" ht="30">
+    <row r="207" spans="1:6" ht="26.25">
       <c r="A207" s="2" t="s">
         <v>462</v>
       </c>
@@ -31849,7 +31849,7 @@
       <c r="E214" s="10"/>
       <c r="F214" s="10"/>
     </row>
-    <row r="215" spans="1:6" ht="30">
+    <row r="215" spans="1:6" ht="26.25">
       <c r="A215" s="2" t="s">
         <v>480</v>
       </c>
@@ -32670,7 +32670,7 @@
       <c r="E282" s="10"/>
       <c r="F282" s="10"/>
     </row>
-    <row r="283" spans="1:6" ht="30">
+    <row r="283" spans="1:6" ht="26.25">
       <c r="A283" s="2" t="s">
         <v>625</v>
       </c>
@@ -32684,7 +32684,7 @@
       </c>
       <c r="F283" s="10"/>
     </row>
-    <row r="284" spans="1:6" ht="30">
+    <row r="284" spans="1:6" ht="26.25">
       <c r="A284" s="2" t="s">
         <v>628</v>
       </c>
@@ -33030,14 +33030,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -35751,12 +35751,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="26.5" style="8" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -35767,7 +35767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="24.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -35835,7 +35835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="39">
       <c r="A10" s="2" t="s">
         <v>1069</v>
       </c>
@@ -35857,7 +35857,7 @@
       <c r="C11" s="10"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="26.25">
       <c r="A12" s="2" t="s">
         <v>1074</v>
       </c>
@@ -35867,7 +35867,7 @@
       <c r="C12" s="10"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4" ht="39">
       <c r="A13" s="2" t="s">
         <v>1076</v>
       </c>
@@ -35877,7 +35877,7 @@
       <c r="C13" s="10"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="26.25">
       <c r="A14" s="2" t="s">
         <v>1078</v>
       </c>
@@ -35887,7 +35887,7 @@
       <c r="C14" s="10"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1080</v>
       </c>
@@ -35897,7 +35897,7 @@
       <c r="C15" s="10"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="30">
+    <row r="16" spans="1:4" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1082</v>
       </c>
@@ -35909,7 +35909,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="45">
+    <row r="17" spans="1:4" ht="39">
       <c r="A17" s="2" t="s">
         <v>1085</v>
       </c>
@@ -35921,7 +35921,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="30">
+    <row r="18" spans="1:4" ht="39">
       <c r="A18" s="2" t="s">
         <v>1088</v>
       </c>
@@ -35931,7 +35931,7 @@
       <c r="C18" s="10"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="45">
+    <row r="19" spans="1:4" ht="39">
       <c r="A19" s="2" t="s">
         <v>1090</v>
       </c>
@@ -35941,7 +35941,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="30">
+    <row r="20" spans="1:4" ht="26.25">
       <c r="A20" s="2" t="s">
         <v>1092</v>
       </c>
@@ -35951,7 +35951,7 @@
       <c r="C20" s="10"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="26.25">
       <c r="A21" s="2" t="s">
         <v>1094</v>
       </c>
@@ -35961,7 +35961,7 @@
       <c r="C21" s="10"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="26.25">
       <c r="A22" s="2" t="s">
         <v>1096</v>
       </c>
@@ -35991,7 +35991,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="26.25">
       <c r="A25" s="2" t="s">
         <v>1102</v>
       </c>
@@ -36021,7 +36021,7 @@
       <c r="C27" s="10"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="30">
+    <row r="28" spans="1:4" ht="26.25">
       <c r="A28" s="2" t="s">
         <v>1107</v>
       </c>
@@ -36033,7 +36033,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="30">
+    <row r="29" spans="1:4" ht="26.25">
       <c r="A29" s="2" t="s">
         <v>1110</v>
       </c>
@@ -36045,7 +36045,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="30">
+    <row r="30" spans="1:4" ht="26.25">
       <c r="A30" s="2" t="s">
         <v>1113</v>
       </c>
@@ -36067,7 +36067,7 @@
       <c r="C31" s="10"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="30">
+    <row r="32" spans="1:4" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1118</v>
       </c>
@@ -36079,7 +36079,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="30">
+    <row r="33" spans="1:4" ht="39">
       <c r="A33" s="2" t="s">
         <v>1121</v>
       </c>
@@ -36091,7 +36091,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="26.25">
       <c r="A34" s="2" t="s">
         <v>1124</v>
       </c>
@@ -36103,7 +36103,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="135">
+    <row r="35" spans="1:4" ht="128.25">
       <c r="A35" s="2" t="s">
         <v>1127</v>
       </c>
@@ -36115,7 +36115,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" ht="135">
+    <row r="36" spans="1:4" ht="128.25">
       <c r="A36" s="2" t="s">
         <v>1130</v>
       </c>
@@ -36199,7 +36199,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="30">
+    <row r="44" spans="1:4" ht="26.25">
       <c r="A44" s="2" t="s">
         <v>1147</v>
       </c>
@@ -36211,7 +36211,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="30">
+    <row r="45" spans="1:4" ht="26.25">
       <c r="A45" s="2" t="s">
         <v>1150</v>
       </c>
@@ -36221,7 +36221,7 @@
       <c r="C45" s="10"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="75">
+    <row r="46" spans="1:4" ht="77.25">
       <c r="A46" s="2" t="s">
         <v>1152</v>
       </c>
@@ -36248,13 +36248,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="39.5" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.1640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -36371,7 +36371,7 @@
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="26.25">
       <c r="A13" s="2" t="s">
         <v>1164</v>
       </c>
@@ -36395,7 +36395,7 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="26.25">
       <c r="A15" s="2" t="s">
         <v>1169</v>
       </c>
@@ -36408,7 +36408,7 @@
       </c>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="26.25">
       <c r="A16" s="2" t="s">
         <v>1172</v>
       </c>
@@ -36432,7 +36432,7 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" ht="40">
+    <row r="18" spans="1:5" ht="48.75">
       <c r="A18" s="2" t="s">
         <v>1177</v>
       </c>
@@ -36445,7 +36445,7 @@
       </c>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" ht="60">
+    <row r="19" spans="1:5" ht="64.5">
       <c r="A19" s="2" t="s">
         <v>1180</v>
       </c>
@@ -36594,7 +36594,7 @@
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="26.25">
       <c r="A32" s="2" t="s">
         <v>1209</v>
       </c>
@@ -36607,7 +36607,7 @@
       </c>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" spans="1:5" ht="30">
+    <row r="33" spans="1:5" ht="26.25">
       <c r="A33" s="2" t="s">
         <v>1212</v>
       </c>
@@ -36694,7 +36694,7 @@
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
     </row>
-    <row r="40" spans="1:5" ht="45">
+    <row r="40" spans="1:5" ht="51.75">
       <c r="A40" s="2" t="s">
         <v>1231</v>
       </c>
@@ -36731,7 +36731,7 @@
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
     </row>
-    <row r="43" spans="1:5" ht="30">
+    <row r="43" spans="1:5" ht="26.25">
       <c r="A43" s="2" t="s">
         <v>1239</v>
       </c>
@@ -36744,7 +36744,7 @@
       </c>
       <c r="E43" s="10"/>
     </row>
-    <row r="44" spans="1:5" ht="30">
+    <row r="44" spans="1:5" ht="39">
       <c r="A44" s="2" t="s">
         <v>1240</v>
       </c>
@@ -36803,7 +36803,7 @@
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
     </row>
-    <row r="49" spans="1:5" ht="30">
+    <row r="49" spans="1:5" ht="26.25">
       <c r="A49" s="2" t="s">
         <v>1252</v>
       </c>
@@ -36838,7 +36838,7 @@
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
     </row>
-    <row r="52" spans="1:5" ht="30">
+    <row r="52" spans="1:5" ht="26.25">
       <c r="A52" s="2" t="s">
         <v>1259</v>
       </c>
@@ -36932,7 +36932,7 @@
       </c>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:5" ht="45">
+    <row r="60" spans="1:5" ht="39">
       <c r="A60" s="2" t="s">
         <v>1278</v>
       </c>
@@ -36970,17 +36970,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE84B961-E28E-4D68-86C8-B0BB636BCA52}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -37064,7 +37064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="32" customFormat="1" ht="16">
+    <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="69" t="s">
         <v>2082</v>
       </c>
@@ -37845,15 +37845,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -37905,6 +37896,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1BDBD4-E316-45AC-920A-A6692C88096C}">
   <ds:schemaRefs>
@@ -37926,27 +37926,27 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.08.08 11:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1188" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{739887B1-65CF-401B-A28D-6954AE777C11}"/>
+  <xr:revisionPtr revIDLastSave="1248" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1B3EBB9-F032-40D7-8986-D047B67A78F5}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="150" windowWidth="24300" windowHeight="14370" tabRatio="877" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -43,16 +43,17 @@
     <sheet name="Type de ressource" sheetId="36" r:id="rId28"/>
     <sheet name="Type de vecteurs" sheetId="37" r:id="rId29"/>
     <sheet name="Niveau de prise en charge" sheetId="31" r:id="rId30"/>
-    <sheet name="Type de devenir du patient" sheetId="35" r:id="rId31"/>
+    <sheet name="#Type de devenir du patient" sheetId="35" r:id="rId31"/>
     <sheet name="Type de destination" sheetId="61" r:id="rId32"/>
     <sheet name="Effet à obtenir" sheetId="10" r:id="rId33"/>
     <sheet name="Cadre conventionnel" sheetId="43" r:id="rId34"/>
     <sheet name="Delai d'intervention souhaite" sheetId="40" r:id="rId35"/>
-    <sheet name="Statut du vecteur" sheetId="42" r:id="rId36"/>
+    <sheet name="Annulation DR" sheetId="62" r:id="rId36"/>
     <sheet name="Reponse demande ressources" sheetId="59" r:id="rId37"/>
+    <sheet name="Statut du vecteur" sheetId="42" r:id="rId38"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$2:$L$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$2:$L$39</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3050" uniqueCount="2102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3070" uniqueCount="2110">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -6582,12 +6583,36 @@
   <si>
     <t>Décrit le délai d'intervention attendu ou souhaité pour une ressource ou un vecteur.</t>
   </si>
+  <si>
+    <t>Ressource engagée</t>
+  </si>
+  <si>
+    <t>resourcesRequest</t>
+  </si>
+  <si>
+    <t>ANNULEE</t>
+  </si>
+  <si>
+    <t>La demande de concours est annulée dans son intégralité</t>
+  </si>
+  <si>
+    <t>STATUS_DR</t>
+  </si>
+  <si>
+    <t>Annulation de la demande de ressources</t>
+  </si>
+  <si>
+    <t>Décrit l'état de l'annulation de demande de ressources</t>
+  </si>
+  <si>
+    <t>Etat annulation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37">
+  <fonts count="44">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6813,12 +6838,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
@@ -6829,6 +6848,46 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -6960,7 +7019,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7099,9 +7158,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -7115,10 +7171,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7128,6 +7184,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="42" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60 % - Accent5" xfId="1" builtinId="48"/>
@@ -7135,7 +7204,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
-  <dxfs count="196">
+  <dxfs count="187">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7154,13 +7230,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7193,114 +7262,134 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10684,342 +10773,364 @@
 </styleSheet>
 </file>
 
+<file path=xl/namedSheetViews/namedSheetView1.xml><?xml version="1.0" encoding="utf-8"?>
+<namedSheetViews xmlns="http://schemas.microsoft.com/office/spreadsheetml/2019/namedsheetviews" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8CBD23D8-3CB7-491B-B00E-5486B907388F}" name="Table13611123111813" displayName="Table13611123111813" ref="A9:E55" totalsRowShown="0" headerRowDxfId="195" dataDxfId="194">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{8CBD23D8-3CB7-491B-B00E-5486B907388F}" name="Table13611123111813" displayName="Table13611123111813" ref="A9:E55" totalsRowShown="0" headerRowDxfId="186" dataDxfId="185">
   <autoFilter ref="A9:E55" xr:uid="{8CBD23D8-3CB7-491B-B00E-5486B907388F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E0E4BEF8-D213-4F3F-97E1-4EF95756B90E}" name="Code" dataDxfId="193"/>
-    <tableColumn id="2" xr3:uid="{3431D095-AE1F-4ABA-9D63-EC4DB501B423}" name="Libellé niveau 1" dataDxfId="192"/>
-    <tableColumn id="5" xr3:uid="{97BD8D92-80A6-4F7F-9379-59C2B46726A3}" name="Libellé niveau 2" dataDxfId="191"/>
-    <tableColumn id="3" xr3:uid="{127B5052-742A-4FFC-ABFE-8F7750C796F5}" name="Description" dataDxfId="190"/>
-    <tableColumn id="4" xr3:uid="{166EA99C-D40A-41CA-8E35-76670A47C2FF}" name="Commentaire" dataDxfId="189"/>
+    <tableColumn id="1" xr3:uid="{E0E4BEF8-D213-4F3F-97E1-4EF95756B90E}" name="Code" dataDxfId="184"/>
+    <tableColumn id="2" xr3:uid="{3431D095-AE1F-4ABA-9D63-EC4DB501B423}" name="Libellé niveau 1" dataDxfId="183"/>
+    <tableColumn id="5" xr3:uid="{97BD8D92-80A6-4F7F-9379-59C2B46726A3}" name="Libellé niveau 2" dataDxfId="182"/>
+    <tableColumn id="3" xr3:uid="{127B5052-742A-4FFC-ABFE-8F7750C796F5}" name="Description" dataDxfId="181"/>
+    <tableColumn id="4" xr3:uid="{166EA99C-D40A-41CA-8E35-76670A47C2FF}" name="Commentaire" dataDxfId="180"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{823C2F13-948D-4974-9C9C-1AD390776B68}" name="Table136111235" displayName="Table136111235" ref="A9:E55" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{823C2F13-948D-4974-9C9C-1AD390776B68}" name="Table136111235" displayName="Table136111235" ref="A9:E55" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
   <autoFilter ref="A9:E55" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C65B8274-E954-4CBF-8B3B-6DACFEF3D09F}" name="Code" dataDxfId="129"/>
-    <tableColumn id="2" xr3:uid="{84ACD83D-893A-4B00-89F4-93AEE374E815}" name="Libellé niveau 1" dataDxfId="128"/>
-    <tableColumn id="5" xr3:uid="{E64A61DE-4BB8-4C3E-B7B9-726F1A447BD7}" name="Libellé niveau 2" dataDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{B1043381-4D28-4782-8747-DA98FAFD4504}" name="Description" dataDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{DF53D3E2-A057-4D40-BE92-9E7F311D817E}" name="Commentaire" dataDxfId="125"/>
+    <tableColumn id="1" xr3:uid="{C65B8274-E954-4CBF-8B3B-6DACFEF3D09F}" name="Code" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{84ACD83D-893A-4B00-89F4-93AEE374E815}" name="Libellé niveau 1" dataDxfId="119"/>
+    <tableColumn id="5" xr3:uid="{E64A61DE-4BB8-4C3E-B7B9-726F1A447BD7}" name="Libellé niveau 2" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{B1043381-4D28-4782-8747-DA98FAFD4504}" name="Description" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{DF53D3E2-A057-4D40-BE92-9E7F311D817E}" name="Commentaire" dataDxfId="116"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C3C96985-E377-4F48-BA27-F14A223DCC95}" name="Table1361112311" displayName="Table1361112311" ref="A9:E55" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C3C96985-E377-4F48-BA27-F14A223DCC95}" name="Table1361112311" displayName="Table1361112311" ref="A9:E55" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114">
   <autoFilter ref="A9:E55" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{888FD29E-2275-4F75-ADD9-E04935713E5C}" name="Code" dataDxfId="122"/>
-    <tableColumn id="2" xr3:uid="{49B955E3-E63C-42E4-A3D1-7E9F8878B275}" name="Libellé niveau 1" dataDxfId="121"/>
-    <tableColumn id="5" xr3:uid="{C2281989-9EA7-462C-90E1-C689C38F32FC}" name="Libellé niveau 2" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{693429A6-E746-47FF-A745-B1D8AFE53E56}" name="Description" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{91A2BB1F-5F3A-47DF-86F4-E97AB53ADD89}" name="Commentaire" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{888FD29E-2275-4F75-ADD9-E04935713E5C}" name="Code" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{49B955E3-E63C-42E4-A3D1-7E9F8878B275}" name="Libellé niveau 1" dataDxfId="112"/>
+    <tableColumn id="5" xr3:uid="{C2281989-9EA7-462C-90E1-C689C38F32FC}" name="Libellé niveau 2" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{693429A6-E746-47FF-A745-B1D8AFE53E56}" name="Description" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{91A2BB1F-5F3A-47DF-86F4-E97AB53ADD89}" name="Commentaire" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FCFF9977-C677-479A-85FC-B06533A394C5}" name="Table136111231115" displayName="Table136111231115" ref="A9:E55" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FCFF9977-C677-479A-85FC-B06533A394C5}" name="Table136111231115" displayName="Table136111231115" ref="A9:E55" totalsRowShown="0" headerRowDxfId="108" dataDxfId="107">
   <autoFilter ref="A9:E55" xr:uid="{FCFF9977-C677-479A-85FC-B06533A394C5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4A576D64-7823-4B55-BF7E-F5CB76EA3E3E}" name="Code" dataDxfId="115"/>
-    <tableColumn id="2" xr3:uid="{CBBE7E46-1033-4C8A-AE13-078E2F5F30BD}" name="Libellé niveau 1" dataDxfId="114"/>
-    <tableColumn id="5" xr3:uid="{294792C7-CE9D-42DF-96E0-1035ACCFF003}" name="Libellé niveau 2" dataDxfId="113"/>
-    <tableColumn id="3" xr3:uid="{CA095527-FAAE-4845-8EC8-35CF34674BD1}" name="Description" dataDxfId="112"/>
-    <tableColumn id="4" xr3:uid="{D599D956-3DCB-49BC-91E2-9495FEFE3A0D}" name="Commentaire" dataDxfId="111"/>
+    <tableColumn id="1" xr3:uid="{4A576D64-7823-4B55-BF7E-F5CB76EA3E3E}" name="Code" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{CBBE7E46-1033-4C8A-AE13-078E2F5F30BD}" name="Libellé niveau 1" dataDxfId="105"/>
+    <tableColumn id="5" xr3:uid="{294792C7-CE9D-42DF-96E0-1035ACCFF003}" name="Libellé niveau 2" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{CA095527-FAAE-4845-8EC8-35CF34674BD1}" name="Description" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{D599D956-3DCB-49BC-91E2-9495FEFE3A0D}" name="Commentaire" dataDxfId="102"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{2A2AD6DF-70D1-4862-8B6B-3EA16EA226E8}" name="Table136111231116" displayName="Table136111231116" ref="A9:E55" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{2A2AD6DF-70D1-4862-8B6B-3EA16EA226E8}" name="Table136111231116" displayName="Table136111231116" ref="A9:E55" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
   <autoFilter ref="A9:E55" xr:uid="{2A2AD6DF-70D1-4862-8B6B-3EA16EA226E8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DAD71D71-B89C-4E24-B32B-350EE5ECD2D7}" name="Code" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{9814D279-C1B5-40C4-8A18-1E240B57B85C}" name="Libellé niveau 1" dataDxfId="107"/>
-    <tableColumn id="5" xr3:uid="{4BFAD3EE-A659-4BE0-8AAB-3469FECB5643}" name="Libellé niveau 2" dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{96657DDA-8D57-40A2-B54B-E4AC1B489A0D}" name="Description" dataDxfId="105"/>
-    <tableColumn id="4" xr3:uid="{12AB4119-159D-434F-85AA-2B89F1A63856}" name="Commentaire" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{DAD71D71-B89C-4E24-B32B-350EE5ECD2D7}" name="Code" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{9814D279-C1B5-40C4-8A18-1E240B57B85C}" name="Libellé niveau 1" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{4BFAD3EE-A659-4BE0-8AAB-3469FECB5643}" name="Libellé niveau 2" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{96657DDA-8D57-40A2-B54B-E4AC1B489A0D}" name="Description" dataDxfId="96"/>
+    <tableColumn id="4" xr3:uid="{12AB4119-159D-434F-85AA-2B89F1A63856}" name="Commentaire" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{4D2E6F8C-DACC-4A26-AF1C-27A96B5B0CEB}" name="Table136111231117" displayName="Table136111231117" ref="A9:E55" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{4D2E6F8C-DACC-4A26-AF1C-27A96B5B0CEB}" name="Table136111231117" displayName="Table136111231117" ref="A9:E55" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
   <autoFilter ref="A9:E55" xr:uid="{4D2E6F8C-DACC-4A26-AF1C-27A96B5B0CEB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{73A28F86-A0B9-4591-B8D2-0160E457A112}" name="Code" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{F7506F92-2DA9-4093-9FDA-9893B7117480}" name="Libellé niveau 1" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{87CA381F-E725-4FBA-9AD1-5C61C6B110A7}" name="Libellé niveau 2" dataDxfId="99"/>
-    <tableColumn id="3" xr3:uid="{39D920FE-DBE6-4BFE-9670-1D3E45145CF4}" name="Description" dataDxfId="98"/>
-    <tableColumn id="4" xr3:uid="{6A637CD0-E4AE-4CBB-B448-5134035C720F}" name="Commentaire" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{73A28F86-A0B9-4591-B8D2-0160E457A112}" name="Code" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{F7506F92-2DA9-4093-9FDA-9893B7117480}" name="Libellé niveau 1" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{87CA381F-E725-4FBA-9AD1-5C61C6B110A7}" name="Libellé niveau 2" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{39D920FE-DBE6-4BFE-9670-1D3E45145CF4}" name="Description" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{6A637CD0-E4AE-4CBB-B448-5134035C720F}" name="Commentaire" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{E64CCCB9-2511-4EC1-8A5A-FF1038C81F09}" name="Table136111231118" displayName="Table136111231118" ref="A9:E55" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{E64CCCB9-2511-4EC1-8A5A-FF1038C81F09}" name="Table136111231118" displayName="Table136111231118" ref="A9:E55" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
   <autoFilter ref="A9:E55" xr:uid="{E64CCCB9-2511-4EC1-8A5A-FF1038C81F09}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{09E6D0E8-8FB6-4435-A553-92417353F896}" name="Code" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{A213C1A0-1722-4289-A2D1-5A6EB30EA09B}" name="Libellé niveau 1" dataDxfId="93"/>
-    <tableColumn id="5" xr3:uid="{53CF9BCE-0E7D-4BDE-B31F-55A8819FC0A0}" name="Libellé niveau 2" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{514C1BC9-9ADF-4004-BAB2-15D24A3A1D09}" name="Description" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{B12E6EEC-3F2C-407F-9AA7-389D7A17FCF7}" name="Commentaire" dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{09E6D0E8-8FB6-4435-A553-92417353F896}" name="Code" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{A213C1A0-1722-4289-A2D1-5A6EB30EA09B}" name="Libellé niveau 1" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{53CF9BCE-0E7D-4BDE-B31F-55A8819FC0A0}" name="Libellé niveau 2" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{514C1BC9-9ADF-4004-BAB2-15D24A3A1D09}" name="Description" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{B12E6EEC-3F2C-407F-9AA7-389D7A17FCF7}" name="Commentaire" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{E49A72A2-799E-4EB5-A633-DA9AD17ABED3}" name="Table136111231119" displayName="Table136111231119" ref="A9:E55" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{E49A72A2-799E-4EB5-A633-DA9AD17ABED3}" name="Table136111231119" displayName="Table136111231119" ref="A9:E55" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <autoFilter ref="A9:E55" xr:uid="{E49A72A2-799E-4EB5-A633-DA9AD17ABED3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:E55">
     <sortCondition ref="A10:A55"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7BFF7477-5274-4DF2-96EF-E56B7D69958A}" name="Code" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{FA4C3FFB-F1E7-4D2E-A4DD-0D3DF4405172}" name="Libellé niveau 1" dataDxfId="86"/>
-    <tableColumn id="5" xr3:uid="{A8127A8F-6B34-448D-A889-6BE2CE9E132C}" name="Libellé niveau 2" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{7B4AEDBA-3677-4E04-9052-1F30AB73A25F}" name="Description" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{9F627AE1-28AD-49D7-815A-4D3C089B24ED}" name="Commentaire" dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{7BFF7477-5274-4DF2-96EF-E56B7D69958A}" name="Code" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{FA4C3FFB-F1E7-4D2E-A4DD-0D3DF4405172}" name="Libellé niveau 1" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{A8127A8F-6B34-448D-A889-6BE2CE9E132C}" name="Libellé niveau 2" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{7B4AEDBA-3677-4E04-9052-1F30AB73A25F}" name="Description" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{9F627AE1-28AD-49D7-815A-4D3C089B24ED}" name="Commentaire" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{4B4CDC31-DA4C-4411-9B0D-8DA3539A0493}" name="Table136111231120" displayName="Table136111231120" ref="A9:E55" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{4B4CDC31-DA4C-4411-9B0D-8DA3539A0493}" name="Table136111231120" displayName="Table136111231120" ref="A9:E55" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="A9:E55" xr:uid="{4B4CDC31-DA4C-4411-9B0D-8DA3539A0493}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{317D1C42-0F4B-4773-8F99-F1B182F45481}" name="Code" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{77113B58-1151-4391-BEF5-DB56D3F4E4D5}" name="Libellé niveau 1" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{1CB9B5EC-80A3-4CA4-A035-92C9648D737A}" name="Libellé niveau 2" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{5FD1FD14-CDEB-40D4-9245-CD50BA9263BB}" name="Description" dataDxfId="77"/>
-    <tableColumn id="4" xr3:uid="{84BF17F5-072D-4227-B551-BE57A4509B17}" name="Commentaire" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{317D1C42-0F4B-4773-8F99-F1B182F45481}" name="Code" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{77113B58-1151-4391-BEF5-DB56D3F4E4D5}" name="Libellé niveau 1" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{1CB9B5EC-80A3-4CA4-A035-92C9648D737A}" name="Libellé niveau 2" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{5FD1FD14-CDEB-40D4-9245-CD50BA9263BB}" name="Description" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{84BF17F5-072D-4227-B551-BE57A4509B17}" name="Commentaire" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}" name="Table134" displayName="Table134" ref="A9:E30" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="A9:E30" xr:uid="{58BAE6F7-D01C-41AD-9846-4ED090DE684C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{865D8B57-135B-4BFA-938D-B62BC39AC970}" name="Code"/>
     <tableColumn id="2" xr3:uid="{E07D1CE2-997E-4A59-9869-D1EFB60F0809}" name="Libellé niveau 1"/>
     <tableColumn id="5" xr3:uid="{A8693491-C517-461F-B62C-F068AE507B25}" name="Libellé niveau 2"/>
-    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{5BEB0E75-8B05-44A8-99B9-CB9CB8DD7E0C}" name="Description" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{0C12ADAB-8B2E-4D44-B007-B1D25D7BAB07}" name="Commentaire" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}" name="Table13410" displayName="Table13410" ref="A9:F30" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A9:F30" xr:uid="{91C84658-0601-42A2-85F6-BBDF103A10CD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9B470DB1-BD5A-4D37-B9A2-613B4968664F}" name="Code"/>
-    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{C642441E-F665-4E14-A6AD-9D3C8769E0C7}" name="Libellé niveau 1" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{2FD7C62E-F3A8-479C-9488-B45577D597CB}" name="Libellé niveau 2" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{E474BB77-DCDC-415E-B7AC-9F51B933F4E0}" name="Libellé niveau 3" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{39AFB611-6F39-4451-B931-6D448FB9F381}" name="Description" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{2D0AD57C-4196-46DA-AA26-8087A6B411DB}" name="Commentaire" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3B0BCC87-0508-4B50-B37F-D0A3A984A79D}" name="Table13611123111814" displayName="Table13611123111814" ref="A9:E55" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3B0BCC87-0508-4B50-B37F-D0A3A984A79D}" name="Table13611123111814" displayName="Table13611123111814" ref="A9:E55" totalsRowShown="0" headerRowDxfId="179" dataDxfId="178">
   <autoFilter ref="A9:E55" xr:uid="{3B0BCC87-0508-4B50-B37F-D0A3A984A79D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{526E210B-F075-426E-960B-2873C3BD0C3B}" name="Code" dataDxfId="186"/>
-    <tableColumn id="2" xr3:uid="{2DA7E824-8886-4D58-ADE6-5377ED969D2A}" name="Libellé niveau 1" dataDxfId="185"/>
-    <tableColumn id="5" xr3:uid="{5D94993D-C9B5-47AD-AE15-32C420404C57}" name="Libellé niveau 2" dataDxfId="184"/>
-    <tableColumn id="3" xr3:uid="{436A1EAF-13B2-4CB3-9DDA-971E988E804D}" name="Description" dataDxfId="183"/>
-    <tableColumn id="4" xr3:uid="{82927005-4386-4694-9FA0-CF3D6DDB541C}" name="Commentaire" dataDxfId="182"/>
+    <tableColumn id="1" xr3:uid="{526E210B-F075-426E-960B-2873C3BD0C3B}" name="Code" dataDxfId="177"/>
+    <tableColumn id="2" xr3:uid="{2DA7E824-8886-4D58-ADE6-5377ED969D2A}" name="Libellé niveau 1" dataDxfId="176"/>
+    <tableColumn id="5" xr3:uid="{5D94993D-C9B5-47AD-AE15-32C420404C57}" name="Libellé niveau 2" dataDxfId="175"/>
+    <tableColumn id="3" xr3:uid="{436A1EAF-13B2-4CB3-9DDA-971E988E804D}" name="Description" dataDxfId="174"/>
+    <tableColumn id="4" xr3:uid="{82927005-4386-4694-9FA0-CF3D6DDB541C}" name="Commentaire" dataDxfId="173"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{53E2508C-FDA4-492A-BCC5-54C2C9927701}" name="Table1361112311182122" displayName="Table1361112311182122" ref="A9:E55" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{53E2508C-FDA4-492A-BCC5-54C2C9927701}" name="Table1361112311182122" displayName="Table1361112311182122" ref="A9:E55" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="A9:E55" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{61EFFEA6-F404-4D86-AF5A-470909BE208C}" name="Code" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{03E7B1DA-4913-4752-81D9-0DC5A650C798}" name="Libellé niveau 1" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{37E58575-3D14-49D7-8CD2-5DBE167C1AB2}" name="Libellé niveau 2" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{A2966C92-9801-4F74-B82F-3949B0B677E2}" name="Description" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{024E1FD3-4136-4C4D-9326-7EB1C41CE3F6}" name="Commentaire" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{61EFFEA6-F404-4D86-AF5A-470909BE208C}" name="Code" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{03E7B1DA-4913-4752-81D9-0DC5A650C798}" name="Libellé niveau 1" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{37E58575-3D14-49D7-8CD2-5DBE167C1AB2}" name="Libellé niveau 2" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{A2966C92-9801-4F74-B82F-3949B0B677E2}" name="Description" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{024E1FD3-4136-4C4D-9326-7EB1C41CE3F6}" name="Commentaire" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B9D58545-FB9E-446E-B811-6132BB1C3102}" name="Table136111231118212223" displayName="Table136111231118212223" ref="A9:E56" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{B9D58545-FB9E-446E-B811-6132BB1C3102}" name="Table136111231118212223" displayName="Table136111231118212223" ref="A9:E56" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="A9:E56" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E024BFB1-D7BC-4643-A173-73487B8EA76A}" name="Code" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{1FF3D037-3DC1-4032-AEEC-DB4E0FB2E125}" name="Libellé niveau 1" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{62B7E7BB-D7DB-42E9-9D6E-BCC352A62FAB}" name="Libellé niveau 2" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{D76DC12D-18A0-4B2C-9CCF-77E99D26B9F8}" name="Description" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{76F1640A-E1D7-412F-8753-57C0DE81055A}" name="Commentaire" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{E024BFB1-D7BC-4643-A173-73487B8EA76A}" name="Code" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{1FF3D037-3DC1-4032-AEEC-DB4E0FB2E125}" name="Libellé niveau 1" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{62B7E7BB-D7DB-42E9-9D6E-BCC352A62FAB}" name="Libellé niveau 2" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{D76DC12D-18A0-4B2C-9CCF-77E99D26B9F8}" name="Description" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{76F1640A-E1D7-412F-8753-57C0DE81055A}" name="Commentaire" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{02356107-77B0-4BE5-BEAF-E473DB32590C}" name="Table1361112311181325" displayName="Table1361112311181325" ref="A9:E55" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{02356107-77B0-4BE5-BEAF-E473DB32590C}" name="Table1361112311181325" displayName="Table1361112311181325" ref="A9:E55" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A9:E55" xr:uid="{02356107-77B0-4BE5-BEAF-E473DB32590C}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A3539628-1B96-4BB4-8A92-807D3B263DB7}" name="Code" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{AB8BA679-7023-4CF4-9883-6EE0FCD762F0}" name="Libellé niveau 1" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{5539128F-5313-4E5E-9C65-3502BDA2C44F}" name="Libellé niveau 2" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{D014B530-2E82-44D4-8C35-E5E40F3B9E3F}" name="Description" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{70515DEB-B1E5-4074-8DF3-44DBE6841499}" name="Commentaire" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{A3539628-1B96-4BB4-8A92-807D3B263DB7}" name="Code" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{AB8BA679-7023-4CF4-9883-6EE0FCD762F0}" name="Libellé niveau 1" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{5539128F-5313-4E5E-9C65-3502BDA2C44F}" name="Libellé niveau 2" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{D014B530-2E82-44D4-8C35-E5E40F3B9E3F}" name="Description" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{70515DEB-B1E5-4074-8DF3-44DBE6841499}" name="Commentaire" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DACF081D-DC50-403B-ADE1-57E5CB746E1E}" name="Table136" displayName="Table136" ref="A9:E55" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A9:E55" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{B3B3839E-7AA1-40F2-8D40-8B4C4130C33F}" name="Code" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{5B41AD54-EF54-419D-9557-D10165E3ECF6}" name="Libellé niveau 1" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{653C927B-56B9-4E39-8BC4-421DABCEC24B}" name="Libellé niveau 2" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{582D657A-1BB1-4D1A-882E-2FC91EF4A158}" name="Description" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{DD9122FE-5E05-4333-A4C2-0761574C47AC}" name="Commentaire" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADC06F70-889C-49F4-A602-458A21122DFC}" name="Table1361112" displayName="Table1361112" ref="A9:E55" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A9:E55" xr:uid="{EB7ACF14-FFBA-43E8-87A9-ACD7498B7895}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{73A2FECF-6CB9-4077-B0C7-A871C559AE83}" name="Code" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{FF04C7BE-CF51-4071-983D-631D78CC4E8F}" name="Libellé niveau 1" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{2BC45373-CCDD-4D71-AED7-35BA573538EC}" name="Libellé niveau 2" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{F975606E-B093-444F-A92B-4454E9D1F6FB}" name="Description" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{7F0D53E8-DCA3-4B3E-9BD7-47FE9D948220}" name="Commentaire" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{AEC31045-4022-46B3-A929-AC0614C9B5F7}" name="Table1361112311181326" displayName="Table1361112311181326" ref="A9:E55" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A9:E55" xr:uid="{AEC31045-4022-46B3-A929-AC0614C9B5F7}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A5939715-FD43-4BD9-9C9E-8B871392B9D8}" name="Code" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{9073BE50-9BBC-4E46-B62A-844A341664A8}" name="Libellé niveau 1" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{F39E1D91-61EC-4575-AA3A-5D7CC1F29201}" name="Libellé niveau 2" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{14836D78-1246-412B-B7ED-D773520414B3}" name="Description" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{4CB87313-3FCB-452A-BD3F-F57E778C5817}" name="Commentaire" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}" name="Table13611123111821" displayName="Table13611123111821" ref="A9:E55" totalsRowShown="0" headerRowDxfId="181" dataDxfId="180">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}" name="Table13611123111821" displayName="Table13611123111821" ref="A9:E55" totalsRowShown="0" headerRowDxfId="172" dataDxfId="171">
   <autoFilter ref="A9:E55" xr:uid="{17969914-72E8-45E0-B159-7FC4D4E17FB0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E79380D3-D068-423A-A034-02D5BAD28B34}" name="Code" dataDxfId="179"/>
-    <tableColumn id="2" xr3:uid="{38AD2FF1-8A7F-4689-AF86-3D0B5B4171F9}" name="Libellé niveau 1" dataDxfId="178"/>
-    <tableColumn id="5" xr3:uid="{F5EB8D60-F8AE-488C-8A75-B040D771B063}" name="Libellé niveau 2" dataDxfId="177"/>
-    <tableColumn id="3" xr3:uid="{1346777B-B4B8-4C5A-A2A0-C55CA418799A}" name="Description" dataDxfId="176"/>
-    <tableColumn id="4" xr3:uid="{7565A967-B560-4204-9869-CC57B1587900}" name="Commentaire" dataDxfId="175"/>
+    <tableColumn id="1" xr3:uid="{E79380D3-D068-423A-A034-02D5BAD28B34}" name="Code" dataDxfId="170"/>
+    <tableColumn id="2" xr3:uid="{38AD2FF1-8A7F-4689-AF86-3D0B5B4171F9}" name="Libellé niveau 1" dataDxfId="169"/>
+    <tableColumn id="5" xr3:uid="{F5EB8D60-F8AE-488C-8A75-B040D771B063}" name="Libellé niveau 2" dataDxfId="168"/>
+    <tableColumn id="3" xr3:uid="{1346777B-B4B8-4C5A-A2A0-C55CA418799A}" name="Description" dataDxfId="167"/>
+    <tableColumn id="4" xr3:uid="{7565A967-B560-4204-9869-CC57B1587900}" name="Commentaire" dataDxfId="166"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="174" dataDxfId="173">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}" name="Table137" displayName="Table137" ref="A9:F308" totalsRowShown="0" headerRowDxfId="165" dataDxfId="164">
   <autoFilter ref="A9:F308" xr:uid="{09B386D5-C588-4FF7-932D-04D6B9913019}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="172"/>
-    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="171"/>
-    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="170"/>
-    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="169"/>
-    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="168"/>
-    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="167"/>
+    <tableColumn id="1" xr3:uid="{F19F314C-B88E-48A0-9134-0480F8CF5303}" name="Code" dataDxfId="163"/>
+    <tableColumn id="2" xr3:uid="{600128F5-608F-4F75-ADD7-09E47F508C64}" name="Libellé niveau 1" dataDxfId="162"/>
+    <tableColumn id="6" xr3:uid="{69B015DB-FEAC-41E1-97CC-32D2D70D1E5F}" name="Libellé niveau 2" dataDxfId="161"/>
+    <tableColumn id="7" xr3:uid="{DDCC42E9-EE40-4BB4-8B10-7F7964B45C24}" name="Libellé niveau 3" dataDxfId="160"/>
+    <tableColumn id="3" xr3:uid="{B18EF0E1-670C-4280-93AF-67B4FB66EE2F}" name="Description" dataDxfId="159"/>
+    <tableColumn id="4" xr3:uid="{B87504F2-E81C-4AC3-AFB9-7F1544707E97}" name="Commentaire" dataDxfId="158"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}" name="Table138" displayName="Table138" ref="A9:F188" totalsRowShown="0" headerRowDxfId="157" dataDxfId="156">
   <autoFilter ref="A9:F188" xr:uid="{1926E7F2-C41A-49BC-938F-DC437CDBFF61}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="164"/>
-    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="163"/>
-    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="162"/>
-    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="159"/>
+    <tableColumn id="1" xr3:uid="{68E43B73-9A3F-4404-BFFA-9D2C83024853}" name="Code" dataDxfId="155"/>
+    <tableColumn id="2" xr3:uid="{4EE1502F-9D93-480B-9E76-CF9D4340C70D}" name="Libellé niveau 1" dataDxfId="154"/>
+    <tableColumn id="5" xr3:uid="{7B9C8786-A455-41BE-8B0E-D205B49FACF5}" name="Libellé niveau 2" dataDxfId="153"/>
+    <tableColumn id="6" xr3:uid="{254DB673-9BA3-42AE-9511-308D7BCD2FC5}" name="Libellé niveau 3" dataDxfId="152"/>
+    <tableColumn id="3" xr3:uid="{704D9D94-904F-4137-9FA6-AF5A0D326491}" name="Description" dataDxfId="151"/>
+    <tableColumn id="4" xr3:uid="{E0842B8F-A591-4C1E-A821-41D16E287145}" name="Commentaire" dataDxfId="150"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}" name="Table1" displayName="Table1" ref="A9:D46" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
   <autoFilter ref="A9:D46" xr:uid="{57784127-1058-49CC-86D5-E956DD9E7341}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="156"/>
-    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="155"/>
-    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="154"/>
-    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="153"/>
+    <tableColumn id="1" xr3:uid="{41A202AF-0A91-4C8F-B1DD-1D8B78C88B67}" name="Code" dataDxfId="147"/>
+    <tableColumn id="2" xr3:uid="{787839B6-641F-4C38-B883-AA61D5F0F7BA}" name="Libellé niveau 1" dataDxfId="146"/>
+    <tableColumn id="3" xr3:uid="{EA8B2165-6449-4C73-AB38-E548BEDD1CC6}" name="Description" dataDxfId="145"/>
+    <tableColumn id="4" xr3:uid="{E8FC5318-5334-4D19-B99B-DF7F88C59DC8}" name="Commentaire" dataDxfId="144"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="152" dataDxfId="151">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}" name="Table139" displayName="Table139" ref="A9:E61" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142">
   <autoFilter ref="A9:E61" xr:uid="{B5CED85C-8B87-4150-8F6E-210F8E0A2FFA}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="148"/>
-    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="147"/>
-    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="146"/>
+    <tableColumn id="1" xr3:uid="{1E16E225-2AC0-42BC-891A-DE42FEC023D6}" name="Code" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{EAF0C6A6-B766-472E-B250-B4F25993D46E}" name="Libellé niveau 1" dataDxfId="140"/>
+    <tableColumn id="5" xr3:uid="{81750735-53CA-440E-972E-333E415A08B6}" name="Libellé niveau 2" dataDxfId="139"/>
+    <tableColumn id="3" xr3:uid="{D8928B6E-6058-44ED-A422-FB52AA55B676}" name="Description" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{8EE4E12B-725F-47C8-B534-7688D1544C58}" name="Commentaire" dataDxfId="137"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B4F34E16-6907-43F3-BE39-7236A5E958C1}" name="Table1361112311181324" displayName="Table1361112311181324" ref="A9:E55" totalsRowShown="0" headerRowDxfId="145" dataDxfId="144">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B4F34E16-6907-43F3-BE39-7236A5E958C1}" name="Table1361112311181324" displayName="Table1361112311181324" ref="A9:E55" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135">
   <autoFilter ref="A9:E55" xr:uid="{B4F34E16-6907-43F3-BE39-7236A5E958C1}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{E04E8FE3-37D1-4BCD-B413-743E4DC4D779}" name="Code" dataDxfId="143"/>
-    <tableColumn id="2" xr3:uid="{AD3A7356-1689-4604-9ECC-BE119363210C}" name="Libellé niveau 1" dataDxfId="142"/>
-    <tableColumn id="5" xr3:uid="{2348B431-9FD0-4141-896C-0D101A9A5F99}" name="Libellé niveau 2" dataDxfId="141"/>
-    <tableColumn id="3" xr3:uid="{4B8B8570-D8A1-4AEA-90A5-8E0E9C6DD58C}" name="Description" dataDxfId="140"/>
-    <tableColumn id="4" xr3:uid="{B436BE35-AE75-458E-BF9D-1A1F55295033}" name="Commentaire" dataDxfId="139"/>
+    <tableColumn id="1" xr3:uid="{E04E8FE3-37D1-4BCD-B413-743E4DC4D779}" name="Code" dataDxfId="134"/>
+    <tableColumn id="2" xr3:uid="{AD3A7356-1689-4604-9ECC-BE119363210C}" name="Libellé niveau 1" dataDxfId="133"/>
+    <tableColumn id="5" xr3:uid="{2348B431-9FD0-4141-896C-0D101A9A5F99}" name="Libellé niveau 2" dataDxfId="132"/>
+    <tableColumn id="3" xr3:uid="{4B8B8570-D8A1-4AEA-90A5-8E0E9C6DD58C}" name="Description" dataDxfId="131"/>
+    <tableColumn id="4" xr3:uid="{B436BE35-AE75-458E-BF9D-1A1F55295033}" name="Commentaire" dataDxfId="130"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}" name="Table13611123" displayName="Table13611123" ref="A9:E55" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}" name="Table13611123" displayName="Table13611123" ref="A9:E55" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
   <autoFilter ref="A9:E55" xr:uid="{B647832F-37DE-421D-B1F3-9D38947A9A6A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A5D7830D-ADAE-49D1-AC01-5A1DFA001520}" name="Code" dataDxfId="136"/>
-    <tableColumn id="2" xr3:uid="{314EEFD1-40EA-4FC8-B871-E91D87553FAE}" name="Libellé niveau 1" dataDxfId="135"/>
-    <tableColumn id="5" xr3:uid="{2A634FA7-602A-4CA9-B5C2-AF22E2C2C4B5}" name="Libellé niveau 2" dataDxfId="134"/>
-    <tableColumn id="3" xr3:uid="{110DEB60-AD15-400E-BCE9-BFB19B19C22B}" name="Description" dataDxfId="133"/>
-    <tableColumn id="4" xr3:uid="{946798AA-F310-452C-873A-8DEE9082FA3D}" name="Commentaire" dataDxfId="132"/>
+    <tableColumn id="1" xr3:uid="{A5D7830D-ADAE-49D1-AC01-5A1DFA001520}" name="Code" dataDxfId="127"/>
+    <tableColumn id="2" xr3:uid="{314EEFD1-40EA-4FC8-B871-E91D87553FAE}" name="Libellé niveau 1" dataDxfId="126"/>
+    <tableColumn id="5" xr3:uid="{2A634FA7-602A-4CA9-B5C2-AF22E2C2C4B5}" name="Libellé niveau 2" dataDxfId="125"/>
+    <tableColumn id="3" xr3:uid="{110DEB60-AD15-400E-BCE9-BFB19B19C22B}" name="Description" dataDxfId="124"/>
+    <tableColumn id="4" xr3:uid="{946798AA-F310-452C-873A-8DEE9082FA3D}" name="Commentaire" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11288,13 +11399,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}">
-  <dimension ref="A1:M224"/>
+  <dimension ref="A1:M225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -11364,7 +11475,7 @@
       <c r="B3" s="33" t="s">
         <v>2022</v>
       </c>
-      <c r="C3" s="78" t="str">
+      <c r="C3" s="77" t="str">
         <f>Filiere!$B$8</f>
         <v>Décrit la filière compétente pour traiter le dossier.</v>
       </c>
@@ -11398,7 +11509,7 @@
       <c r="B4" s="33" t="s">
         <v>2003</v>
       </c>
-      <c r="C4" s="79" t="str">
+      <c r="C4" s="78" t="str">
         <f>'Type d''intervention'!$B$8</f>
         <v>Décrit le type d'intervention (primaire, secondaire, etc.)</v>
       </c>
@@ -11432,7 +11543,7 @@
       <c r="B5" s="33" t="s">
         <v>2054</v>
       </c>
-      <c r="C5" s="79" t="str">
+      <c r="C5" s="78" t="str">
         <f>'Origine de l''appel'!$B$8</f>
         <v>Décrit l'origine de l'appel</v>
       </c>
@@ -11466,7 +11577,7 @@
       <c r="B6" s="33" t="s">
         <v>1727</v>
       </c>
-      <c r="C6" s="79" t="str">
+      <c r="C6" s="78" t="str">
         <f>'Nature de fait'!$B$8</f>
         <v>Décrit la nature de fait de l'affaire/dossier</v>
       </c>
@@ -11502,7 +11613,7 @@
       <c r="B7" s="34" t="s">
         <v>1733</v>
       </c>
-      <c r="C7" s="79" t="str">
+      <c r="C7" s="78" t="str">
         <f>'Type de lieu'!$B$8</f>
         <v>Décrit le type de lieu où se situe l'affaire/dossier</v>
       </c>
@@ -11538,7 +11649,7 @@
       <c r="B8" s="34" t="s">
         <v>1734</v>
       </c>
-      <c r="C8" s="79" t="str">
+      <c r="C8" s="78" t="str">
         <f>'Risque, menace et sensibilité'!$B$8</f>
         <v>Décrit les risques, menaces ou sensibilités de l'affaire/dossier</v>
       </c>
@@ -11574,7 +11685,7 @@
       <c r="B9" s="34" t="s">
         <v>1754</v>
       </c>
-      <c r="C9" s="78" t="str">
+      <c r="C9" s="77" t="str">
         <f>'Motif de recours médico-secouri'!$B$8</f>
         <v>Décrit le motif de recours médico-secouriste.</v>
       </c>
@@ -11610,7 +11721,7 @@
       <c r="B10" s="34" t="s">
         <v>2075</v>
       </c>
-      <c r="C10" s="78" t="str">
+      <c r="C10" s="77" t="str">
         <f>'Etats du dossier'!$B$8</f>
         <v>Décrit la filière compétente pour traiter le dossier.</v>
       </c>
@@ -11644,7 +11755,7 @@
       <c r="B11" s="31" t="s">
         <v>1992</v>
       </c>
-      <c r="C11" s="80" t="str">
+      <c r="C11" s="79" t="str">
         <f>'Nombre de patients-victimes'!$B$8</f>
         <v>Décrit le nombre de patient/victimes</v>
       </c>
@@ -11678,7 +11789,7 @@
       <c r="B12" s="31" t="s">
         <v>2000</v>
       </c>
-      <c r="C12" s="80" t="str">
+      <c r="C12" s="79" t="str">
         <f>'Type du patient-victime'!$B$8</f>
         <v>Décrit le type de patient/victime principal</v>
       </c>
@@ -11712,7 +11823,7 @@
       <c r="B13" s="34" t="s">
         <v>1730</v>
       </c>
-      <c r="C13" s="78" t="str">
+      <c r="C13" s="77" t="str">
         <f>'Attribution du dossier'!$B$8</f>
         <v>Décrit le type de dossier, et son attribution</v>
       </c>
@@ -11746,7 +11857,7 @@
       <c r="B14" s="34" t="s">
         <v>1738</v>
       </c>
-      <c r="C14" s="78" t="str">
+      <c r="C14" s="77" t="str">
         <f>'Priorité de régulation médicale'!$B$8</f>
         <v>Décrit la priorité de régulation médicale.</v>
       </c>
@@ -11780,7 +11891,7 @@
       <c r="B15" s="31" t="s">
         <v>2004</v>
       </c>
-      <c r="C15" s="80" t="str">
+      <c r="C15" s="79" t="str">
         <f>'Lieu - Source ou type d''id'!$B$8</f>
         <v>Décrit le type d'idenfiant possible pour un lieu  (société / établissement)</v>
       </c>
@@ -11816,7 +11927,7 @@
       <c r="B16" s="31" t="s">
         <v>1998</v>
       </c>
-      <c r="C16" s="80" t="str">
+      <c r="C16" s="79" t="str">
         <f>Precision!$B$8</f>
         <v>Décrit le niveau de précision des coordonnées GPS envoyées</v>
       </c>
@@ -11852,7 +11963,7 @@
       <c r="B17" s="31" t="s">
         <v>1993</v>
       </c>
-      <c r="C17" s="80" t="str">
+      <c r="C17" s="79" t="str">
         <f>'Nom de la source'!$B$8</f>
         <v>Décrit le système fournissant le localisant</v>
       </c>
@@ -11888,7 +11999,7 @@
       <c r="B18" s="31" t="s">
         <v>1997</v>
       </c>
-      <c r="C18" s="80" t="str">
+      <c r="C18" s="79" t="str">
         <f>'Type d''objet'!$B$8</f>
         <v>Décrit le type d'objet dans le système</v>
       </c>
@@ -11924,7 +12035,7 @@
       <c r="B19" s="31" t="s">
         <v>1994</v>
       </c>
-      <c r="C19" s="80" t="str">
+      <c r="C19" s="79" t="str">
         <f>Signalement!$B$8</f>
         <v>Décrit le niveau de signalement de l'alerte</v>
       </c>
@@ -11958,7 +12069,7 @@
       <c r="B20" s="31" t="s">
         <v>1995</v>
       </c>
-      <c r="C20" s="80" t="str">
+      <c r="C20" s="79" t="str">
         <f>Canal!$B$8</f>
         <v>Décrit le type de canal utilisé pour le contact</v>
       </c>
@@ -11994,7 +12105,7 @@
       <c r="B21" s="31" t="s">
         <v>1996</v>
       </c>
-      <c r="C21" s="80" t="str">
+      <c r="C21" s="79" t="str">
         <f>'Type de contact'!$B$8</f>
         <v>Décrit le type de contact</v>
       </c>
@@ -12030,7 +12141,7 @@
       <c r="B22" s="34" t="s">
         <v>1735</v>
       </c>
-      <c r="C22" s="78" t="str">
+      <c r="C22" s="77" t="str">
         <f>'Type de requérant'!$B$8</f>
         <v>Décrit le type de requérant/appelant</v>
       </c>
@@ -12066,7 +12177,7 @@
       <c r="B23" s="34" t="s">
         <v>1736</v>
       </c>
-      <c r="C23" s="78" t="str">
+      <c r="C23" s="77" t="str">
         <f>'Difficultés de communication'!$B$8</f>
         <v>Décrit les difficultés de communication potentielles du requérant/appelant</v>
       </c>
@@ -12102,7 +12213,7 @@
       <c r="B24" s="34" t="s">
         <v>2055</v>
       </c>
-      <c r="C24" s="78" t="str">
+      <c r="C24" s="77" t="str">
         <f>'Patient - type d''Id'!$B$8</f>
         <v>Décrit le type d'identifiant fourni</v>
       </c>
@@ -12136,7 +12247,7 @@
       <c r="B25" s="34" t="s">
         <v>1739</v>
       </c>
-      <c r="C25" s="78" t="str">
+      <c r="C25" s="77" t="str">
         <f>Sexe!$B$8</f>
         <v>Décrit le sexe du patient</v>
       </c>
@@ -12172,7 +12283,7 @@
       <c r="B26" s="34" t="s">
         <v>1740</v>
       </c>
-      <c r="C26" s="78" t="str">
+      <c r="C26" s="77" t="str">
         <f>'Niveau de soin'!$B$8</f>
         <v>Décrit le niveau de soins : le plus grave est retenu pour qualifier le dossier/affaire. Pour chaque patient/victime, le motif spécifique est indiqué.</v>
       </c>
@@ -12206,7 +12317,7 @@
       <c r="B27" s="34" t="s">
         <v>2057</v>
       </c>
-      <c r="C27" s="78" t="str">
+      <c r="C27" s="77" t="str">
         <f>Role!$B$8</f>
         <v>Décrit le rôle de l'opérateur dans l'organisation à laquelle il appartient</v>
       </c>
@@ -12240,7 +12351,7 @@
       <c r="B28" s="34" t="s">
         <v>2069</v>
       </c>
-      <c r="C28" s="78" t="str">
+      <c r="C28" s="77" t="str">
         <f>'Type de decision'!$B$8</f>
         <v>Décrit le type de décision prise</v>
       </c>
@@ -12258,10 +12369,8 @@
       <c r="G28" s="28" t="s">
         <v>1743</v>
       </c>
-      <c r="H28" s="70" t="s">
-        <v>1748</v>
-      </c>
-      <c r="I28" s="70" t="s">
+      <c r="H28" s="80"/>
+      <c r="I28" s="80" t="s">
         <v>1748</v>
       </c>
       <c r="J28" s="30"/>
@@ -12276,7 +12385,7 @@
       <c r="B29" s="34" t="s">
         <v>1742</v>
       </c>
-      <c r="C29" s="78" t="str">
+      <c r="C29" s="77" t="str">
         <f>'Type de ressource'!$B$8</f>
         <v xml:space="preserve">Décrit le type de moyen/ressources, dans un sens plus large que type de vecteur/véhicule. N.B. dans OPG pour les message EMSI.
 </v>
@@ -12315,7 +12424,7 @@
       <c r="B30" s="34" t="s">
         <v>1753</v>
       </c>
-      <c r="C30" s="78" t="str">
+      <c r="C30" s="77" t="str">
         <f>'Type de vecteurs'!$B$8</f>
         <v>Décrit le type de vecteur/véhicule ou de ressource mobilisée, avec plus de précision que simplement le type de ressources. Utilisée exclusivement en inter-santé (cf. EMSI-OPG pour 15-NexSIS)</v>
       </c>
@@ -12348,12 +12457,12 @@
     </row>
     <row r="31" spans="1:13" ht="15">
       <c r="A31" s="27" t="s">
-        <v>1751</v>
+        <v>2102</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>1749</v>
       </c>
-      <c r="C31" s="79" t="str">
+      <c r="C31" s="78" t="str">
         <f>'Niveau de prise en charge'!$B$8</f>
         <v>Décrit le niveau de prise en charge exigé.</v>
       </c>
@@ -12371,9 +12480,7 @@
       <c r="G31" s="28" t="s">
         <v>1743</v>
       </c>
-      <c r="H31" s="30" t="s">
-        <v>1748</v>
-      </c>
+      <c r="H31" s="30"/>
       <c r="I31" s="30" t="s">
         <v>1748</v>
       </c>
@@ -12387,22 +12494,20 @@
       <c r="M31" s="30"/>
     </row>
     <row r="32" spans="1:13" ht="15">
-      <c r="A32" s="27" t="s">
-        <v>1745</v>
-      </c>
+      <c r="A32" s="27"/>
       <c r="B32" s="34" t="s">
         <v>1741</v>
       </c>
-      <c r="C32" s="79" t="str">
-        <f>'Type de devenir du patient'!$B$8</f>
+      <c r="C32" s="78" t="str">
+        <f>'#Type de devenir du patient'!$B$8</f>
         <v>Décrit le devenir du patient</v>
       </c>
       <c r="D32" s="27" t="str">
-        <f>'Type de devenir du patient'!$B$1</f>
+        <f>'#Type de devenir du patient'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
       <c r="E32" s="27" t="str">
-        <f>'Type de devenir du patient'!$B$2</f>
+        <f>'#Type de devenir du patient'!$B$2</f>
         <v>NOMENC_DEVENIR_PAT</v>
       </c>
       <c r="F32" s="29" t="s">
@@ -12411,12 +12516,8 @@
       <c r="G32" s="28" t="s">
         <v>1743</v>
       </c>
-      <c r="H32" s="30" t="s">
-        <v>1748</v>
-      </c>
-      <c r="I32" s="30" t="s">
-        <v>1748</v>
-      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
       <c r="L32" s="30"/>
@@ -12429,7 +12530,7 @@
       <c r="B33" s="34" t="s">
         <v>2084</v>
       </c>
-      <c r="C33" s="79" t="str">
+      <c r="C33" s="78" t="str">
         <f>'Type de destination'!$B$8</f>
         <v>Décrit la filière compétente pour traiter le dossier.</v>
       </c>
@@ -12463,7 +12564,7 @@
       <c r="B34" s="34" t="s">
         <v>1737</v>
       </c>
-      <c r="C34" s="79" t="str">
+      <c r="C34" s="78" t="str">
         <f>'Effet à obtenir'!$B$8</f>
         <v>Décrit les effets à obtenir utilisés uniquement entre SAMU, en intersanté.</v>
       </c>
@@ -12497,7 +12598,7 @@
       <c r="B35" s="31" t="s">
         <v>1882</v>
       </c>
-      <c r="C35" s="79" t="str">
+      <c r="C35" s="78" t="str">
         <f>'Cadre conventionnel'!$B$8</f>
         <v xml:space="preserve">Décrit le cadre conventionnel dans lequel s'inscrit une demande de ressources. Codes inter-santé uniquement (voir EMSI pour lien 15-Nexsis). </v>
       </c>
@@ -12529,7 +12630,7 @@
       <c r="B36" s="31" t="s">
         <v>2002</v>
       </c>
-      <c r="C36" s="79" t="str">
+      <c r="C36" s="78" t="str">
         <f>'Delai d''intervention souhaite'!$B$8</f>
         <v>Décrit le délai d'intervention attendu ou souhaité pour une ressource ou un vecteur.</v>
       </c>
@@ -12558,24 +12659,24 @@
     </row>
     <row r="37" spans="1:13" ht="15">
       <c r="A37" s="28" t="s">
-        <v>2068</v>
+        <v>2103</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>2067</v>
-      </c>
-      <c r="C37" s="79" t="str">
-        <f>'Reponse demande ressources'!$B$8</f>
-        <v>Décrit la réponse à une demande de ressources</v>
+        <v>2109</v>
+      </c>
+      <c r="C37" s="87" t="str">
+        <f>'Annulation DR'!$B$8</f>
+        <v>Décrit l'état de l'annulation de demande de ressources</v>
       </c>
       <c r="D37" s="27" t="str">
-        <f>'Reponse demande ressources'!$B$1</f>
+        <f>'Annulation DR'!B1</f>
         <v>ENUM</v>
       </c>
       <c r="E37" s="27" t="str">
-        <f>'Reponse demande ressources'!$B$2</f>
-        <v>REPONSE</v>
-      </c>
-      <c r="F37" s="29" t="s">
+        <f>'Annulation DR'!B2</f>
+        <v>STATUS_DR</v>
+      </c>
+      <c r="F37" s="88" t="s">
         <v>1728</v>
       </c>
       <c r="G37" s="28" t="s">
@@ -12584,64 +12685,83 @@
       <c r="H37" s="30"/>
       <c r="I37" s="30"/>
       <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30" t="s">
+      <c r="K37" s="30" t="s">
         <v>1748</v>
       </c>
+      <c r="L37" s="30"/>
       <c r="M37" s="30"/>
     </row>
     <row r="38" spans="1:13" ht="15">
       <c r="A38" s="28" t="s">
+        <v>2068</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C38" s="78" t="str">
+        <f>'Reponse demande ressources'!$B$8</f>
+        <v>Décrit la réponse à une demande de ressources</v>
+      </c>
+      <c r="D38" s="27" t="str">
+        <f>'Reponse demande ressources'!$B$1</f>
+        <v>ENUM</v>
+      </c>
+      <c r="E38" s="27" t="str">
+        <f>'Reponse demande ressources'!$B$2</f>
+        <v>REPONSE</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>1728</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>1743</v>
+      </c>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30" t="s">
+        <v>1748</v>
+      </c>
+      <c r="M38" s="30"/>
+    </row>
+    <row r="39" spans="1:13" ht="15">
+      <c r="A39" s="28" t="s">
         <v>1883</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B39" s="31" t="s">
         <v>1884</v>
       </c>
-      <c r="C38" s="79" t="str">
+      <c r="C39" s="78" t="str">
         <f>'Statut du vecteur'!$B$8</f>
         <v>Décrit le statut du vecteur/véhicule mobilisé</v>
       </c>
-      <c r="D38" s="27" t="str">
+      <c r="D39" s="27" t="str">
         <f>'Statut du vecteur'!$B$1</f>
         <v>SI-SAMU</v>
       </c>
-      <c r="E38" s="27" t="str">
+      <c r="E39" s="27" t="str">
         <f>'Statut du vecteur'!$B$2</f>
         <v>STATUS_VECTEUR</v>
       </c>
-      <c r="F38" s="29" t="s">
+      <c r="F39" s="29" t="s">
         <v>1728</v>
       </c>
-      <c r="G38" s="28" t="s">
+      <c r="G39" s="28" t="s">
         <v>1743</v>
       </c>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30" t="s">
-        <v>1748</v>
-      </c>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="30" t="s">
-        <v>1748</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="15">
-      <c r="B39" s="31"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
       <c r="H39" s="30"/>
       <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
+      <c r="J39" s="30" t="s">
+        <v>1748</v>
+      </c>
       <c r="K39" s="30"/>
       <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
+      <c r="M39" s="30" t="s">
+        <v>1748</v>
+      </c>
     </row>
     <row r="40" spans="1:13" ht="15">
-      <c r="A40" s="28"/>
       <c r="B40" s="31"/>
       <c r="C40" s="28"/>
       <c r="D40" s="28"/>
@@ -12670,9 +12790,9 @@
       <c r="L41" s="30"/>
       <c r="M41" s="30"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" ht="15">
       <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="28"/>
       <c r="D42" s="28"/>
       <c r="E42" s="28"/>
@@ -12783,12 +12903,12 @@
       <c r="E49" s="28"/>
       <c r="F49" s="28"/>
       <c r="G49" s="28"/>
-      <c r="H49" s="28"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="28"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="30"/>
+      <c r="L49" s="30"/>
+      <c r="M49" s="30"/>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="28"/>
@@ -15415,48 +15535,61 @@
       <c r="L224" s="28"/>
       <c r="M224" s="28"/>
     </row>
+    <row r="225" spans="1:13">
+      <c r="A225" s="28"/>
+      <c r="B225" s="28"/>
+      <c r="C225" s="28"/>
+      <c r="D225" s="28"/>
+      <c r="E225" s="28"/>
+      <c r="F225" s="28"/>
+      <c r="G225" s="28"/>
+      <c r="H225" s="28"/>
+      <c r="I225" s="28"/>
+      <c r="J225" s="28"/>
+      <c r="K225" s="28"/>
+      <c r="L225" s="28"/>
+      <c r="M225" s="28"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:L38" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}"/>
+  <autoFilter ref="A2:L39" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}"/>
   <conditionalFormatting sqref="A19:F21">
-    <cfRule type="expression" dxfId="15" priority="31">
+    <cfRule type="expression" dxfId="7" priority="31">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
     <cfRule type="expression" priority="32">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39:M39 A40:M224 A3:M38">
-    <cfRule type="expression" dxfId="14" priority="53">
+  <conditionalFormatting sqref="B40:M40 A41:M225 A3:M39">
+    <cfRule type="expression" dxfId="6" priority="53">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39:M39 A40:M224 A3:M38">
     <cfRule type="expression" priority="55">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:M5">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>H3=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>H3="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:M45">
-    <cfRule type="expression" dxfId="11" priority="52">
+  <conditionalFormatting sqref="H6:M46">
+    <cfRule type="expression" dxfId="3" priority="10" stopIfTrue="1">
+      <formula>H6="X"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="52">
       <formula>H6=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
-      <formula>H6="X"</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M35:M38">
+    <cfRule type="expression" dxfId="1" priority="9" stopIfTrue="1">
+      <formula>M35="X"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M35:M37">
-    <cfRule type="expression" dxfId="9" priority="54">
+    <cfRule type="expression" dxfId="0" priority="54">
       <formula>M35=""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
-      <formula>M35="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -15475,8 +15608,8 @@
     <hyperlink ref="F31" location="'Niveau de prise en charge'!A1" display="Lien nomenclature" xr:uid="{2154EBB7-71EE-44B5-BBEE-716579483CDC}"/>
     <hyperlink ref="F32" location="'Type de devenir du patient'!A1" display="Lien nomenclature" xr:uid="{0E2A9314-0B8D-4156-A7C3-BC0E2885D9D2}"/>
     <hyperlink ref="F34" location="'Effet à obtenir'!A1" display="Lien nomenclature" xr:uid="{F32B9CB2-26FC-4D51-B612-B9EB269DC3B1}"/>
-    <hyperlink ref="F38" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{9DFDDF82-C842-46CA-9B9A-3545027D4646}"/>
-    <hyperlink ref="F38" location="'Statut du vecteur'!A1" display="Lien nomenclature" xr:uid="{CBB6C543-B740-4053-95FD-E8C10E8B561C}"/>
+    <hyperlink ref="F39" location="'Attribution du dossier'!A1" display="Lien nomenclature" xr:uid="{9DFDDF82-C842-46CA-9B9A-3545027D4646}"/>
+    <hyperlink ref="F39" location="'Statut du vecteur'!A1" display="Lien nomenclature" xr:uid="{CBB6C543-B740-4053-95FD-E8C10E8B561C}"/>
     <hyperlink ref="F35" location="'Cadre conventionnel'!A1" display="Lien nomenclature" xr:uid="{018B40BB-963F-4A1C-AF4F-5EA9FD5F329B}"/>
     <hyperlink ref="F36" location="'Delai d''intervention souhaite'!A1" display="Lien nomenclature" xr:uid="{FA2A5069-90AE-4459-B4C7-F1CDCCD8EAB0}"/>
     <hyperlink ref="F11" location="'Nombre de patients-victimes'!A1" display="Lien nomenclature" xr:uid="{6309BD82-9F33-4F60-88D8-A0006F1258C1}"/>
@@ -15494,9 +15627,10 @@
     <hyperlink ref="F24" location="'Patient - type d''Id'!A1" display="Lien nomenclature" xr:uid="{679AF562-7FA0-4BA2-9C4D-AA1F96F40CFA}"/>
     <hyperlink ref="F28" location="'Type de decision'!A1" display="Lien nomenclature" xr:uid="{4F195D5A-2BD1-4EA9-BE69-3011CC92C820}"/>
     <hyperlink ref="F27" location="Role!A1" display="Lien nomenclature" xr:uid="{582C01B4-1165-40A4-A66C-114EB3863727}"/>
-    <hyperlink ref="F37" location="'Reponse demande ressources'!A1" display="Lien nomenclature" xr:uid="{A5992456-8F22-45CA-B0C9-B24FF1D02C76}"/>
+    <hyperlink ref="F38" location="'Reponse demande ressources'!A1" display="Lien nomenclature" xr:uid="{A5992456-8F22-45CA-B0C9-B24FF1D02C76}"/>
     <hyperlink ref="F10" location="'Etats du dossier'!A1" display="Lien nomenclature" xr:uid="{E2F3E3CE-6DF1-437C-A6B6-E5C58AA762D2}"/>
     <hyperlink ref="F33" location="'Type de destination'!A1" display="Lien nomenclature" xr:uid="{D62BADA3-6E05-4387-BA31-BBD4E4D70DB5}"/>
+    <hyperlink ref="F37" location="'Annulation DR'!A1" display="Lien nomenclature" xr:uid="{81CA3C32-8B71-4375-8729-60148FE0E1D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20146,9 +20280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52670871-FFE0-4B71-AFFC-AFEDF834F777}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
@@ -20364,200 +20496,200 @@
       <c r="K22"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="2"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="2"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="83"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="2"/>
-      <c r="B25" s="38"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="2"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="2"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="43"/>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="2"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="83"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="85"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="2"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="86"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="2"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="83"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="2"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="A31" s="83"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="43"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="2"/>
+      <c r="A32" s="83"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="C32" s="83"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="A33" s="83"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="43"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="83"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="83"/>
+      <c r="B35" s="83"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="85"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="86"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="83"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="D37" s="83"/>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="A38" s="83"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="83"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="83"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="D39" s="83"/>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="A40" s="83"/>
+      <c r="B40" s="83"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="83"/>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="83"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="D41" s="83"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="A42" s="84"/>
+      <c r="B42" s="83"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="83"/>
+      <c r="E42" s="85"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
+      <c r="A43" s="86"/>
+      <c r="B43" s="83"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="86"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="B44" s="83"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="83"/>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
+      <c r="A45" s="83"/>
+      <c r="B45" s="83"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="D45" s="83"/>
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="A46" s="83"/>
+      <c r="B46" s="83"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="83"/>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="83"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="D47" s="83"/>
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
+      <c r="A48" s="83"/>
+      <c r="B48" s="83"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="D48" s="83"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
+      <c r="A49" s="84"/>
+      <c r="B49" s="84"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="E49" s="85"/>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="A50" s="86"/>
+      <c r="B50" s="86"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="86"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2"/>
@@ -22923,10 +23055,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="71" t="s">
         <v>2042</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="71" t="s">
         <v>2042</v>
       </c>
       <c r="C10" s="43"/>
@@ -22936,23 +23068,23 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="72" t="s">
         <v>2043</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="72" t="s">
         <v>2043</v>
       </c>
       <c r="C11" s="43"/>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="73" t="s">
         <v>2049</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="72" t="s">
         <v>2044</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="72" t="s">
         <v>2044</v>
       </c>
       <c r="C12" s="43"/>
@@ -22962,10 +23094,10 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="72" t="s">
         <v>2045</v>
       </c>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="72" t="s">
         <v>2045</v>
       </c>
       <c r="C13" s="43"/>
@@ -22975,10 +23107,10 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="72" t="s">
         <v>1343</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="72" t="s">
         <v>1343</v>
       </c>
       <c r="C14" s="43"/>
@@ -22988,10 +23120,10 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="72" t="s">
         <v>1346</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="72" t="s">
         <v>1346</v>
       </c>
       <c r="C15" s="43"/>
@@ -23822,7 +23954,7 @@
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="48.75">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="74" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="66" t="s">
@@ -25153,9 +25285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCC278-4076-404C-8EB9-6697AFDA1197}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
@@ -26235,7 +26365,7 @@
       <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="76" t="s">
         <v>2095</v>
       </c>
       <c r="B18" s="23" t="s">
@@ -26631,7 +26761,7 @@
       <c r="A10" s="69" t="s">
         <v>2092</v>
       </c>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="75" t="s">
         <v>2087</v>
       </c>
       <c r="C10" s="43"/>
@@ -26642,7 +26772,7 @@
       <c r="A11" s="52" t="s">
         <v>1317</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="75" t="s">
         <v>2088</v>
       </c>
       <c r="C11" s="43"/>
@@ -26653,7 +26783,7 @@
       <c r="A12" s="52" t="s">
         <v>2093</v>
       </c>
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="75" t="s">
         <v>2089</v>
       </c>
       <c r="C12" s="43"/>
@@ -26664,7 +26794,7 @@
       <c r="A13" s="52" t="s">
         <v>2086</v>
       </c>
-      <c r="B13" s="76" t="s">
+      <c r="B13" s="75" t="s">
         <v>683</v>
       </c>
       <c r="C13" s="43"/>
@@ -26675,7 +26805,7 @@
       <c r="A14" s="52" t="s">
         <v>2094</v>
       </c>
-      <c r="B14" s="76" t="s">
+      <c r="B14" s="75" t="s">
         <v>2090</v>
       </c>
       <c r="C14" s="43"/>
@@ -26686,7 +26816,7 @@
       <c r="A15" s="52" t="s">
         <v>1343</v>
       </c>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="75" t="s">
         <v>2091</v>
       </c>
       <c r="C15" s="43"/>
@@ -28236,470 +28366,442 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B730C132-AF0D-4124-AB29-0565D21E3ED1}">
-  <dimension ref="A1:F64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D07CCD-8605-4E9E-B9C4-85FB17F9209F}">
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" style="52" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="52" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" style="52" customWidth="1"/>
-    <col min="5" max="5" width="88.7109375" style="52" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="52" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="52"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
-        <v>1284</v>
-      </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="54" t="s">
+      <c r="B1" s="22" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="55" t="s">
-        <v>1852</v>
-      </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="54" t="s">
+      <c r="B2" s="81" t="s">
+        <v>2106</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="54" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="54" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="54" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="54" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="58" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="54" t="s">
+      <c r="B7" s="6" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="64" t="s">
-        <v>1902</v>
-      </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="59" t="s">
+      <c r="B8" s="82" t="s">
+        <v>2108</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="59" t="s">
+      <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="60" t="s">
-        <v>1800</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>1801</v>
-      </c>
-      <c r="C10" s="61"/>
-      <c r="E10" s="61" t="s">
-        <v>1802</v>
-      </c>
-      <c r="F10" s="52" t="s">
-        <v>1803</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="46" t="s">
-        <v>1804</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>1805</v>
-      </c>
-      <c r="E11" s="52" t="s">
-        <v>1806</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="46" t="s">
-        <v>1807</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>1808</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>1809</v>
-      </c>
-      <c r="F12" s="52" t="s">
-        <v>1810</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="46" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>1812</v>
-      </c>
-      <c r="C13"/>
-      <c r="E13" s="52" t="s">
-        <v>1813</v>
-      </c>
-      <c r="F13" s="52" t="s">
-        <v>1814</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="60" t="s">
-        <v>1815</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>1816</v>
-      </c>
-      <c r="E14" s="52" t="s">
-        <v>1817</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="46" t="s">
-        <v>1818</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>1819</v>
-      </c>
-      <c r="C15"/>
-      <c r="E15" s="52" t="s">
-        <v>1885</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="60" t="s">
-        <v>1820</v>
-      </c>
-      <c r="B16" s="52" t="s">
-        <v>1821</v>
-      </c>
-      <c r="C16" s="50"/>
-      <c r="F16" s="52" t="s">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="60" t="s">
-        <v>1589</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>1823</v>
-      </c>
-      <c r="C17" s="61"/>
-      <c r="E17" s="52" t="s">
-        <v>1824</v>
-      </c>
-      <c r="F17" s="52" t="s">
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="60" t="s">
-        <v>1826</v>
-      </c>
-      <c r="C18" s="50" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="60" t="s">
-        <v>1828</v>
-      </c>
-      <c r="C19" s="50" t="s">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="60" t="s">
-        <v>1830</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>1831</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="60" t="s">
-        <v>1832</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="46" t="s">
-        <v>1834</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>1835</v>
-      </c>
-      <c r="C22"/>
-      <c r="E22" s="52" t="s">
-        <v>1836</v>
-      </c>
-      <c r="F22" s="52" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="46" t="s">
-        <v>1838</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>1839</v>
-      </c>
-      <c r="C23"/>
-      <c r="E23" s="52" t="s">
-        <v>1840</v>
-      </c>
-      <c r="F23" s="52" t="s">
-        <v>1841</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="46" t="s">
-        <v>1842</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>1843</v>
-      </c>
-      <c r="C24"/>
-      <c r="E24" s="52" t="s">
-        <v>1844</v>
-      </c>
-      <c r="F24" s="52" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="60" t="s">
-        <v>1846</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>1847</v>
-      </c>
-      <c r="E25" s="52" t="s">
-        <v>1848</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="60" t="s">
-        <v>1849</v>
-      </c>
-      <c r="B26" s="52" t="s">
-        <v>1850</v>
-      </c>
-      <c r="E26" s="52" t="s">
-        <v>1851</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28"/>
-      <c r="C28"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29"/>
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30"/>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31"/>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32"/>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33"/>
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34"/>
-      <c r="F34"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35"/>
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36"/>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37"/>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38"/>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39"/>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40"/>
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41"/>
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42"/>
-      <c r="F42"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43"/>
-      <c r="F43"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44"/>
-      <c r="F44"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45"/>
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46"/>
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47"/>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48"/>
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49"/>
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50"/>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51"/>
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52"/>
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53"/>
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54"/>
-      <c r="F54"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55"/>
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56"/>
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57"/>
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58"/>
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59"/>
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60"/>
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61"/>
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62"/>
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63"/>
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64"/>
-      <c r="F64"/>
+    <row r="10" spans="1:5" s="32" customFormat="1">
+      <c r="A10" s="69" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="83" t="s">
+        <v>2105</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" s="32" customFormat="1">
+      <c r="A11" s="83"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" s="32" customFormat="1">
+      <c r="A12" s="83"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" s="32" customFormat="1">
+      <c r="A13" s="83"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" s="32" customFormat="1">
+      <c r="A14" s="83"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" s="32" customFormat="1">
+      <c r="A15" s="83"/>
+      <c r="B15" s="83"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" s="32" customFormat="1">
+      <c r="A16" s="83"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" s="32" customFormat="1">
+      <c r="A17" s="83"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="2"/>
+      <c r="J17"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:11" s="32" customFormat="1">
+      <c r="A18" s="83"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="2"/>
+      <c r="J18"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:11" s="32" customFormat="1">
+      <c r="A19" s="83"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="2"/>
+      <c r="J19"/>
+      <c r="K19"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="83"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="84"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="85"/>
+    </row>
+    <row r="22" spans="1:11" s="42" customFormat="1">
+      <c r="A22" s="86"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="86"/>
+      <c r="J22"/>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="83"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="83"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="83"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="83"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="84"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="84"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="83"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" s="83"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" s="83"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" s="83"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="83"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="84"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="84"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="83"/>
+      <c r="B33" s="83"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="83"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="83"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="83"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="83"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="84"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="84"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="83"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="83"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="83"/>
+      <c r="B40" s="83"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="83"/>
+      <c r="B41" s="83"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="83"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="84"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="84"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="83"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="83"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="83"/>
+      <c r="B44" s="83"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="83"/>
+      <c r="E44" s="83"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="83"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="83"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="83"/>
+      <c r="B46" s="83"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="83"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="84"/>
+      <c r="B47" s="84"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="84"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="83"/>
+      <c r="B48" s="83"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="83"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="83"/>
+      <c r="B49" s="83"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="83"/>
+      <c r="E49" s="83"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="83"/>
+      <c r="B50" s="83"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="83"/>
+      <c r="E50" s="83"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="83"/>
+      <c r="B51" s="83"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="83"/>
+      <c r="E51" s="83"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="84"/>
+      <c r="B52" s="84"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="84"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="83"/>
+      <c r="B53" s="83"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="83"/>
+      <c r="E53" s="83"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="83"/>
+      <c r="B54" s="83"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="83"/>
+      <c r="E54" s="83"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="83"/>
+      <c r="B55" s="83"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="83"/>
+      <c r="E55" s="83"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -29123,6 +29225,474 @@
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B730C132-AF0D-4124-AB29-0565D21E3ED1}">
+  <dimension ref="A1:F64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="52" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="52" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="52" customWidth="1"/>
+    <col min="5" max="5" width="88.7109375" style="52" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" style="52" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="52"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="64" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="60" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C10" s="61"/>
+      <c r="E10" s="61" t="s">
+        <v>1802</v>
+      </c>
+      <c r="F10" s="52" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="46" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>1805</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="46" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>1808</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>1809</v>
+      </c>
+      <c r="F12" s="52" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="46" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>1812</v>
+      </c>
+      <c r="C13"/>
+      <c r="E13" s="52" t="s">
+        <v>1813</v>
+      </c>
+      <c r="F13" s="52" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="60" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>1816</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="46" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>1819</v>
+      </c>
+      <c r="C15"/>
+      <c r="E15" s="52" t="s">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="60" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C16" s="50"/>
+      <c r="F16" s="52" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="60" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C17" s="61"/>
+      <c r="E17" s="52" t="s">
+        <v>1824</v>
+      </c>
+      <c r="F17" s="52" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="60" t="s">
+        <v>1826</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="60" t="s">
+        <v>1828</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="60" t="s">
+        <v>1830</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="60" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="46" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C22"/>
+      <c r="E22" s="52" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="46" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C23"/>
+      <c r="E23" s="52" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F23" s="52" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="46" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C24"/>
+      <c r="E24" s="52" t="s">
+        <v>1844</v>
+      </c>
+      <c r="F24" s="52" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="60" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>1847</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="60" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>1850</v>
+      </c>
+      <c r="E26" s="52" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28"/>
+      <c r="C28"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29"/>
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30"/>
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33"/>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34"/>
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35"/>
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37"/>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41"/>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42"/>
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43"/>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45"/>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46"/>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47"/>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48"/>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49"/>
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50"/>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51"/>
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52"/>
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53"/>
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54"/>
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55"/>
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56"/>
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57"/>
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58"/>
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59"/>
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60"/>
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61"/>
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62"/>
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63"/>
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64"/>
+      <c r="F64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29227,10 +29797,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
-      <c r="A10" s="71">
+      <c r="A10" s="70">
         <v>15</v>
       </c>
-      <c r="B10" s="71">
+      <c r="B10" s="70">
         <v>15</v>
       </c>
       <c r="C10" s="43"/>
@@ -29582,22 +30152,22 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="O27">
-    <cfRule type="expression" dxfId="29" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>OR($AD27="X",$AC27="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>AND($AD27=1,$AC27=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>$AD27=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>$AC27=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>AND(NOT(ISBLANK($V27)),ISBLANK($AC27),ISBLANK($AD27))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="6">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>AND($Q27="X",OR($B27&lt;&gt;"",$C27&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33467,17 +34037,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3991FE2B-C9FE-43D1-B302-70CA3C5EF889}">
   <dimension ref="A1:H188"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -37373,7 +37943,7 @@
       </c>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:5" ht="39">
+    <row r="60" spans="1:5" ht="51.75">
       <c r="A60" s="2" t="s">
         <v>1278</v>
       </c>
@@ -37881,58 +38451,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -38346,6 +38864,58 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
@@ -38355,24 +38925,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1BDBD4-E316-45AC-920A-A6692C88096C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -38390,4 +38942,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.08.28 09:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1286" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45C4BA62-3063-2C41-BD49-6E027B24B112}"/>
+  <xr:revisionPtr revIDLastSave="1292" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C604EB38-E752-3A4D-A9F8-EF9536B01774}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26040" yWindow="2980" windowWidth="26040" windowHeight="20480" tabRatio="877" firstSheet="13" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -7264,14 +7264,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="6" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -15794,19 +15794,19 @@
   </sheetData>
   <autoFilter ref="A2:N38" xr:uid="{C501F445-31F5-46E1-AB08-5738D3066605}"/>
   <conditionalFormatting sqref="A3:N38">
+    <cfRule type="expression" dxfId="17" priority="61">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
     <cfRule type="expression" priority="62">
       <formula>ISODD(ROW())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="61">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:N39 A40:N224">
+    <cfRule type="expression" dxfId="16" priority="63">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39:N39 A40:N224">
     <cfRule type="expression" priority="64">
       <formula>ISODD(ROW())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="63">
-      <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:N5">
@@ -15850,11 +15850,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34:N37">
-    <cfRule type="expression" dxfId="7" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="16">
+      <formula>N34=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="40" stopIfTrue="1">
       <formula>N34="X"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="16">
-      <formula>N34=""</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -21453,7 +21453,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29F356B-BB22-47DE-A619-877383F0285B}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
@@ -30446,8 +30448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24418BCA-6BA9-46F7-8F30-546B2F7203DE}">
   <dimension ref="A1:F317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -38706,67 +38708,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="5a233c5be867259e7f523794110a7773">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71fc54e2a62b1985aea6da9d2195ce0c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -39180,20 +39121,83 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A0C22BD-AC09-42A1-93D5-445ECA25C3E7}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -39207,5 +39211,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A0C22BD-AC09-42A1-93D5-445ECA25C3E7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.08.29 11:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1356" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD31257F-106F-42B4-B411-A3BE63D29032}"/>
+  <xr:revisionPtr revIDLastSave="1358" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E8EE5F5-F8C2-4098-9266-F2A678286D6B}"/>
   <bookViews>
-    <workbookView xWindow="9090" yWindow="645" windowWidth="18135" windowHeight="11865" tabRatio="877" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -6077,9 +6077,6 @@
     <t>Décrit le niveau de précision des coordonnées GPS envoyées</t>
   </si>
   <si>
-    <t xml:space="preserve">Précision à l'échelle de la ville, </t>
-  </si>
-  <si>
     <t>Précision à l'échelle de la rue</t>
   </si>
   <si>
@@ -6089,9 +6086,6 @@
     <t>Point coordonnée GPS exact</t>
   </si>
   <si>
-    <t xml:space="preserve"> Précision de la localisation non évaluable par l'émetteur</t>
-  </si>
-  <si>
     <t>NEXSIS</t>
   </si>
   <si>
@@ -6672,6 +6666,12 @@
   </si>
   <si>
     <t>SP</t>
+  </si>
+  <si>
+    <t>Précision à l'échelle de la ville</t>
+  </si>
+  <si>
+    <t>Précision de la localisation non évaluable par l'émetteur</t>
   </si>
 </sst>
 </file>
@@ -11488,10 +11488,10 @@
   <dimension ref="A1:N224"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -11542,7 +11542,7 @@
         <v>1738</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
       <c r="K2" s="25" t="s">
         <v>1782</v>
@@ -11559,10 +11559,10 @@
     </row>
     <row r="3" spans="1:14" ht="15">
       <c r="A3" s="27" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="C3" s="76" t="str">
         <f>Filiere!$B$8</f>
@@ -11594,10 +11594,10 @@
     </row>
     <row r="4" spans="1:14" ht="15">
       <c r="A4" s="27" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="C4" s="77" t="str">
         <f>'Type d''intervention'!$B$8</f>
@@ -11632,7 +11632,7 @@
         <v>1719</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="C5" s="77" t="str">
         <f>'Origine de l''appel'!$B$8</f>
@@ -11821,7 +11821,7 @@
         <v>1719</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>2048</v>
+        <v>2046</v>
       </c>
       <c r="C10" s="76" t="str">
         <f>'Etats du dossier'!$B$8</f>
@@ -11856,7 +11856,7 @@
         <v>1719</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="C11" s="78" t="str">
         <f>'Nombre de patients-victimes'!$B$8</f>
@@ -11891,7 +11891,7 @@
         <v>1719</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="C12" s="78" t="str">
         <f>'Type du patient-victime'!$B$8</f>
@@ -11993,10 +11993,10 @@
     </row>
     <row r="15" spans="1:14" ht="15">
       <c r="A15" s="27" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>1976</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>1978</v>
       </c>
       <c r="C15" s="78" t="str">
         <f>'Lieu - Source ou type d''id'!$B$8</f>
@@ -12030,10 +12030,10 @@
     </row>
     <row r="16" spans="1:14" ht="15">
       <c r="A16" s="27" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="C16" s="78" t="str">
         <f>Precision!$B$8</f>
@@ -12067,10 +12067,10 @@
     </row>
     <row r="17" spans="1:14" ht="15">
       <c r="A17" s="27" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
       <c r="C17" s="78" t="str">
         <f>'Nom de la source'!$B$8</f>
@@ -12104,10 +12104,10 @@
     </row>
     <row r="18" spans="1:14" ht="15">
       <c r="A18" s="27" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="C18" s="78" t="str">
         <f>'Type d''objet'!$B$8</f>
@@ -12144,7 +12144,7 @@
         <v>1722</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
       <c r="C19" s="78" t="str">
         <f>Signalement!$B$8</f>
@@ -12179,7 +12179,7 @@
         <v>1722</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="C20" s="78" t="str">
         <f>Canal!$B$8</f>
@@ -12216,7 +12216,7 @@
         <v>1722</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="C21" s="78" t="str">
         <f>'Type de contact'!$B$8</f>
@@ -12327,7 +12327,7 @@
         <v>1736</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="C24" s="76" t="str">
         <f>'Patient - type d''Id'!$B$8</f>
@@ -12398,7 +12398,7 @@
     </row>
     <row r="26" spans="1:14" ht="15">
       <c r="A26" s="28" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>1733</v>
@@ -12433,10 +12433,10 @@
     </row>
     <row r="27" spans="1:14" ht="15">
       <c r="A27" s="28" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="C27" s="76" t="str">
         <f>Role!$B$8</f>
@@ -12471,7 +12471,7 @@
         <v>1737</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>2043</v>
+        <v>2041</v>
       </c>
       <c r="C28" s="76" t="str">
         <f>'Type de decision'!$B$8</f>
@@ -12586,7 +12586,7 @@
     </row>
     <row r="31" spans="1:14" ht="15">
       <c r="A31" s="27" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>1741</v>
@@ -12628,7 +12628,7 @@
         <v>1737</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
       <c r="C32" s="77" t="str">
         <f>'Type de destination'!$B$8</f>
@@ -12731,7 +12731,7 @@
         <v>1744</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>2125</v>
+        <v>2123</v>
       </c>
       <c r="C35" s="77" t="str">
         <f>'Delai d''intervention'!$B$8</f>
@@ -12765,10 +12765,10 @@
     </row>
     <row r="36" spans="1:14" ht="15">
       <c r="A36" s="28" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
       <c r="C36" s="86" t="str">
         <f>'Annulation DR'!$B$8</f>
@@ -12800,10 +12800,10 @@
     </row>
     <row r="37" spans="1:14" ht="15">
       <c r="A37" s="28" t="s">
-        <v>2042</v>
+        <v>2040</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>2041</v>
+        <v>2039</v>
       </c>
       <c r="C37" s="77" t="str">
         <f>'Reponse demande ressources'!$B$8</f>
@@ -17939,7 +17939,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -18360,8 +18360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B0CB38-6314-4064-A5AE-C4AA5D27D31D}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -18463,7 +18463,7 @@
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52" t="s">
-        <v>1933</v>
+        <v>2130</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -18476,7 +18476,7 @@
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -18489,7 +18489,7 @@
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -18502,7 +18502,7 @@
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -18515,7 +18515,7 @@
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52" t="s">
-        <v>1937</v>
+        <v>2131</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -18842,7 +18842,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -18888,7 +18888,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -18911,10 +18911,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="52" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -18922,10 +18922,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -18933,10 +18933,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -19282,7 +19282,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -19328,7 +19328,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -19351,10 +19351,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="52" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -19362,10 +19362,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -19384,10 +19384,10 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52"/>
@@ -19395,10 +19395,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -19727,7 +19727,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -19773,7 +19773,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -19796,10 +19796,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="52" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -19807,10 +19807,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -20163,7 +20163,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -20209,7 +20209,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -20232,10 +20232,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="52" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -20243,10 +20243,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -20254,10 +20254,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -20265,10 +20265,10 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52"/>
@@ -20276,10 +20276,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -20287,10 +20287,10 @@
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1">
       <c r="A15" s="52" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52"/>
@@ -20588,7 +20588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52670871-FFE0-4B71-AFFC-AFEDF834F777}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -20615,7 +20615,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -20661,7 +20661,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -20684,27 +20684,27 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="68" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -20713,24 +20713,24 @@
         <v>1389</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -21074,7 +21074,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -21120,7 +21120,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -21143,10 +21143,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="52" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -21154,10 +21154,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -21176,10 +21176,10 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52"/>
@@ -21187,10 +21187,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -21198,10 +21198,10 @@
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1">
       <c r="A15" s="52" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52"/>
@@ -22245,7 +22245,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -22291,7 +22291,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -22314,66 +22314,66 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="52" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="2" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="2" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="2" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="2" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="2" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -23285,7 +23285,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -23331,7 +23331,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -23354,53 +23354,53 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="70" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="71" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B11" s="71" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="72" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="71" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B12" s="71" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="71" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="B13" s="71" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -23413,7 +23413,7 @@
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -23426,7 +23426,7 @@
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -24204,7 +24204,7 @@
         <v>1545</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
       <c r="D2" s="3"/>
     </row>
@@ -24300,7 +24300,7 @@
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19" t="s">
-        <v>2126</v>
+        <v>2124</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="19"/>
@@ -24346,18 +24346,18 @@
     </row>
     <row r="15" spans="1:6" s="19" customFormat="1" ht="12.75">
       <c r="A15" s="19" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="19" customFormat="1" ht="12.75">
       <c r="A16" s="19" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>2095</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="19" customFormat="1" ht="12.75">
@@ -24370,10 +24370,10 @@
     </row>
     <row r="18" spans="1:6" s="19" customFormat="1" ht="12.75">
       <c r="A18" s="19" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="19" customFormat="1" ht="12.75">
@@ -24381,7 +24381,7 @@
         <v>1380</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>2098</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="19" customFormat="1" ht="12.75">
@@ -24389,7 +24389,7 @@
         <v>1684</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -24418,27 +24418,27 @@
     </row>
     <row r="23" spans="1:6" s="32" customFormat="1">
       <c r="A23" s="19" t="s">
-        <v>2127</v>
+        <v>2125</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19" t="s">
-        <v>2128</v>
+        <v>2126</v>
       </c>
       <c r="E23" s="19"/>
     </row>
     <row r="24" spans="1:6" s="32" customFormat="1">
       <c r="A24" s="19" t="s">
-        <v>2129</v>
+        <v>2127</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19" t="s">
-        <v>2130</v>
+        <v>2128</v>
       </c>
       <c r="E24" s="19"/>
     </row>
     <row r="25" spans="1:6" s="32" customFormat="1">
       <c r="A25" s="19" t="s">
-        <v>2131</v>
+        <v>2129</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="19" t="s">
@@ -24476,7 +24476,7 @@
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19" t="s">
-        <v>2099</v>
+        <v>2097</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
@@ -24487,7 +24487,7 @@
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19" t="s">
-        <v>2100</v>
+        <v>2098</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
@@ -24498,18 +24498,18 @@
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19" t="s">
-        <v>2101</v>
+        <v>2099</v>
       </c>
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="1:6" s="53" customFormat="1">
       <c r="A31" s="19" t="s">
-        <v>2102</v>
+        <v>2100</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19" t="s">
-        <v>2103</v>
+        <v>2101</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
@@ -24533,7 +24533,7 @@
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="19" t="s">
-        <v>2104</v>
+        <v>2102</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
@@ -24541,11 +24541,11 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="19" t="s">
-        <v>2105</v>
+        <v>2103</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
@@ -24557,7 +24557,7 @@
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="19" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
@@ -24838,7 +24838,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -25015,7 +25015,7 @@
       </c>
       <c r="B21" s="53"/>
       <c r="C21" s="53" t="s">
-        <v>2044</v>
+        <v>2042</v>
       </c>
       <c r="D21" s="53"/>
       <c r="E21" s="52" t="s">
@@ -25141,7 +25141,7 @@
       </c>
       <c r="B31" s="52"/>
       <c r="C31" s="52" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
       <c r="D31" s="52"/>
       <c r="E31" s="52" t="s">
@@ -25668,7 +25668,7 @@
       </c>
       <c r="B72" s="52"/>
       <c r="C72" s="52" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
       <c r="D72" s="52"/>
       <c r="E72" s="52" t="s">
@@ -25765,7 +25765,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -25811,7 +25811,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -25834,10 +25834,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="68" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -25845,10 +25845,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -25856,10 +25856,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -26625,7 +26625,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2057</v>
+        <v>2055</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -26671,7 +26671,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -26694,10 +26694,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="68" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -26708,7 +26708,7 @@
         <v>1312</v>
       </c>
       <c r="B11" s="74" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -26716,10 +26716,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
       <c r="B12" s="74" t="s">
-        <v>2061</v>
+        <v>2059</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -26727,7 +26727,7 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="B13" s="74" t="s">
         <v>679</v>
@@ -26738,10 +26738,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -26752,7 +26752,7 @@
         <v>1338</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>2063</v>
+        <v>2061</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52"/>
@@ -27641,7 +27641,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
@@ -27861,7 +27861,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -27906,7 +27906,7 @@
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -27914,14 +27914,14 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2109</v>
+        <v>2107</v>
       </c>
       <c r="B12" s="52" t="s">
         <v>1894</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52" t="s">
-        <v>2117</v>
+        <v>2115</v>
       </c>
       <c r="E12" s="2">
         <v>3</v>
@@ -27929,14 +27929,14 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2110</v>
+        <v>2108</v>
       </c>
       <c r="B13" s="52" t="s">
         <v>1895</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52" t="s">
-        <v>2118</v>
+        <v>2116</v>
       </c>
       <c r="E13" s="2">
         <v>4</v>
@@ -27944,14 +27944,14 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
       <c r="B14" s="52" t="s">
         <v>1896</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52" t="s">
-        <v>2119</v>
+        <v>2117</v>
       </c>
       <c r="E14" s="2">
         <v>5</v>
@@ -27959,14 +27959,14 @@
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1">
       <c r="A15" s="52" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
       <c r="B15" s="52" t="s">
         <v>1897</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52" t="s">
-        <v>2120</v>
+        <v>2118</v>
       </c>
       <c r="E15" s="2">
         <v>6</v>
@@ -27974,14 +27974,14 @@
     </row>
     <row r="16" spans="1:5" s="32" customFormat="1">
       <c r="A16" s="52" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="B16" s="52" t="s">
         <v>1898</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="52" t="s">
-        <v>2121</v>
+        <v>2119</v>
       </c>
       <c r="E16" s="2">
         <v>7</v>
@@ -27989,14 +27989,14 @@
     </row>
     <row r="17" spans="1:5" s="32" customFormat="1">
       <c r="A17" s="52" t="s">
-        <v>2114</v>
+        <v>2112</v>
       </c>
       <c r="B17" s="52" t="s">
         <v>1899</v>
       </c>
       <c r="C17" s="43"/>
       <c r="D17" s="52" t="s">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="E17" s="2">
         <v>8</v>
@@ -28004,14 +28004,14 @@
     </row>
     <row r="18" spans="1:5" s="32" customFormat="1">
       <c r="A18" s="52" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
       <c r="B18" s="52" t="s">
         <v>1900</v>
       </c>
       <c r="C18" s="43"/>
       <c r="D18" s="52" t="s">
-        <v>2123</v>
+        <v>2121</v>
       </c>
       <c r="E18" s="2">
         <v>9</v>
@@ -28019,14 +28019,14 @@
     </row>
     <row r="19" spans="1:5" s="32" customFormat="1">
       <c r="A19" s="52" t="s">
-        <v>2116</v>
+        <v>2114</v>
       </c>
       <c r="B19" s="52" t="s">
         <v>1901</v>
       </c>
       <c r="C19" s="43"/>
       <c r="D19" s="52" t="s">
-        <v>2124</v>
+        <v>2122</v>
       </c>
       <c r="E19" s="2">
         <v>10</v>
@@ -28329,7 +28329,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -28375,7 +28375,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="81" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -28398,14 +28398,14 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="68" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
       <c r="B10" s="82" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="82" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -28772,7 +28772,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -28824,7 +28824,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>2033</v>
+        <v>2031</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -28851,57 +28851,57 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="60" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="19" t="s">
-        <v>2038</v>
+        <v>2036</v>
       </c>
       <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="46" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="19" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="46" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>2036</v>
+        <v>2034</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="19" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
       <c r="F12" s="16"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="46" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>2037</v>
+        <v>2035</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="19" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="F13" s="16"/>
     </row>
@@ -29857,7 +29857,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="75" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>1594</v>
@@ -30180,7 +30180,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -30226,7 +30226,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -30256,7 +30256,7 @@
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="2" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -30269,7 +30269,7 @@
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="2" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -30282,7 +30282,7 @@
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="2" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -30295,7 +30295,7 @@
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="2" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -30308,7 +30308,7 @@
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="2" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -31769,7 +31769,7 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -31781,7 +31781,7 @@
     </row>
     <row r="93" spans="1:6" ht="26.25">
       <c r="A93" s="2" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -31795,7 +31795,7 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
@@ -31808,7 +31808,7 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="2" t="s">
@@ -31820,7 +31820,7 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2" t="s">
-        <v>2086</v>
+        <v>2084</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -31832,7 +31832,7 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2" t="s">
-        <v>2087</v>
+        <v>2085</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -31844,7 +31844,7 @@
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="2" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -38437,7 +38437,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>2056</v>
+        <v>2054</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -38483,7 +38483,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -38506,10 +38506,10 @@
     </row>
     <row r="10" spans="1:5" s="32" customFormat="1">
       <c r="A10" s="68" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>2052</v>
+        <v>2050</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="52"/>
@@ -38517,10 +38517,10 @@
     </row>
     <row r="11" spans="1:5" s="32" customFormat="1">
       <c r="A11" s="52" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>2051</v>
+        <v>2049</v>
       </c>
       <c r="C11" s="43"/>
       <c r="D11" s="52"/>
@@ -38528,10 +38528,10 @@
     </row>
     <row r="12" spans="1:5" s="32" customFormat="1">
       <c r="A12" s="52" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="52"/>
@@ -38539,10 +38539,10 @@
     </row>
     <row r="13" spans="1:5" s="32" customFormat="1">
       <c r="A13" s="52" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="52"/>
@@ -38550,10 +38550,10 @@
     </row>
     <row r="14" spans="1:5" s="32" customFormat="1">
       <c r="A14" s="52" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="C14" s="43"/>
       <c r="D14" s="52"/>
@@ -38561,10 +38561,10 @@
     </row>
     <row r="15" spans="1:5" s="32" customFormat="1">
       <c r="A15" s="52" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="C15" s="43"/>
       <c r="D15" s="52"/>
@@ -38572,10 +38572,10 @@
     </row>
     <row r="16" spans="1:5" s="32" customFormat="1">
       <c r="A16" s="52" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="52"/>

</xml_diff>

<commit_message>
[24.09.05 15:38] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1358" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E8EE5F5-F8C2-4098-9266-F2A678286D6B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="1590" windowWidth="21045" windowHeight="14610" tabRatio="877" firstSheet="14" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -18360,7 +18360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B0CB38-6314-4064-A5AE-C4AA5D27D31D}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -23729,8 +23729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DA8262-2222-433E-B162-3866A2FDA084}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -38372,7 +38372,7 @@
       </c>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:5" ht="39">
+    <row r="60" spans="1:5" ht="51.75">
       <c r="A60" s="2" t="s">
         <v>1274</v>
       </c>
@@ -38871,67 +38871,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -39345,33 +39284,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D81159C-31FE-4FCD-8462-8FEDAB97280E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -39389,4 +39363,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.09.11 17:40] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1358" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E8EE5F5-F8C2-4098-9266-F2A678286D6B}"/>
+  <xr:revisionPtr revIDLastSave="1359" documentId="13_ncr:1_{39F4392A-9E63-F244-B431-F45D1B40DCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F871DD72-3148-4B80-ADC0-CBAF93145BE2}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2340" yWindow="1590" windowWidth="21045" windowHeight="14610" tabRatio="877" firstSheet="14" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="345" windowWidth="28110" windowHeight="15225" tabRatio="877" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="38" r:id="rId1"/>
@@ -11790,7 +11790,7 @@
       </c>
       <c r="D9" s="49" t="str">
         <f>'Motif de recours médico-secouri'!$B$1</f>
-        <v>SI-SAMU</v>
+        <v>CISU</v>
       </c>
       <c r="E9" s="27" t="str">
         <f>'Motif de recours médico-secouri'!$B$2</f>
@@ -23729,7 +23729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DA8262-2222-433E-B162-3866A2FDA084}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -37690,8 +37690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8116353-BC00-4857-8D37-9470DD9A948C}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -37708,7 +37708,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1280</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -38372,7 +38372,7 @@
       </c>
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:5" ht="51.75">
+    <row r="60" spans="1:5" ht="39">
       <c r="A60" s="2" t="s">
         <v>1274</v>
       </c>
@@ -38871,6 +38871,67 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -39284,68 +39345,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D81159C-31FE-4FCD-8462-8FEDAB97280E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -39363,30 +39389,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBBB1551-8692-41DC-9582-B0EFCC1A2247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.11.25 17:11] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="196" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{981E77C6-8E74-4021-B42D-A7C3EEDD3006}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="765" windowWidth="24765" windowHeight="14145" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -9286,7 +9286,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9433,10 +9433,9 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -9449,885 +9448,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in 60% - Accent5" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="143">
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF58383"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10374,74 +9512,44 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
+          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
+          <bgColor rgb="FFFFE1FF"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF58383"/>
         </patternFill>
       </fill>
     </dxf>
@@ -11198,25 +10306,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P224"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="69.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="69.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="16" width="12.7109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="30.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16" width="12.6640625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -11226,7 +10334,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" ht="15">
+    <row r="2" spans="1:16" s="4" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -11276,7 +10384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15">
+    <row r="3" spans="1:16">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -11315,7 +10423,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="15">
+    <row r="4" spans="1:16">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -11354,7 +10462,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
     </row>
-    <row r="5" spans="1:16" ht="15">
+    <row r="5" spans="1:16">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -11393,7 +10501,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
     </row>
-    <row r="6" spans="1:16" ht="15">
+    <row r="6" spans="1:16">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -11436,7 +10544,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
     </row>
-    <row r="7" spans="1:16" ht="15">
+    <row r="7" spans="1:16">
       <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
@@ -11481,7 +10589,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
     </row>
-    <row r="8" spans="1:16" ht="15">
+    <row r="8" spans="1:16">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -11522,7 +10630,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" spans="1:16" ht="15">
+    <row r="9" spans="1:16">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -11565,7 +10673,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="1:16" ht="15">
+    <row r="10" spans="1:16">
       <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
@@ -11604,7 +10712,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="1:16" ht="15">
+    <row r="11" spans="1:16">
       <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
@@ -11643,7 +10751,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="1:16" ht="15">
+    <row r="12" spans="1:16">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -11682,7 +10790,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="1:16" ht="15">
+    <row r="13" spans="1:16">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -11721,7 +10829,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="1:16" ht="15">
+    <row r="14" spans="1:16">
       <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
@@ -11760,7 +10868,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="1:16" ht="15">
+    <row r="15" spans="1:16">
       <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
@@ -11801,7 +10909,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="1:16" ht="15">
+    <row r="16" spans="1:16">
       <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
@@ -11842,7 +10950,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:16" ht="15">
+    <row r="17" spans="1:16">
       <c r="A17" s="5" t="s">
         <v>49</v>
       </c>
@@ -11883,7 +10991,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="1:16" ht="15">
+    <row r="18" spans="1:16">
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
@@ -11924,7 +11032,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
     </row>
-    <row r="19" spans="1:16" ht="15">
+    <row r="19" spans="1:16">
       <c r="A19" s="5" t="s">
         <v>53</v>
       </c>
@@ -11963,7 +11071,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" spans="1:16" ht="15">
+    <row r="20" spans="1:16">
       <c r="A20" s="5" t="s">
         <v>56</v>
       </c>
@@ -12004,7 +11112,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
     </row>
-    <row r="21" spans="1:16" ht="15">
+    <row r="21" spans="1:16">
       <c r="A21" s="5" t="s">
         <v>58</v>
       </c>
@@ -12045,7 +11153,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="1:16" ht="15">
+    <row r="22" spans="1:16">
       <c r="A22" s="9" t="s">
         <v>60</v>
       </c>
@@ -12083,7 +11191,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" spans="1:16" ht="15">
+    <row r="23" spans="1:16">
       <c r="A23" s="5" t="s">
         <v>63</v>
       </c>
@@ -12124,7 +11232,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
     </row>
-    <row r="24" spans="1:16" ht="15">
+    <row r="24" spans="1:16">
       <c r="A24" s="5" t="s">
         <v>65</v>
       </c>
@@ -12165,7 +11273,7 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="1:16" ht="15">
+    <row r="25" spans="1:16">
       <c r="A25" s="9" t="s">
         <v>67</v>
       </c>
@@ -12206,7 +11314,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="1:16" ht="15">
+    <row r="26" spans="1:16">
       <c r="A26" s="9" t="s">
         <v>70</v>
       </c>
@@ -12251,7 +11359,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="1:16" ht="15">
+    <row r="27" spans="1:16">
       <c r="A27" s="9" t="s">
         <v>72</v>
       </c>
@@ -12290,7 +11398,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="1:16" ht="15">
+    <row r="28" spans="1:16">
       <c r="A28" s="9" t="s">
         <v>75</v>
       </c>
@@ -12331,7 +11439,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="1:16" ht="15">
+    <row r="29" spans="1:16">
       <c r="A29" s="5" t="s">
         <v>78</v>
       </c>
@@ -12370,7 +11478,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="1:16" ht="15">
+    <row r="30" spans="1:16">
       <c r="A30" s="5" t="s">
         <v>81</v>
       </c>
@@ -12416,7 +11524,7 @@
       </c>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" spans="1:16" ht="15">
+    <row r="31" spans="1:16">
       <c r="A31" s="9" t="s">
         <v>84</v>
       </c>
@@ -12461,7 +11569,7 @@
       </c>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="1:16" ht="15">
+    <row r="32" spans="1:16">
       <c r="A32" s="5" t="s">
         <v>86</v>
       </c>
@@ -12504,7 +11612,7 @@
       </c>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="1:16" ht="15">
+    <row r="33" spans="1:16">
       <c r="A33" s="5" t="s">
         <v>89</v>
       </c>
@@ -12543,7 +11651,7 @@
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="1:16" ht="15">
+    <row r="34" spans="1:16">
       <c r="A34" s="9" t="s">
         <v>91</v>
       </c>
@@ -12582,7 +11690,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="1:16" ht="15">
+    <row r="35" spans="1:16">
       <c r="A35" s="9" t="s">
         <v>94</v>
       </c>
@@ -12619,7 +11727,7 @@
       </c>
       <c r="P35" s="10"/>
     </row>
-    <row r="36" spans="1:16" ht="15">
+    <row r="36" spans="1:16">
       <c r="A36" s="9" t="s">
         <v>96</v>
       </c>
@@ -12660,7 +11768,7 @@
       </c>
       <c r="P36" s="10"/>
     </row>
-    <row r="37" spans="1:16" ht="15">
+    <row r="37" spans="1:16">
       <c r="A37" s="9" t="s">
         <v>98</v>
       </c>
@@ -12699,7 +11807,7 @@
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
     </row>
-    <row r="38" spans="1:16" ht="15">
+    <row r="38" spans="1:16">
       <c r="A38" s="9" t="s">
         <v>101</v>
       </c>
@@ -12738,7 +11846,7 @@
       </c>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="1:16" ht="15">
+    <row r="39" spans="1:16">
       <c r="A39" s="9" t="s">
         <v>104</v>
       </c>
@@ -12779,7 +11887,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15">
+    <row r="40" spans="1:16">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="14"/>
@@ -12797,7 +11905,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="1:16" ht="15">
+    <row r="41" spans="1:16">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="14"/>
@@ -16112,93 +15220,93 @@
   </sheetData>
   <autoFilter ref="A2:P2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="142" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:A224">
-    <cfRule type="expression" dxfId="141" priority="9">
+    <cfRule type="expression" dxfId="30" priority="9">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:P39">
-    <cfRule type="expression" dxfId="140" priority="7">
+    <cfRule type="expression" dxfId="29" priority="7">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:P224">
-    <cfRule type="expression" dxfId="139" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:G22">
-    <cfRule type="expression" dxfId="138" priority="5">
+    <cfRule type="expression" dxfId="27" priority="5">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:P22">
-    <cfRule type="expression" dxfId="137" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:P22 B40:P224">
-    <cfRule type="expression" dxfId="136" priority="23">
+    <cfRule type="expression" dxfId="25" priority="23">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:J22">
-    <cfRule type="expression" dxfId="135" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:P45">
-    <cfRule type="expression" dxfId="134" priority="21">
+    <cfRule type="expression" dxfId="23" priority="21">
       <formula>I3="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:P122">
-    <cfRule type="expression" dxfId="133" priority="17">
+    <cfRule type="expression" dxfId="22" priority="17">
       <formula>I3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:P122">
-    <cfRule type="expression" dxfId="132" priority="18">
+    <cfRule type="expression" dxfId="21" priority="18">
       <formula>I46="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:L7">
-    <cfRule type="expression" dxfId="131" priority="16">
+    <cfRule type="expression" dxfId="20" priority="16">
       <formula>K6="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:L9">
-    <cfRule type="expression" dxfId="130" priority="15">
+    <cfRule type="expression" dxfId="19" priority="15">
       <formula>K9="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:L26">
-    <cfRule type="expression" dxfId="129" priority="14">
+    <cfRule type="expression" dxfId="18" priority="14">
       <formula>K26="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:L32">
-    <cfRule type="expression" dxfId="128" priority="13">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>K30="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25:L26">
-    <cfRule type="expression" dxfId="127" priority="11">
+    <cfRule type="expression" dxfId="16" priority="11">
       <formula>L25="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="expression" dxfId="126" priority="12">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>L28="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P35:P38">
-    <cfRule type="expression" dxfId="125" priority="19">
+    <cfRule type="expression" dxfId="14" priority="19">
       <formula>P35=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="20">
+    <cfRule type="expression" dxfId="13" priority="20">
       <formula>P35="X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16254,12 +15362,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16475,12 +15583,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16692,14 +15800,14 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="67.5" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17220,14 +16328,14 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="51.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="51.83203125" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17622,12 +16730,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17839,12 +16947,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="154.83203125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18059,12 +17167,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18238,13 +17346,13 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18428,12 +17536,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18632,13 +17740,13 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18849,17 +17957,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18924,7 +18032,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="25" customFormat="1">
+    <row r="7" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A7" s="22" t="s">
         <v>119</v>
       </c>
@@ -19220,11 +18328,11 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19423,12 +18531,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="104.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="104.5" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -21699,7 +20807,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="54" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -21714,13 +20822,13 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="86.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="86.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -21785,7 +20893,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="7" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A7" s="25" t="s">
         <v>2164</v>
       </c>
@@ -21797,7 +20905,7 @@
       </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="8" spans="1:5" s="25" customFormat="1" ht="45">
+    <row r="8" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A8" s="25" t="s">
         <v>2167</v>
       </c>
@@ -21809,7 +20917,7 @@
       </c>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="9" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A9" s="25" t="s">
         <v>2170</v>
       </c>
@@ -21821,7 +20929,7 @@
       </c>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="10" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A10" s="25" t="s">
         <v>2173</v>
       </c>
@@ -21833,7 +20941,7 @@
       </c>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="11" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A11" s="25" t="s">
         <v>2176</v>
       </c>
@@ -21845,7 +20953,7 @@
       </c>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="12" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A12" s="25" t="s">
         <v>2179</v>
       </c>
@@ -21857,7 +20965,7 @@
       </c>
       <c r="E12" s="23"/>
     </row>
-    <row r="13" spans="1:5" s="25" customFormat="1">
+    <row r="13" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A13" s="25" t="s">
         <v>2182</v>
       </c>
@@ -21869,7 +20977,7 @@
       </c>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="14" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A14" s="25" t="s">
         <v>2185</v>
       </c>
@@ -21881,7 +20989,7 @@
       </c>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="15" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A15" s="25" t="s">
         <v>2187</v>
       </c>
@@ -21893,7 +21001,7 @@
       </c>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="16" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A16" s="25" t="s">
         <v>2190</v>
       </c>
@@ -21905,7 +21013,7 @@
       </c>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" spans="1:5" s="25" customFormat="1" ht="45">
+    <row r="17" spans="1:5" s="25" customFormat="1" ht="48">
       <c r="A17" s="25" t="s">
         <v>2193</v>
       </c>
@@ -21917,7 +21025,7 @@
       </c>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" spans="1:5" s="25" customFormat="1" ht="60">
+    <row r="18" spans="1:5" s="25" customFormat="1" ht="48">
       <c r="A18" s="25" t="s">
         <v>2196</v>
       </c>
@@ -21929,7 +21037,7 @@
       </c>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" spans="1:5" s="25" customFormat="1" ht="45">
+    <row r="19" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A19" s="25" t="s">
         <v>2199</v>
       </c>
@@ -21941,7 +21049,7 @@
       </c>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="20" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A20" s="25" t="s">
         <v>2202</v>
       </c>
@@ -21953,7 +21061,7 @@
       </c>
       <c r="E20" s="23"/>
     </row>
-    <row r="21" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="21" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A21" s="25" t="s">
         <v>2205</v>
       </c>
@@ -21965,7 +21073,7 @@
       </c>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="22" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A22" s="25" t="s">
         <v>2208</v>
       </c>
@@ -21977,7 +21085,7 @@
       </c>
       <c r="E22" s="23"/>
     </row>
-    <row r="23" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="23" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A23" s="25" t="s">
         <v>2211</v>
       </c>
@@ -21989,7 +21097,7 @@
       </c>
       <c r="E23" s="23"/>
     </row>
-    <row r="24" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="24" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A24" s="25" t="s">
         <v>2214</v>
       </c>
@@ -22001,7 +21109,7 @@
       </c>
       <c r="E24" s="23"/>
     </row>
-    <row r="25" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="25" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A25" s="25" t="s">
         <v>2217</v>
       </c>
@@ -22013,7 +21121,7 @@
       </c>
       <c r="E25" s="23"/>
     </row>
-    <row r="26" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="26" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A26" s="25" t="s">
         <v>2220</v>
       </c>
@@ -22025,7 +21133,7 @@
       </c>
       <c r="E26" s="23"/>
     </row>
-    <row r="27" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="27" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A27" s="25" t="s">
         <v>2223</v>
       </c>
@@ -22067,7 +21175,7 @@
       <c r="D30" s="22"/>
       <c r="E30" s="23"/>
     </row>
-    <row r="31" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="31" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A31" s="25" t="s">
         <v>2232</v>
       </c>
@@ -22079,7 +21187,7 @@
       </c>
       <c r="E31" s="23"/>
     </row>
-    <row r="32" spans="1:5" s="25" customFormat="1">
+    <row r="32" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A32" s="25" t="s">
         <v>2235</v>
       </c>
@@ -22091,7 +21199,7 @@
       </c>
       <c r="E32" s="23"/>
     </row>
-    <row r="33" spans="1:5" s="25" customFormat="1" ht="30">
+    <row r="33" spans="1:5" s="25" customFormat="1" ht="32">
       <c r="A33" s="25" t="s">
         <v>2236</v>
       </c>
@@ -22103,7 +21211,7 @@
       </c>
       <c r="E33" s="23"/>
     </row>
-    <row r="34" spans="1:5" s="25" customFormat="1">
+    <row r="34" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A34" s="25" t="s">
         <v>1586</v>
       </c>
@@ -22115,7 +21223,7 @@
       </c>
       <c r="E34" s="23"/>
     </row>
-    <row r="35" spans="1:5" s="25" customFormat="1">
+    <row r="35" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A35" s="25" t="s">
         <v>1420</v>
       </c>
@@ -22144,12 +21252,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="4" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="2" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22222,7 +21330,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="42" t="s">
         <v>2245</v>
       </c>
@@ -22235,7 +21343,7 @@
         <v>2247</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="48">
       <c r="A8" s="42" t="s">
         <v>2248</v>
       </c>
@@ -22248,7 +21356,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45">
+    <row r="9" spans="1:6" ht="32">
       <c r="A9" s="42" t="s">
         <v>2251</v>
       </c>
@@ -22261,7 +21369,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="32">
       <c r="A10" s="42" t="s">
         <v>1611</v>
       </c>
@@ -22274,7 +21382,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6" ht="32">
       <c r="A11" s="42" t="s">
         <v>2256</v>
       </c>
@@ -22287,7 +21395,7 @@
         <v>2258</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30">
+    <row r="12" spans="1:6" ht="32">
       <c r="A12" s="42" t="s">
         <v>2259</v>
       </c>
@@ -22300,7 +21408,7 @@
         <v>2261</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="32">
       <c r="A13" s="42" t="s">
         <v>2262</v>
       </c>
@@ -22313,7 +21421,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45">
+    <row r="14" spans="1:6" ht="48">
       <c r="A14" s="42" t="s">
         <v>1586</v>
       </c>
@@ -22326,7 +21434,7 @@
         <v>2266</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30">
+    <row r="15" spans="1:6" ht="32">
       <c r="A15" s="42" t="s">
         <v>2267</v>
       </c>
@@ -22440,12 +21548,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22665,13 +21773,13 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
-    <col min="6" max="6" width="61.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="6" max="6" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -22802,14 +21910,14 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -23208,12 +22316,12 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="79.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -23278,7 +22386,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="25" customFormat="1">
+    <row r="7" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A7" s="51" t="s">
         <v>2313</v>
       </c>
@@ -23286,7 +22394,7 @@
         <v>2850</v>
       </c>
       <c r="C7" s="23"/>
-      <c r="D7" s="71" t="s">
+      <c r="D7" t="s">
         <v>2314</v>
       </c>
       <c r="E7"/>
@@ -23299,7 +22407,7 @@
         <v>2315</v>
       </c>
       <c r="C8" s="23"/>
-      <c r="D8" s="71" t="s">
+      <c r="D8" t="s">
         <v>2316</v>
       </c>
       <c r="E8"/>
@@ -23446,14 +22554,14 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="170.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="170.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -23868,14 +22976,14 @@
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" customWidth="1"/>
+    <col min="6" max="6" width="69.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -24462,13 +23570,13 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -24533,7 +23641,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="25" customFormat="1">
+    <row r="7" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A7" s="22" t="s">
         <v>2807</v>
       </c>
@@ -24899,15 +24007,15 @@
       <selection activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="25" customWidth="1"/>
     <col min="3" max="3" width="56" style="25" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="25" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="25" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="25"/>
+    <col min="4" max="4" width="17.6640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="25" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" customFormat="1">
@@ -25424,7 +24532,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.75">
+    <row r="49" spans="1:5" ht="16">
       <c r="A49" s="25" t="s">
         <v>2499</v>
       </c>
@@ -25436,7 +24544,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.75">
+    <row r="50" spans="1:5" ht="16">
       <c r="A50" s="25" t="s">
         <v>2501</v>
       </c>
@@ -25448,7 +24556,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75">
+    <row r="51" spans="1:5" ht="16">
       <c r="A51" s="25" t="s">
         <v>2503</v>
       </c>
@@ -25460,7 +24568,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.75">
+    <row r="52" spans="1:5" ht="16">
       <c r="A52" s="25" t="s">
         <v>2505</v>
       </c>
@@ -25472,7 +24580,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.75">
+    <row r="53" spans="1:5" ht="16">
       <c r="A53" s="25" t="s">
         <v>2507</v>
       </c>
@@ -25484,7 +24592,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.75">
+    <row r="54" spans="1:5" ht="16">
       <c r="A54" s="25" t="s">
         <v>2509</v>
       </c>
@@ -25496,7 +24604,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.75">
+    <row r="55" spans="1:5" ht="16">
       <c r="A55" s="25" t="s">
         <v>2511</v>
       </c>
@@ -25508,7 +24616,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.75">
+    <row r="56" spans="1:5" ht="16">
       <c r="A56" s="25" t="s">
         <v>2513</v>
       </c>
@@ -25520,7 +24628,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15.75">
+    <row r="57" spans="1:5" ht="16">
       <c r="A57" s="25" t="s">
         <v>2515</v>
       </c>
@@ -25532,7 +24640,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.75">
+    <row r="58" spans="1:5" ht="16">
       <c r="A58" s="25" t="s">
         <v>2517</v>
       </c>
@@ -25544,7 +24652,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.75">
+    <row r="59" spans="1:5" ht="16">
       <c r="A59" s="25" t="s">
         <v>2519</v>
       </c>
@@ -25556,7 +24664,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15.75">
+    <row r="60" spans="1:5" ht="16">
       <c r="A60" s="25" t="s">
         <v>2521</v>
       </c>
@@ -25568,7 +24676,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.75">
+    <row r="61" spans="1:5" ht="16">
       <c r="A61" s="25" t="s">
         <v>2523</v>
       </c>
@@ -25580,7 +24688,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.75">
+    <row r="62" spans="1:5" ht="16">
       <c r="A62" s="25" t="s">
         <v>2525</v>
       </c>
@@ -25592,7 +24700,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.75">
+    <row r="63" spans="1:5" ht="16">
       <c r="A63" s="25" t="s">
         <v>2527</v>
       </c>
@@ -25723,13 +24831,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26128,13 +25236,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26199,7 +25307,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="25" customFormat="1">
+    <row r="7" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A7" s="22" t="s">
         <v>2550</v>
       </c>
@@ -26210,7 +25318,7 @@
       <c r="D7"/>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:5" s="25" customFormat="1">
+    <row r="8" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A8" s="22" t="s">
         <v>2858</v>
       </c>
@@ -26341,13 +25449,13 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="61.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.5" customWidth="1"/>
+    <col min="4" max="4" width="61.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26412,7 +25520,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="16">
       <c r="A7" s="56" t="s">
         <v>2561</v>
       </c>
@@ -26436,7 +25544,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="16">
       <c r="A9" s="56" t="s">
         <v>2363</v>
       </c>
@@ -26448,7 +25556,7 @@
         <v>2568</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="16">
       <c r="A10" s="56" t="s">
         <v>2348</v>
       </c>
@@ -26460,7 +25568,7 @@
         <v>2570</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="16">
       <c r="A11" s="56" t="s">
         <v>2571</v>
       </c>
@@ -26472,7 +25580,7 @@
         <v>2573</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="16">
       <c r="A12" s="56" t="s">
         <v>2544</v>
       </c>
@@ -26484,7 +25592,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="16">
       <c r="A13" s="56" t="s">
         <v>2576</v>
       </c>
@@ -26496,7 +25604,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="16">
       <c r="A14" s="60" t="s">
         <v>2579</v>
       </c>
@@ -26508,7 +25616,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="16">
       <c r="A15" s="61" t="s">
         <v>2581</v>
       </c>
@@ -26520,7 +25628,7 @@
         <v>2582</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="16">
       <c r="A16" s="56" t="s">
         <v>2583</v>
       </c>
@@ -26532,7 +25640,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="16">
       <c r="A17" s="56" t="s">
         <v>2585</v>
       </c>
@@ -26544,7 +25652,7 @@
         <v>2586</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="16">
       <c r="A18" s="56" t="s">
         <v>2587</v>
       </c>
@@ -26613,13 +25721,13 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="163.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="163.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26819,12 +25927,12 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="154.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="154.83203125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -27083,13 +26191,13 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="52.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -27154,7 +26262,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="25" customFormat="1">
+    <row r="7" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A7" s="22" t="s">
         <v>2656</v>
       </c>
@@ -27352,13 +26460,13 @@
       <selection activeCell="C1" sqref="B1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="74" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27431,7 +26539,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="16">
       <c r="A7" s="63" t="s">
         <v>2661</v>
       </c>
@@ -27445,7 +26553,7 @@
       </c>
       <c r="F7" s="42"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" ht="16">
       <c r="A8" s="56" t="s">
         <v>2663</v>
       </c>
@@ -27459,7 +26567,7 @@
       </c>
       <c r="F8" s="42"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="16">
       <c r="A9" s="56" t="s">
         <v>2665</v>
       </c>
@@ -27473,7 +26581,7 @@
       </c>
       <c r="F9" s="42"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="16">
       <c r="A10" s="56" t="s">
         <v>2667</v>
       </c>
@@ -27751,20 +26859,20 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" customWidth="1"/>
-    <col min="5" max="5" width="88.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+    <col min="5" max="5" width="88.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -27844,7 +26952,7 @@
       <c r="B7" s="57" t="s">
         <v>2672</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" t="s">
         <v>2863</v>
       </c>
       <c r="F7" t="s">
@@ -27858,18 +26966,18 @@
       <c r="B8" s="32" t="s">
         <v>2675</v>
       </c>
-      <c r="E8" s="77" t="s">
+      <c r="E8" s="75" t="s">
         <v>2864</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75">
+    <row r="9" spans="1:7" ht="16">
       <c r="A9" t="s">
         <v>2676</v>
       </c>
       <c r="B9" s="32" t="s">
         <v>2677</v>
       </c>
-      <c r="E9" s="78" t="s">
+      <c r="E9" s="76" t="s">
         <v>2865</v>
       </c>
       <c r="F9" t="s">
@@ -27877,26 +26985,26 @@
       </c>
       <c r="G9" s="64"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75">
+    <row r="10" spans="1:7" ht="16">
       <c r="A10" t="s">
         <v>2679</v>
       </c>
       <c r="B10" t="s">
         <v>2680</v>
       </c>
-      <c r="E10" s="79" t="s">
+      <c r="E10" s="69" t="s">
         <v>2866</v>
       </c>
       <c r="G10" s="54"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75">
+    <row r="11" spans="1:7" ht="16">
       <c r="A11" t="s">
         <v>2681</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>2682</v>
       </c>
-      <c r="E11" s="79" t="s">
+      <c r="E11" s="69" t="s">
         <v>2867</v>
       </c>
       <c r="F11" t="s">
@@ -27911,7 +27019,7 @@
       <c r="B12" s="57" t="s">
         <v>2685</v>
       </c>
-      <c r="E12" s="79" t="s">
+      <c r="E12" s="69" t="s">
         <v>2868</v>
       </c>
     </row>
@@ -27923,35 +27031,35 @@
         <v>2687</v>
       </c>
       <c r="C13" s="57"/>
-      <c r="E13" s="79" t="s">
+      <c r="E13" s="69" t="s">
         <v>2869</v>
       </c>
       <c r="F13" t="s">
         <v>2688</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="69" customFormat="1">
-      <c r="A14" s="72" t="s">
+    <row r="14" spans="1:7" s="69" customFormat="1" ht="16">
+      <c r="A14" s="71" t="s">
         <v>2860</v>
       </c>
-      <c r="B14" s="73" t="s">
+      <c r="B14" s="72" t="s">
         <v>2861</v>
       </c>
-      <c r="C14" s="74"/>
-      <c r="E14" s="77" t="s">
+      <c r="C14" s="73"/>
+      <c r="E14" s="75" t="s">
         <v>2870</v>
       </c>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75">
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+    </row>
+    <row r="15" spans="1:7" ht="16">
       <c r="A15" t="s">
         <v>2689</v>
       </c>
       <c r="B15" s="57" t="s">
         <v>2690</v>
       </c>
-      <c r="E15" s="79" t="s">
+      <c r="E15" s="69" t="s">
         <v>2871</v>
       </c>
       <c r="F15" t="s">
@@ -27966,7 +27074,7 @@
       <c r="B16" s="57" t="s">
         <v>2693</v>
       </c>
-      <c r="E16" s="77" t="s">
+      <c r="E16" s="75" t="s">
         <v>2872</v>
       </c>
     </row>
@@ -27977,30 +27085,30 @@
       <c r="B17" s="57" t="s">
         <v>2695</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="E17" s="75" t="s">
         <v>2873</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75">
+    <row r="18" spans="1:7" ht="16">
       <c r="A18" t="s">
         <v>2696</v>
       </c>
       <c r="B18" s="57" t="s">
         <v>2697</v>
       </c>
-      <c r="E18" s="77" t="s">
+      <c r="E18" s="75" t="s">
         <v>2874</v>
       </c>
       <c r="G18" s="64"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75">
+    <row r="19" spans="1:7" ht="16">
       <c r="A19" t="s">
         <v>2698</v>
       </c>
       <c r="B19" s="57" t="s">
         <v>2699</v>
       </c>
-      <c r="E19" s="77" t="s">
+      <c r="E19" s="75" t="s">
         <v>2875</v>
       </c>
       <c r="G19" s="64"/>
@@ -28012,7 +27120,7 @@
       <c r="B20" s="32" t="s">
         <v>2701</v>
       </c>
-      <c r="E20" s="79" t="s">
+      <c r="E20" s="69" t="s">
         <v>2876</v>
       </c>
       <c r="F20" t="s">
@@ -28026,7 +27134,7 @@
       <c r="B21" s="32" t="s">
         <v>2703</v>
       </c>
-      <c r="E21" s="79" t="s">
+      <c r="E21" s="69" t="s">
         <v>2877</v>
       </c>
       <c r="F21" t="s">
@@ -28040,7 +27148,7 @@
       <c r="B22" s="32" t="s">
         <v>2706</v>
       </c>
-      <c r="E22" s="79" t="s">
+      <c r="E22" s="69" t="s">
         <v>2878</v>
       </c>
       <c r="F22" t="s">
@@ -28054,7 +27162,7 @@
       <c r="B23" s="32" t="s">
         <v>2709</v>
       </c>
-      <c r="E23" s="80" t="s">
+      <c r="E23" s="69" t="s">
         <v>2880</v>
       </c>
     </row>
@@ -28065,15 +27173,9 @@
       <c r="B24" t="s">
         <v>2711</v>
       </c>
-      <c r="E24" s="76" t="s">
+      <c r="E24" t="s">
         <v>2879</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="E25" s="76"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="E26" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -28089,13 +27191,13 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="100.28515625" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="80.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="100.33203125" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="80.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -28582,11 +27684,11 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29040,44 +28142,44 @@
       <c r="E51" s="24"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>OR($AD24="X",$AC24="X")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>AND($AD24=1,$AC24=1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="3">
+      <formula>$AD24=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="4">
+      <formula>$AC24=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>AND(NOT(ISBLANK($V24)),ISBLANK($AC24),ISBLANK($AD24))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="6">
+      <formula>AND($Q24="X",OR($B24&lt;&gt;"",$C24&lt;&gt;""))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="114" priority="30">
+    <cfRule type="expression" dxfId="6" priority="30">
       <formula>OR($AD23="X",$AC23="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="31">
+    <cfRule type="expression" dxfId="5" priority="31">
       <formula>AND($AD23=1,$AC23=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="32">
+    <cfRule type="expression" dxfId="4" priority="32">
       <formula>$AD23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="33">
+    <cfRule type="expression" dxfId="3" priority="33">
       <formula>$AC23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="34">
+    <cfRule type="expression" dxfId="2" priority="34">
       <formula>AND(NOT(ISBLANK($V23)),ISBLANK($AC23),ISBLANK($AD23))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="35">
+    <cfRule type="expression" dxfId="1" priority="35">
       <formula>AND($Q23="X",OR(#REF!&lt;&gt;"",$B23&lt;&gt;""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="108" priority="1">
-      <formula>OR($AD24="X",$AC24="X")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="2">
-      <formula>AND($AD24=1,$AC24=1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="3">
-      <formula>$AD24=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="4">
-      <formula>$AC24=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="5">
-      <formula>AND(NOT(ISBLANK($V24)),ISBLANK($AC24),ISBLANK($AD24))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="6">
-      <formula>AND($Q24="X",OR($B24&lt;&gt;"",$C24&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -29096,14 +28198,14 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" customWidth="1"/>
+    <col min="5" max="5" width="47.83203125" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -29166,7 +28268,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="64.5">
+    <row r="7" spans="1:6" ht="60">
       <c r="A7" s="24" t="s">
         <v>140</v>
       </c>
@@ -29192,7 +28294,7 @@
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
     </row>
-    <row r="9" spans="1:6" ht="26.25">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="24" t="s">
         <v>145</v>
       </c>
@@ -29206,7 +28308,7 @@
       </c>
       <c r="F9" s="24"/>
     </row>
-    <row r="10" spans="1:6" ht="26.25">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="24" t="s">
         <v>148</v>
       </c>
@@ -29220,7 +28322,7 @@
       </c>
       <c r="F10" s="24"/>
     </row>
-    <row r="11" spans="1:6" ht="26.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="24" t="s">
         <v>151</v>
       </c>
@@ -29233,7 +28335,7 @@
       </c>
       <c r="F11" s="24"/>
     </row>
-    <row r="12" spans="1:6" ht="26.25">
+    <row r="12" spans="1:6" ht="30">
       <c r="A12" s="24" t="s">
         <v>154</v>
       </c>
@@ -29261,7 +28363,7 @@
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
     </row>
-    <row r="14" spans="1:6" ht="26.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="24" t="s">
         <v>160</v>
       </c>
@@ -29287,7 +28389,7 @@
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
     </row>
-    <row r="16" spans="1:6" ht="26.25">
+    <row r="16" spans="1:6" ht="30">
       <c r="A16" s="24" t="s">
         <v>165</v>
       </c>
@@ -29302,7 +28404,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="26.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="24" t="s">
         <v>169</v>
       </c>
@@ -29328,7 +28430,7 @@
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
     </row>
-    <row r="19" spans="1:6" ht="39">
+    <row r="19" spans="1:6" ht="30">
       <c r="A19" s="24" t="s">
         <v>174</v>
       </c>
@@ -29342,7 +28444,7 @@
       </c>
       <c r="F19" s="24"/>
     </row>
-    <row r="20" spans="1:6" ht="39">
+    <row r="20" spans="1:6" ht="30">
       <c r="A20" s="24" t="s">
         <v>177</v>
       </c>
@@ -29367,7 +28469,7 @@
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
     </row>
-    <row r="22" spans="1:6" ht="26.25">
+    <row r="22" spans="1:6" ht="30">
       <c r="A22" s="24" t="s">
         <v>182</v>
       </c>
@@ -29381,7 +28483,7 @@
       </c>
       <c r="F22" s="24"/>
     </row>
-    <row r="23" spans="1:6" ht="26.25">
+    <row r="23" spans="1:6" ht="30">
       <c r="A23" s="24" t="s">
         <v>185</v>
       </c>
@@ -29395,7 +28497,7 @@
       </c>
       <c r="F23" s="24"/>
     </row>
-    <row r="24" spans="1:6" ht="26.25">
+    <row r="24" spans="1:6" ht="30">
       <c r="A24" s="24" t="s">
         <v>188</v>
       </c>
@@ -29409,7 +28511,7 @@
       </c>
       <c r="F24" s="24"/>
     </row>
-    <row r="25" spans="1:6" ht="26.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="24" t="s">
         <v>191</v>
       </c>
@@ -29446,7 +28548,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
     </row>
-    <row r="28" spans="1:6" ht="51.75">
+    <row r="28" spans="1:6" ht="60">
       <c r="A28" s="24" t="s">
         <v>198</v>
       </c>
@@ -29460,7 +28562,7 @@
       </c>
       <c r="F28" s="24"/>
     </row>
-    <row r="29" spans="1:6" ht="26.25">
+    <row r="29" spans="1:6" ht="30">
       <c r="A29" s="24" t="s">
         <v>201</v>
       </c>
@@ -29499,7 +28601,7 @@
       </c>
       <c r="F31" s="24"/>
     </row>
-    <row r="32" spans="1:6" ht="26.25">
+    <row r="32" spans="1:6" ht="30">
       <c r="A32" s="24" t="s">
         <v>209</v>
       </c>
@@ -29525,7 +28627,7 @@
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
     </row>
-    <row r="34" spans="1:6" ht="102.75">
+    <row r="34" spans="1:6" ht="120">
       <c r="A34" s="24" t="s">
         <v>214</v>
       </c>
@@ -29539,7 +28641,7 @@
       </c>
       <c r="F34" s="24"/>
     </row>
-    <row r="35" spans="1:6" ht="26.25">
+    <row r="35" spans="1:6" ht="30">
       <c r="A35" s="24" t="s">
         <v>217</v>
       </c>
@@ -29553,7 +28655,7 @@
       </c>
       <c r="F35" s="24"/>
     </row>
-    <row r="36" spans="1:6" ht="39">
+    <row r="36" spans="1:6" ht="30">
       <c r="A36" s="24" t="s">
         <v>220</v>
       </c>
@@ -29578,7 +28680,7 @@
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
     </row>
-    <row r="38" spans="1:6" ht="39">
+    <row r="38" spans="1:6" ht="30">
       <c r="A38" s="24" t="s">
         <v>225</v>
       </c>
@@ -29592,7 +28694,7 @@
       </c>
       <c r="F38" s="24"/>
     </row>
-    <row r="39" spans="1:6" ht="26.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="24" t="s">
         <v>228</v>
       </c>
@@ -29606,7 +28708,7 @@
       </c>
       <c r="F39" s="24"/>
     </row>
-    <row r="40" spans="1:6" ht="39">
+    <row r="40" spans="1:6" ht="30">
       <c r="A40" s="24" t="s">
         <v>231</v>
       </c>
@@ -29631,7 +28733,7 @@
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
     </row>
-    <row r="42" spans="1:6" ht="39">
+    <row r="42" spans="1:6" ht="45">
       <c r="A42" s="24" t="s">
         <v>236</v>
       </c>
@@ -29730,7 +28832,7 @@
       <c r="E49" s="24"/>
       <c r="F49" s="24"/>
     </row>
-    <row r="50" spans="1:6" ht="26.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="24" t="s">
         <v>254</v>
       </c>
@@ -29744,7 +28846,7 @@
       </c>
       <c r="F50" s="24"/>
     </row>
-    <row r="51" spans="1:6" ht="64.5">
+    <row r="51" spans="1:6" ht="60">
       <c r="A51" s="24" t="s">
         <v>257</v>
       </c>
@@ -30117,7 +29219,7 @@
       <c r="E81" s="24"/>
       <c r="F81" s="24"/>
     </row>
-    <row r="82" spans="1:6" ht="39">
+    <row r="82" spans="1:6" ht="45">
       <c r="A82" s="24" t="s">
         <v>323</v>
       </c>
@@ -30143,7 +29245,7 @@
       <c r="E83" s="24"/>
       <c r="F83" s="24"/>
     </row>
-    <row r="84" spans="1:6" ht="128.25">
+    <row r="84" spans="1:6" ht="135">
       <c r="A84" s="24" t="s">
         <v>328</v>
       </c>
@@ -30169,7 +29271,7 @@
       <c r="E85" s="24"/>
       <c r="F85" s="24"/>
     </row>
-    <row r="86" spans="1:6" ht="51.75">
+    <row r="86" spans="1:6" ht="60">
       <c r="A86" s="24" t="s">
         <v>333</v>
       </c>
@@ -30182,7 +29284,7 @@
       </c>
       <c r="F86" s="24"/>
     </row>
-    <row r="87" spans="1:6" ht="26.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="24" t="s">
         <v>336</v>
       </c>
@@ -30222,7 +29324,7 @@
       <c r="E89" s="24"/>
       <c r="F89" s="24"/>
     </row>
-    <row r="90" spans="1:6" ht="26.25">
+    <row r="90" spans="1:6" ht="30">
       <c r="A90" s="24" t="s">
         <v>344</v>
       </c>
@@ -30394,7 +29496,7 @@
       <c r="E103" s="24"/>
       <c r="F103" s="24"/>
     </row>
-    <row r="104" spans="1:6" ht="26.25">
+    <row r="104" spans="1:6" ht="30">
       <c r="A104" s="24" t="s">
         <v>375</v>
       </c>
@@ -30408,7 +29510,7 @@
       </c>
       <c r="F104" s="24"/>
     </row>
-    <row r="105" spans="1:6" ht="26.25">
+    <row r="105" spans="1:6">
       <c r="A105" s="24" t="s">
         <v>378</v>
       </c>
@@ -30532,7 +29634,7 @@
       <c r="E114" s="24"/>
       <c r="F114" s="24"/>
     </row>
-    <row r="115" spans="1:6" ht="26.25">
+    <row r="115" spans="1:6" ht="30">
       <c r="A115" s="24" t="s">
         <v>401</v>
       </c>
@@ -30546,7 +29648,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="26.25">
+    <row r="116" spans="1:6">
       <c r="A116" s="24" t="s">
         <v>404</v>
       </c>
@@ -30559,7 +29661,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="39">
+    <row r="117" spans="1:6" ht="45">
       <c r="A117" s="24" t="s">
         <v>407</v>
       </c>
@@ -30597,7 +29699,7 @@
       <c r="E119" s="24"/>
       <c r="F119" s="24"/>
     </row>
-    <row r="120" spans="1:6" ht="39">
+    <row r="120" spans="1:6" ht="45">
       <c r="A120" s="24" t="s">
         <v>414</v>
       </c>
@@ -30658,7 +29760,7 @@
       <c r="E124" s="24"/>
       <c r="F124" s="24"/>
     </row>
-    <row r="125" spans="1:6" ht="39">
+    <row r="125" spans="1:6" ht="45">
       <c r="A125" s="24" t="s">
         <v>425</v>
       </c>
@@ -30794,7 +29896,7 @@
       <c r="E135" s="24"/>
       <c r="F135" s="24"/>
     </row>
-    <row r="136" spans="1:6" ht="26.25">
+    <row r="136" spans="1:6" ht="30">
       <c r="A136" s="24" t="s">
         <v>450</v>
       </c>
@@ -30820,7 +29922,7 @@
       <c r="E137" s="24"/>
       <c r="F137" s="24"/>
     </row>
-    <row r="138" spans="1:6" ht="26.25">
+    <row r="138" spans="1:6" ht="30">
       <c r="A138" s="24" t="s">
         <v>455</v>
       </c>
@@ -30834,7 +29936,7 @@
       </c>
       <c r="F138" s="24"/>
     </row>
-    <row r="139" spans="1:6" ht="26.25">
+    <row r="139" spans="1:6" ht="30">
       <c r="A139" s="24" t="s">
         <v>456</v>
       </c>
@@ -30848,7 +29950,7 @@
       </c>
       <c r="F139" s="24"/>
     </row>
-    <row r="140" spans="1:6" ht="26.25">
+    <row r="140" spans="1:6">
       <c r="A140" s="24" t="s">
         <v>457</v>
       </c>
@@ -30862,7 +29964,7 @@
       </c>
       <c r="F140" s="24"/>
     </row>
-    <row r="141" spans="1:6" ht="26.25">
+    <row r="141" spans="1:6" ht="30">
       <c r="A141" s="24" t="s">
         <v>458</v>
       </c>
@@ -30891,7 +29993,7 @@
       </c>
       <c r="F142" s="24"/>
     </row>
-    <row r="143" spans="1:6" ht="26.25">
+    <row r="143" spans="1:6">
       <c r="A143" s="24" t="s">
         <v>461</v>
       </c>
@@ -30905,7 +30007,7 @@
       </c>
       <c r="F143" s="24"/>
     </row>
-    <row r="144" spans="1:6" ht="39">
+    <row r="144" spans="1:6" ht="30">
       <c r="A144" s="24" t="s">
         <v>462</v>
       </c>
@@ -30919,7 +30021,7 @@
       </c>
       <c r="F144" s="24"/>
     </row>
-    <row r="145" spans="1:6" ht="39">
+    <row r="145" spans="1:6" ht="30">
       <c r="A145" s="24" t="s">
         <v>463</v>
       </c>
@@ -30933,7 +30035,7 @@
       </c>
       <c r="F145" s="24"/>
     </row>
-    <row r="146" spans="1:6" ht="26.25">
+    <row r="146" spans="1:6" ht="30">
       <c r="A146" s="24" t="s">
         <v>464</v>
       </c>
@@ -30946,7 +30048,7 @@
       </c>
       <c r="F146" s="24"/>
     </row>
-    <row r="147" spans="1:6" ht="26.25">
+    <row r="147" spans="1:6" ht="30">
       <c r="A147" s="24" t="s">
         <v>465</v>
       </c>
@@ -30960,7 +30062,7 @@
       </c>
       <c r="F147" s="24"/>
     </row>
-    <row r="148" spans="1:6" ht="26.25">
+    <row r="148" spans="1:6" ht="30">
       <c r="A148" s="24" t="s">
         <v>466</v>
       </c>
@@ -31092,7 +30194,7 @@
       <c r="E158" s="24"/>
       <c r="F158" s="24"/>
     </row>
-    <row r="159" spans="1:6" ht="39">
+    <row r="159" spans="1:6" ht="30">
       <c r="A159" s="24" t="s">
         <v>487</v>
       </c>
@@ -31106,7 +30208,7 @@
       </c>
       <c r="F159" s="24"/>
     </row>
-    <row r="160" spans="1:6" ht="39">
+    <row r="160" spans="1:6" ht="45">
       <c r="A160" s="24" t="s">
         <v>490</v>
       </c>
@@ -31120,7 +30222,7 @@
       </c>
       <c r="F160" s="24"/>
     </row>
-    <row r="161" spans="1:6" ht="39">
+    <row r="161" spans="1:6" ht="45">
       <c r="A161" s="24" t="s">
         <v>493</v>
       </c>
@@ -31171,7 +30273,7 @@
       <c r="E164" s="24"/>
       <c r="F164" s="24"/>
     </row>
-    <row r="165" spans="1:6" ht="26.25">
+    <row r="165" spans="1:6" ht="30">
       <c r="A165" s="24" t="s">
         <v>503</v>
       </c>
@@ -31388,7 +30490,7 @@
       <c r="E182" s="24"/>
       <c r="F182" s="24"/>
     </row>
-    <row r="183" spans="1:6" ht="26.25">
+    <row r="183" spans="1:6" ht="30">
       <c r="A183" s="24" t="s">
         <v>540</v>
       </c>
@@ -31524,7 +30626,7 @@
       </c>
       <c r="F193" s="24"/>
     </row>
-    <row r="194" spans="1:6" ht="26.25">
+    <row r="194" spans="1:6">
       <c r="A194" s="24" t="s">
         <v>565</v>
       </c>
@@ -31624,7 +30726,7 @@
       <c r="E201" s="24"/>
       <c r="F201" s="24"/>
     </row>
-    <row r="202" spans="1:6" ht="26.25">
+    <row r="202" spans="1:6" ht="30">
       <c r="A202" s="24" t="s">
         <v>584</v>
       </c>
@@ -31650,7 +30752,7 @@
       <c r="E203" s="24"/>
       <c r="F203" s="24"/>
     </row>
-    <row r="204" spans="1:6" ht="26.25">
+    <row r="204" spans="1:6" ht="30">
       <c r="A204" s="24" t="s">
         <v>589</v>
       </c>
@@ -31748,7 +30850,7 @@
       <c r="E211" s="24"/>
       <c r="F211" s="24"/>
     </row>
-    <row r="212" spans="1:6" ht="26.25">
+    <row r="212" spans="1:6" ht="30">
       <c r="A212" s="24" t="s">
         <v>607</v>
       </c>
@@ -32569,7 +31671,7 @@
       <c r="E279" s="24"/>
       <c r="F279" s="24"/>
     </row>
-    <row r="280" spans="1:6" ht="26.25">
+    <row r="280" spans="1:6" ht="30">
       <c r="A280" s="24" t="s">
         <v>752</v>
       </c>
@@ -32583,7 +31685,7 @@
       </c>
       <c r="F280" s="24"/>
     </row>
-    <row r="281" spans="1:6" ht="26.25">
+    <row r="281" spans="1:6" ht="30">
       <c r="A281" s="24" t="s">
         <v>755</v>
       </c>
@@ -32930,14 +32032,14 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" customWidth="1"/>
-    <col min="5" max="5" width="255.7109375" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
+    <col min="4" max="4" width="44.6640625" customWidth="1"/>
+    <col min="5" max="5" width="255.6640625" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -35001,12 +34103,12 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -35063,7 +34165,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="39">
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="24" t="s">
         <v>1194</v>
       </c>
@@ -35083,7 +34185,7 @@
       </c>
       <c r="C8" s="24"/>
     </row>
-    <row r="9" spans="1:4" ht="26.25">
+    <row r="9" spans="1:4" ht="30">
       <c r="A9" s="24" t="s">
         <v>1199</v>
       </c>
@@ -35092,7 +34194,7 @@
       </c>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="1:4" ht="39">
+    <row r="10" spans="1:4" ht="30">
       <c r="A10" s="24" t="s">
         <v>1201</v>
       </c>
@@ -35101,7 +34203,7 @@
       </c>
       <c r="C10" s="24"/>
     </row>
-    <row r="11" spans="1:4" ht="26.25">
+    <row r="11" spans="1:4" ht="30">
       <c r="A11" s="24" t="s">
         <v>1203</v>
       </c>
@@ -35110,7 +34212,7 @@
       </c>
       <c r="C11" s="24"/>
     </row>
-    <row r="12" spans="1:4" ht="26.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="24" t="s">
         <v>1205</v>
       </c>
@@ -35119,7 +34221,7 @@
       </c>
       <c r="C12" s="24"/>
     </row>
-    <row r="13" spans="1:4" ht="26.25">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="24" t="s">
         <v>1207</v>
       </c>
@@ -35130,7 +34232,7 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="39">
+    <row r="14" spans="1:4" ht="45">
       <c r="A14" s="24" t="s">
         <v>1210</v>
       </c>
@@ -35141,7 +34243,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="39">
+    <row r="15" spans="1:4" ht="30">
       <c r="A15" s="24" t="s">
         <v>1213</v>
       </c>
@@ -35150,7 +34252,7 @@
       </c>
       <c r="C15" s="24"/>
     </row>
-    <row r="16" spans="1:4" ht="39">
+    <row r="16" spans="1:4" ht="45">
       <c r="A16" s="24" t="s">
         <v>1215</v>
       </c>
@@ -35159,7 +34261,7 @@
       </c>
       <c r="C16" s="24"/>
     </row>
-    <row r="17" spans="1:3" ht="26.25">
+    <row r="17" spans="1:3" ht="30">
       <c r="A17" s="24" t="s">
         <v>1217</v>
       </c>
@@ -35168,7 +34270,7 @@
       </c>
       <c r="C17" s="24"/>
     </row>
-    <row r="18" spans="1:3" ht="26.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="24" t="s">
         <v>1219</v>
       </c>
@@ -35177,7 +34279,7 @@
       </c>
       <c r="C18" s="24"/>
     </row>
-    <row r="19" spans="1:3" ht="26.25">
+    <row r="19" spans="1:3" ht="30">
       <c r="A19" s="24" t="s">
         <v>1221</v>
       </c>
@@ -35204,7 +34306,7 @@
       </c>
       <c r="C21" s="24"/>
     </row>
-    <row r="22" spans="1:3" ht="26.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="24" t="s">
         <v>1227</v>
       </c>
@@ -35231,7 +34333,7 @@
       </c>
       <c r="C24" s="24"/>
     </row>
-    <row r="25" spans="1:3" ht="26.25">
+    <row r="25" spans="1:3" ht="30">
       <c r="A25" s="24" t="s">
         <v>1232</v>
       </c>
@@ -35242,7 +34344,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="26.25">
+    <row r="26" spans="1:3" ht="30">
       <c r="A26" s="24" t="s">
         <v>1235</v>
       </c>
@@ -35253,7 +34355,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="26.25">
+    <row r="27" spans="1:3" ht="30">
       <c r="A27" s="24" t="s">
         <v>1238</v>
       </c>
@@ -35273,7 +34375,7 @@
       </c>
       <c r="C28" s="24"/>
     </row>
-    <row r="29" spans="1:3" ht="26.25">
+    <row r="29" spans="1:3" ht="30">
       <c r="A29" s="24" t="s">
         <v>1243</v>
       </c>
@@ -35284,7 +34386,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="39">
+    <row r="30" spans="1:3" ht="30">
       <c r="A30" s="24" t="s">
         <v>1246</v>
       </c>
@@ -35295,7 +34397,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="26.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="24" t="s">
         <v>1249</v>
       </c>
@@ -35306,7 +34408,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="128.25">
+    <row r="32" spans="1:3" ht="135">
       <c r="A32" s="24" t="s">
         <v>1252</v>
       </c>
@@ -35317,7 +34419,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="128.25">
+    <row r="33" spans="1:3" ht="135">
       <c r="A33" s="24" t="s">
         <v>1255</v>
       </c>
@@ -35393,7 +34495,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="26.25">
+    <row r="41" spans="1:3" ht="30">
       <c r="A41" s="24" t="s">
         <v>1272</v>
       </c>
@@ -35404,7 +34506,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="26.25">
+    <row r="42" spans="1:3" ht="30">
       <c r="A42" s="24" t="s">
         <v>1275</v>
       </c>
@@ -35413,7 +34515,7 @@
       </c>
       <c r="C42" s="24"/>
     </row>
-    <row r="43" spans="1:3" ht="77.25">
+    <row r="43" spans="1:3" ht="75">
       <c r="A43" s="24" t="s">
         <v>1277</v>
       </c>
@@ -35441,13 +34543,13 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -35539,7 +34641,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:5" ht="26.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="24" t="s">
         <v>1290</v>
       </c>
@@ -35561,7 +34663,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12" spans="1:5" ht="26.25">
+    <row r="12" spans="1:5" ht="30">
       <c r="A12" s="24" t="s">
         <v>1295</v>
       </c>
@@ -35573,7 +34675,7 @@
       </c>
       <c r="E12" s="24"/>
     </row>
-    <row r="13" spans="1:5" ht="26.25">
+    <row r="13" spans="1:5" ht="30">
       <c r="A13" s="24" t="s">
         <v>1298</v>
       </c>
@@ -35595,7 +34697,7 @@
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:5" ht="48.75">
+    <row r="15" spans="1:5" ht="40">
       <c r="A15" s="24" t="s">
         <v>1303</v>
       </c>
@@ -35607,7 +34709,7 @@
       </c>
       <c r="E15" s="24"/>
     </row>
-    <row r="16" spans="1:5" ht="64.5">
+    <row r="16" spans="1:5" ht="60">
       <c r="A16" s="24" t="s">
         <v>1306</v>
       </c>
@@ -35743,7 +34845,7 @@
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
     </row>
-    <row r="29" spans="1:5" ht="26.25">
+    <row r="29" spans="1:5" ht="30">
       <c r="A29" s="24" t="s">
         <v>1335</v>
       </c>
@@ -35755,7 +34857,7 @@
       </c>
       <c r="E29" s="24"/>
     </row>
-    <row r="30" spans="1:5" ht="26.25">
+    <row r="30" spans="1:5" ht="30">
       <c r="A30" s="24" t="s">
         <v>1338</v>
       </c>
@@ -35833,7 +34935,7 @@
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
     </row>
-    <row r="37" spans="1:5" ht="51.75">
+    <row r="37" spans="1:5" ht="45">
       <c r="A37" s="24" t="s">
         <v>1357</v>
       </c>
@@ -35867,7 +34969,7 @@
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
     </row>
-    <row r="40" spans="1:5" ht="26.25">
+    <row r="40" spans="1:5" ht="30">
       <c r="A40" s="24" t="s">
         <v>1365</v>
       </c>
@@ -35879,7 +34981,7 @@
       </c>
       <c r="E40" s="24"/>
     </row>
-    <row r="41" spans="1:5" ht="39">
+    <row r="41" spans="1:5" ht="30">
       <c r="A41" s="24" t="s">
         <v>1366</v>
       </c>
@@ -35933,7 +35035,7 @@
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
     </row>
-    <row r="46" spans="1:5" ht="26.25">
+    <row r="46" spans="1:5" ht="30">
       <c r="A46" s="24" t="s">
         <v>1378</v>
       </c>
@@ -35965,7 +35067,7 @@
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
     </row>
-    <row r="49" spans="1:5" ht="26.25">
+    <row r="49" spans="1:5" ht="30">
       <c r="A49" s="24" t="s">
         <v>1385</v>
       </c>
@@ -36051,7 +35153,7 @@
       </c>
       <c r="E56" s="24"/>
     </row>
-    <row r="57" spans="1:5" ht="39">
+    <row r="57" spans="1:5" ht="45">
       <c r="A57" s="24" t="s">
         <v>1404</v>
       </c>
@@ -36092,13 +35194,13 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -36163,7 +35265,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="25" customFormat="1">
+    <row r="7" spans="1:5" s="25" customFormat="1" ht="16">
       <c r="A7" s="22" t="s">
         <v>2822</v>
       </c>
@@ -36308,15 +35410,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -36366,6 +35459,15 @@
     </l0a6b4600f484920bbceae0813174244>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36783,6 +35885,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -36790,24 +35910,22 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB073A50-F568-4F6E-9BF9-DA8A5B206B6B}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB073A50-F568-4F6E-9BF9-DA8A5B206B6B}"/>
 </file>
</xml_diff>

<commit_message>
[24.11.25 17:30] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="196" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{981E77C6-8E74-4021-B42D-A7C3EEDD3006}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" tabRatio="500" firstSheet="29" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -10306,11 +10306,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P224"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14"/>
@@ -27187,8 +27187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -35410,6 +35410,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -35459,15 +35468,6 @@
     </l0a6b4600f484920bbceae0813174244>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -35885,24 +35885,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -35910,8 +35892,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB073A50-F568-4F6E-9BF9-DA8A5B206B6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27FF8B5-506F-46C5-AD7B-D0EA568E0AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>

<commit_message>
[25.01.07 15:43] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="409" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{674EC906-8686-418C-9D95-7D6304D11899}"/>
+  <xr:revisionPtr revIDLastSave="413" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ED9049A-2E58-40EA-A1D3-061D3064025B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="34" activeTab="38" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -9361,7 +9361,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9545,7 +9545,6 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in 60% - Accent5" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -9553,75 +9552,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="60">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9642,171 +9577,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF58383"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE1FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF58383"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9940,7 +9711,267 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF58383"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE1FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF58383"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10572,11 +10603,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q224"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
+      <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -15732,147 +15763,117 @@
   </sheetData>
   <autoFilter ref="A2:P39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="56" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:A224">
-    <cfRule type="expression" dxfId="55" priority="28">
+    <cfRule type="expression" dxfId="45" priority="29">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:H40">
+    <cfRule type="expression" dxfId="44" priority="2">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:P39">
-    <cfRule type="expression" dxfId="54" priority="26">
+    <cfRule type="expression" dxfId="43" priority="27">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:P224">
-    <cfRule type="expression" dxfId="53" priority="27">
+  <conditionalFormatting sqref="A3:Q224">
+    <cfRule type="expression" dxfId="42" priority="6">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:G22">
-    <cfRule type="expression" dxfId="52" priority="24">
+    <cfRule type="expression" dxfId="41" priority="25">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:Q22">
-    <cfRule type="expression" dxfId="51" priority="23">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41:Q224 H22:Q22 B40:F40 H40:Q40">
-    <cfRule type="expression" dxfId="50" priority="42">
+  <conditionalFormatting sqref="H22:Q22 H40:Q40 B41:Q224">
+    <cfRule type="expression" dxfId="39" priority="43">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:J22">
-    <cfRule type="expression" dxfId="49" priority="22">
+    <cfRule type="expression" dxfId="38" priority="23">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:P45">
-    <cfRule type="expression" dxfId="48" priority="40">
+    <cfRule type="expression" dxfId="37" priority="41">
       <formula>I3="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:P122">
-    <cfRule type="expression" dxfId="47" priority="36">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula>I3=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:P122">
-    <cfRule type="expression" dxfId="46" priority="37">
+    <cfRule type="expression" dxfId="35" priority="38">
       <formula>I46="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:L7">
-    <cfRule type="expression" dxfId="45" priority="35">
+    <cfRule type="expression" dxfId="34" priority="36">
       <formula>K6="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:L9">
-    <cfRule type="expression" dxfId="44" priority="34">
+    <cfRule type="expression" dxfId="33" priority="35">
       <formula>K9="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:L26">
-    <cfRule type="expression" dxfId="43" priority="33">
+    <cfRule type="expression" dxfId="32" priority="34">
       <formula>K26="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:L32">
-    <cfRule type="expression" dxfId="42" priority="32">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>K30="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25:L26">
-    <cfRule type="expression" dxfId="41" priority="30">
+    <cfRule type="expression" dxfId="30" priority="31">
       <formula>L25="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="expression" dxfId="40" priority="31">
+    <cfRule type="expression" dxfId="29" priority="32">
       <formula>L28="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P35:P38">
-    <cfRule type="expression" dxfId="39" priority="38">
+    <cfRule type="expression" dxfId="28" priority="39">
       <formula>P35=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="27" priority="40">
       <formula>P35="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40">
-    <cfRule type="expression" dxfId="24" priority="17">
+  <conditionalFormatting sqref="Q3:Q39">
+    <cfRule type="expression" dxfId="26" priority="5">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q39">
-    <cfRule type="expression" dxfId="17" priority="4">
-      <formula>ISEVEN(ROW())</formula>
+  <conditionalFormatting sqref="Q3:Q122">
+    <cfRule type="expression" dxfId="25" priority="7">
+      <formula>Q3=""</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q224">
-    <cfRule type="expression" dxfId="16" priority="5">
-      <formula>ISODD(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q45">
-    <cfRule type="expression" dxfId="15" priority="10">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>Q3="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q122">
-    <cfRule type="expression" dxfId="14" priority="6">
-      <formula>Q3=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q46:Q122">
-    <cfRule type="expression" dxfId="13" priority="7">
-      <formula>Q46="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q35:Q38">
-    <cfRule type="expression" dxfId="12" priority="8">
-      <formula>Q35=""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="9">
-      <formula>Q35="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ISEVEN(ROW())</formula>
+  <conditionalFormatting sqref="I1:Q1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>X</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -21373,7 +21374,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="25" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -27751,7 +27752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1D2C4D-5188-41FB-B7BD-758B830952F8}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -27834,7 +27835,7 @@
         <v>2890</v>
       </c>
       <c r="C7" s="22"/>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="25" t="s">
         <v>2895</v>
       </c>
       <c r="E7" s="24"/>
@@ -27847,7 +27848,7 @@
         <v>2891</v>
       </c>
       <c r="C8" s="22"/>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="25" t="s">
         <v>2894</v>
       </c>
       <c r="E8" s="24"/>
@@ -27860,7 +27861,7 @@
         <v>2898</v>
       </c>
       <c r="C9" s="22"/>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="25" t="s">
         <v>2899</v>
       </c>
       <c r="E9" s="24"/>
@@ -27873,7 +27874,7 @@
         <v>2900</v>
       </c>
       <c r="C10" s="22"/>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="25" t="s">
         <v>2901</v>
       </c>
       <c r="E10" s="24"/>
@@ -27886,7 +27887,7 @@
         <v>2892</v>
       </c>
       <c r="C11" s="22"/>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="25" t="s">
         <v>2893</v>
       </c>
       <c r="E11" s="24"/>
@@ -28586,42 +28587,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="37" priority="1">
+    <cfRule type="expression" dxfId="59" priority="1">
       <formula>OR($AD24="X",$AC24="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="2">
+    <cfRule type="expression" dxfId="58" priority="2">
       <formula>AND($AD24=1,$AC24=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="3">
+    <cfRule type="expression" dxfId="57" priority="3">
       <formula>$AD24=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="4">
+    <cfRule type="expression" dxfId="56" priority="4">
       <formula>$AC24=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="5">
+    <cfRule type="expression" dxfId="55" priority="5">
       <formula>AND(NOT(ISBLANK($V24)),ISBLANK($AC24),ISBLANK($AD24))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="6">
+    <cfRule type="expression" dxfId="54" priority="6">
       <formula>AND($Q24="X",OR($B24&lt;&gt;"",$C24&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="31" priority="30">
+    <cfRule type="expression" dxfId="53" priority="30">
       <formula>OR($AD23="X",$AC23="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="31">
+    <cfRule type="expression" dxfId="52" priority="31">
       <formula>AND($AD23=1,$AC23=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="32">
+    <cfRule type="expression" dxfId="51" priority="32">
       <formula>$AD23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="33">
+    <cfRule type="expression" dxfId="50" priority="33">
       <formula>$AC23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="34">
+    <cfRule type="expression" dxfId="49" priority="34">
       <formula>AND(NOT(ISBLANK($V23)),ISBLANK($AC23),ISBLANK($AD23))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="35">
+    <cfRule type="expression" dxfId="48" priority="35">
       <formula>AND($Q23="X",OR(#REF!&lt;&gt;"",$B23&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36823,17 +36824,17 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[25.01.08 15:43] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="413" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6ED9049A-2E58-40EA-A1D3-061D3064025B}"/>
+  <xr:revisionPtr revIDLastSave="427" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C27853-17FA-4EC7-9472-16726E49915A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4290" yWindow="1005" windowWidth="21600" windowHeight="13095" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -9361,7 +9361,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9545,6 +9545,9 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in 60% - Accent5" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -9552,7 +9555,177 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="143">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -9620,34 +9793,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9796,6 +9941,450 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10604,10 +11193,10 @@
   <dimension ref="A1:Q224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M28" sqref="M28"/>
+      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -11884,7 +12473,7 @@
       <c r="J31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K31" s="10" t="s">
+      <c r="K31" s="83" t="s">
         <v>20</v>
       </c>
       <c r="L31" s="10"/>
@@ -15762,118 +16351,60 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:P39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="46" priority="22"/>
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="duplicateValues" dxfId="23" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:A224">
-    <cfRule type="expression" dxfId="45" priority="29">
+    <cfRule type="expression" dxfId="22" priority="31">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:H40">
-    <cfRule type="expression" dxfId="44" priority="2">
+    <cfRule type="expression" dxfId="21" priority="4">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:P39">
-    <cfRule type="expression" dxfId="43" priority="27">
+  <conditionalFormatting sqref="A3:P6 A7:J7 M7:P7 A8:P39">
+    <cfRule type="expression" dxfId="20" priority="29">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:Q224">
-    <cfRule type="expression" dxfId="42" priority="6">
+  <conditionalFormatting sqref="A3:Q6 A7:J7 M7:Q7 A8:Q224">
+    <cfRule type="expression" dxfId="19" priority="8">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:G22">
-    <cfRule type="expression" dxfId="41" priority="25">
+    <cfRule type="expression" dxfId="18" priority="27">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:Q22">
-    <cfRule type="expression" dxfId="40" priority="24">
+    <cfRule type="expression" dxfId="17" priority="26">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:Q22 H40:Q40 B41:Q224">
-    <cfRule type="expression" dxfId="39" priority="43">
+    <cfRule type="expression" dxfId="16" priority="45">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:J22">
-    <cfRule type="expression" dxfId="38" priority="23">
+    <cfRule type="expression" dxfId="15" priority="25">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:P45">
-    <cfRule type="expression" dxfId="37" priority="41">
-      <formula>I3="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:P122">
-    <cfRule type="expression" dxfId="36" priority="37">
-      <formula>I3=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I46:P122">
-    <cfRule type="expression" dxfId="35" priority="38">
-      <formula>I46="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6:L7">
-    <cfRule type="expression" dxfId="34" priority="36">
-      <formula>K6="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9:L9">
-    <cfRule type="expression" dxfId="33" priority="35">
-      <formula>K9="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K26:L26">
-    <cfRule type="expression" dxfId="32" priority="34">
-      <formula>K26="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K30:L32">
-    <cfRule type="expression" dxfId="31" priority="33">
-      <formula>K30="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L25:L26">
-    <cfRule type="expression" dxfId="30" priority="31">
-      <formula>L25="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L28">
-    <cfRule type="expression" dxfId="29" priority="32">
-      <formula>L28="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P35:P38">
-    <cfRule type="expression" dxfId="28" priority="39">
-      <formula>P35=""</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="40">
-      <formula>P35="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q39">
-    <cfRule type="expression" dxfId="26" priority="5">
+    <cfRule type="expression" dxfId="14" priority="7">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q122">
-    <cfRule type="expression" dxfId="25" priority="7">
-      <formula>Q3=""</formula>
+  <conditionalFormatting sqref="I2:CB1048576">
+    <cfRule type="expression" dxfId="13" priority="2">
+      <formula>I2="X"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="8">
-      <formula>Q3="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:Q1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>X</formula>
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>ISBLANK(I2)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -21374,7 +21905,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="47" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -28587,42 +29118,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="59" priority="1">
+    <cfRule type="expression" dxfId="142" priority="1">
       <formula>OR($AD24="X",$AC24="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="2">
+    <cfRule type="expression" dxfId="141" priority="2">
       <formula>AND($AD24=1,$AC24=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="3">
+    <cfRule type="expression" dxfId="140" priority="3">
       <formula>$AD24=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="4">
+    <cfRule type="expression" dxfId="139" priority="4">
       <formula>$AC24=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="5">
+    <cfRule type="expression" dxfId="138" priority="5">
       <formula>AND(NOT(ISBLANK($V24)),ISBLANK($AC24),ISBLANK($AD24))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="6">
+    <cfRule type="expression" dxfId="137" priority="6">
       <formula>AND($Q24="X",OR($B24&lt;&gt;"",$C24&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="53" priority="30">
+    <cfRule type="expression" dxfId="136" priority="30">
       <formula>OR($AD23="X",$AC23="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="31">
+    <cfRule type="expression" dxfId="135" priority="31">
       <formula>AND($AD23=1,$AC23=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="32">
+    <cfRule type="expression" dxfId="134" priority="32">
       <formula>$AD23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="33">
+    <cfRule type="expression" dxfId="133" priority="33">
       <formula>$AC23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="34">
+    <cfRule type="expression" dxfId="132" priority="34">
       <formula>AND(NOT(ISBLANK($V23)),ISBLANK($AC23),ISBLANK($AD23))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="35">
+    <cfRule type="expression" dxfId="131" priority="35">
       <formula>AND($Q23="X",OR(#REF!&lt;&gt;"",$B23&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35476,9 +36007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -36347,67 +36876,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -36821,33 +37289,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27FF8B5-506F-46C5-AD7B-D0EA568E0AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36865,4 +37368,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[25.01.08 17:43] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="427" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C27853-17FA-4EC7-9472-16726E49915A}"/>
+  <xr:revisionPtr revIDLastSave="461" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E93BA5E5-8124-4821-9E09-DC2B3995B271}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4290" yWindow="1005" windowWidth="21600" windowHeight="13095" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29340" yWindow="360" windowWidth="24030" windowHeight="12285" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
     <sheet name="#Type de devenir du patient" sheetId="39" r:id="rId40"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$2:$P$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'#Sommaire'!$A$2:$Q$39</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3797" uniqueCount="2902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="2903">
   <si>
     <t>ID unique</t>
   </si>
@@ -8930,6 +8930,9 @@
   </si>
   <si>
     <t>Le dossier a été ouvert  par un utilisateur humain (à la première ouverture uniquement)</t>
+  </si>
+  <si>
+    <t>RS-EDA-MAJ</t>
   </si>
 </sst>
 </file>
@@ -9198,6 +9201,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -9361,7 +9365,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9545,9 +9549,6 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in 60% - Accent5" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -9555,14 +9556,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
-  <dxfs count="143">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -9573,38 +9567,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9617,859 +9580,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59987182226020086"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10561,6 +9671,58 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFF58383"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -11190,13 +10352,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q224"/>
+  <dimension ref="A1:R224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -11209,18 +10371,18 @@
     <col min="6" max="6" width="30.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="21.28515625" style="1" customWidth="1"/>
-    <col min="9" max="17" width="12.7109375" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="11.42578125" style="1"/>
+    <col min="9" max="18" width="12.7109375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="77"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" ht="15">
+    <row r="2" spans="1:18" s="4" customFormat="1" ht="15">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -11252,28 +10414,31 @@
         <v>9</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>2902</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>2883</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:18" ht="15">
       <c r="A3" s="82" t="s">
         <v>16</v>
       </c>
@@ -11305,15 +10470,18 @@
       <c r="J3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="10"/>
+      <c r="K3" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="1:17" ht="15">
+      <c r="R3" s="10"/>
+    </row>
+    <row r="4" spans="1:18" ht="15">
       <c r="A4" s="78" t="s">
         <v>21</v>
       </c>
@@ -11352,8 +10520,9 @@
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="1:17" ht="15">
+      <c r="R4" s="10"/>
+    </row>
+    <row r="5" spans="1:18" ht="15">
       <c r="A5" s="78" t="s">
         <v>23</v>
       </c>
@@ -11392,8 +10561,9 @@
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:17" ht="15">
+      <c r="R5" s="10"/>
+    </row>
+    <row r="6" spans="1:18" ht="15">
       <c r="A6" s="78" t="s">
         <v>26</v>
       </c>
@@ -11427,17 +10597,18 @@
       <c r="J6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" ht="15">
+      <c r="R6" s="10"/>
+    </row>
+    <row r="7" spans="1:18" ht="15">
       <c r="A7" s="78" t="s">
         <v>28</v>
       </c>
@@ -11471,19 +10642,20 @@
       <c r="J7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="K7" s="10"/>
       <c r="L7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
-    </row>
-    <row r="8" spans="1:17" ht="15">
+      <c r="R7" s="10"/>
+    </row>
+    <row r="8" spans="1:18" ht="15">
       <c r="A8" s="78" t="s">
         <v>30</v>
       </c>
@@ -11517,15 +10689,18 @@
       <c r="J8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
-    </row>
-    <row r="9" spans="1:17" ht="15">
+      <c r="R8" s="10"/>
+    </row>
+    <row r="9" spans="1:18" ht="15">
       <c r="A9" s="78" t="s">
         <v>32</v>
       </c>
@@ -11559,17 +10734,18 @@
       <c r="J9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="10"/>
+      <c r="L9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
-    </row>
-    <row r="10" spans="1:17" ht="15">
+      <c r="R9" s="10"/>
+    </row>
+    <row r="10" spans="1:18" ht="15">
       <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
@@ -11601,15 +10777,18 @@
       <c r="J10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" ht="15">
+      <c r="R10" s="10"/>
+    </row>
+    <row r="11" spans="1:18" ht="15">
       <c r="A11" s="78" t="s">
         <v>36</v>
       </c>
@@ -11648,8 +10827,9 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
-    </row>
-    <row r="12" spans="1:17" ht="15">
+      <c r="R11" s="10"/>
+    </row>
+    <row r="12" spans="1:18" ht="15">
       <c r="A12" s="78" t="s">
         <v>38</v>
       </c>
@@ -11688,8 +10868,9 @@
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
-    </row>
-    <row r="13" spans="1:17" ht="15">
+      <c r="R12" s="10"/>
+    </row>
+    <row r="13" spans="1:18" ht="15">
       <c r="A13" s="78" t="s">
         <v>40</v>
       </c>
@@ -11728,8 +10909,9 @@
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
-    </row>
-    <row r="14" spans="1:17" ht="15">
+      <c r="R13" s="10"/>
+    </row>
+    <row r="14" spans="1:18" ht="15">
       <c r="A14" s="78" t="s">
         <v>42</v>
       </c>
@@ -11761,15 +10943,18 @@
       <c r="J14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="10"/>
+      <c r="K14" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
-    </row>
-    <row r="15" spans="1:17" ht="15">
+      <c r="R14" s="10"/>
+    </row>
+    <row r="15" spans="1:18" ht="15">
       <c r="A15" s="78" t="s">
         <v>44</v>
       </c>
@@ -11803,15 +10988,18 @@
       <c r="J15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="10"/>
+      <c r="K15" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" ht="15">
+      <c r="R15" s="10"/>
+    </row>
+    <row r="16" spans="1:18" ht="15">
       <c r="A16" s="78" t="s">
         <v>47</v>
       </c>
@@ -11852,8 +11040,9 @@
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
-    </row>
-    <row r="17" spans="1:17" ht="15">
+      <c r="R16" s="10"/>
+    </row>
+    <row r="17" spans="1:18" ht="15">
       <c r="A17" s="78" t="s">
         <v>49</v>
       </c>
@@ -11887,15 +11076,18 @@
       <c r="J17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="10"/>
+      <c r="K17" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
-    </row>
-    <row r="18" spans="1:17" ht="15">
+      <c r="R17" s="10"/>
+    </row>
+    <row r="18" spans="1:18" ht="15">
       <c r="A18" s="78" t="s">
         <v>51</v>
       </c>
@@ -11929,15 +11121,18 @@
       <c r="J18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K18" s="10"/>
+      <c r="K18" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
-    </row>
-    <row r="19" spans="1:17" ht="15">
+      <c r="R18" s="10"/>
+    </row>
+    <row r="19" spans="1:18" ht="15">
       <c r="A19" s="78" t="s">
         <v>53</v>
       </c>
@@ -11976,8 +11171,9 @@
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
-    </row>
-    <row r="20" spans="1:17" ht="15">
+      <c r="R19" s="10"/>
+    </row>
+    <row r="20" spans="1:18" ht="15">
       <c r="A20" s="81" t="s">
         <v>56</v>
       </c>
@@ -12018,8 +11214,9 @@
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
-    </row>
-    <row r="21" spans="1:17" ht="15">
+      <c r="R20" s="10"/>
+    </row>
+    <row r="21" spans="1:18" ht="15">
       <c r="A21" s="78" t="s">
         <v>58</v>
       </c>
@@ -12053,15 +11250,18 @@
       <c r="J21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K21" s="10"/>
+      <c r="K21" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
       <c r="Q21" s="10"/>
-    </row>
-    <row r="22" spans="1:17" ht="15">
+      <c r="R21" s="10"/>
+    </row>
+    <row r="22" spans="1:18" ht="15">
       <c r="A22" s="79" t="s">
         <v>60</v>
       </c>
@@ -12099,8 +11299,9 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
-    </row>
-    <row r="23" spans="1:17" ht="15">
+      <c r="R22" s="10"/>
+    </row>
+    <row r="23" spans="1:18" ht="15">
       <c r="A23" s="78" t="s">
         <v>63</v>
       </c>
@@ -12141,8 +11342,9 @@
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
-    </row>
-    <row r="24" spans="1:17" ht="15">
+      <c r="R23" s="10"/>
+    </row>
+    <row r="24" spans="1:18" ht="15">
       <c r="A24" s="78" t="s">
         <v>65</v>
       </c>
@@ -12183,8 +11385,9 @@
       <c r="O24" s="10"/>
       <c r="P24" s="10"/>
       <c r="Q24" s="10"/>
-    </row>
-    <row r="25" spans="1:17" ht="15">
+      <c r="R24" s="10"/>
+    </row>
+    <row r="25" spans="1:18" ht="15">
       <c r="A25" s="79" t="s">
         <v>67</v>
       </c>
@@ -12216,17 +11419,20 @@
       <c r="J25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10" t="s">
+      <c r="K25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="10"/>
-    </row>
-    <row r="26" spans="1:17" ht="15">
+      <c r="R25" s="10"/>
+    </row>
+    <row r="26" spans="1:18" ht="15">
       <c r="A26" s="78" t="s">
         <v>70</v>
       </c>
@@ -12266,13 +11472,16 @@
       <c r="L26" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="10"/>
+      <c r="M26" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
-    </row>
-    <row r="27" spans="1:17" ht="15">
+      <c r="R26" s="10"/>
+    </row>
+    <row r="27" spans="1:18" ht="15">
       <c r="A27" s="79" t="s">
         <v>72</v>
       </c>
@@ -12304,15 +11513,18 @@
       <c r="J27" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K27" s="10"/>
+      <c r="K27" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
-    </row>
-    <row r="28" spans="1:17" ht="15">
+      <c r="R27" s="10"/>
+    </row>
+    <row r="28" spans="1:18" ht="15">
       <c r="A28" s="79" t="s">
         <v>75</v>
       </c>
@@ -12344,17 +11556,20 @@
       <c r="J28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10" t="s">
+      <c r="K28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="10"/>
-    </row>
-    <row r="29" spans="1:17" ht="15">
+      <c r="R28" s="10"/>
+    </row>
+    <row r="29" spans="1:18" ht="15">
       <c r="A29" s="78" t="s">
         <v>78</v>
       </c>
@@ -12386,15 +11601,18 @@
       <c r="J29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="K29" s="16"/>
+      <c r="K29" s="16" t="s">
+        <v>20</v>
+      </c>
       <c r="L29" s="16"/>
-      <c r="M29" s="10"/>
+      <c r="M29" s="16"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="10"/>
-    </row>
-    <row r="30" spans="1:17" ht="15">
+      <c r="R29" s="10"/>
+    </row>
+    <row r="30" spans="1:18" ht="15">
       <c r="A30" s="78" t="s">
         <v>81</v>
       </c>
@@ -12430,18 +11648,21 @@
       <c r="K30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10" t="s">
+      <c r="L30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N30" s="10"/>
-      <c r="O30" s="10" t="s">
+      <c r="M30" s="10"/>
+      <c r="N30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="Q30" s="10"/>
-    </row>
-    <row r="31" spans="1:17" ht="15">
+      <c r="R30" s="10"/>
+    </row>
+    <row r="31" spans="1:18" ht="15">
       <c r="A31" s="79" t="s">
         <v>84</v>
       </c>
@@ -12470,24 +11691,23 @@
         <v>19</v>
       </c>
       <c r="I31" s="10"/>
-      <c r="J31" s="10" t="s">
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K31" s="83" t="s">
+      <c r="M31" s="10"/>
+      <c r="N31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10" t="s">
+      <c r="O31" s="10"/>
+      <c r="P31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
-    </row>
-    <row r="32" spans="1:17" ht="15">
+      <c r="R31" s="10"/>
+    </row>
+    <row r="32" spans="1:18" ht="15">
       <c r="A32" s="78" t="s">
         <v>86</v>
       </c>
@@ -12517,21 +11737,22 @@
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
-      <c r="K32" s="10" t="s">
+      <c r="K32" s="10"/>
+      <c r="L32" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10" t="s">
+      <c r="M32" s="10"/>
+      <c r="N32" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10" t="s">
+      <c r="O32" s="10"/>
+      <c r="P32" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P32" s="10"/>
       <c r="Q32" s="10"/>
-    </row>
-    <row r="33" spans="1:17" ht="15">
+      <c r="R32" s="10"/>
+    </row>
+    <row r="33" spans="1:18" ht="15">
       <c r="A33" s="78" t="s">
         <v>89</v>
       </c>
@@ -12563,15 +11784,18 @@
       <c r="J33" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K33" s="10"/>
+      <c r="K33" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
       <c r="Q33" s="10"/>
-    </row>
-    <row r="34" spans="1:17" ht="15">
+      <c r="R33" s="10"/>
+    </row>
+    <row r="34" spans="1:18" ht="15">
       <c r="A34" s="79" t="s">
         <v>91</v>
       </c>
@@ -12604,14 +11828,15 @@
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
-      <c r="N34" s="10" t="s">
+      <c r="N34" s="10"/>
+      <c r="O34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O34" s="10"/>
       <c r="P34" s="10"/>
       <c r="Q34" s="10"/>
-    </row>
-    <row r="35" spans="1:17" ht="15">
+      <c r="R34" s="10"/>
+    </row>
+    <row r="35" spans="1:18" ht="15">
       <c r="A35" s="79" t="s">
         <v>94</v>
       </c>
@@ -12643,15 +11868,16 @@
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="10" t="s">
+      <c r="M35" s="10"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O35" s="80"/>
-      <c r="P35" s="10"/>
+      <c r="P35" s="80"/>
       <c r="Q35" s="10"/>
-    </row>
-    <row r="36" spans="1:17" ht="15">
+      <c r="R35" s="10"/>
+    </row>
+    <row r="36" spans="1:18" ht="15">
       <c r="A36" s="79" t="s">
         <v>96</v>
       </c>
@@ -12684,16 +11910,17 @@
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
-      <c r="N36" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N36" s="10"/>
       <c r="O36" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P36" s="10"/>
+      <c r="P36" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="Q36" s="10"/>
-    </row>
-    <row r="37" spans="1:17" ht="15">
+      <c r="R36" s="10"/>
+    </row>
+    <row r="37" spans="1:18" ht="15">
       <c r="A37" s="79" t="s">
         <v>98</v>
       </c>
@@ -12726,14 +11953,15 @@
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
-      <c r="N37" s="10" t="s">
+      <c r="N37" s="10"/>
+      <c r="O37" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O37" s="10"/>
       <c r="P37" s="10"/>
       <c r="Q37" s="10"/>
-    </row>
-    <row r="38" spans="1:17" ht="15">
+      <c r="R37" s="10"/>
+    </row>
+    <row r="38" spans="1:18" ht="15">
       <c r="A38" s="79" t="s">
         <v>101</v>
       </c>
@@ -12767,13 +11995,14 @@
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
-      <c r="O38" s="10" t="s">
+      <c r="O38" s="10"/>
+      <c r="P38" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P38" s="10"/>
       <c r="Q38" s="10"/>
-    </row>
-    <row r="39" spans="1:17" ht="15">
+      <c r="R38" s="10"/>
+    </row>
+    <row r="39" spans="1:18" ht="15">
       <c r="A39" s="79" t="s">
         <v>104</v>
       </c>
@@ -12805,17 +12034,18 @@
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
       <c r="L39" s="10"/>
-      <c r="M39" s="10" t="s">
+      <c r="M39" s="10"/>
+      <c r="N39" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="N39" s="10"/>
       <c r="O39" s="10"/>
-      <c r="P39" s="10" t="s">
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Q39" s="10"/>
-    </row>
-    <row r="40" spans="1:17" ht="15">
+      <c r="R39" s="10"/>
+    </row>
+    <row r="40" spans="1:18" ht="15">
       <c r="A40" s="79" t="s">
         <v>2881</v>
       </c>
@@ -12849,11 +12079,12 @@
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
-      <c r="Q40" s="10" t="s">
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15">
+    <row r="41" spans="1:18" ht="15">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="14"/>
@@ -12871,8 +12102,9 @@
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
       <c r="Q41" s="10"/>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="R41" s="10"/>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -12890,8 +12122,9 @@
       <c r="O42" s="10"/>
       <c r="P42" s="10"/>
       <c r="Q42" s="10"/>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="R42" s="10"/>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -12909,8 +12142,9 @@
       <c r="O43" s="10"/>
       <c r="P43" s="10"/>
       <c r="Q43" s="10"/>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="R43" s="10"/>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -12928,8 +12162,9 @@
       <c r="O44" s="10"/>
       <c r="P44" s="10"/>
       <c r="Q44" s="10"/>
-    </row>
-    <row r="45" spans="1:17">
+      <c r="R44" s="10"/>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -12947,8 +12182,9 @@
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
       <c r="Q45" s="10"/>
-    </row>
-    <row r="46" spans="1:17">
+      <c r="R45" s="10"/>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
@@ -12966,8 +12202,9 @@
       <c r="O46" s="10"/>
       <c r="P46" s="10"/>
       <c r="Q46" s="10"/>
-    </row>
-    <row r="47" spans="1:17">
+      <c r="R46" s="10"/>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -12985,8 +12222,9 @@
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
       <c r="Q47" s="10"/>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="R47" s="10"/>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -13004,8 +12242,9 @@
       <c r="O48" s="10"/>
       <c r="P48" s="10"/>
       <c r="Q48" s="10"/>
-    </row>
-    <row r="49" spans="1:17">
+      <c r="R48" s="10"/>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -13023,8 +12262,9 @@
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
       <c r="Q49" s="10"/>
-    </row>
-    <row r="50" spans="1:17">
+      <c r="R49" s="10"/>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -13042,8 +12282,9 @@
       <c r="O50" s="10"/>
       <c r="P50" s="10"/>
       <c r="Q50" s="10"/>
-    </row>
-    <row r="51" spans="1:17">
+      <c r="R50" s="10"/>
+    </row>
+    <row r="51" spans="1:18">
       <c r="A51" s="9"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -13061,8 +12302,9 @@
       <c r="O51" s="10"/>
       <c r="P51" s="10"/>
       <c r="Q51" s="10"/>
-    </row>
-    <row r="52" spans="1:17">
+      <c r="R51" s="10"/>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -13080,8 +12322,9 @@
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
       <c r="Q52" s="10"/>
-    </row>
-    <row r="53" spans="1:17">
+      <c r="R52" s="10"/>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -13099,8 +12342,9 @@
       <c r="O53" s="10"/>
       <c r="P53" s="10"/>
       <c r="Q53" s="10"/>
-    </row>
-    <row r="54" spans="1:17">
+      <c r="R53" s="10"/>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -13118,8 +12362,9 @@
       <c r="O54" s="10"/>
       <c r="P54" s="10"/>
       <c r="Q54" s="10"/>
-    </row>
-    <row r="55" spans="1:17">
+      <c r="R54" s="10"/>
+    </row>
+    <row r="55" spans="1:18">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -13137,8 +12382,9 @@
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
       <c r="Q55" s="10"/>
-    </row>
-    <row r="56" spans="1:17">
+      <c r="R55" s="10"/>
+    </row>
+    <row r="56" spans="1:18">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -13156,8 +12402,9 @@
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
       <c r="Q56" s="10"/>
-    </row>
-    <row r="57" spans="1:17">
+      <c r="R56" s="10"/>
+    </row>
+    <row r="57" spans="1:18">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -13175,8 +12422,9 @@
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
       <c r="Q57" s="10"/>
-    </row>
-    <row r="58" spans="1:17">
+      <c r="R57" s="10"/>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -13194,8 +12442,9 @@
       <c r="O58" s="10"/>
       <c r="P58" s="10"/>
       <c r="Q58" s="10"/>
-    </row>
-    <row r="59" spans="1:17">
+      <c r="R58" s="10"/>
+    </row>
+    <row r="59" spans="1:18">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -13213,8 +12462,9 @@
       <c r="O59" s="10"/>
       <c r="P59" s="10"/>
       <c r="Q59" s="10"/>
-    </row>
-    <row r="60" spans="1:17">
+      <c r="R59" s="10"/>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -13232,8 +12482,9 @@
       <c r="O60" s="10"/>
       <c r="P60" s="10"/>
       <c r="Q60" s="10"/>
-    </row>
-    <row r="61" spans="1:17">
+      <c r="R60" s="10"/>
+    </row>
+    <row r="61" spans="1:18">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -13251,8 +12502,9 @@
       <c r="O61" s="10"/>
       <c r="P61" s="10"/>
       <c r="Q61" s="10"/>
-    </row>
-    <row r="62" spans="1:17">
+      <c r="R61" s="10"/>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -13270,8 +12522,9 @@
       <c r="O62" s="10"/>
       <c r="P62" s="10"/>
       <c r="Q62" s="10"/>
-    </row>
-    <row r="63" spans="1:17">
+      <c r="R62" s="10"/>
+    </row>
+    <row r="63" spans="1:18">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -13289,8 +12542,9 @@
       <c r="O63" s="10"/>
       <c r="P63" s="10"/>
       <c r="Q63" s="10"/>
-    </row>
-    <row r="64" spans="1:17">
+      <c r="R63" s="10"/>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -13308,8 +12562,9 @@
       <c r="O64" s="10"/>
       <c r="P64" s="10"/>
       <c r="Q64" s="10"/>
-    </row>
-    <row r="65" spans="1:17">
+      <c r="R64" s="10"/>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -13327,8 +12582,9 @@
       <c r="O65" s="10"/>
       <c r="P65" s="10"/>
       <c r="Q65" s="10"/>
-    </row>
-    <row r="66" spans="1:17">
+      <c r="R65" s="10"/>
+    </row>
+    <row r="66" spans="1:18">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -13346,8 +12602,9 @@
       <c r="O66" s="10"/>
       <c r="P66" s="10"/>
       <c r="Q66" s="10"/>
-    </row>
-    <row r="67" spans="1:17">
+      <c r="R66" s="10"/>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -13365,8 +12622,9 @@
       <c r="O67" s="10"/>
       <c r="P67" s="10"/>
       <c r="Q67" s="10"/>
-    </row>
-    <row r="68" spans="1:17">
+      <c r="R67" s="10"/>
+    </row>
+    <row r="68" spans="1:18">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -13384,8 +12642,9 @@
       <c r="O68" s="10"/>
       <c r="P68" s="10"/>
       <c r="Q68" s="10"/>
-    </row>
-    <row r="69" spans="1:17">
+      <c r="R68" s="10"/>
+    </row>
+    <row r="69" spans="1:18">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -13403,8 +12662,9 @@
       <c r="O69" s="10"/>
       <c r="P69" s="10"/>
       <c r="Q69" s="10"/>
-    </row>
-    <row r="70" spans="1:17">
+      <c r="R69" s="10"/>
+    </row>
+    <row r="70" spans="1:18">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -13422,8 +12682,9 @@
       <c r="O70" s="10"/>
       <c r="P70" s="10"/>
       <c r="Q70" s="10"/>
-    </row>
-    <row r="71" spans="1:17">
+      <c r="R70" s="10"/>
+    </row>
+    <row r="71" spans="1:18">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -13441,8 +12702,9 @@
       <c r="O71" s="10"/>
       <c r="P71" s="10"/>
       <c r="Q71" s="10"/>
-    </row>
-    <row r="72" spans="1:17">
+      <c r="R71" s="10"/>
+    </row>
+    <row r="72" spans="1:18">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -13460,8 +12722,9 @@
       <c r="O72" s="10"/>
       <c r="P72" s="10"/>
       <c r="Q72" s="10"/>
-    </row>
-    <row r="73" spans="1:17">
+      <c r="R72" s="10"/>
+    </row>
+    <row r="73" spans="1:18">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -13479,8 +12742,9 @@
       <c r="O73" s="10"/>
       <c r="P73" s="10"/>
       <c r="Q73" s="10"/>
-    </row>
-    <row r="74" spans="1:17">
+      <c r="R73" s="10"/>
+    </row>
+    <row r="74" spans="1:18">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -13498,8 +12762,9 @@
       <c r="O74" s="10"/>
       <c r="P74" s="10"/>
       <c r="Q74" s="10"/>
-    </row>
-    <row r="75" spans="1:17">
+      <c r="R74" s="10"/>
+    </row>
+    <row r="75" spans="1:18">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -13517,8 +12782,9 @@
       <c r="O75" s="10"/>
       <c r="P75" s="10"/>
       <c r="Q75" s="10"/>
-    </row>
-    <row r="76" spans="1:17">
+      <c r="R75" s="10"/>
+    </row>
+    <row r="76" spans="1:18">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -13536,8 +12802,9 @@
       <c r="O76" s="10"/>
       <c r="P76" s="10"/>
       <c r="Q76" s="10"/>
-    </row>
-    <row r="77" spans="1:17">
+      <c r="R76" s="10"/>
+    </row>
+    <row r="77" spans="1:18">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -13555,8 +12822,9 @@
       <c r="O77" s="10"/>
       <c r="P77" s="10"/>
       <c r="Q77" s="10"/>
-    </row>
-    <row r="78" spans="1:17">
+      <c r="R77" s="10"/>
+    </row>
+    <row r="78" spans="1:18">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -13574,8 +12842,9 @@
       <c r="O78" s="10"/>
       <c r="P78" s="10"/>
       <c r="Q78" s="10"/>
-    </row>
-    <row r="79" spans="1:17">
+      <c r="R78" s="10"/>
+    </row>
+    <row r="79" spans="1:18">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -13593,8 +12862,9 @@
       <c r="O79" s="10"/>
       <c r="P79" s="10"/>
       <c r="Q79" s="10"/>
-    </row>
-    <row r="80" spans="1:17">
+      <c r="R79" s="10"/>
+    </row>
+    <row r="80" spans="1:18">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -13612,8 +12882,9 @@
       <c r="O80" s="10"/>
       <c r="P80" s="10"/>
       <c r="Q80" s="10"/>
-    </row>
-    <row r="81" spans="1:17">
+      <c r="R80" s="10"/>
+    </row>
+    <row r="81" spans="1:18">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -13631,8 +12902,9 @@
       <c r="O81" s="10"/>
       <c r="P81" s="10"/>
       <c r="Q81" s="10"/>
-    </row>
-    <row r="82" spans="1:17">
+      <c r="R81" s="10"/>
+    </row>
+    <row r="82" spans="1:18">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -13650,8 +12922,9 @@
       <c r="O82" s="10"/>
       <c r="P82" s="10"/>
       <c r="Q82" s="10"/>
-    </row>
-    <row r="83" spans="1:17">
+      <c r="R82" s="10"/>
+    </row>
+    <row r="83" spans="1:18">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -13669,8 +12942,9 @@
       <c r="O83" s="10"/>
       <c r="P83" s="10"/>
       <c r="Q83" s="10"/>
-    </row>
-    <row r="84" spans="1:17">
+      <c r="R83" s="10"/>
+    </row>
+    <row r="84" spans="1:18">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -13688,8 +12962,9 @@
       <c r="O84" s="10"/>
       <c r="P84" s="10"/>
       <c r="Q84" s="10"/>
-    </row>
-    <row r="85" spans="1:17">
+      <c r="R84" s="10"/>
+    </row>
+    <row r="85" spans="1:18">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -13707,8 +12982,9 @@
       <c r="O85" s="10"/>
       <c r="P85" s="10"/>
       <c r="Q85" s="10"/>
-    </row>
-    <row r="86" spans="1:17">
+      <c r="R85" s="10"/>
+    </row>
+    <row r="86" spans="1:18">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -13726,8 +13002,9 @@
       <c r="O86" s="10"/>
       <c r="P86" s="10"/>
       <c r="Q86" s="10"/>
-    </row>
-    <row r="87" spans="1:17">
+      <c r="R86" s="10"/>
+    </row>
+    <row r="87" spans="1:18">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -13745,8 +13022,9 @@
       <c r="O87" s="10"/>
       <c r="P87" s="10"/>
       <c r="Q87" s="10"/>
-    </row>
-    <row r="88" spans="1:17">
+      <c r="R87" s="10"/>
+    </row>
+    <row r="88" spans="1:18">
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -13764,8 +13042,9 @@
       <c r="O88" s="10"/>
       <c r="P88" s="10"/>
       <c r="Q88" s="10"/>
-    </row>
-    <row r="89" spans="1:17">
+      <c r="R88" s="10"/>
+    </row>
+    <row r="89" spans="1:18">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -13783,8 +13062,9 @@
       <c r="O89" s="10"/>
       <c r="P89" s="10"/>
       <c r="Q89" s="10"/>
-    </row>
-    <row r="90" spans="1:17">
+      <c r="R89" s="10"/>
+    </row>
+    <row r="90" spans="1:18">
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -13802,8 +13082,9 @@
       <c r="O90" s="10"/>
       <c r="P90" s="10"/>
       <c r="Q90" s="10"/>
-    </row>
-    <row r="91" spans="1:17">
+      <c r="R90" s="10"/>
+    </row>
+    <row r="91" spans="1:18">
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -13821,8 +13102,9 @@
       <c r="O91" s="10"/>
       <c r="P91" s="10"/>
       <c r="Q91" s="10"/>
-    </row>
-    <row r="92" spans="1:17">
+      <c r="R91" s="10"/>
+    </row>
+    <row r="92" spans="1:18">
       <c r="A92" s="9"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -13840,8 +13122,9 @@
       <c r="O92" s="10"/>
       <c r="P92" s="10"/>
       <c r="Q92" s="10"/>
-    </row>
-    <row r="93" spans="1:17">
+      <c r="R92" s="10"/>
+    </row>
+    <row r="93" spans="1:18">
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -13859,8 +13142,9 @@
       <c r="O93" s="10"/>
       <c r="P93" s="10"/>
       <c r="Q93" s="10"/>
-    </row>
-    <row r="94" spans="1:17">
+      <c r="R93" s="10"/>
+    </row>
+    <row r="94" spans="1:18">
       <c r="A94" s="9"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -13878,8 +13162,9 @@
       <c r="O94" s="10"/>
       <c r="P94" s="10"/>
       <c r="Q94" s="10"/>
-    </row>
-    <row r="95" spans="1:17">
+      <c r="R94" s="10"/>
+    </row>
+    <row r="95" spans="1:18">
       <c r="A95" s="9"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -13897,8 +13182,9 @@
       <c r="O95" s="10"/>
       <c r="P95" s="10"/>
       <c r="Q95" s="10"/>
-    </row>
-    <row r="96" spans="1:17">
+      <c r="R95" s="10"/>
+    </row>
+    <row r="96" spans="1:18">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -13916,8 +13202,9 @@
       <c r="O96" s="10"/>
       <c r="P96" s="10"/>
       <c r="Q96" s="10"/>
-    </row>
-    <row r="97" spans="1:17">
+      <c r="R96" s="10"/>
+    </row>
+    <row r="97" spans="1:18">
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -13935,8 +13222,9 @@
       <c r="O97" s="10"/>
       <c r="P97" s="10"/>
       <c r="Q97" s="10"/>
-    </row>
-    <row r="98" spans="1:17">
+      <c r="R97" s="10"/>
+    </row>
+    <row r="98" spans="1:18">
       <c r="A98" s="9"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -13954,8 +13242,9 @@
       <c r="O98" s="10"/>
       <c r="P98" s="10"/>
       <c r="Q98" s="10"/>
-    </row>
-    <row r="99" spans="1:17">
+      <c r="R98" s="10"/>
+    </row>
+    <row r="99" spans="1:18">
       <c r="A99" s="9"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -13973,8 +13262,9 @@
       <c r="O99" s="10"/>
       <c r="P99" s="10"/>
       <c r="Q99" s="10"/>
-    </row>
-    <row r="100" spans="1:17">
+      <c r="R99" s="10"/>
+    </row>
+    <row r="100" spans="1:18">
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -13992,8 +13282,9 @@
       <c r="O100" s="10"/>
       <c r="P100" s="10"/>
       <c r="Q100" s="10"/>
-    </row>
-    <row r="101" spans="1:17">
+      <c r="R100" s="10"/>
+    </row>
+    <row r="101" spans="1:18">
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -14011,8 +13302,9 @@
       <c r="O101" s="10"/>
       <c r="P101" s="10"/>
       <c r="Q101" s="10"/>
-    </row>
-    <row r="102" spans="1:17">
+      <c r="R101" s="10"/>
+    </row>
+    <row r="102" spans="1:18">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -14030,8 +13322,9 @@
       <c r="O102" s="10"/>
       <c r="P102" s="10"/>
       <c r="Q102" s="10"/>
-    </row>
-    <row r="103" spans="1:17">
+      <c r="R102" s="10"/>
+    </row>
+    <row r="103" spans="1:18">
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
@@ -14049,8 +13342,9 @@
       <c r="O103" s="10"/>
       <c r="P103" s="10"/>
       <c r="Q103" s="10"/>
-    </row>
-    <row r="104" spans="1:17">
+      <c r="R103" s="10"/>
+    </row>
+    <row r="104" spans="1:18">
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
@@ -14068,8 +13362,9 @@
       <c r="O104" s="10"/>
       <c r="P104" s="10"/>
       <c r="Q104" s="10"/>
-    </row>
-    <row r="105" spans="1:17">
+      <c r="R104" s="10"/>
+    </row>
+    <row r="105" spans="1:18">
       <c r="A105" s="9"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -14087,8 +13382,9 @@
       <c r="O105" s="10"/>
       <c r="P105" s="10"/>
       <c r="Q105" s="10"/>
-    </row>
-    <row r="106" spans="1:17">
+      <c r="R105" s="10"/>
+    </row>
+    <row r="106" spans="1:18">
       <c r="A106" s="9"/>
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
@@ -14106,8 +13402,9 @@
       <c r="O106" s="10"/>
       <c r="P106" s="10"/>
       <c r="Q106" s="10"/>
-    </row>
-    <row r="107" spans="1:17">
+      <c r="R106" s="10"/>
+    </row>
+    <row r="107" spans="1:18">
       <c r="A107" s="9"/>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
@@ -14125,8 +13422,9 @@
       <c r="O107" s="10"/>
       <c r="P107" s="10"/>
       <c r="Q107" s="10"/>
-    </row>
-    <row r="108" spans="1:17">
+      <c r="R107" s="10"/>
+    </row>
+    <row r="108" spans="1:18">
       <c r="A108" s="9"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
@@ -14144,8 +13442,9 @@
       <c r="O108" s="10"/>
       <c r="P108" s="10"/>
       <c r="Q108" s="10"/>
-    </row>
-    <row r="109" spans="1:17">
+      <c r="R108" s="10"/>
+    </row>
+    <row r="109" spans="1:18">
       <c r="A109" s="9"/>
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
@@ -14163,8 +13462,9 @@
       <c r="O109" s="10"/>
       <c r="P109" s="10"/>
       <c r="Q109" s="10"/>
-    </row>
-    <row r="110" spans="1:17">
+      <c r="R109" s="10"/>
+    </row>
+    <row r="110" spans="1:18">
       <c r="A110" s="9"/>
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
@@ -14182,8 +13482,9 @@
       <c r="O110" s="10"/>
       <c r="P110" s="10"/>
       <c r="Q110" s="10"/>
-    </row>
-    <row r="111" spans="1:17">
+      <c r="R110" s="10"/>
+    </row>
+    <row r="111" spans="1:18">
       <c r="A111" s="9"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
@@ -14201,8 +13502,9 @@
       <c r="O111" s="10"/>
       <c r="P111" s="10"/>
       <c r="Q111" s="10"/>
-    </row>
-    <row r="112" spans="1:17">
+      <c r="R111" s="10"/>
+    </row>
+    <row r="112" spans="1:18">
       <c r="A112" s="9"/>
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
@@ -14220,8 +13522,9 @@
       <c r="O112" s="10"/>
       <c r="P112" s="10"/>
       <c r="Q112" s="10"/>
-    </row>
-    <row r="113" spans="1:17">
+      <c r="R112" s="10"/>
+    </row>
+    <row r="113" spans="1:18">
       <c r="A113" s="9"/>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
@@ -14239,8 +13542,9 @@
       <c r="O113" s="10"/>
       <c r="P113" s="10"/>
       <c r="Q113" s="10"/>
-    </row>
-    <row r="114" spans="1:17">
+      <c r="R113" s="10"/>
+    </row>
+    <row r="114" spans="1:18">
       <c r="A114" s="9"/>
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
@@ -14258,8 +13562,9 @@
       <c r="O114" s="10"/>
       <c r="P114" s="10"/>
       <c r="Q114" s="10"/>
-    </row>
-    <row r="115" spans="1:17">
+      <c r="R114" s="10"/>
+    </row>
+    <row r="115" spans="1:18">
       <c r="A115" s="9"/>
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
@@ -14277,8 +13582,9 @@
       <c r="O115" s="10"/>
       <c r="P115" s="10"/>
       <c r="Q115" s="10"/>
-    </row>
-    <row r="116" spans="1:17">
+      <c r="R115" s="10"/>
+    </row>
+    <row r="116" spans="1:18">
       <c r="A116" s="9"/>
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
@@ -14296,8 +13602,9 @@
       <c r="O116" s="10"/>
       <c r="P116" s="10"/>
       <c r="Q116" s="10"/>
-    </row>
-    <row r="117" spans="1:17">
+      <c r="R116" s="10"/>
+    </row>
+    <row r="117" spans="1:18">
       <c r="A117" s="9"/>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
@@ -14315,8 +13622,9 @@
       <c r="O117" s="10"/>
       <c r="P117" s="10"/>
       <c r="Q117" s="10"/>
-    </row>
-    <row r="118" spans="1:17">
+      <c r="R117" s="10"/>
+    </row>
+    <row r="118" spans="1:18">
       <c r="A118" s="9"/>
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
@@ -14334,8 +13642,9 @@
       <c r="O118" s="10"/>
       <c r="P118" s="10"/>
       <c r="Q118" s="10"/>
-    </row>
-    <row r="119" spans="1:17">
+      <c r="R118" s="10"/>
+    </row>
+    <row r="119" spans="1:18">
       <c r="A119" s="9"/>
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
@@ -14353,8 +13662,9 @@
       <c r="O119" s="10"/>
       <c r="P119" s="10"/>
       <c r="Q119" s="10"/>
-    </row>
-    <row r="120" spans="1:17">
+      <c r="R119" s="10"/>
+    </row>
+    <row r="120" spans="1:18">
       <c r="A120" s="9"/>
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
@@ -14372,8 +13682,9 @@
       <c r="O120" s="10"/>
       <c r="P120" s="10"/>
       <c r="Q120" s="10"/>
-    </row>
-    <row r="121" spans="1:17">
+      <c r="R120" s="10"/>
+    </row>
+    <row r="121" spans="1:18">
       <c r="A121" s="9"/>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
@@ -14391,8 +13702,9 @@
       <c r="O121" s="10"/>
       <c r="P121" s="10"/>
       <c r="Q121" s="10"/>
-    </row>
-    <row r="122" spans="1:17">
+      <c r="R121" s="10"/>
+    </row>
+    <row r="122" spans="1:18">
       <c r="A122" s="9"/>
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
@@ -14410,8 +13722,9 @@
       <c r="O122" s="10"/>
       <c r="P122" s="10"/>
       <c r="Q122" s="10"/>
-    </row>
-    <row r="123" spans="1:17">
+      <c r="R122" s="10"/>
+    </row>
+    <row r="123" spans="1:18">
       <c r="A123" s="9"/>
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
@@ -14429,8 +13742,9 @@
       <c r="O123" s="9"/>
       <c r="P123" s="9"/>
       <c r="Q123" s="9"/>
-    </row>
-    <row r="124" spans="1:17">
+      <c r="R123" s="9"/>
+    </row>
+    <row r="124" spans="1:18">
       <c r="A124" s="9"/>
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
@@ -14448,8 +13762,9 @@
       <c r="O124" s="9"/>
       <c r="P124" s="9"/>
       <c r="Q124" s="9"/>
-    </row>
-    <row r="125" spans="1:17">
+      <c r="R124" s="9"/>
+    </row>
+    <row r="125" spans="1:18">
       <c r="A125" s="9"/>
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
@@ -14467,8 +13782,9 @@
       <c r="O125" s="9"/>
       <c r="P125" s="9"/>
       <c r="Q125" s="9"/>
-    </row>
-    <row r="126" spans="1:17">
+      <c r="R125" s="9"/>
+    </row>
+    <row r="126" spans="1:18">
       <c r="A126" s="9"/>
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
@@ -14486,8 +13802,9 @@
       <c r="O126" s="9"/>
       <c r="P126" s="9"/>
       <c r="Q126" s="9"/>
-    </row>
-    <row r="127" spans="1:17">
+      <c r="R126" s="9"/>
+    </row>
+    <row r="127" spans="1:18">
       <c r="A127" s="9"/>
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
@@ -14505,8 +13822,9 @@
       <c r="O127" s="9"/>
       <c r="P127" s="9"/>
       <c r="Q127" s="9"/>
-    </row>
-    <row r="128" spans="1:17">
+      <c r="R127" s="9"/>
+    </row>
+    <row r="128" spans="1:18">
       <c r="A128" s="9"/>
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
@@ -14524,8 +13842,9 @@
       <c r="O128" s="9"/>
       <c r="P128" s="9"/>
       <c r="Q128" s="9"/>
-    </row>
-    <row r="129" spans="1:17">
+      <c r="R128" s="9"/>
+    </row>
+    <row r="129" spans="1:18">
       <c r="A129" s="9"/>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
@@ -14543,8 +13862,9 @@
       <c r="O129" s="9"/>
       <c r="P129" s="9"/>
       <c r="Q129" s="9"/>
-    </row>
-    <row r="130" spans="1:17">
+      <c r="R129" s="9"/>
+    </row>
+    <row r="130" spans="1:18">
       <c r="A130" s="9"/>
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
@@ -14562,8 +13882,9 @@
       <c r="O130" s="9"/>
       <c r="P130" s="9"/>
       <c r="Q130" s="9"/>
-    </row>
-    <row r="131" spans="1:17">
+      <c r="R130" s="9"/>
+    </row>
+    <row r="131" spans="1:18">
       <c r="A131" s="9"/>
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
@@ -14581,8 +13902,9 @@
       <c r="O131" s="9"/>
       <c r="P131" s="9"/>
       <c r="Q131" s="9"/>
-    </row>
-    <row r="132" spans="1:17">
+      <c r="R131" s="9"/>
+    </row>
+    <row r="132" spans="1:18">
       <c r="A132" s="9"/>
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
@@ -14600,8 +13922,9 @@
       <c r="O132" s="9"/>
       <c r="P132" s="9"/>
       <c r="Q132" s="9"/>
-    </row>
-    <row r="133" spans="1:17">
+      <c r="R132" s="9"/>
+    </row>
+    <row r="133" spans="1:18">
       <c r="A133" s="9"/>
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
@@ -14619,8 +13942,9 @@
       <c r="O133" s="9"/>
       <c r="P133" s="9"/>
       <c r="Q133" s="9"/>
-    </row>
-    <row r="134" spans="1:17">
+      <c r="R133" s="9"/>
+    </row>
+    <row r="134" spans="1:18">
       <c r="A134" s="9"/>
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
@@ -14638,8 +13962,9 @@
       <c r="O134" s="9"/>
       <c r="P134" s="9"/>
       <c r="Q134" s="9"/>
-    </row>
-    <row r="135" spans="1:17">
+      <c r="R134" s="9"/>
+    </row>
+    <row r="135" spans="1:18">
       <c r="A135" s="9"/>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
@@ -14657,8 +13982,9 @@
       <c r="O135" s="9"/>
       <c r="P135" s="9"/>
       <c r="Q135" s="9"/>
-    </row>
-    <row r="136" spans="1:17">
+      <c r="R135" s="9"/>
+    </row>
+    <row r="136" spans="1:18">
       <c r="A136" s="9"/>
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
@@ -14676,8 +14002,9 @@
       <c r="O136" s="9"/>
       <c r="P136" s="9"/>
       <c r="Q136" s="9"/>
-    </row>
-    <row r="137" spans="1:17">
+      <c r="R136" s="9"/>
+    </row>
+    <row r="137" spans="1:18">
       <c r="A137" s="9"/>
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
@@ -14695,8 +14022,9 @@
       <c r="O137" s="9"/>
       <c r="P137" s="9"/>
       <c r="Q137" s="9"/>
-    </row>
-    <row r="138" spans="1:17">
+      <c r="R137" s="9"/>
+    </row>
+    <row r="138" spans="1:18">
       <c r="A138" s="9"/>
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
@@ -14714,8 +14042,9 @@
       <c r="O138" s="9"/>
       <c r="P138" s="9"/>
       <c r="Q138" s="9"/>
-    </row>
-    <row r="139" spans="1:17">
+      <c r="R138" s="9"/>
+    </row>
+    <row r="139" spans="1:18">
       <c r="A139" s="9"/>
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
@@ -14733,8 +14062,9 @@
       <c r="O139" s="9"/>
       <c r="P139" s="9"/>
       <c r="Q139" s="9"/>
-    </row>
-    <row r="140" spans="1:17">
+      <c r="R139" s="9"/>
+    </row>
+    <row r="140" spans="1:18">
       <c r="A140" s="9"/>
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
@@ -14752,8 +14082,9 @@
       <c r="O140" s="9"/>
       <c r="P140" s="9"/>
       <c r="Q140" s="9"/>
-    </row>
-    <row r="141" spans="1:17">
+      <c r="R140" s="9"/>
+    </row>
+    <row r="141" spans="1:18">
       <c r="A141" s="9"/>
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
@@ -14771,8 +14102,9 @@
       <c r="O141" s="9"/>
       <c r="P141" s="9"/>
       <c r="Q141" s="9"/>
-    </row>
-    <row r="142" spans="1:17">
+      <c r="R141" s="9"/>
+    </row>
+    <row r="142" spans="1:18">
       <c r="A142" s="9"/>
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
@@ -14790,8 +14122,9 @@
       <c r="O142" s="9"/>
       <c r="P142" s="9"/>
       <c r="Q142" s="9"/>
-    </row>
-    <row r="143" spans="1:17">
+      <c r="R142" s="9"/>
+    </row>
+    <row r="143" spans="1:18">
       <c r="A143" s="9"/>
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
@@ -14809,8 +14142,9 @@
       <c r="O143" s="9"/>
       <c r="P143" s="9"/>
       <c r="Q143" s="9"/>
-    </row>
-    <row r="144" spans="1:17">
+      <c r="R143" s="9"/>
+    </row>
+    <row r="144" spans="1:18">
       <c r="A144" s="9"/>
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
@@ -14828,8 +14162,9 @@
       <c r="O144" s="9"/>
       <c r="P144" s="9"/>
       <c r="Q144" s="9"/>
-    </row>
-    <row r="145" spans="1:17">
+      <c r="R144" s="9"/>
+    </row>
+    <row r="145" spans="1:18">
       <c r="A145" s="9"/>
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
@@ -14847,8 +14182,9 @@
       <c r="O145" s="9"/>
       <c r="P145" s="9"/>
       <c r="Q145" s="9"/>
-    </row>
-    <row r="146" spans="1:17">
+      <c r="R145" s="9"/>
+    </row>
+    <row r="146" spans="1:18">
       <c r="A146" s="9"/>
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
@@ -14866,8 +14202,9 @@
       <c r="O146" s="9"/>
       <c r="P146" s="9"/>
       <c r="Q146" s="9"/>
-    </row>
-    <row r="147" spans="1:17">
+      <c r="R146" s="9"/>
+    </row>
+    <row r="147" spans="1:18">
       <c r="A147" s="9"/>
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
@@ -14885,8 +14222,9 @@
       <c r="O147" s="9"/>
       <c r="P147" s="9"/>
       <c r="Q147" s="9"/>
-    </row>
-    <row r="148" spans="1:17">
+      <c r="R147" s="9"/>
+    </row>
+    <row r="148" spans="1:18">
       <c r="A148" s="9"/>
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
@@ -14904,8 +14242,9 @@
       <c r="O148" s="9"/>
       <c r="P148" s="9"/>
       <c r="Q148" s="9"/>
-    </row>
-    <row r="149" spans="1:17">
+      <c r="R148" s="9"/>
+    </row>
+    <row r="149" spans="1:18">
       <c r="A149" s="9"/>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
@@ -14923,8 +14262,9 @@
       <c r="O149" s="9"/>
       <c r="P149" s="9"/>
       <c r="Q149" s="9"/>
-    </row>
-    <row r="150" spans="1:17">
+      <c r="R149" s="9"/>
+    </row>
+    <row r="150" spans="1:18">
       <c r="A150" s="9"/>
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
@@ -14942,8 +14282,9 @@
       <c r="O150" s="9"/>
       <c r="P150" s="9"/>
       <c r="Q150" s="9"/>
-    </row>
-    <row r="151" spans="1:17">
+      <c r="R150" s="9"/>
+    </row>
+    <row r="151" spans="1:18">
       <c r="A151" s="9"/>
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
@@ -14961,8 +14302,9 @@
       <c r="O151" s="9"/>
       <c r="P151" s="9"/>
       <c r="Q151" s="9"/>
-    </row>
-    <row r="152" spans="1:17">
+      <c r="R151" s="9"/>
+    </row>
+    <row r="152" spans="1:18">
       <c r="A152" s="9"/>
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
@@ -14980,8 +14322,9 @@
       <c r="O152" s="9"/>
       <c r="P152" s="9"/>
       <c r="Q152" s="9"/>
-    </row>
-    <row r="153" spans="1:17">
+      <c r="R152" s="9"/>
+    </row>
+    <row r="153" spans="1:18">
       <c r="A153" s="9"/>
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
@@ -14999,8 +14342,9 @@
       <c r="O153" s="9"/>
       <c r="P153" s="9"/>
       <c r="Q153" s="9"/>
-    </row>
-    <row r="154" spans="1:17">
+      <c r="R153" s="9"/>
+    </row>
+    <row r="154" spans="1:18">
       <c r="A154" s="9"/>
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
@@ -15018,8 +14362,9 @@
       <c r="O154" s="9"/>
       <c r="P154" s="9"/>
       <c r="Q154" s="9"/>
-    </row>
-    <row r="155" spans="1:17">
+      <c r="R154" s="9"/>
+    </row>
+    <row r="155" spans="1:18">
       <c r="A155" s="9"/>
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
@@ -15037,8 +14382,9 @@
       <c r="O155" s="9"/>
       <c r="P155" s="9"/>
       <c r="Q155" s="9"/>
-    </row>
-    <row r="156" spans="1:17">
+      <c r="R155" s="9"/>
+    </row>
+    <row r="156" spans="1:18">
       <c r="A156" s="9"/>
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
@@ -15056,8 +14402,9 @@
       <c r="O156" s="9"/>
       <c r="P156" s="9"/>
       <c r="Q156" s="9"/>
-    </row>
-    <row r="157" spans="1:17">
+      <c r="R156" s="9"/>
+    </row>
+    <row r="157" spans="1:18">
       <c r="A157" s="9"/>
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
@@ -15075,8 +14422,9 @@
       <c r="O157" s="9"/>
       <c r="P157" s="9"/>
       <c r="Q157" s="9"/>
-    </row>
-    <row r="158" spans="1:17">
+      <c r="R157" s="9"/>
+    </row>
+    <row r="158" spans="1:18">
       <c r="A158" s="9"/>
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
@@ -15094,8 +14442,9 @@
       <c r="O158" s="9"/>
       <c r="P158" s="9"/>
       <c r="Q158" s="9"/>
-    </row>
-    <row r="159" spans="1:17">
+      <c r="R158" s="9"/>
+    </row>
+    <row r="159" spans="1:18">
       <c r="A159" s="9"/>
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
@@ -15113,8 +14462,9 @@
       <c r="O159" s="9"/>
       <c r="P159" s="9"/>
       <c r="Q159" s="9"/>
-    </row>
-    <row r="160" spans="1:17">
+      <c r="R159" s="9"/>
+    </row>
+    <row r="160" spans="1:18">
       <c r="A160" s="9"/>
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
@@ -15132,8 +14482,9 @@
       <c r="O160" s="9"/>
       <c r="P160" s="9"/>
       <c r="Q160" s="9"/>
-    </row>
-    <row r="161" spans="1:17">
+      <c r="R160" s="9"/>
+    </row>
+    <row r="161" spans="1:18">
       <c r="A161" s="9"/>
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
@@ -15151,8 +14502,9 @@
       <c r="O161" s="9"/>
       <c r="P161" s="9"/>
       <c r="Q161" s="9"/>
-    </row>
-    <row r="162" spans="1:17">
+      <c r="R161" s="9"/>
+    </row>
+    <row r="162" spans="1:18">
       <c r="A162" s="9"/>
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
@@ -15170,8 +14522,9 @@
       <c r="O162" s="9"/>
       <c r="P162" s="9"/>
       <c r="Q162" s="9"/>
-    </row>
-    <row r="163" spans="1:17">
+      <c r="R162" s="9"/>
+    </row>
+    <row r="163" spans="1:18">
       <c r="A163" s="9"/>
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
@@ -15189,8 +14542,9 @@
       <c r="O163" s="9"/>
       <c r="P163" s="9"/>
       <c r="Q163" s="9"/>
-    </row>
-    <row r="164" spans="1:17">
+      <c r="R163" s="9"/>
+    </row>
+    <row r="164" spans="1:18">
       <c r="A164" s="9"/>
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
@@ -15208,8 +14562,9 @@
       <c r="O164" s="9"/>
       <c r="P164" s="9"/>
       <c r="Q164" s="9"/>
-    </row>
-    <row r="165" spans="1:17">
+      <c r="R164" s="9"/>
+    </row>
+    <row r="165" spans="1:18">
       <c r="A165" s="9"/>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
@@ -15227,8 +14582,9 @@
       <c r="O165" s="9"/>
       <c r="P165" s="9"/>
       <c r="Q165" s="9"/>
-    </row>
-    <row r="166" spans="1:17">
+      <c r="R165" s="9"/>
+    </row>
+    <row r="166" spans="1:18">
       <c r="A166" s="9"/>
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
@@ -15246,8 +14602,9 @@
       <c r="O166" s="9"/>
       <c r="P166" s="9"/>
       <c r="Q166" s="9"/>
-    </row>
-    <row r="167" spans="1:17">
+      <c r="R166" s="9"/>
+    </row>
+    <row r="167" spans="1:18">
       <c r="A167" s="9"/>
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
@@ -15265,8 +14622,9 @@
       <c r="O167" s="9"/>
       <c r="P167" s="9"/>
       <c r="Q167" s="9"/>
-    </row>
-    <row r="168" spans="1:17">
+      <c r="R167" s="9"/>
+    </row>
+    <row r="168" spans="1:18">
       <c r="A168" s="9"/>
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
@@ -15284,8 +14642,9 @@
       <c r="O168" s="9"/>
       <c r="P168" s="9"/>
       <c r="Q168" s="9"/>
-    </row>
-    <row r="169" spans="1:17">
+      <c r="R168" s="9"/>
+    </row>
+    <row r="169" spans="1:18">
       <c r="A169" s="9"/>
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
@@ -15303,8 +14662,9 @@
       <c r="O169" s="9"/>
       <c r="P169" s="9"/>
       <c r="Q169" s="9"/>
-    </row>
-    <row r="170" spans="1:17">
+      <c r="R169" s="9"/>
+    </row>
+    <row r="170" spans="1:18">
       <c r="A170" s="9"/>
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
@@ -15322,8 +14682,9 @@
       <c r="O170" s="9"/>
       <c r="P170" s="9"/>
       <c r="Q170" s="9"/>
-    </row>
-    <row r="171" spans="1:17">
+      <c r="R170" s="9"/>
+    </row>
+    <row r="171" spans="1:18">
       <c r="A171" s="9"/>
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
@@ -15341,8 +14702,9 @@
       <c r="O171" s="9"/>
       <c r="P171" s="9"/>
       <c r="Q171" s="9"/>
-    </row>
-    <row r="172" spans="1:17">
+      <c r="R171" s="9"/>
+    </row>
+    <row r="172" spans="1:18">
       <c r="A172" s="9"/>
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
@@ -15360,8 +14722,9 @@
       <c r="O172" s="9"/>
       <c r="P172" s="9"/>
       <c r="Q172" s="9"/>
-    </row>
-    <row r="173" spans="1:17">
+      <c r="R172" s="9"/>
+    </row>
+    <row r="173" spans="1:18">
       <c r="A173" s="9"/>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
@@ -15379,8 +14742,9 @@
       <c r="O173" s="9"/>
       <c r="P173" s="9"/>
       <c r="Q173" s="9"/>
-    </row>
-    <row r="174" spans="1:17">
+      <c r="R173" s="9"/>
+    </row>
+    <row r="174" spans="1:18">
       <c r="A174" s="9"/>
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
@@ -15398,8 +14762,9 @@
       <c r="O174" s="9"/>
       <c r="P174" s="9"/>
       <c r="Q174" s="9"/>
-    </row>
-    <row r="175" spans="1:17">
+      <c r="R174" s="9"/>
+    </row>
+    <row r="175" spans="1:18">
       <c r="A175" s="9"/>
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
@@ -15417,8 +14782,9 @@
       <c r="O175" s="9"/>
       <c r="P175" s="9"/>
       <c r="Q175" s="9"/>
-    </row>
-    <row r="176" spans="1:17">
+      <c r="R175" s="9"/>
+    </row>
+    <row r="176" spans="1:18">
       <c r="A176" s="9"/>
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
@@ -15436,8 +14802,9 @@
       <c r="O176" s="9"/>
       <c r="P176" s="9"/>
       <c r="Q176" s="9"/>
-    </row>
-    <row r="177" spans="1:17">
+      <c r="R176" s="9"/>
+    </row>
+    <row r="177" spans="1:18">
       <c r="A177" s="9"/>
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
@@ -15455,8 +14822,9 @@
       <c r="O177" s="9"/>
       <c r="P177" s="9"/>
       <c r="Q177" s="9"/>
-    </row>
-    <row r="178" spans="1:17">
+      <c r="R177" s="9"/>
+    </row>
+    <row r="178" spans="1:18">
       <c r="A178" s="9"/>
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
@@ -15474,8 +14842,9 @@
       <c r="O178" s="9"/>
       <c r="P178" s="9"/>
       <c r="Q178" s="9"/>
-    </row>
-    <row r="179" spans="1:17">
+      <c r="R178" s="9"/>
+    </row>
+    <row r="179" spans="1:18">
       <c r="A179" s="9"/>
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
@@ -15493,8 +14862,9 @@
       <c r="O179" s="9"/>
       <c r="P179" s="9"/>
       <c r="Q179" s="9"/>
-    </row>
-    <row r="180" spans="1:17">
+      <c r="R179" s="9"/>
+    </row>
+    <row r="180" spans="1:18">
       <c r="A180" s="9"/>
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
@@ -15512,8 +14882,9 @@
       <c r="O180" s="9"/>
       <c r="P180" s="9"/>
       <c r="Q180" s="9"/>
-    </row>
-    <row r="181" spans="1:17">
+      <c r="R180" s="9"/>
+    </row>
+    <row r="181" spans="1:18">
       <c r="A181" s="9"/>
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
@@ -15531,8 +14902,9 @@
       <c r="O181" s="9"/>
       <c r="P181" s="9"/>
       <c r="Q181" s="9"/>
-    </row>
-    <row r="182" spans="1:17">
+      <c r="R181" s="9"/>
+    </row>
+    <row r="182" spans="1:18">
       <c r="A182" s="9"/>
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
@@ -15550,8 +14922,9 @@
       <c r="O182" s="9"/>
       <c r="P182" s="9"/>
       <c r="Q182" s="9"/>
-    </row>
-    <row r="183" spans="1:17">
+      <c r="R182" s="9"/>
+    </row>
+    <row r="183" spans="1:18">
       <c r="A183" s="9"/>
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
@@ -15569,8 +14942,9 @@
       <c r="O183" s="9"/>
       <c r="P183" s="9"/>
       <c r="Q183" s="9"/>
-    </row>
-    <row r="184" spans="1:17">
+      <c r="R183" s="9"/>
+    </row>
+    <row r="184" spans="1:18">
       <c r="A184" s="9"/>
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
@@ -15588,8 +14962,9 @@
       <c r="O184" s="9"/>
       <c r="P184" s="9"/>
       <c r="Q184" s="9"/>
-    </row>
-    <row r="185" spans="1:17">
+      <c r="R184" s="9"/>
+    </row>
+    <row r="185" spans="1:18">
       <c r="A185" s="9"/>
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
@@ -15607,8 +14982,9 @@
       <c r="O185" s="9"/>
       <c r="P185" s="9"/>
       <c r="Q185" s="9"/>
-    </row>
-    <row r="186" spans="1:17">
+      <c r="R185" s="9"/>
+    </row>
+    <row r="186" spans="1:18">
       <c r="A186" s="9"/>
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
@@ -15626,8 +15002,9 @@
       <c r="O186" s="9"/>
       <c r="P186" s="9"/>
       <c r="Q186" s="9"/>
-    </row>
-    <row r="187" spans="1:17">
+      <c r="R186" s="9"/>
+    </row>
+    <row r="187" spans="1:18">
       <c r="A187" s="9"/>
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
@@ -15645,8 +15022,9 @@
       <c r="O187" s="9"/>
       <c r="P187" s="9"/>
       <c r="Q187" s="9"/>
-    </row>
-    <row r="188" spans="1:17">
+      <c r="R187" s="9"/>
+    </row>
+    <row r="188" spans="1:18">
       <c r="A188" s="9"/>
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
@@ -15664,8 +15042,9 @@
       <c r="O188" s="9"/>
       <c r="P188" s="9"/>
       <c r="Q188" s="9"/>
-    </row>
-    <row r="189" spans="1:17">
+      <c r="R188" s="9"/>
+    </row>
+    <row r="189" spans="1:18">
       <c r="A189" s="9"/>
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
@@ -15683,8 +15062,9 @@
       <c r="O189" s="9"/>
       <c r="P189" s="9"/>
       <c r="Q189" s="9"/>
-    </row>
-    <row r="190" spans="1:17">
+      <c r="R189" s="9"/>
+    </row>
+    <row r="190" spans="1:18">
       <c r="A190" s="9"/>
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
@@ -15702,8 +15082,9 @@
       <c r="O190" s="9"/>
       <c r="P190" s="9"/>
       <c r="Q190" s="9"/>
-    </row>
-    <row r="191" spans="1:17">
+      <c r="R190" s="9"/>
+    </row>
+    <row r="191" spans="1:18">
       <c r="A191" s="9"/>
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
@@ -15721,8 +15102,9 @@
       <c r="O191" s="9"/>
       <c r="P191" s="9"/>
       <c r="Q191" s="9"/>
-    </row>
-    <row r="192" spans="1:17">
+      <c r="R191" s="9"/>
+    </row>
+    <row r="192" spans="1:18">
       <c r="A192" s="9"/>
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
@@ -15740,8 +15122,9 @@
       <c r="O192" s="9"/>
       <c r="P192" s="9"/>
       <c r="Q192" s="9"/>
-    </row>
-    <row r="193" spans="1:17">
+      <c r="R192" s="9"/>
+    </row>
+    <row r="193" spans="1:18">
       <c r="A193" s="9"/>
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
@@ -15759,8 +15142,9 @@
       <c r="O193" s="9"/>
       <c r="P193" s="9"/>
       <c r="Q193" s="9"/>
-    </row>
-    <row r="194" spans="1:17">
+      <c r="R193" s="9"/>
+    </row>
+    <row r="194" spans="1:18">
       <c r="A194" s="9"/>
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
@@ -15778,8 +15162,9 @@
       <c r="O194" s="9"/>
       <c r="P194" s="9"/>
       <c r="Q194" s="9"/>
-    </row>
-    <row r="195" spans="1:17">
+      <c r="R194" s="9"/>
+    </row>
+    <row r="195" spans="1:18">
       <c r="A195" s="9"/>
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
@@ -15797,8 +15182,9 @@
       <c r="O195" s="9"/>
       <c r="P195" s="9"/>
       <c r="Q195" s="9"/>
-    </row>
-    <row r="196" spans="1:17">
+      <c r="R195" s="9"/>
+    </row>
+    <row r="196" spans="1:18">
       <c r="A196" s="9"/>
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
@@ -15816,8 +15202,9 @@
       <c r="O196" s="9"/>
       <c r="P196" s="9"/>
       <c r="Q196" s="9"/>
-    </row>
-    <row r="197" spans="1:17">
+      <c r="R196" s="9"/>
+    </row>
+    <row r="197" spans="1:18">
       <c r="A197" s="9"/>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
@@ -15835,8 +15222,9 @@
       <c r="O197" s="9"/>
       <c r="P197" s="9"/>
       <c r="Q197" s="9"/>
-    </row>
-    <row r="198" spans="1:17">
+      <c r="R197" s="9"/>
+    </row>
+    <row r="198" spans="1:18">
       <c r="A198" s="9"/>
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
@@ -15854,8 +15242,9 @@
       <c r="O198" s="9"/>
       <c r="P198" s="9"/>
       <c r="Q198" s="9"/>
-    </row>
-    <row r="199" spans="1:17">
+      <c r="R198" s="9"/>
+    </row>
+    <row r="199" spans="1:18">
       <c r="A199" s="9"/>
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
@@ -15873,8 +15262,9 @@
       <c r="O199" s="9"/>
       <c r="P199" s="9"/>
       <c r="Q199" s="9"/>
-    </row>
-    <row r="200" spans="1:17">
+      <c r="R199" s="9"/>
+    </row>
+    <row r="200" spans="1:18">
       <c r="A200" s="9"/>
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
@@ -15892,8 +15282,9 @@
       <c r="O200" s="9"/>
       <c r="P200" s="9"/>
       <c r="Q200" s="9"/>
-    </row>
-    <row r="201" spans="1:17">
+      <c r="R200" s="9"/>
+    </row>
+    <row r="201" spans="1:18">
       <c r="A201" s="9"/>
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
@@ -15911,8 +15302,9 @@
       <c r="O201" s="9"/>
       <c r="P201" s="9"/>
       <c r="Q201" s="9"/>
-    </row>
-    <row r="202" spans="1:17">
+      <c r="R201" s="9"/>
+    </row>
+    <row r="202" spans="1:18">
       <c r="A202" s="9"/>
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
@@ -15930,8 +15322,9 @@
       <c r="O202" s="9"/>
       <c r="P202" s="9"/>
       <c r="Q202" s="9"/>
-    </row>
-    <row r="203" spans="1:17">
+      <c r="R202" s="9"/>
+    </row>
+    <row r="203" spans="1:18">
       <c r="A203" s="9"/>
       <c r="B203" s="9"/>
       <c r="C203" s="9"/>
@@ -15949,8 +15342,9 @@
       <c r="O203" s="9"/>
       <c r="P203" s="9"/>
       <c r="Q203" s="9"/>
-    </row>
-    <row r="204" spans="1:17">
+      <c r="R203" s="9"/>
+    </row>
+    <row r="204" spans="1:18">
       <c r="A204" s="9"/>
       <c r="B204" s="9"/>
       <c r="C204" s="9"/>
@@ -15968,8 +15362,9 @@
       <c r="O204" s="9"/>
       <c r="P204" s="9"/>
       <c r="Q204" s="9"/>
-    </row>
-    <row r="205" spans="1:17">
+      <c r="R204" s="9"/>
+    </row>
+    <row r="205" spans="1:18">
       <c r="A205" s="9"/>
       <c r="B205" s="9"/>
       <c r="C205" s="9"/>
@@ -15987,8 +15382,9 @@
       <c r="O205" s="9"/>
       <c r="P205" s="9"/>
       <c r="Q205" s="9"/>
-    </row>
-    <row r="206" spans="1:17">
+      <c r="R205" s="9"/>
+    </row>
+    <row r="206" spans="1:18">
       <c r="A206" s="9"/>
       <c r="B206" s="9"/>
       <c r="C206" s="9"/>
@@ -16006,8 +15402,9 @@
       <c r="O206" s="9"/>
       <c r="P206" s="9"/>
       <c r="Q206" s="9"/>
-    </row>
-    <row r="207" spans="1:17">
+      <c r="R206" s="9"/>
+    </row>
+    <row r="207" spans="1:18">
       <c r="A207" s="9"/>
       <c r="B207" s="9"/>
       <c r="C207" s="9"/>
@@ -16025,8 +15422,9 @@
       <c r="O207" s="9"/>
       <c r="P207" s="9"/>
       <c r="Q207" s="9"/>
-    </row>
-    <row r="208" spans="1:17">
+      <c r="R207" s="9"/>
+    </row>
+    <row r="208" spans="1:18">
       <c r="A208" s="9"/>
       <c r="B208" s="9"/>
       <c r="C208" s="9"/>
@@ -16044,8 +15442,9 @@
       <c r="O208" s="9"/>
       <c r="P208" s="9"/>
       <c r="Q208" s="9"/>
-    </row>
-    <row r="209" spans="1:17">
+      <c r="R208" s="9"/>
+    </row>
+    <row r="209" spans="1:18">
       <c r="A209" s="9"/>
       <c r="B209" s="9"/>
       <c r="C209" s="9"/>
@@ -16063,8 +15462,9 @@
       <c r="O209" s="9"/>
       <c r="P209" s="9"/>
       <c r="Q209" s="9"/>
-    </row>
-    <row r="210" spans="1:17">
+      <c r="R209" s="9"/>
+    </row>
+    <row r="210" spans="1:18">
       <c r="A210" s="9"/>
       <c r="B210" s="9"/>
       <c r="C210" s="9"/>
@@ -16082,8 +15482,9 @@
       <c r="O210" s="9"/>
       <c r="P210" s="9"/>
       <c r="Q210" s="9"/>
-    </row>
-    <row r="211" spans="1:17">
+      <c r="R210" s="9"/>
+    </row>
+    <row r="211" spans="1:18">
       <c r="A211" s="9"/>
       <c r="B211" s="9"/>
       <c r="C211" s="9"/>
@@ -16101,8 +15502,9 @@
       <c r="O211" s="9"/>
       <c r="P211" s="9"/>
       <c r="Q211" s="9"/>
-    </row>
-    <row r="212" spans="1:17">
+      <c r="R211" s="9"/>
+    </row>
+    <row r="212" spans="1:18">
       <c r="A212" s="9"/>
       <c r="B212" s="9"/>
       <c r="C212" s="9"/>
@@ -16120,8 +15522,9 @@
       <c r="O212" s="9"/>
       <c r="P212" s="9"/>
       <c r="Q212" s="9"/>
-    </row>
-    <row r="213" spans="1:17">
+      <c r="R212" s="9"/>
+    </row>
+    <row r="213" spans="1:18">
       <c r="A213" s="9"/>
       <c r="B213" s="9"/>
       <c r="C213" s="9"/>
@@ -16139,8 +15542,9 @@
       <c r="O213" s="9"/>
       <c r="P213" s="9"/>
       <c r="Q213" s="9"/>
-    </row>
-    <row r="214" spans="1:17">
+      <c r="R213" s="9"/>
+    </row>
+    <row r="214" spans="1:18">
       <c r="A214" s="9"/>
       <c r="B214" s="9"/>
       <c r="C214" s="9"/>
@@ -16158,8 +15562,9 @@
       <c r="O214" s="9"/>
       <c r="P214" s="9"/>
       <c r="Q214" s="9"/>
-    </row>
-    <row r="215" spans="1:17">
+      <c r="R214" s="9"/>
+    </row>
+    <row r="215" spans="1:18">
       <c r="A215" s="9"/>
       <c r="B215" s="9"/>
       <c r="C215" s="9"/>
@@ -16177,8 +15582,9 @@
       <c r="O215" s="9"/>
       <c r="P215" s="9"/>
       <c r="Q215" s="9"/>
-    </row>
-    <row r="216" spans="1:17">
+      <c r="R215" s="9"/>
+    </row>
+    <row r="216" spans="1:18">
       <c r="A216" s="9"/>
       <c r="B216" s="9"/>
       <c r="C216" s="9"/>
@@ -16196,8 +15602,9 @@
       <c r="O216" s="9"/>
       <c r="P216" s="9"/>
       <c r="Q216" s="9"/>
-    </row>
-    <row r="217" spans="1:17">
+      <c r="R216" s="9"/>
+    </row>
+    <row r="217" spans="1:18">
       <c r="A217" s="9"/>
       <c r="B217" s="9"/>
       <c r="C217" s="9"/>
@@ -16215,8 +15622,9 @@
       <c r="O217" s="9"/>
       <c r="P217" s="9"/>
       <c r="Q217" s="9"/>
-    </row>
-    <row r="218" spans="1:17">
+      <c r="R217" s="9"/>
+    </row>
+    <row r="218" spans="1:18">
       <c r="A218" s="9"/>
       <c r="B218" s="9"/>
       <c r="C218" s="9"/>
@@ -16234,8 +15642,9 @@
       <c r="O218" s="9"/>
       <c r="P218" s="9"/>
       <c r="Q218" s="9"/>
-    </row>
-    <row r="219" spans="1:17">
+      <c r="R218" s="9"/>
+    </row>
+    <row r="219" spans="1:18">
       <c r="A219" s="9"/>
       <c r="B219" s="9"/>
       <c r="C219" s="9"/>
@@ -16253,8 +15662,9 @@
       <c r="O219" s="9"/>
       <c r="P219" s="9"/>
       <c r="Q219" s="9"/>
-    </row>
-    <row r="220" spans="1:17">
+      <c r="R219" s="9"/>
+    </row>
+    <row r="220" spans="1:18">
       <c r="A220" s="9"/>
       <c r="B220" s="9"/>
       <c r="C220" s="9"/>
@@ -16272,8 +15682,9 @@
       <c r="O220" s="9"/>
       <c r="P220" s="9"/>
       <c r="Q220" s="9"/>
-    </row>
-    <row r="221" spans="1:17">
+      <c r="R220" s="9"/>
+    </row>
+    <row r="221" spans="1:18">
       <c r="A221" s="9"/>
       <c r="B221" s="9"/>
       <c r="C221" s="9"/>
@@ -16291,8 +15702,9 @@
       <c r="O221" s="9"/>
       <c r="P221" s="9"/>
       <c r="Q221" s="9"/>
-    </row>
-    <row r="222" spans="1:17">
+      <c r="R221" s="9"/>
+    </row>
+    <row r="222" spans="1:18">
       <c r="A222" s="9"/>
       <c r="B222" s="9"/>
       <c r="C222" s="9"/>
@@ -16310,8 +15722,9 @@
       <c r="O222" s="9"/>
       <c r="P222" s="9"/>
       <c r="Q222" s="9"/>
-    </row>
-    <row r="223" spans="1:17">
+      <c r="R222" s="9"/>
+    </row>
+    <row r="223" spans="1:18">
       <c r="A223" s="9"/>
       <c r="B223" s="9"/>
       <c r="C223" s="9"/>
@@ -16329,8 +15742,9 @@
       <c r="O223" s="9"/>
       <c r="P223" s="9"/>
       <c r="Q223" s="9"/>
-    </row>
-    <row r="224" spans="1:17">
+      <c r="R223" s="9"/>
+    </row>
+    <row r="224" spans="1:18">
       <c r="A224" s="9"/>
       <c r="B224" s="9"/>
       <c r="C224" s="9"/>
@@ -16348,9 +15762,10 @@
       <c r="O224" s="9"/>
       <c r="P224" s="9"/>
       <c r="Q224" s="9"/>
+      <c r="R224" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:P39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:Q39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="duplicateValues" dxfId="23" priority="24"/>
   </conditionalFormatting>
@@ -16359,52 +15774,45 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A40:H40">
+  <conditionalFormatting sqref="A7:K7 A8:Q39 N7:Q7 A3:Q6">
+    <cfRule type="expression" dxfId="3" priority="29">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:K7 N7:R7 A8:R224 A3:R6">
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>ISODD(ROW())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:R40">
     <cfRule type="expression" dxfId="21" priority="4">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:P6 A7:J7 M7:P7 A8:P39">
-    <cfRule type="expression" dxfId="20" priority="29">
+  <conditionalFormatting sqref="B41:R224">
+    <cfRule type="expression" dxfId="20" priority="45">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:Q6 A7:J7 M7:Q7 A8:Q224">
-    <cfRule type="expression" dxfId="19" priority="8">
+  <conditionalFormatting sqref="C22:R22">
+    <cfRule type="expression" dxfId="19" priority="25">
+      <formula>ISEVEN(ROW())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="26">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:G22">
-    <cfRule type="expression" dxfId="18" priority="27">
-      <formula>ISEVEN(ROW())</formula>
+  <conditionalFormatting sqref="I2:CC1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>ISBLANK(I2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>I2="X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:Q22">
-    <cfRule type="expression" dxfId="17" priority="26">
-      <formula>ISODD(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22:Q22 H40:Q40 B41:Q224">
-    <cfRule type="expression" dxfId="16" priority="45">
+  <conditionalFormatting sqref="R3:R39">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I22:J22">
-    <cfRule type="expression" dxfId="15" priority="25">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q39">
-    <cfRule type="expression" dxfId="14" priority="7">
-      <formula>ISEVEN(ROW())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:CB1048576">
-    <cfRule type="expression" dxfId="13" priority="2">
-      <formula>I2="X"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="1">
-      <formula>ISBLANK(I2)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -21905,7 +21313,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="130" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -29118,42 +28526,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="142" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>OR($AD24="X",$AC24="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AND($AD24=1,$AC24=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="3">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>$AD24=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>$AC24=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="5">
+    <cfRule type="expression" dxfId="12" priority="5">
       <formula>AND(NOT(ISBLANK($V24)),ISBLANK($AC24),ISBLANK($AD24))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>AND($Q24="X",OR($B24&lt;&gt;"",$C24&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="136" priority="30">
+    <cfRule type="expression" dxfId="10" priority="30">
       <formula>OR($AD23="X",$AC23="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="31">
+    <cfRule type="expression" dxfId="9" priority="31">
       <formula>AND($AD23=1,$AC23=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="32">
+    <cfRule type="expression" dxfId="8" priority="32">
       <formula>$AD23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="33">
+    <cfRule type="expression" dxfId="7" priority="33">
       <formula>$AC23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="34">
+    <cfRule type="expression" dxfId="6" priority="34">
       <formula>AND(NOT(ISBLANK($V23)),ISBLANK($AC23),ISBLANK($AD23))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="35">
+    <cfRule type="expression" dxfId="5" priority="35">
       <formula>AND($Q23="X",OR(#REF!&lt;&gt;"",$B23&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36876,6 +36284,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -37289,7 +36706,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -37341,16 +36758,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27FF8B5-506F-46C5-AD7B-D0EA568E0AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37370,28 +36786,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[25.01.09 11:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="461" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E93BA5E5-8124-4821-9E09-DC2B3995B271}"/>
+  <xr:revisionPtr revIDLastSave="463" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7F91A53-AE62-4A9D-AADE-18F18D1157B3}"/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="360" windowWidth="24030" windowHeight="12285" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="33120" yWindow="3135" windowWidth="21600" windowHeight="11295" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -9560,32 +9560,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79989013336588644"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -9682,6 +9656,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -9704,6 +9692,18 @@
           <bgColor theme="4" tint="0.79989013336588644"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -10354,11 +10354,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R224"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -15774,44 +15774,44 @@
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:K7 A8:Q39 N7:Q7 A3:Q6">
-    <cfRule type="expression" dxfId="3" priority="29">
+  <conditionalFormatting sqref="A3:Q6 A7:K7 A8:Q39 N7:Q7">
+    <cfRule type="expression" dxfId="21" priority="29">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:K7 N7:R7 A8:R224 A3:R6">
-    <cfRule type="expression" dxfId="2" priority="8">
+  <conditionalFormatting sqref="A3:R6 A7:K7 N7:R7 A8:R224">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:R40">
-    <cfRule type="expression" dxfId="21" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:R224">
-    <cfRule type="expression" dxfId="20" priority="45">
+    <cfRule type="expression" dxfId="18" priority="45">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:R22">
-    <cfRule type="expression" dxfId="19" priority="25">
+    <cfRule type="expression" dxfId="17" priority="25">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="26">
+    <cfRule type="expression" dxfId="16" priority="26">
       <formula>ISODD(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:CC1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>ISBLANK(I2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>I2="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R39">
-    <cfRule type="expression" dxfId="17" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19439,7 +19439,7 @@
       </c>
       <c r="D33" s="47"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="25.5">
       <c r="A34" s="47" t="s">
         <v>1781</v>
       </c>
@@ -21313,7 +21313,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -28526,42 +28526,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B24">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>OR($AD24="X",$AC24="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>AND($AD24=1,$AC24=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>$AD24=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>$AC24=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>AND(NOT(ISBLANK($V24)),ISBLANK($AC24),ISBLANK($AD24))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>AND($Q24="X",OR($B24&lt;&gt;"",$C24&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O23">
-    <cfRule type="expression" dxfId="10" priority="30">
+    <cfRule type="expression" dxfId="6" priority="30">
       <formula>OR($AD23="X",$AC23="X")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="31">
+    <cfRule type="expression" dxfId="5" priority="31">
       <formula>AND($AD23=1,$AC23=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="32">
+    <cfRule type="expression" dxfId="4" priority="32">
       <formula>$AD23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="33">
+    <cfRule type="expression" dxfId="3" priority="33">
       <formula>$AC23=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="34">
+    <cfRule type="expression" dxfId="2" priority="34">
       <formula>AND(NOT(ISBLANK($V23)),ISBLANK($AC23),ISBLANK($AD23))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="35">
+    <cfRule type="expression" dxfId="1" priority="35">
       <formula>AND($Q23="X",OR(#REF!&lt;&gt;"",$B23&lt;&gt;""))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35415,12 +35415,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="44.28515625" customWidth="1"/>
     <col min="5" max="5" width="42.140625" customWidth="1"/>
@@ -36284,6 +36286,58 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -36292,7 +36346,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -36706,59 +36760,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -36766,7 +36786,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27FF8B5-506F-46C5-AD7B-D0EA568E0AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36784,22 +36804,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[25.01.13 17:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="463" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7F91A53-AE62-4A9D-AADE-18F18D1157B3}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88AE1070-121B-44F9-BB0D-D192835F3267}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="33120" yWindow="3135" windowWidth="21600" windowHeight="11295" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="990" yWindow="2115" windowWidth="25605" windowHeight="11940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="2903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3811" uniqueCount="2903">
   <si>
     <t>ID unique</t>
   </si>
@@ -10354,11 +10354,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R224"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="H28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -11652,9 +11652,7 @@
         <v>20</v>
       </c>
       <c r="M30" s="10"/>
-      <c r="N30" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="10" t="s">
         <v>20</v>
@@ -19439,7 +19437,7 @@
       </c>
       <c r="D33" s="47"/>
     </row>
-    <row r="34" spans="1:4" ht="25.5">
+    <row r="34" spans="1:4">
       <c r="A34" s="47" t="s">
         <v>1781</v>
       </c>
@@ -35415,7 +35413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -36286,67 +36284,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -36760,33 +36697,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27FF8B5-506F-46C5-AD7B-D0EA568E0AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36804,4 +36776,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[25.01.14 11:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="464" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88AE1070-121B-44F9-BB0D-D192835F3267}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="990" yWindow="2115" windowWidth="25605" windowHeight="11940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -9807,6 +9807,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13611123111813" displayName="Table13611123111813" ref="A6:E52" totalsRowShown="0">
   <autoFilter ref="A6:E52" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
@@ -10354,11 +10358,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R224"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="H28" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -19437,7 +19441,7 @@
       </c>
       <c r="D33" s="47"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" ht="25.5">
       <c r="A34" s="47" t="s">
         <v>1781</v>
       </c>
@@ -35413,8 +35417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -36284,6 +36288,67 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -36697,68 +36762,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27FF8B5-506F-46C5-AD7B-D0EA568E0AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36776,30 +36806,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[25.01.20 13:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="464" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88AE1070-121B-44F9-BB0D-D192835F3267}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="656" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -9807,10 +9807,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13611123111813" displayName="Table13611123111813" ref="A6:E52" totalsRowShown="0">
   <autoFilter ref="A6:E52" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
@@ -29072,8 +29068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F314"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -32907,7 +32903,7 @@
   <dimension ref="A1:H185"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -34977,8 +34973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35417,8 +35413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -36288,67 +36284,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -36762,33 +36697,68 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27FF8B5-506F-46C5-AD7B-D0EA568E0AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36806,4 +36776,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[25.01.27 15:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="464" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88AE1070-121B-44F9-BB0D-D192835F3267}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="656" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="656" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -16084,7 +16084,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -29068,8 +29068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F314"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -34973,8 +34973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -36284,6 +36284,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="52" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="a24e46c8e369b0d0dbf292fc067594e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b005a03a4b86eaa0f9218a8d7ff13ee" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -36697,7 +36706,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
@@ -36749,16 +36758,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C27FF8B5-506F-46C5-AD7B-D0EA568E0AF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -36778,28 +36786,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A00B4654-0C09-4F85-99FD-FA4928CBD3A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E158D6-857B-4A1D-8488-366612583065}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[25.01.28 11:42] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
+++ b/nomenclature_parser/in/Nomenclatures RC-EDA et messages RS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="464" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88AE1070-121B-44F9-BB0D-D192835F3267}"/>
+  <xr:revisionPtr revIDLastSave="474" documentId="11_3C80A0E040A7A70446C1793E9590B8BC49BCD1F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17DE9581-1348-4B8C-A850-C46B1E9A2DEB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="656" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="525" yWindow="315" windowWidth="21690" windowHeight="15150" tabRatio="656" firstSheet="18" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#Sommaire" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3811" uniqueCount="2903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3811" uniqueCount="2902">
   <si>
     <t>ID unique</t>
   </si>
@@ -7320,12 +7320,6 @@
     <t>Numéro d'identification SINUS</t>
   </si>
   <si>
-    <t>SI-VIC</t>
-  </si>
-  <si>
-    <t>Numéro d'identification SI-VIC</t>
-  </si>
-  <si>
     <t>DOSSARD</t>
   </si>
   <si>
@@ -8933,6 +8927,9 @@
   </si>
   <si>
     <t>RS-EDA-MAJ</t>
+  </si>
+  <si>
+    <t>Autre identifiant</t>
   </si>
 </sst>
 </file>
@@ -9365,7 +9362,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -9549,6 +9546,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in 60% - Accent5" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -9977,8 +9975,8 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table1361112311182122" displayName="Table1361112311182122" ref="A6:E52" totalsRowShown="0">
-  <autoFilter ref="A6:E52" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table1361112311182122" displayName="Table1361112311182122" ref="A6:E51" totalsRowShown="0">
+  <autoFilter ref="A6:E51" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="Code"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="Libellé niveau 1"/>
@@ -10355,10 +10353,10 @@
   <dimension ref="A1:R224"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
@@ -10414,7 +10412,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>2902</v>
+        <v>2900</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>10</v>
@@ -10435,7 +10433,7 @@
         <v>15</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15">
@@ -12045,11 +12043,11 @@
     </row>
     <row r="40" spans="1:18" ht="15">
       <c r="A40" s="79" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="14" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
       <c r="D40" s="9" t="str">
         <f>'Etape message'!B5</f>
@@ -12067,7 +12065,7 @@
         <v>18</v>
       </c>
       <c r="H40" s="9" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
@@ -21753,7 +21751,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -22046,10 +22044,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -22130,7 +22128,7 @@
         <v>2361</v>
       </c>
       <c r="C7" s="23"/>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="83" t="s">
         <v>2362</v>
       </c>
       <c r="E7"/>
@@ -22143,7 +22141,7 @@
         <v>2363</v>
       </c>
       <c r="C8" s="23"/>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="83" t="s">
         <v>2364</v>
       </c>
       <c r="E8"/>
@@ -22156,7 +22154,7 @@
         <v>2365</v>
       </c>
       <c r="C9" s="23"/>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="83" t="s">
         <v>2366</v>
       </c>
       <c r="E9"/>
@@ -22169,21 +22167,21 @@
         <v>2367</v>
       </c>
       <c r="C10" s="23"/>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="83" t="s">
         <v>2368</v>
       </c>
       <c r="E10"/>
     </row>
     <row r="11" spans="1:5" s="25" customFormat="1">
       <c r="A11" t="s">
-        <v>2369</v>
+        <v>199</v>
       </c>
       <c r="B11" t="s">
-        <v>2369</v>
+        <v>199</v>
       </c>
       <c r="C11" s="23"/>
-      <c r="D11" s="24" t="s">
-        <v>2370</v>
+      <c r="D11" s="83" t="s">
+        <v>2901</v>
       </c>
       <c r="E11"/>
     </row>
@@ -22215,50 +22213,12 @@
       <c r="D15"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:5" s="25" customFormat="1">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="23"/>
-      <c r="D16"/>
-      <c r="E16"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-    </row>
-    <row r="19" spans="1:5" s="30" customFormat="1">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="B20" s="31"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" s="32"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" s="31"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" s="32"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" s="33"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" s="33"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" s="33"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" s="33"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" s="34"/>
+    <row r="18" spans="1:5" s="30" customFormat="1">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -22301,7 +22261,7 @@
         <v>108</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>2371</v>
+        <v>2369</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -22311,7 +22271,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2372</v>
+        <v>2370</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -22331,7 +22291,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2373</v>
+        <v>2371</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -22358,46 +22318,46 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
+        <v>2372</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2373</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>2374</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2375</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2376</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
+        <v>2375</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2376</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>2377</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>2378</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>2379</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
+        <v>2378</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2379</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>2380</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>2381</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>2382</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
+        <v>2381</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2382</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>2383</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>2384</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>2385</v>
       </c>
     </row>
   </sheetData>
@@ -22449,7 +22409,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2386</v>
+        <v>2384</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -22469,7 +22429,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2387</v>
+        <v>2385</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -22496,57 +22456,57 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="42" t="s">
-        <v>2388</v>
+        <v>2386</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>2389</v>
+        <v>2387</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="2" t="s">
-        <v>2390</v>
+        <v>2388</v>
       </c>
       <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="42" t="s">
-        <v>2391</v>
+        <v>2389</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>2392</v>
+        <v>2390</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
       <c r="E8" s="2" t="s">
-        <v>2393</v>
+        <v>2391</v>
       </c>
       <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="42" t="s">
-        <v>2394</v>
+        <v>2392</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>2395</v>
+        <v>2393</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
       <c r="E9" s="2" t="s">
-        <v>2396</v>
+        <v>2394</v>
       </c>
       <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="42" t="s">
-        <v>2397</v>
+        <v>2395</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>2398</v>
+        <v>2396</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
       <c r="E10" s="2" t="s">
-        <v>2399</v>
+        <v>2397</v>
       </c>
       <c r="F10" s="42"/>
     </row>
@@ -22851,7 +22811,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2400</v>
+        <v>2398</v>
       </c>
       <c r="C3" s="19"/>
     </row>
@@ -22869,7 +22829,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2401</v>
+        <v>2399</v>
       </c>
       <c r="C5" s="20"/>
     </row>
@@ -22892,79 +22852,79 @@
     </row>
     <row r="7" spans="1:5" s="25" customFormat="1">
       <c r="A7" s="51" t="s">
-        <v>2402</v>
+        <v>2400</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>2403</v>
+        <v>2401</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" t="s">
-        <v>2404</v>
+        <v>2402</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8" spans="1:5" s="25" customFormat="1">
       <c r="A8" s="35" t="s">
-        <v>2405</v>
+        <v>2403</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>2405</v>
+        <v>2403</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" t="s">
-        <v>2406</v>
+        <v>2404</v>
       </c>
       <c r="E8"/>
     </row>
     <row r="9" spans="1:5" s="25" customFormat="1">
       <c r="A9" s="35" t="s">
-        <v>2407</v>
+        <v>2405</v>
       </c>
       <c r="B9" s="35" t="s">
         <v>2291</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" t="s">
-        <v>2408</v>
+        <v>2406</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10" spans="1:5" s="25" customFormat="1">
       <c r="A10" s="35" t="s">
-        <v>2409</v>
+        <v>2407</v>
       </c>
       <c r="B10" s="35" t="s">
         <v>2276</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" t="s">
-        <v>2410</v>
+        <v>2408</v>
       </c>
       <c r="E10"/>
     </row>
     <row r="11" spans="1:5" s="25" customFormat="1">
       <c r="A11" t="s">
-        <v>2411</v>
+        <v>2409</v>
       </c>
       <c r="B11" t="s">
-        <v>2412</v>
+        <v>2410</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>2413</v>
+        <v>2411</v>
       </c>
       <c r="E11"/>
     </row>
     <row r="12" spans="1:5" s="25" customFormat="1">
       <c r="A12" t="s">
-        <v>2414</v>
+        <v>2412</v>
       </c>
       <c r="B12" t="s">
-        <v>2415</v>
+        <v>2413</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" t="s">
-        <v>2416</v>
+        <v>2414</v>
       </c>
       <c r="E12"/>
     </row>
@@ -22973,11 +22933,11 @@
         <v>199</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>2417</v>
+        <v>2415</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" t="s">
-        <v>2418</v>
+        <v>2416</v>
       </c>
       <c r="E13"/>
     </row>
@@ -22986,11 +22946,11 @@
         <v>1503</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>2384</v>
+        <v>2382</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" t="s">
-        <v>2419</v>
+        <v>2417</v>
       </c>
       <c r="E14"/>
     </row>
@@ -23093,7 +23053,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2420</v>
+        <v>2418</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -23113,7 +23073,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2421</v>
+        <v>2419</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -23140,81 +23100,81 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="42" t="s">
+        <v>2420</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>2421</v>
+      </c>
+      <c r="C7" s="42" t="s">
         <v>2422</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>2423</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>2424</v>
       </c>
       <c r="D7" s="42"/>
       <c r="E7" s="42" t="s">
-        <v>2425</v>
+        <v>2423</v>
       </c>
       <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="42" t="s">
+        <v>2424</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>2425</v>
+      </c>
+      <c r="C8" s="42" t="s">
         <v>2426</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>2427</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>2428</v>
       </c>
       <c r="D8" s="42"/>
       <c r="E8" s="42" t="s">
-        <v>2429</v>
+        <v>2427</v>
       </c>
       <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="42" t="s">
+        <v>2428</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C9" s="42" t="s">
         <v>2430</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>2431</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>2432</v>
       </c>
       <c r="D9" s="42"/>
       <c r="E9" s="42" t="s">
-        <v>2433</v>
+        <v>2431</v>
       </c>
       <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="42" t="s">
+        <v>2432</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>2433</v>
+      </c>
+      <c r="C10" s="42" t="s">
         <v>2434</v>
-      </c>
-      <c r="B10" s="42" t="s">
-        <v>2435</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>2436</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42" t="s">
-        <v>2437</v>
+        <v>2435</v>
       </c>
       <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="42" t="s">
+        <v>2436</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>2437</v>
+      </c>
+      <c r="C11" s="42" t="s">
         <v>2438</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>2439</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>2440</v>
       </c>
       <c r="D11" s="42"/>
       <c r="E11" s="42" t="s">
-        <v>2441</v>
+        <v>2439</v>
       </c>
       <c r="F11" s="42"/>
     </row>
@@ -23515,10 +23475,10 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2442</v>
+        <v>2440</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>2443</v>
+        <v>2441</v>
       </c>
       <c r="D3" s="19"/>
     </row>
@@ -23537,7 +23497,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2444</v>
+        <v>2442</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -23565,108 +23525,108 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>2445</v>
+        <v>2443</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>2446</v>
+        <v>2444</v>
       </c>
       <c r="D7" s="42"/>
       <c r="E7" s="25" t="s">
-        <v>2447</v>
+        <v>2445</v>
       </c>
       <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>2448</v>
+        <v>2446</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="25" t="s">
-        <v>2449</v>
+        <v>2447</v>
       </c>
       <c r="D8" s="42"/>
       <c r="E8" s="25"/>
       <c r="F8" s="42" t="s">
-        <v>2450</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>2451</v>
+        <v>2449</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25" t="s">
-        <v>2452</v>
+        <v>2450</v>
       </c>
       <c r="D9" s="42"/>
       <c r="E9" s="25"/>
       <c r="F9" s="42" t="s">
-        <v>2453</v>
+        <v>2451</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>2454</v>
+        <v>2452</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" t="s">
-        <v>2455</v>
+        <v>2453</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="25" t="s">
-        <v>2456</v>
+        <v>2454</v>
       </c>
       <c r="F10" s="42" t="s">
-        <v>2457</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>2458</v>
+        <v>2456</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" t="s">
-        <v>2459</v>
+        <v>2457</v>
       </c>
       <c r="D11" s="42"/>
       <c r="E11" s="25"/>
       <c r="F11" s="42" t="s">
-        <v>2460</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="25" t="s">
+        <v>2459</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>2460</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>2461</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>2462</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>2463</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="25" t="s">
+        <v>2462</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>2463</v>
+      </c>
+      <c r="E13" s="25" t="s">
         <v>2464</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>2465</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>2466</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>2467</v>
+        <v>2465</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>2468</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>2469</v>
+        <v>2467</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>2303</v>
@@ -23674,7 +23634,7 @@
     </row>
     <row r="16" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>2470</v>
+        <v>2468</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>2291</v>
@@ -23682,19 +23642,19 @@
     </row>
     <row r="17" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>2471</v>
+        <v>2469</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>2472</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>2473</v>
+        <v>2471</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
       <c r="D18" s="42"/>
       <c r="E18" s="25"/>
@@ -23702,39 +23662,39 @@
     </row>
     <row r="19" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="25" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="25" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="25" t="s">
-        <v>2481</v>
+        <v>2479</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>2482</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="25" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>2306</v>
@@ -23742,11 +23702,11 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="25" t="s">
-        <v>2484</v>
+        <v>2482</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
       <c r="D24" s="42"/>
       <c r="E24" s="25"/>
@@ -23754,49 +23714,49 @@
     </row>
     <row r="25" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A25" s="25" t="s">
-        <v>2486</v>
+        <v>2484</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>2487</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A26" s="25" t="s">
+        <v>2486</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>2487</v>
+      </c>
+      <c r="E26" s="25" t="s">
         <v>2488</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>2489</v>
-      </c>
-      <c r="E26" s="25" t="s">
-        <v>2490</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="25" t="s">
+        <v>2489</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>2490</v>
+      </c>
+      <c r="E27" s="25" t="s">
         <v>2491</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>2492</v>
-      </c>
-      <c r="E27" s="25" t="s">
-        <v>2493</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="25" customFormat="1" ht="15.75" customHeight="1">
       <c r="A28" s="25" t="s">
-        <v>2494</v>
+        <v>2492</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>2495</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="25" t="s">
-        <v>2496</v>
+        <v>2494</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" t="s">
-        <v>2497</v>
+        <v>2495</v>
       </c>
       <c r="D29" s="42"/>
       <c r="E29" s="25"/>
@@ -23804,11 +23764,11 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="25" t="s">
-        <v>2498</v>
+        <v>2496</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="25" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
       <c r="D30" s="25"/>
       <c r="E30" s="25"/>
@@ -23816,15 +23776,15 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="25" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>2501</v>
+        <v>2499</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="25"/>
       <c r="E31" s="25" t="s">
-        <v>2502</v>
+        <v>2500</v>
       </c>
       <c r="F31" s="42"/>
     </row>
@@ -23833,22 +23793,22 @@
         <v>179</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>2503</v>
+        <v>2501</v>
       </c>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25" t="s">
-        <v>2504</v>
+        <v>2502</v>
       </c>
       <c r="F32" s="42"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="42" t="s">
-        <v>2505</v>
+        <v>2503</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="42" t="s">
-        <v>2506</v>
+        <v>2504</v>
       </c>
       <c r="D33" s="42"/>
       <c r="E33" s="42"/>
@@ -23856,11 +23816,11 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34" s="42" t="s">
-        <v>2507</v>
+        <v>2505</v>
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="42" t="s">
-        <v>2508</v>
+        <v>2506</v>
       </c>
       <c r="D34" s="42"/>
       <c r="E34" s="42"/>
@@ -23868,11 +23828,11 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="42" t="s">
-        <v>2509</v>
+        <v>2507</v>
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="42" t="s">
-        <v>2510</v>
+        <v>2508</v>
       </c>
       <c r="D35" s="42"/>
       <c r="E35" s="42"/>
@@ -23880,11 +23840,11 @@
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="42" t="s">
-        <v>2511</v>
+        <v>2509</v>
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="42" t="s">
-        <v>2512</v>
+        <v>2510</v>
       </c>
       <c r="D36" s="42"/>
       <c r="E36" s="42"/>
@@ -23895,22 +23855,22 @@
         <v>199</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>2513</v>
+        <v>2511</v>
       </c>
       <c r="C37" s="42"/>
       <c r="D37" s="42"/>
       <c r="E37" s="42" t="s">
-        <v>2514</v>
+        <v>2512</v>
       </c>
       <c r="F37" s="42"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38" s="42" t="s">
-        <v>2515</v>
+        <v>2513</v>
       </c>
       <c r="B38" s="42"/>
       <c r="C38" s="42" t="s">
-        <v>2516</v>
+        <v>2514</v>
       </c>
       <c r="D38" s="42"/>
       <c r="E38" s="42"/>
@@ -23918,11 +23878,11 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="42" t="s">
-        <v>2517</v>
+        <v>2515</v>
       </c>
       <c r="B39" s="42"/>
       <c r="C39" s="42" t="s">
-        <v>2518</v>
+        <v>2516</v>
       </c>
       <c r="D39" s="42"/>
       <c r="E39" s="42"/>
@@ -23930,11 +23890,11 @@
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40" s="42" t="s">
-        <v>2519</v>
+        <v>2517</v>
       </c>
       <c r="B40" s="42"/>
       <c r="C40" s="42" t="s">
-        <v>2520</v>
+        <v>2518</v>
       </c>
       <c r="D40" s="42"/>
       <c r="E40" s="42"/>
@@ -24547,7 +24507,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2521</v>
+        <v>2519</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -24567,7 +24527,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2522</v>
+        <v>2520</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -24594,48 +24554,48 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="25" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="25" t="s">
+        <v>2521</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>2522</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>2523</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>2524</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>2525</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="25" t="s">
+        <v>2524</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>2525</v>
+      </c>
+      <c r="E9" s="25" t="s">
         <v>2526</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>2527</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>2528</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="25" t="s">
-        <v>2529</v>
+        <v>2527</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>2530</v>
+        <v>2528</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="25" t="s">
-        <v>2531</v>
+        <v>2529</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>199</v>
@@ -24643,640 +24603,640 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="25" t="s">
-        <v>2532</v>
+        <v>2530</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>2533</v>
+        <v>2531</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="25" t="s">
-        <v>2534</v>
+        <v>2532</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>2535</v>
+        <v>2533</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="25" t="s">
-        <v>2536</v>
+        <v>2534</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>2537</v>
+        <v>2535</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="25" t="s">
-        <v>2538</v>
+        <v>2536</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>2539</v>
+        <v>2537</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="25" t="s">
-        <v>2540</v>
+        <v>2538</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>2541</v>
+        <v>2539</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="25" t="s">
-        <v>2542</v>
+        <v>2540</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>2543</v>
+        <v>2541</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="25" t="s">
+        <v>2542</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>2543</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>2544</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>2545</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>2546</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="25" t="s">
-        <v>2547</v>
+        <v>2545</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>2548</v>
+        <v>2546</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="25" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>2549</v>
+        <v>2547</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="25" t="s">
-        <v>2550</v>
+        <v>2548</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>2551</v>
+        <v>2549</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="25" t="s">
-        <v>2552</v>
+        <v>2550</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>2553</v>
+        <v>2551</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="25" t="s">
-        <v>2554</v>
+        <v>2552</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>2555</v>
+        <v>2553</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="25" t="s">
-        <v>2556</v>
+        <v>2554</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>2557</v>
+        <v>2555</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="25" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>2558</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="25" t="s">
-        <v>2559</v>
+        <v>2557</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>2276</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="25" t="s">
-        <v>2560</v>
+        <v>2558</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>2291</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="25" t="s">
-        <v>2561</v>
+        <v>2559</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>2487</v>
+        <v>2485</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="25" t="s">
-        <v>2491</v>
+        <v>2489</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>2491</v>
+        <v>2489</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="25" t="s">
-        <v>2562</v>
+        <v>2560</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>2563</v>
+        <v>2561</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="25" t="s">
-        <v>2564</v>
+        <v>2562</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="25" t="s">
-        <v>2566</v>
+        <v>2564</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>2567</v>
+        <v>2565</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="25" t="s">
-        <v>2568</v>
+        <v>2566</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>2569</v>
+        <v>2567</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="25" t="s">
-        <v>2570</v>
+        <v>2568</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>2571</v>
+        <v>2569</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="25" t="s">
-        <v>2572</v>
+        <v>2570</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>2573</v>
+        <v>2571</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="25" t="s">
-        <v>2574</v>
+        <v>2572</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>2575</v>
+        <v>2573</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="25" t="s">
-        <v>2576</v>
+        <v>2574</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>2577</v>
+        <v>2575</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="25" t="s">
-        <v>2578</v>
+        <v>2576</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>2579</v>
+        <v>2577</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="25" t="s">
-        <v>2580</v>
+        <v>2578</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>2581</v>
+        <v>2579</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="25" t="s">
-        <v>2582</v>
+        <v>2580</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>2583</v>
+        <v>2581</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="25" t="s">
-        <v>2584</v>
+        <v>2582</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>2585</v>
+        <v>2583</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="25" t="s">
-        <v>2586</v>
+        <v>2584</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>2587</v>
+        <v>2585</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="25" t="s">
-        <v>2588</v>
+        <v>2586</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>2589</v>
+        <v>2587</v>
       </c>
       <c r="E43" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="25" t="s">
-        <v>2590</v>
+        <v>2588</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>2591</v>
+        <v>2589</v>
       </c>
       <c r="E44" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="25" t="s">
-        <v>2592</v>
+        <v>2590</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>2593</v>
+        <v>2591</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="25" t="s">
-        <v>2594</v>
+        <v>2592</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>2595</v>
+        <v>2593</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="25" t="s">
-        <v>2596</v>
+        <v>2594</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>2597</v>
+        <v>2595</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>2525</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="25" t="s">
-        <v>2445</v>
+        <v>2443</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>2445</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75">
       <c r="A49" s="25" t="s">
-        <v>2598</v>
+        <v>2596</v>
       </c>
       <c r="B49" s="54"/>
       <c r="C49" s="25" t="s">
-        <v>2599</v>
+        <v>2597</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75">
       <c r="A50" s="25" t="s">
-        <v>2600</v>
+        <v>2598</v>
       </c>
       <c r="B50" s="54"/>
       <c r="C50" s="25" t="s">
-        <v>2601</v>
+        <v>2599</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75">
       <c r="A51" s="25" t="s">
-        <v>2602</v>
+        <v>2600</v>
       </c>
       <c r="B51" s="54"/>
       <c r="C51" s="25" t="s">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75">
       <c r="A52" s="25" t="s">
-        <v>2604</v>
+        <v>2602</v>
       </c>
       <c r="B52" s="54"/>
       <c r="C52" s="25" t="s">
-        <v>2605</v>
+        <v>2603</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75">
       <c r="A53" s="25" t="s">
-        <v>2606</v>
+        <v>2604</v>
       </c>
       <c r="B53" s="54"/>
       <c r="C53" s="25" t="s">
-        <v>2607</v>
+        <v>2605</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75">
       <c r="A54" s="25" t="s">
-        <v>2608</v>
+        <v>2606</v>
       </c>
       <c r="B54" s="54"/>
       <c r="C54" s="25" t="s">
-        <v>2609</v>
+        <v>2607</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75">
       <c r="A55" s="25" t="s">
-        <v>2610</v>
+        <v>2608</v>
       </c>
       <c r="B55" s="54"/>
       <c r="C55" s="25" t="s">
-        <v>2611</v>
+        <v>2609</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>2546</v>
+        <v>2544</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75">
       <c r="A56" s="25" t="s">
-        <v>2612</v>
+        <v>2610</v>
       </c>
       <c r="B56" s="54"/>
       <c r="C56" s="25" t="s">
-        <v>2613</v>
+        <v>2611</v>
       </c>
       <c r="E56" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75">
       <c r="A57" s="25" t="s">
-        <v>2614</v>
+        <v>2612</v>
       </c>
       <c r="B57" s="54"/>
       <c r="C57" s="25" t="s">
-        <v>2615</v>
+        <v>2613</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15.75">
       <c r="A58" s="25" t="s">
-        <v>2616</v>
+        <v>2614</v>
       </c>
       <c r="B58" s="54"/>
       <c r="C58" s="25" t="s">
-        <v>2617</v>
+        <v>2615</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75">
       <c r="A59" s="25" t="s">
-        <v>2618</v>
+        <v>2616</v>
       </c>
       <c r="B59" s="54"/>
       <c r="C59" s="25" t="s">
-        <v>2619</v>
+        <v>2617</v>
       </c>
       <c r="E59" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75">
       <c r="A60" s="25" t="s">
-        <v>2620</v>
+        <v>2618</v>
       </c>
       <c r="B60" s="54"/>
       <c r="C60" s="25" t="s">
-        <v>2621</v>
+        <v>2619</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75">
       <c r="A61" s="25" t="s">
-        <v>2622</v>
+        <v>2620</v>
       </c>
       <c r="B61" s="54"/>
       <c r="C61" s="25" t="s">
-        <v>2623</v>
+        <v>2621</v>
       </c>
       <c r="E61" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15.75">
       <c r="A62" s="25" t="s">
-        <v>2624</v>
+        <v>2622</v>
       </c>
       <c r="B62" s="54"/>
       <c r="C62" s="25" t="s">
-        <v>2625</v>
+        <v>2623</v>
       </c>
       <c r="E62" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75">
       <c r="A63" s="25" t="s">
-        <v>2626</v>
+        <v>2624</v>
       </c>
       <c r="B63" s="54"/>
       <c r="C63" s="25" t="s">
-        <v>2627</v>
+        <v>2625</v>
       </c>
       <c r="E63" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="25" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>2628</v>
+        <v>2626</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="25" t="s">
-        <v>2629</v>
+        <v>2627</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>2630</v>
+        <v>2628</v>
       </c>
       <c r="E65" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="25" t="s">
-        <v>2631</v>
+        <v>2629</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>2632</v>
+        <v>2630</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="25" t="s">
-        <v>2633</v>
+        <v>2631</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>2634</v>
+        <v>2632</v>
       </c>
       <c r="E67" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="25" t="s">
-        <v>2635</v>
+        <v>2633</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>2636</v>
+        <v>2634</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="25" t="s">
-        <v>2637</v>
+        <v>2635</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>2638</v>
+        <v>2636</v>
       </c>
       <c r="E69" s="25" t="s">
-        <v>2528</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -25369,7 +25329,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2639</v>
+        <v>2637</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -25389,7 +25349,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2640</v>
+        <v>2638</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -25419,54 +25379,54 @@
         <v>2275</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>2641</v>
+        <v>2639</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="26" t="s">
-        <v>2642</v>
+        <v>2640</v>
       </c>
       <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="26" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>2644</v>
+        <v>2642</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
       <c r="E8" s="26" t="s">
-        <v>2645</v>
+        <v>2643</v>
       </c>
       <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="26" t="s">
-        <v>2646</v>
+        <v>2644</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
       <c r="E9" s="26" t="s">
-        <v>2647</v>
+        <v>2645</v>
       </c>
       <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="26" t="s">
-        <v>2648</v>
+        <v>2646</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>2649</v>
+        <v>2647</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
       <c r="E10" s="26" t="s">
-        <v>2650</v>
+        <v>2648</v>
       </c>
       <c r="F10" s="42"/>
     </row>
@@ -25772,7 +25732,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2651</v>
+        <v>2649</v>
       </c>
       <c r="C3" s="19"/>
     </row>
@@ -25813,10 +25773,10 @@
     </row>
     <row r="7" spans="1:5" s="25" customFormat="1">
       <c r="A7" s="22" t="s">
-        <v>2652</v>
+        <v>2650</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>2653</v>
+        <v>2651</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7"/>
@@ -25824,10 +25784,10 @@
     </row>
     <row r="8" spans="1:5" s="25" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>2654</v>
+        <v>2652</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>2655</v>
+        <v>2653</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8"/>
@@ -25838,7 +25798,7 @@
         <v>2287</v>
       </c>
       <c r="B9" s="55" t="s">
-        <v>2656</v>
+        <v>2654</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9"/>
@@ -25846,10 +25806,10 @@
     </row>
     <row r="10" spans="1:5" s="25" customFormat="1">
       <c r="A10" t="s">
-        <v>2657</v>
+        <v>2655</v>
       </c>
       <c r="B10" s="55" t="s">
-        <v>2658</v>
+        <v>2656</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10"/>
@@ -25857,7 +25817,7 @@
     </row>
     <row r="11" spans="1:5" s="25" customFormat="1">
       <c r="A11" t="s">
-        <v>2659</v>
+        <v>2657</v>
       </c>
       <c r="B11" s="55" t="s">
         <v>878</v>
@@ -25868,10 +25828,10 @@
     </row>
     <row r="12" spans="1:5" s="25" customFormat="1">
       <c r="A12" t="s">
-        <v>2660</v>
+        <v>2658</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>2661</v>
+        <v>2659</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12"/>
@@ -25882,7 +25842,7 @@
         <v>199</v>
       </c>
       <c r="B13" s="55" t="s">
-        <v>2417</v>
+        <v>2415</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13"/>
@@ -25985,7 +25945,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2662</v>
+        <v>2660</v>
       </c>
       <c r="C3" s="19"/>
     </row>
@@ -26003,7 +25963,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2663</v>
+        <v>2661</v>
       </c>
       <c r="C5" s="20"/>
     </row>
@@ -26026,146 +25986,146 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="56" t="s">
-        <v>2664</v>
+        <v>2662</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>2665</v>
+        <v>2663</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="57" t="s">
-        <v>2666</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="58" t="s">
-        <v>2667</v>
+        <v>2665</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>2668</v>
+        <v>2666</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="57" t="s">
-        <v>2669</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="56" t="s">
-        <v>2460</v>
+        <v>2458</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>2670</v>
+        <v>2668</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="57" t="s">
-        <v>2671</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="56" t="s">
-        <v>2445</v>
+        <v>2443</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>2672</v>
+        <v>2670</v>
       </c>
       <c r="C10" s="33"/>
       <c r="D10" s="57" t="s">
-        <v>2673</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="56" t="s">
-        <v>2674</v>
+        <v>2672</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>2675</v>
+        <v>2673</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="57" t="s">
-        <v>2676</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="56" t="s">
-        <v>2643</v>
+        <v>2641</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>2677</v>
+        <v>2675</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="57" t="s">
-        <v>2678</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="56" t="s">
-        <v>2679</v>
+        <v>2677</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>2680</v>
+        <v>2678</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="57" t="s">
-        <v>2681</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="60" t="s">
-        <v>2682</v>
+        <v>2680</v>
       </c>
       <c r="B14" s="57" t="s">
-        <v>2683</v>
+        <v>2681</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="57" t="s">
-        <v>2683</v>
+        <v>2681</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="61" t="s">
-        <v>2684</v>
+        <v>2682</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>2685</v>
+        <v>2683</v>
       </c>
       <c r="C15" s="33"/>
       <c r="D15" s="57" t="s">
-        <v>2685</v>
+        <v>2683</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="56" t="s">
-        <v>2686</v>
+        <v>2684</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>2687</v>
+        <v>2685</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="57" t="s">
-        <v>2687</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="56" t="s">
-        <v>2688</v>
+        <v>2686</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>2689</v>
+        <v>2687</v>
       </c>
       <c r="C17" s="33"/>
       <c r="D17" s="57" t="s">
-        <v>2689</v>
+        <v>2687</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="56" t="s">
-        <v>2690</v>
+        <v>2688</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>2691</v>
+        <v>2689</v>
       </c>
       <c r="C18" s="33"/>
       <c r="D18" s="57" t="s">
-        <v>2691</v>
+        <v>2689</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -26259,7 +26219,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2692</v>
+        <v>2690</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
@@ -26279,7 +26239,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2693</v>
+        <v>2691</v>
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
@@ -26306,112 +26266,112 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>2692</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2693</v>
+      </c>
+      <c r="E7" t="s">
         <v>2694</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2695</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2696</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>2695</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2696</v>
+      </c>
+      <c r="E8" t="s">
         <v>2697</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2698</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2699</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2699</v>
+      </c>
+      <c r="E9" t="s">
         <v>2700</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2701</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2702</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>2701</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2702</v>
+      </c>
+      <c r="E10" t="s">
         <v>2703</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2704</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2705</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>2704</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2705</v>
+      </c>
+      <c r="E11" t="s">
         <v>2706</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2707</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2708</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
+        <v>2707</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2708</v>
+      </c>
+      <c r="E12" t="s">
         <v>2709</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2710</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2711</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>2710</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2711</v>
+      </c>
+      <c r="E13" t="s">
         <v>2712</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2713</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2714</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>2713</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2714</v>
+      </c>
+      <c r="E14" t="s">
         <v>2715</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2716</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2717</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>2718</v>
+        <v>2716</v>
       </c>
       <c r="B15" t="s">
-        <v>2719</v>
+        <v>2717</v>
       </c>
       <c r="E15" t="s">
-        <v>2717</v>
+        <v>2715</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>2720</v>
+        <v>2718</v>
       </c>
       <c r="B16" t="s">
-        <v>2721</v>
+        <v>2719</v>
       </c>
       <c r="E16" t="s">
-        <v>2717</v>
+        <v>2715</v>
       </c>
     </row>
   </sheetData>
@@ -26463,7 +26423,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2722</v>
+        <v>2720</v>
       </c>
       <c r="C3" s="19"/>
     </row>
@@ -26481,7 +26441,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2723</v>
+        <v>2721</v>
       </c>
       <c r="C5" s="20"/>
     </row>
@@ -26504,14 +26464,14 @@
     </row>
     <row r="7" spans="1:5" s="25" customFormat="1">
       <c r="A7" s="62" t="s">
-        <v>2724</v>
+        <v>2722</v>
       </c>
       <c r="B7" t="s">
-        <v>2725</v>
+        <v>2723</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" t="s">
-        <v>2726</v>
+        <v>2724</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -26519,14 +26479,14 @@
     </row>
     <row r="8" spans="1:5" s="25" customFormat="1">
       <c r="A8" t="s">
-        <v>2727</v>
+        <v>2725</v>
       </c>
       <c r="B8" t="s">
-        <v>2728</v>
+        <v>2726</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" t="s">
-        <v>2729</v>
+        <v>2727</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -26534,14 +26494,14 @@
     </row>
     <row r="9" spans="1:5" s="25" customFormat="1">
       <c r="A9" t="s">
-        <v>2730</v>
+        <v>2728</v>
       </c>
       <c r="B9" t="s">
-        <v>2731</v>
+        <v>2729</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" t="s">
-        <v>2732</v>
+        <v>2730</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -26549,14 +26509,14 @@
     </row>
     <row r="10" spans="1:5" s="25" customFormat="1">
       <c r="A10" t="s">
-        <v>2733</v>
+        <v>2731</v>
       </c>
       <c r="B10" t="s">
-        <v>2734</v>
+        <v>2732</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" t="s">
-        <v>2735</v>
+        <v>2733</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -26564,14 +26524,14 @@
     </row>
     <row r="11" spans="1:5" s="25" customFormat="1">
       <c r="A11" t="s">
-        <v>2736</v>
+        <v>2734</v>
       </c>
       <c r="B11" t="s">
-        <v>2737</v>
+        <v>2735</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" t="s">
-        <v>2738</v>
+        <v>2736</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -26579,14 +26539,14 @@
     </row>
     <row r="12" spans="1:5" s="25" customFormat="1">
       <c r="A12" t="s">
-        <v>2739</v>
+        <v>2737</v>
       </c>
       <c r="B12" t="s">
-        <v>2740</v>
+        <v>2738</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" t="s">
-        <v>2741</v>
+        <v>2739</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -26594,14 +26554,14 @@
     </row>
     <row r="13" spans="1:5" s="25" customFormat="1">
       <c r="A13" t="s">
-        <v>2742</v>
+        <v>2740</v>
       </c>
       <c r="B13" t="s">
-        <v>2743</v>
+        <v>2741</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" t="s">
-        <v>2744</v>
+        <v>2742</v>
       </c>
       <c r="E13">
         <v>7</v>
@@ -26609,14 +26569,14 @@
     </row>
     <row r="14" spans="1:5" s="25" customFormat="1">
       <c r="A14" t="s">
-        <v>2745</v>
+        <v>2743</v>
       </c>
       <c r="B14" t="s">
-        <v>2746</v>
+        <v>2744</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" t="s">
-        <v>2747</v>
+        <v>2745</v>
       </c>
       <c r="E14">
         <v>8</v>
@@ -26624,14 +26584,14 @@
     </row>
     <row r="15" spans="1:5" s="25" customFormat="1">
       <c r="A15" t="s">
-        <v>2748</v>
+        <v>2746</v>
       </c>
       <c r="B15" t="s">
-        <v>2749</v>
+        <v>2747</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" t="s">
-        <v>2750</v>
+        <v>2748</v>
       </c>
       <c r="E15">
         <v>9</v>
@@ -26639,14 +26599,14 @@
     </row>
     <row r="16" spans="1:5" s="25" customFormat="1">
       <c r="A16" t="s">
-        <v>2751</v>
+        <v>2749</v>
       </c>
       <c r="B16" t="s">
-        <v>2752</v>
+        <v>2750</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" t="s">
-        <v>2753</v>
+        <v>2751</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -26654,13 +26614,13 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2753</v>
+      </c>
+      <c r="D17" t="s">
         <v>2754</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2755</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2756</v>
       </c>
       <c r="E17">
         <v>11</v>
@@ -26727,7 +26687,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2757</v>
+        <v>2755</v>
       </c>
       <c r="C3" s="19"/>
     </row>
@@ -26745,7 +26705,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2758</v>
+        <v>2756</v>
       </c>
       <c r="C5" s="20"/>
     </row>
@@ -26768,14 +26728,14 @@
     </row>
     <row r="7" spans="1:5" s="25" customFormat="1">
       <c r="A7" s="22" t="s">
-        <v>2759</v>
+        <v>2757</v>
       </c>
       <c r="B7" t="s">
-        <v>2760</v>
+        <v>2758</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" t="s">
-        <v>2761</v>
+        <v>2759</v>
       </c>
       <c r="E7"/>
     </row>
@@ -26996,7 +26956,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2762</v>
+        <v>2760</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="19"/>
@@ -27016,7 +26976,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2763</v>
+        <v>2761</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="20"/>
@@ -27043,57 +27003,57 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="63" t="s">
-        <v>2764</v>
+        <v>2762</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>2764</v>
+        <v>2762</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="26" t="s">
-        <v>2765</v>
+        <v>2763</v>
       </c>
       <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="56" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="B8" s="56" t="s">
-        <v>2766</v>
+        <v>2764</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
       <c r="E8" s="26" t="s">
-        <v>2767</v>
+        <v>2765</v>
       </c>
       <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="56" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>2768</v>
+        <v>2766</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
       <c r="E9" s="26" t="s">
-        <v>2769</v>
+        <v>2767</v>
       </c>
       <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="56" t="s">
-        <v>2770</v>
+        <v>2768</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>2770</v>
+        <v>2768</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
       <c r="E10" s="26" t="s">
-        <v>2771</v>
+        <v>2769</v>
       </c>
       <c r="F10" s="42"/>
     </row>
@@ -27402,7 +27362,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2772</v>
+        <v>2770</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
@@ -27422,7 +27382,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2773</v>
+        <v>2771</v>
       </c>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
@@ -27449,234 +27409,234 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>2772</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>2773</v>
+      </c>
+      <c r="E7" t="s">
         <v>2774</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="F7" t="s">
         <v>2775</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2776</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2777</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
+        <v>2776</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>2777</v>
+      </c>
+      <c r="E8" s="75" t="s">
         <v>2778</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>2779</v>
-      </c>
-      <c r="E8" s="75" t="s">
-        <v>2780</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75">
       <c r="A9" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>2780</v>
+      </c>
+      <c r="E9" s="76" t="s">
         <v>2781</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="F9" t="s">
         <v>2782</v>
-      </c>
-      <c r="E9" s="76" t="s">
-        <v>2783</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2784</v>
       </c>
       <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15.75">
       <c r="A10" t="s">
+        <v>2783</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2784</v>
+      </c>
+      <c r="E10" s="69" t="s">
         <v>2785</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2786</v>
-      </c>
-      <c r="E10" s="69" t="s">
-        <v>2787</v>
       </c>
       <c r="G10" s="54"/>
     </row>
     <row r="11" spans="1:7" ht="15.75">
       <c r="A11" t="s">
+        <v>2786</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>2787</v>
+      </c>
+      <c r="E11" s="69" t="s">
         <v>2788</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="F11" t="s">
         <v>2789</v>
-      </c>
-      <c r="E11" s="69" t="s">
-        <v>2790</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2791</v>
       </c>
       <c r="G11" s="64"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
+        <v>2790</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>2791</v>
+      </c>
+      <c r="E12" s="69" t="s">
         <v>2792</v>
-      </c>
-      <c r="B12" s="57" t="s">
-        <v>2793</v>
-      </c>
-      <c r="E12" s="69" t="s">
-        <v>2794</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>2795</v>
+        <v>2793</v>
       </c>
       <c r="B13" t="s">
-        <v>2796</v>
+        <v>2794</v>
       </c>
       <c r="C13" s="57"/>
       <c r="E13" s="69" t="s">
-        <v>2797</v>
+        <v>2795</v>
       </c>
       <c r="F13" t="s">
-        <v>2798</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="69" customFormat="1">
       <c r="A14" s="71" t="s">
-        <v>2799</v>
+        <v>2797</v>
       </c>
       <c r="B14" s="72" t="s">
-        <v>2800</v>
+        <v>2798</v>
       </c>
       <c r="C14" s="73"/>
       <c r="E14" s="75" t="s">
-        <v>2801</v>
+        <v>2799</v>
       </c>
       <c r="F14" s="74"/>
       <c r="G14" s="74"/>
     </row>
     <row r="15" spans="1:7" ht="15.75">
       <c r="A15" t="s">
+        <v>2800</v>
+      </c>
+      <c r="B15" s="57" t="s">
+        <v>2801</v>
+      </c>
+      <c r="E15" s="69" t="s">
         <v>2802</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="F15" t="s">
         <v>2803</v>
-      </c>
-      <c r="E15" s="69" t="s">
-        <v>2804</v>
-      </c>
-      <c r="F15" t="s">
-        <v>2805</v>
       </c>
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
+        <v>2804</v>
+      </c>
+      <c r="B16" s="57" t="s">
+        <v>2805</v>
+      </c>
+      <c r="E16" s="75" t="s">
         <v>2806</v>
-      </c>
-      <c r="B16" s="57" t="s">
-        <v>2807</v>
-      </c>
-      <c r="E16" s="75" t="s">
-        <v>2808</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>2807</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>2808</v>
+      </c>
+      <c r="E17" s="75" t="s">
         <v>2809</v>
-      </c>
-      <c r="B17" s="57" t="s">
-        <v>2810</v>
-      </c>
-      <c r="E17" s="75" t="s">
-        <v>2811</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75">
       <c r="A18" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B18" s="57" t="s">
+        <v>2811</v>
+      </c>
+      <c r="E18" s="75" t="s">
         <v>2812</v>
-      </c>
-      <c r="B18" s="57" t="s">
-        <v>2813</v>
-      </c>
-      <c r="E18" s="75" t="s">
-        <v>2814</v>
       </c>
       <c r="G18" s="64"/>
     </row>
     <row r="19" spans="1:7" ht="15.75">
       <c r="A19" t="s">
+        <v>2813</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>2814</v>
+      </c>
+      <c r="E19" s="75" t="s">
         <v>2815</v>
-      </c>
-      <c r="B19" s="57" t="s">
-        <v>2816</v>
-      </c>
-      <c r="E19" s="75" t="s">
-        <v>2817</v>
       </c>
       <c r="G19" s="64"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>2817</v>
+      </c>
+      <c r="E20" s="69" t="s">
         <v>2818</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="F20" t="s">
         <v>2819</v>
-      </c>
-      <c r="E20" s="69" t="s">
-        <v>2820</v>
-      </c>
-      <c r="F20" t="s">
-        <v>2821</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>2821</v>
+      </c>
+      <c r="E21" s="69" t="s">
         <v>2822</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="F21" t="s">
         <v>2823</v>
-      </c>
-      <c r="E21" s="69" t="s">
-        <v>2824</v>
-      </c>
-      <c r="F21" t="s">
-        <v>2825</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
+        <v>2824</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>2825</v>
+      </c>
+      <c r="E22" s="69" t="s">
         <v>2826</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="F22" t="s">
         <v>2827</v>
-      </c>
-      <c r="E22" s="69" t="s">
-        <v>2828</v>
-      </c>
-      <c r="F22" t="s">
-        <v>2829</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>2828</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>2829</v>
+      </c>
+      <c r="E23" s="69" t="s">
         <v>2830</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>2831</v>
-      </c>
-      <c r="E23" s="69" t="s">
-        <v>2832</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
+        <v>2831</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2832</v>
+      </c>
+      <c r="E24" t="s">
         <v>2833</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2834</v>
-      </c>
-      <c r="E24" t="s">
-        <v>2835</v>
       </c>
     </row>
   </sheetData>
@@ -27707,7 +27667,7 @@
         <v>107</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
       <c r="C1" s="19"/>
     </row>
@@ -27725,7 +27685,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2896</v>
+        <v>2894</v>
       </c>
       <c r="C3" s="19"/>
     </row>
@@ -27743,7 +27703,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
       <c r="C5" s="20"/>
     </row>
@@ -27766,66 +27726,66 @@
     </row>
     <row r="7" spans="1:5" s="25" customFormat="1">
       <c r="A7" s="22" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="25" t="s">
-        <v>2895</v>
+        <v>2893</v>
       </c>
       <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" s="25" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
       <c r="C8" s="22"/>
       <c r="D8" s="25" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
       <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" s="25" customFormat="1">
       <c r="A9" s="22" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="25" t="s">
-        <v>2899</v>
+        <v>2897</v>
       </c>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:5" s="25" customFormat="1">
       <c r="A10" s="22" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="25" t="s">
-        <v>2901</v>
+        <v>2899</v>
       </c>
       <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" s="25" customFormat="1">
       <c r="A11" s="22" t="s">
-        <v>2889</v>
+        <v>2887</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="25" t="s">
-        <v>2893</v>
+        <v>2891</v>
       </c>
       <c r="E11" s="24"/>
     </row>
@@ -28611,7 +28571,7 @@
         <v>110</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -28631,7 +28591,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="C5" s=